<commit_message>
TTD JatA ParaayaNam as of 14/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -146,6 +146,81 @@
   </si>
   <si>
     <t>samhitA</t>
+  </si>
+  <si>
+    <t>1.2.11.1</t>
+  </si>
+  <si>
+    <t>1.2.12.1</t>
+  </si>
+  <si>
+    <t>1.2.13.1</t>
+  </si>
+  <si>
+    <t>1.2.14.6</t>
+  </si>
+  <si>
+    <t>13/07/2020</t>
+  </si>
+  <si>
+    <t>1.2.14.7</t>
+  </si>
+  <si>
+    <t>1.3.1.1</t>
+  </si>
+  <si>
+    <t>1.3.2.1</t>
+  </si>
+  <si>
+    <t>1.3.3.1</t>
+  </si>
+  <si>
+    <t>1.3.4.1</t>
+  </si>
+  <si>
+    <t>1.3.5.1</t>
+  </si>
+  <si>
+    <t>1.3.6.1</t>
+  </si>
+  <si>
+    <t>1.3.7.1</t>
+  </si>
+  <si>
+    <t>14/07/2020</t>
+  </si>
+  <si>
+    <t>1.3.8.1</t>
+  </si>
+  <si>
+    <t>1.3.9.1</t>
+  </si>
+  <si>
+    <t>1.3.10.1</t>
+  </si>
+  <si>
+    <t>1.3.11.1</t>
+  </si>
+  <si>
+    <t>1.3.12.1</t>
+  </si>
+  <si>
+    <t>1.3.13.1</t>
+  </si>
+  <si>
+    <t>1.3.14.1</t>
+  </si>
+  <si>
+    <t>upto 1.3.14.4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hPGh9CKobF8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4CipAIdR0nU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LT9kGdY_iUo</t>
   </si>
 </sst>
 </file>
@@ -200,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -212,6 +287,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,8 +598,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -527,9 +609,9 @@
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.77734375" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="42.33203125" customWidth="1"/>
   </cols>
@@ -540,16 +622,16 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -571,16 +653,16 @@
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="3"/>
@@ -604,10 +686,10 @@
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="6">
         <v>5.0199999999999996</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="6">
         <v>8.44</v>
       </c>
       <c r="H7" s="1"/>
@@ -628,10 +710,10 @@
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="6">
         <v>8.44</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="6">
         <v>14.48</v>
       </c>
       <c r="H8" s="1"/>
@@ -650,10 +732,10 @@
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="6">
         <v>14.48</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="6">
         <v>19.16</v>
       </c>
       <c r="H9" s="1"/>
@@ -672,10 +754,10 @@
       <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="6">
         <v>19.16</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="6">
         <v>26.04</v>
       </c>
       <c r="H10" s="1"/>
@@ -694,10 +776,10 @@
       <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="6">
         <v>26.04</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="6">
         <v>33.380000000000003</v>
       </c>
       <c r="H11" s="1"/>
@@ -712,8 +794,8 @@
       <c r="C12" s="1"/>
       <c r="D12" s="4"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -740,7 +822,7 @@
       <c r="F13" s="6">
         <v>2.5</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="6">
         <v>7.39</v>
       </c>
       <c r="H13" s="1"/>
@@ -761,7 +843,7 @@
       <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="6">
         <v>7.39</v>
       </c>
       <c r="G14" s="6">
@@ -786,7 +868,7 @@
       <c r="F15" s="6">
         <v>14.3</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="6">
         <v>19.52</v>
       </c>
       <c r="H15" s="1"/>
@@ -805,10 +887,10 @@
       <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="6">
         <v>19.52</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="6">
         <v>30.56</v>
       </c>
       <c r="H16" s="1"/>
@@ -827,10 +909,10 @@
       <c r="E17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="6">
         <v>30.56</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="6">
         <v>43.12</v>
       </c>
       <c r="H17" s="1"/>
@@ -849,10 +931,10 @@
       <c r="E18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="6">
         <v>43.12</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="6">
         <v>52.12</v>
       </c>
       <c r="H18" s="1"/>
@@ -865,10 +947,10 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="4"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -892,10 +974,10 @@
       <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="6">
         <v>1.36</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="6">
         <v>6.06</v>
       </c>
       <c r="H20" s="1"/>
@@ -916,11 +998,11 @@
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="6">
         <f>+G20</f>
         <v>6.06</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="6">
         <v>16.29</v>
       </c>
       <c r="H21" s="1"/>
@@ -939,11 +1021,11 @@
       <c r="E22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="6">
         <f t="shared" ref="F22:F25" si="0">+G21</f>
         <v>16.29</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="6">
         <v>29.49</v>
       </c>
       <c r="H22" s="1"/>
@@ -962,11 +1044,11 @@
       <c r="E23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="6">
         <f t="shared" si="0"/>
         <v>29.49</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="6">
         <v>36.57</v>
       </c>
       <c r="H23" s="1"/>
@@ -985,11 +1067,11 @@
       <c r="E24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="6">
         <f t="shared" si="0"/>
         <v>36.57</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="6">
         <v>45.53</v>
       </c>
       <c r="H24" s="1"/>
@@ -1008,11 +1090,11 @@
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="6">
         <f t="shared" si="0"/>
         <v>45.53</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="6">
         <v>49.18</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -1027,10 +1109,10 @@
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="D26" s="4"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1055,7 +1137,7 @@
       <c r="F27" s="6">
         <v>5</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="6">
         <v>12.23</v>
       </c>
       <c r="H27" s="1"/>
@@ -1077,11 +1159,11 @@
       <c r="E28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="6">
         <f>+G27</f>
         <v>12.23</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="6">
         <v>18.510000000000002</v>
       </c>
       <c r="H28" s="1"/>
@@ -1101,11 +1183,11 @@
       <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="6">
         <f t="shared" ref="F29:F34" si="2">+G28</f>
         <v>18.510000000000002</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="6">
         <v>23.47</v>
       </c>
       <c r="H29" s="1"/>
@@ -1125,11 +1207,11 @@
       <c r="E30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="6">
         <f t="shared" si="2"/>
         <v>23.47</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="6">
         <v>27.34</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -1151,10 +1233,10 @@
       <c r="E31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="6">
         <v>28.52</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="6">
         <v>34.01</v>
       </c>
       <c r="I31" s="1"/>
@@ -1173,11 +1255,11 @@
       <c r="E32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="6">
         <f t="shared" si="2"/>
         <v>34.01</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="6">
         <v>39.36</v>
       </c>
       <c r="H32" s="1"/>
@@ -1187,7 +1269,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="4">
@@ -1197,11 +1279,11 @@
       <c r="E33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="6">
         <f t="shared" si="2"/>
         <v>39.36</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="6">
         <v>44.39</v>
       </c>
       <c r="H33" s="1"/>
@@ -1211,7 +1293,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="4">
@@ -1221,11 +1303,11 @@
       <c r="E34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="6">
         <f t="shared" si="2"/>
         <v>44.39</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="6">
         <v>51.52</v>
       </c>
       <c r="H34" s="1"/>
@@ -1235,13 +1317,13 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="D35" s="4"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1249,27 +1331,54 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2">
+        <v>44172</v>
+      </c>
+      <c r="C36" s="1">
+        <v>55.25</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="6">
+        <v>7.33</v>
+      </c>
+      <c r="G36" s="6">
+        <v>13.1</v>
+      </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="D37" s="4">
+        <f>+D36+1</f>
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="6">
+        <f>+G36</f>
+        <v>13.1</v>
+      </c>
+      <c r="G37" s="6">
+        <v>23.04</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -1277,13 +1386,23 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+      <c r="D38" s="4">
+        <f t="shared" ref="D38:D40" si="3">+D37+1</f>
+        <v>3</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="6">
+        <f t="shared" ref="F38:F40" si="4">+G37</f>
+        <v>23.04</v>
+      </c>
+      <c r="G38" s="6">
+        <v>32.42</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -1291,13 +1410,23 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="D39" s="4">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" s="6">
+        <f t="shared" si="4"/>
+        <v>32.42</v>
+      </c>
+      <c r="G39" s="6">
+        <v>51.4</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -1305,13 +1434,13 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
+      <c r="D40" s="4"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -1319,27 +1448,54 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="1">
+        <v>58.07</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="6">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="G41" s="6">
+        <v>7.05</v>
+      </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="I41" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="D42" s="4">
+        <f>+D41+1</f>
+        <v>2</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="6">
+        <f>+G41</f>
+        <v>7.05</v>
+      </c>
+      <c r="G42" s="6">
+        <v>15.42</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -1347,13 +1503,23 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="D43" s="4">
+        <f t="shared" ref="D43:D48" si="5">+D42+1</f>
+        <v>3</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F43" s="6">
+        <f t="shared" ref="F43:F48" si="6">+G42</f>
+        <v>15.42</v>
+      </c>
+      <c r="G43" s="6">
+        <v>24.17</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -1361,13 +1527,23 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="D44" s="4">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="6">
+        <f t="shared" si="6"/>
+        <v>24.17</v>
+      </c>
+      <c r="G44" s="6">
+        <v>27.47</v>
+      </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -1375,13 +1551,23 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="D45" s="4">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F45" s="6">
+        <f t="shared" si="6"/>
+        <v>27.47</v>
+      </c>
+      <c r="G45" s="6">
+        <v>37.08</v>
+      </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -1389,13 +1575,23 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="D46" s="4">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="6">
+        <f t="shared" si="6"/>
+        <v>37.08</v>
+      </c>
+      <c r="G46" s="6">
+        <v>41.1</v>
+      </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -1403,13 +1599,23 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="D47" s="4">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F47" s="6">
+        <f t="shared" si="6"/>
+        <v>41.1</v>
+      </c>
+      <c r="G47" s="6">
+        <v>49.11</v>
+      </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -1417,13 +1623,23 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
+      <c r="D48" s="4">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F48" s="6">
+        <f t="shared" si="6"/>
+        <v>49.11</v>
+      </c>
+      <c r="G48" s="6">
+        <v>54.26</v>
+      </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -1431,13 +1647,13 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
+      <c r="D49" s="4"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -1445,27 +1661,54 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="1">
+        <v>56.28</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F50" s="6">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="G50" s="6">
+        <v>11.48</v>
+      </c>
       <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
+      <c r="I50" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="D51" s="4">
+        <f>+D50+1</f>
+        <v>2</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" s="6">
+        <f t="shared" ref="F51:F56" si="7">+G50</f>
+        <v>11.48</v>
+      </c>
+      <c r="G51" s="6">
+        <v>18.12</v>
+      </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -1473,13 +1716,23 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="D52" s="4">
+        <f t="shared" ref="D52:D56" si="8">+D51+1</f>
+        <v>3</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F52" s="6">
+        <f t="shared" si="7"/>
+        <v>18.12</v>
+      </c>
+      <c r="G52" s="6">
+        <v>24.08</v>
+      </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
@@ -1487,13 +1740,23 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="D53" s="4">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F53" s="6">
+        <f t="shared" si="7"/>
+        <v>24.08</v>
+      </c>
+      <c r="G53" s="6">
+        <v>29.13</v>
+      </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -1501,13 +1764,23 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
+      <c r="D54" s="4">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F54" s="6">
+        <f t="shared" si="7"/>
+        <v>29.13</v>
+      </c>
+      <c r="G54" s="6">
+        <v>32.14</v>
+      </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -1515,13 +1788,23 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="D55" s="4">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F55" s="6">
+        <f t="shared" si="7"/>
+        <v>32.14</v>
+      </c>
+      <c r="G55" s="6">
+        <v>39.090000000000003</v>
+      </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
@@ -1529,27 +1812,39 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
+      <c r="D56" s="4">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" s="6">
+        <f t="shared" si="7"/>
+        <v>39.090000000000003</v>
+      </c>
+      <c r="G56" s="6">
+        <v>50.43</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+      <c r="D57" s="4"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -1557,13 +1852,13 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
+      <c r="D58" s="4"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -1571,13 +1866,13 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="D59" s="4"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -1585,13 +1880,13 @@
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
+      <c r="D60" s="4"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -1599,13 +1894,13 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+      <c r="D61" s="4"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -1613,13 +1908,13 @@
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
+      <c r="D62" s="4"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -1627,13 +1922,13 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
+      <c r="D63" s="4"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -1641,13 +1936,13 @@
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
+      <c r="D64" s="4"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -1658,10 +1953,10 @@
     <row r="65" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
+      <c r="D65" s="4"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
@@ -1672,10 +1967,10 @@
     <row r="66" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="D66" s="4"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
@@ -1686,10 +1981,10 @@
     <row r="67" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+      <c r="D67" s="4"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -1700,10 +1995,10 @@
     <row r="68" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+      <c r="D68" s="4"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -1714,10 +2009,10 @@
     <row r="69" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="D69" s="4"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
@@ -1728,10 +2023,10 @@
     <row r="70" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
+      <c r="D70" s="4"/>
       <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
@@ -1742,10 +2037,10 @@
     <row r="71" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
+      <c r="D71" s="4"/>
       <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
@@ -1756,10 +2051,10 @@
     <row r="72" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+      <c r="D72" s="4"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
@@ -1770,10 +2065,10 @@
     <row r="73" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+      <c r="D73" s="4"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -1784,10 +2079,10 @@
     <row r="74" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+      <c r="D74" s="4"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
@@ -1798,10 +2093,10 @@
     <row r="75" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
+      <c r="D75" s="4"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
@@ -1812,10 +2107,10 @@
     <row r="76" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
+      <c r="D76" s="4"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -1826,10 +2121,10 @@
     <row r="77" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
+      <c r="D77" s="4"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
@@ -1840,10 +2135,10 @@
     <row r="78" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
+      <c r="D78" s="4"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
@@ -1854,10 +2149,10 @@
     <row r="79" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
+      <c r="D79" s="4"/>
       <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
@@ -1868,10 +2163,10 @@
     <row r="80" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
+      <c r="D80" s="4"/>
       <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
@@ -1882,10 +2177,10 @@
     <row r="81" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
+      <c r="D81" s="4"/>
       <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -1896,10 +2191,10 @@
     <row r="82" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
+      <c r="D82" s="4"/>
       <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -1910,10 +2205,10 @@
     <row r="83" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
+      <c r="D83" s="4"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -1924,10 +2219,10 @@
     <row r="84" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
+      <c r="D84" s="4"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>

</xml_diff>

<commit_message>
TS 1.1 Files with Kampam pushed 15/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=LT9kGdY_iUo</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>Archieve.org =52.08</t>
   </si>
 </sst>
 </file>
@@ -249,7 +255,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +265,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -292,6 +304,7 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,7 +614,7 @@
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -782,8 +795,12 @@
       <c r="G11" s="6">
         <v>33.380000000000003</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="H11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1390,14 +1407,14 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="4">
-        <f t="shared" ref="D38:D40" si="3">+D37+1</f>
+        <f t="shared" ref="D38:D39" si="3">+D37+1</f>
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>46</v>
       </c>
       <c r="F38" s="6">
-        <f t="shared" ref="F38:F40" si="4">+G37</f>
+        <f t="shared" ref="F38:F39" si="4">+G37</f>
         <v>23.04</v>
       </c>
       <c r="G38" s="6">

</xml_diff>

<commit_message>
TS Jata Darapanam and other files 18/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -654,9 +654,9 @@
   <dimension ref="A4:M84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
+      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Jata Working as of 19/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="126">
   <si>
     <t>Date</t>
   </si>
@@ -268,7 +268,130 @@
     <t>1.4.11.1</t>
   </si>
   <si>
-    <t>55.3.1</t>
+    <t>16/07/2020</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LuXq5_W4nfw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-4tnrZNPY58</t>
+  </si>
+  <si>
+    <t>1.4.12.1</t>
+  </si>
+  <si>
+    <t>1.4.13.1</t>
+  </si>
+  <si>
+    <t>1.4.14.1</t>
+  </si>
+  <si>
+    <t>1.4.16.1</t>
+  </si>
+  <si>
+    <t>1.4.17.1</t>
+  </si>
+  <si>
+    <t>1.4.15.1</t>
+  </si>
+  <si>
+    <t>1.4.18.1</t>
+  </si>
+  <si>
+    <t>1.4.19.1</t>
+  </si>
+  <si>
+    <t>1.4.20.1</t>
+  </si>
+  <si>
+    <t>1.4.21.1</t>
+  </si>
+  <si>
+    <t>1.4.22.1</t>
+  </si>
+  <si>
+    <t>1.4.23.1</t>
+  </si>
+  <si>
+    <t>1.4.24.1</t>
+  </si>
+  <si>
+    <t>1.4.25.1</t>
+  </si>
+  <si>
+    <t>1.4.26.1</t>
+  </si>
+  <si>
+    <t>1.4.27.1</t>
+  </si>
+  <si>
+    <t>1.4.28.1</t>
+  </si>
+  <si>
+    <t>1.4.29.1</t>
+  </si>
+  <si>
+    <t>1.4.30.1</t>
+  </si>
+  <si>
+    <t>1.4.31.1</t>
+  </si>
+  <si>
+    <t>1.4.32.1</t>
+  </si>
+  <si>
+    <t>1.4.33.1</t>
+  </si>
+  <si>
+    <t>1.4.34.1</t>
+  </si>
+  <si>
+    <t>1.4.35.1</t>
+  </si>
+  <si>
+    <t>1.4.36.1</t>
+  </si>
+  <si>
+    <t>1.4.37.1</t>
+  </si>
+  <si>
+    <t>1.4.38.1</t>
+  </si>
+  <si>
+    <t>1.4.39.1</t>
+  </si>
+  <si>
+    <t>17/07/2020</t>
+  </si>
+  <si>
+    <t>1.4.40.1</t>
+  </si>
+  <si>
+    <t>1.4.41.1</t>
+  </si>
+  <si>
+    <t>1.4.42.1</t>
+  </si>
+  <si>
+    <t>1.4.43.1</t>
+  </si>
+  <si>
+    <t>1.4.44.1</t>
+  </si>
+  <si>
+    <t>1.4.45.1</t>
+  </si>
+  <si>
+    <t>1.4.46.1</t>
+  </si>
+  <si>
+    <t>cut 1 jatai</t>
+  </si>
+  <si>
+    <t>18/07/2020</t>
+  </si>
+  <si>
+    <t>TTD</t>
   </si>
 </sst>
 </file>
@@ -297,7 +420,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +439,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -329,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -347,6 +476,7 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,12 +781,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:M84"/>
+  <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -974,7 +1104,9 @@
       <c r="G17" s="6">
         <v>43.12</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1918,8 +2050,8 @@
       <c r="B58" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>84</v>
+      <c r="C58" s="1">
+        <v>55.31</v>
       </c>
       <c r="D58" s="4">
         <v>1</v>
@@ -1934,7 +2066,9 @@
         <v>19.57</v>
       </c>
       <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
+      <c r="I58" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -2084,7 +2218,7 @@
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="4">
@@ -2108,7 +2242,7 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="4">
@@ -2132,7 +2266,7 @@
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="4">
@@ -2156,7 +2290,7 @@
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="4">
@@ -2180,7 +2314,7 @@
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="4">
@@ -2204,7 +2338,7 @@
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="4"/>
@@ -2218,27 +2352,54 @@
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>6</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" s="1">
+        <v>56.28</v>
+      </c>
+      <c r="D71" s="4">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F71" s="6">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="G71" s="6">
+        <v>5.59</v>
+      </c>
       <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
+      <c r="I71" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
+      <c r="D72" s="4">
+        <f>+D71+1</f>
+        <v>2</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F72" s="6">
+        <f>+G71</f>
+        <v>5.59</v>
+      </c>
+      <c r="G72" s="6">
+        <v>9.0399999999999991</v>
+      </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
@@ -2246,13 +2407,23 @@
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
+      <c r="D73" s="4">
+        <f t="shared" ref="D73:D106" si="11">+D72+1</f>
+        <v>3</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F73" s="6">
+        <f t="shared" ref="F73:F106" si="12">+G72</f>
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="G73" s="6">
+        <v>10.5</v>
+      </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -2260,13 +2431,23 @@
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
+      <c r="D74" s="4">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F74" s="6">
+        <f t="shared" si="12"/>
+        <v>10.5</v>
+      </c>
+      <c r="G74" s="6">
+        <v>12.28</v>
+      </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
@@ -2274,13 +2455,23 @@
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
+      <c r="D75" s="4">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F75" s="6">
+        <f t="shared" si="12"/>
+        <v>12.28</v>
+      </c>
+      <c r="G75" s="6">
+        <v>14.01</v>
+      </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
@@ -2288,13 +2479,23 @@
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
+      <c r="D76" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F76" s="6">
+        <f t="shared" si="12"/>
+        <v>14.01</v>
+      </c>
+      <c r="G76" s="6">
+        <v>15.53</v>
+      </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -2302,13 +2503,23 @@
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
+      <c r="D77" s="4">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F77" s="6">
+        <f t="shared" si="12"/>
+        <v>15.53</v>
+      </c>
+      <c r="G77" s="6">
+        <v>17.46</v>
+      </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
@@ -2316,13 +2527,23 @@
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
+      <c r="D78" s="4">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F78" s="6">
+        <f t="shared" si="12"/>
+        <v>17.46</v>
+      </c>
+      <c r="G78" s="6">
+        <v>19.41</v>
+      </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
@@ -2330,13 +2551,23 @@
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
+      <c r="D79" s="4">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F79" s="6">
+        <f t="shared" si="12"/>
+        <v>19.41</v>
+      </c>
+      <c r="G79" s="6">
+        <v>21.08</v>
+      </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
@@ -2344,13 +2575,23 @@
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
+      <c r="D80" s="4">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F80" s="6">
+        <f t="shared" si="12"/>
+        <v>21.08</v>
+      </c>
+      <c r="G80" s="6">
+        <v>23.18</v>
+      </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
@@ -2361,10 +2602,20 @@
     <row r="81" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
+      <c r="D81" s="4">
+        <f t="shared" si="11"/>
+        <v>11</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F81" s="6">
+        <f t="shared" si="12"/>
+        <v>23.18</v>
+      </c>
+      <c r="G81" s="6">
+        <v>27.5</v>
+      </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -2375,10 +2626,20 @@
     <row r="82" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
+      <c r="D82" s="4">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F82" s="6">
+        <f t="shared" si="12"/>
+        <v>27.5</v>
+      </c>
+      <c r="G82" s="6">
+        <v>29.24</v>
+      </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -2389,10 +2650,20 @@
     <row r="83" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="6"/>
-      <c r="G83" s="6"/>
+      <c r="D83" s="4">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F83" s="6">
+        <f t="shared" si="12"/>
+        <v>29.24</v>
+      </c>
+      <c r="G83" s="6">
+        <v>30.55</v>
+      </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -2403,10 +2674,20 @@
     <row r="84" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
+      <c r="D84" s="4">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F84" s="6">
+        <f t="shared" si="12"/>
+        <v>30.55</v>
+      </c>
+      <c r="G84" s="6">
+        <v>31.52</v>
+      </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
@@ -2414,6 +2695,2092 @@
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
     </row>
+    <row r="85" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D85" s="4">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F85" s="6">
+        <f t="shared" si="12"/>
+        <v>31.52</v>
+      </c>
+      <c r="G85" s="6">
+        <v>32.44</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D86" s="4">
+        <f t="shared" si="11"/>
+        <v>16</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F86" s="6">
+        <f t="shared" si="12"/>
+        <v>32.44</v>
+      </c>
+      <c r="G86" s="6">
+        <v>34.42</v>
+      </c>
+    </row>
+    <row r="87" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D87" s="4">
+        <f t="shared" si="11"/>
+        <v>17</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F87" s="6">
+        <f t="shared" si="12"/>
+        <v>34.42</v>
+      </c>
+      <c r="G87" s="6">
+        <v>37.020000000000003</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D88" s="4">
+        <f t="shared" si="11"/>
+        <v>18</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F88" s="6">
+        <f t="shared" si="12"/>
+        <v>37.020000000000003</v>
+      </c>
+      <c r="G88" s="6">
+        <v>38.24</v>
+      </c>
+    </row>
+    <row r="89" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D89" s="4">
+        <f t="shared" si="11"/>
+        <v>19</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F89" s="6">
+        <f t="shared" si="12"/>
+        <v>38.24</v>
+      </c>
+      <c r="G89" s="6">
+        <v>39.479999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D90" s="4">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F90" s="6">
+        <f t="shared" si="12"/>
+        <v>39.479999999999997</v>
+      </c>
+      <c r="G90" s="6">
+        <v>41.14</v>
+      </c>
+    </row>
+    <row r="91" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D91" s="4">
+        <f t="shared" si="11"/>
+        <v>21</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F91" s="6">
+        <f t="shared" si="12"/>
+        <v>41.14</v>
+      </c>
+      <c r="G91" s="6">
+        <v>41.49</v>
+      </c>
+    </row>
+    <row r="92" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D92" s="4">
+        <f t="shared" si="11"/>
+        <v>22</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F92" s="6">
+        <f t="shared" si="12"/>
+        <v>41.49</v>
+      </c>
+      <c r="G92" s="6">
+        <v>43.08</v>
+      </c>
+    </row>
+    <row r="93" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D93" s="4">
+        <f t="shared" si="11"/>
+        <v>23</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F93" s="6">
+        <f t="shared" si="12"/>
+        <v>43.08</v>
+      </c>
+      <c r="G93" s="6">
+        <v>46.09</v>
+      </c>
+    </row>
+    <row r="94" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D94" s="4">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F94" s="6">
+        <f t="shared" si="12"/>
+        <v>46.09</v>
+      </c>
+      <c r="G94" s="6">
+        <v>48.37</v>
+      </c>
+    </row>
+    <row r="95" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D95" s="4">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F95" s="6">
+        <f t="shared" si="12"/>
+        <v>48.37</v>
+      </c>
+      <c r="G95" s="6">
+        <v>50.39</v>
+      </c>
+    </row>
+    <row r="96" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D96" s="4">
+        <f t="shared" si="11"/>
+        <v>26</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F96" s="6">
+        <f t="shared" si="12"/>
+        <v>50.39</v>
+      </c>
+      <c r="G96" s="6">
+        <v>52.16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>7</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C98" s="1">
+        <v>50.24</v>
+      </c>
+      <c r="D98" s="4">
+        <v>1</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F98" s="6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G98" s="6">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="4">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F99" s="6">
+        <f t="shared" si="12"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="G99" s="6">
+        <v>3.52</v>
+      </c>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="4">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F100" s="6">
+        <f t="shared" si="12"/>
+        <v>3.52</v>
+      </c>
+      <c r="G100" s="6">
+        <v>5.56</v>
+      </c>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="4">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F101" s="6">
+        <f t="shared" si="12"/>
+        <v>5.56</v>
+      </c>
+      <c r="G101" s="6">
+        <v>7.56</v>
+      </c>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="4">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F102" s="6">
+        <f t="shared" si="12"/>
+        <v>7.56</v>
+      </c>
+      <c r="G102" s="6">
+        <v>10.06</v>
+      </c>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="4">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F103" s="6">
+        <f t="shared" si="12"/>
+        <v>10.06</v>
+      </c>
+      <c r="G103" s="6">
+        <v>18.149999999999999</v>
+      </c>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="4">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F104" s="6">
+        <f t="shared" si="12"/>
+        <v>18.149999999999999</v>
+      </c>
+      <c r="G104" s="6">
+        <v>27.26</v>
+      </c>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="4">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F105" s="6">
+        <f t="shared" si="12"/>
+        <v>27.26</v>
+      </c>
+      <c r="G105" s="6">
+        <v>37.22</v>
+      </c>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="4">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F106" s="6">
+        <f t="shared" si="12"/>
+        <v>37.22</v>
+      </c>
+      <c r="G106" s="6">
+        <v>47.51</v>
+      </c>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>8</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="4">
+        <v>1</v>
+      </c>
+      <c r="E108" s="1"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="1"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+    </row>
+    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="1"/>
+      <c r="I129" s="1"/>
+    </row>
+    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="6"/>
+      <c r="G136" s="6"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
+    </row>
+    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="6"/>
+      <c r="G137" s="6"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="6"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="1"/>
+      <c r="I140" s="1"/>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="6"/>
+      <c r="G141" s="6"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
+    </row>
+    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B142" s="1"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
+    </row>
+    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="1"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="1"/>
+    </row>
+    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="1"/>
+      <c r="F144" s="6"/>
+      <c r="G144" s="6"/>
+      <c r="H144" s="1"/>
+      <c r="I144" s="1"/>
+    </row>
+    <row r="145" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B145" s="1"/>
+      <c r="C145" s="1"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="1"/>
+      <c r="F145" s="6"/>
+      <c r="G145" s="6"/>
+      <c r="H145" s="1"/>
+      <c r="I145" s="1"/>
+    </row>
+    <row r="146" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="6"/>
+      <c r="G146" s="6"/>
+      <c r="H146" s="1"/>
+      <c r="I146" s="1"/>
+    </row>
+    <row r="147" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="1"/>
+      <c r="F147" s="6"/>
+      <c r="G147" s="6"/>
+      <c r="H147" s="1"/>
+      <c r="I147" s="1"/>
+    </row>
+    <row r="148" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B148" s="1"/>
+      <c r="C148" s="1"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="1"/>
+      <c r="F148" s="6"/>
+      <c r="G148" s="6"/>
+      <c r="H148" s="1"/>
+      <c r="I148" s="1"/>
+    </row>
+    <row r="149" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="6"/>
+      <c r="G149" s="6"/>
+      <c r="H149" s="1"/>
+      <c r="I149" s="1"/>
+    </row>
+    <row r="150" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="6"/>
+      <c r="G150" s="6"/>
+      <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
+    </row>
+    <row r="151" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="6"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+    </row>
+    <row r="152" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="6"/>
+      <c r="G152" s="6"/>
+      <c r="H152" s="1"/>
+      <c r="I152" s="1"/>
+    </row>
+    <row r="153" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B153" s="1"/>
+      <c r="C153" s="1"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="1"/>
+      <c r="F153" s="6"/>
+      <c r="G153" s="6"/>
+      <c r="H153" s="1"/>
+      <c r="I153" s="1"/>
+    </row>
+    <row r="154" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B154" s="1"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="1"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="6"/>
+      <c r="H154" s="1"/>
+      <c r="I154" s="1"/>
+    </row>
+    <row r="155" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="1"/>
+      <c r="F155" s="6"/>
+      <c r="G155" s="6"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+    </row>
+    <row r="156" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="6"/>
+      <c r="G156" s="6"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+    </row>
+    <row r="157" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="4"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="6"/>
+      <c r="G157" s="6"/>
+      <c r="H157" s="1"/>
+      <c r="I157" s="1"/>
+    </row>
+    <row r="158" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="1"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="6"/>
+      <c r="H158" s="1"/>
+      <c r="I158" s="1"/>
+    </row>
+    <row r="159" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="1"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
+    </row>
+    <row r="160" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="1"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
+    </row>
+    <row r="161" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="4"/>
+      <c r="E161" s="1"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="1"/>
+      <c r="I161" s="1"/>
+    </row>
+    <row r="162" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="4"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="1"/>
+      <c r="I162" s="1"/>
+    </row>
+    <row r="163" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="1"/>
+      <c r="I163" s="1"/>
+    </row>
+    <row r="164" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="1"/>
+      <c r="I164" s="1"/>
+    </row>
+    <row r="165" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="6"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="1"/>
+      <c r="I165" s="1"/>
+    </row>
+    <row r="166" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="4"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="6"/>
+      <c r="H166" s="1"/>
+      <c r="I166" s="1"/>
+    </row>
+    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="4"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="6"/>
+      <c r="G167" s="6"/>
+      <c r="H167" s="1"/>
+      <c r="I167" s="1"/>
+    </row>
+    <row r="168" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="4"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="6"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="1"/>
+      <c r="I168" s="1"/>
+    </row>
+    <row r="169" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="4"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="6"/>
+      <c r="G169" s="6"/>
+      <c r="H169" s="1"/>
+      <c r="I169" s="1"/>
+    </row>
+    <row r="170" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="4"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="6"/>
+      <c r="G170" s="6"/>
+      <c r="H170" s="1"/>
+      <c r="I170" s="1"/>
+    </row>
+    <row r="171" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="4"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="1"/>
+      <c r="I171" s="1"/>
+    </row>
+    <row r="172" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="1"/>
+      <c r="F172" s="6"/>
+      <c r="G172" s="6"/>
+      <c r="H172" s="1"/>
+      <c r="I172" s="1"/>
+    </row>
+    <row r="173" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="4"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="6"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="1"/>
+      <c r="I173" s="1"/>
+    </row>
+    <row r="174" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="4"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
+      <c r="H174" s="1"/>
+      <c r="I174" s="1"/>
+    </row>
+    <row r="175" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="4"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="6"/>
+      <c r="G175" s="6"/>
+      <c r="H175" s="1"/>
+      <c r="I175" s="1"/>
+    </row>
+    <row r="176" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="4"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="6"/>
+      <c r="G176" s="6"/>
+      <c r="H176" s="1"/>
+      <c r="I176" s="1"/>
+    </row>
+    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="6"/>
+      <c r="G177" s="6"/>
+      <c r="H177" s="1"/>
+      <c r="I177" s="1"/>
+    </row>
+    <row r="178" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="6"/>
+      <c r="G178" s="6"/>
+      <c r="H178" s="1"/>
+      <c r="I178" s="1"/>
+    </row>
+    <row r="179" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="4"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="6"/>
+      <c r="G179" s="6"/>
+      <c r="H179" s="1"/>
+      <c r="I179" s="1"/>
+    </row>
+    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="4"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="6"/>
+      <c r="G180" s="6"/>
+      <c r="H180" s="1"/>
+      <c r="I180" s="1"/>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="4"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="6"/>
+      <c r="G181" s="6"/>
+      <c r="H181" s="1"/>
+      <c r="I181" s="1"/>
+    </row>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B182" s="1"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="4"/>
+      <c r="E182" s="1"/>
+      <c r="F182" s="6"/>
+      <c r="G182" s="6"/>
+      <c r="H182" s="1"/>
+      <c r="I182" s="1"/>
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+      <c r="D183" s="4"/>
+      <c r="E183" s="1"/>
+      <c r="F183" s="6"/>
+      <c r="G183" s="6"/>
+      <c r="H183" s="1"/>
+      <c r="I183" s="1"/>
+    </row>
+    <row r="184" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
+      <c r="D184" s="4"/>
+      <c r="E184" s="1"/>
+      <c r="F184" s="6"/>
+      <c r="G184" s="6"/>
+      <c r="H184" s="1"/>
+      <c r="I184" s="1"/>
+    </row>
+    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+      <c r="D185" s="4"/>
+      <c r="E185" s="1"/>
+      <c r="F185" s="6"/>
+      <c r="G185" s="6"/>
+      <c r="H185" s="1"/>
+      <c r="I185" s="1"/>
+    </row>
+    <row r="186" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B186" s="1"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="4"/>
+      <c r="E186" s="1"/>
+      <c r="F186" s="6"/>
+      <c r="G186" s="6"/>
+      <c r="H186" s="1"/>
+      <c r="I186" s="1"/>
+    </row>
+    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B187" s="1"/>
+      <c r="C187" s="1"/>
+      <c r="D187" s="4"/>
+      <c r="E187" s="1"/>
+      <c r="F187" s="6"/>
+      <c r="G187" s="6"/>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1"/>
+    </row>
+    <row r="188" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B188" s="1"/>
+      <c r="C188" s="1"/>
+      <c r="D188" s="4"/>
+      <c r="E188" s="1"/>
+      <c r="F188" s="6"/>
+      <c r="G188" s="6"/>
+      <c r="H188" s="1"/>
+      <c r="I188" s="1"/>
+    </row>
+    <row r="189" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B189" s="1"/>
+      <c r="C189" s="1"/>
+      <c r="D189" s="4"/>
+      <c r="E189" s="1"/>
+      <c r="F189" s="6"/>
+      <c r="G189" s="6"/>
+      <c r="H189" s="1"/>
+      <c r="I189" s="1"/>
+    </row>
+    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B190" s="1"/>
+      <c r="C190" s="1"/>
+      <c r="D190" s="4"/>
+      <c r="E190" s="1"/>
+      <c r="F190" s="6"/>
+      <c r="G190" s="6"/>
+      <c r="H190" s="1"/>
+      <c r="I190" s="1"/>
+    </row>
+    <row r="191" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B191" s="1"/>
+      <c r="C191" s="1"/>
+      <c r="D191" s="4"/>
+      <c r="E191" s="1"/>
+      <c r="F191" s="6"/>
+      <c r="G191" s="6"/>
+      <c r="H191" s="1"/>
+      <c r="I191" s="1"/>
+    </row>
+    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B192" s="1"/>
+      <c r="C192" s="1"/>
+      <c r="D192" s="4"/>
+      <c r="E192" s="1"/>
+      <c r="F192" s="6"/>
+      <c r="G192" s="6"/>
+      <c r="H192" s="1"/>
+      <c r="I192" s="1"/>
+    </row>
+    <row r="193" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
+      <c r="D193" s="4"/>
+      <c r="E193" s="1"/>
+      <c r="F193" s="6"/>
+      <c r="G193" s="6"/>
+      <c r="H193" s="1"/>
+      <c r="I193" s="1"/>
+    </row>
+    <row r="194" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B194" s="1"/>
+      <c r="C194" s="1"/>
+      <c r="D194" s="4"/>
+      <c r="E194" s="1"/>
+      <c r="F194" s="6"/>
+      <c r="G194" s="6"/>
+      <c r="H194" s="1"/>
+      <c r="I194" s="1"/>
+    </row>
+    <row r="195" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B195" s="1"/>
+      <c r="C195" s="1"/>
+      <c r="D195" s="4"/>
+      <c r="E195" s="1"/>
+      <c r="F195" s="6"/>
+      <c r="G195" s="6"/>
+      <c r="H195" s="1"/>
+      <c r="I195" s="1"/>
+    </row>
+    <row r="196" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B196" s="1"/>
+      <c r="C196" s="1"/>
+      <c r="D196" s="4"/>
+      <c r="E196" s="1"/>
+      <c r="F196" s="6"/>
+      <c r="G196" s="6"/>
+      <c r="H196" s="1"/>
+      <c r="I196" s="1"/>
+    </row>
+    <row r="197" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B197" s="1"/>
+      <c r="C197" s="1"/>
+      <c r="D197" s="4"/>
+      <c r="E197" s="1"/>
+      <c r="F197" s="6"/>
+      <c r="G197" s="6"/>
+      <c r="H197" s="1"/>
+      <c r="I197" s="1"/>
+    </row>
+    <row r="198" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B198" s="1"/>
+      <c r="C198" s="1"/>
+      <c r="D198" s="4"/>
+      <c r="E198" s="1"/>
+      <c r="F198" s="6"/>
+      <c r="G198" s="6"/>
+      <c r="H198" s="1"/>
+      <c r="I198" s="1"/>
+    </row>
+    <row r="199" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B199" s="1"/>
+      <c r="C199" s="1"/>
+      <c r="D199" s="4"/>
+      <c r="E199" s="1"/>
+      <c r="F199" s="6"/>
+      <c r="G199" s="6"/>
+      <c r="H199" s="1"/>
+      <c r="I199" s="1"/>
+    </row>
+    <row r="200" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B200" s="1"/>
+      <c r="C200" s="1"/>
+      <c r="D200" s="4"/>
+      <c r="E200" s="1"/>
+      <c r="F200" s="6"/>
+      <c r="G200" s="6"/>
+      <c r="H200" s="1"/>
+      <c r="I200" s="1"/>
+    </row>
+    <row r="201" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B201" s="1"/>
+      <c r="C201" s="1"/>
+      <c r="D201" s="4"/>
+      <c r="E201" s="1"/>
+      <c r="F201" s="6"/>
+      <c r="G201" s="6"/>
+      <c r="H201" s="1"/>
+      <c r="I201" s="1"/>
+    </row>
+    <row r="202" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B202" s="1"/>
+      <c r="C202" s="1"/>
+      <c r="D202" s="4"/>
+      <c r="E202" s="1"/>
+      <c r="F202" s="6"/>
+      <c r="G202" s="6"/>
+      <c r="H202" s="1"/>
+      <c r="I202" s="1"/>
+    </row>
+    <row r="203" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B203" s="1"/>
+      <c r="C203" s="1"/>
+      <c r="D203" s="4"/>
+      <c r="E203" s="1"/>
+      <c r="F203" s="6"/>
+      <c r="G203" s="6"/>
+      <c r="H203" s="1"/>
+      <c r="I203" s="1"/>
+    </row>
+    <row r="204" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B204" s="1"/>
+      <c r="C204" s="1"/>
+      <c r="D204" s="4"/>
+      <c r="E204" s="1"/>
+      <c r="F204" s="6"/>
+      <c r="G204" s="6"/>
+      <c r="H204" s="1"/>
+      <c r="I204" s="1"/>
+    </row>
+    <row r="205" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+      <c r="D205" s="4"/>
+      <c r="E205" s="1"/>
+      <c r="F205" s="6"/>
+      <c r="G205" s="6"/>
+      <c r="H205" s="1"/>
+      <c r="I205" s="1"/>
+    </row>
+    <row r="206" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B206" s="1"/>
+      <c r="C206" s="1"/>
+      <c r="D206" s="4"/>
+      <c r="E206" s="1"/>
+      <c r="F206" s="6"/>
+      <c r="G206" s="6"/>
+      <c r="H206" s="1"/>
+      <c r="I206" s="1"/>
+    </row>
+    <row r="207" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B207" s="1"/>
+      <c r="C207" s="1"/>
+      <c r="D207" s="4"/>
+      <c r="E207" s="1"/>
+      <c r="F207" s="6"/>
+      <c r="G207" s="6"/>
+      <c r="H207" s="1"/>
+      <c r="I207" s="1"/>
+    </row>
+    <row r="208" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B208" s="1"/>
+      <c r="C208" s="1"/>
+      <c r="D208" s="4"/>
+      <c r="E208" s="1"/>
+      <c r="F208" s="6"/>
+      <c r="G208" s="6"/>
+      <c r="H208" s="1"/>
+      <c r="I208" s="1"/>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B209" s="1"/>
+      <c r="C209" s="1"/>
+      <c r="D209" s="4"/>
+      <c r="E209" s="1"/>
+      <c r="F209" s="6"/>
+      <c r="G209" s="6"/>
+      <c r="H209" s="1"/>
+      <c r="I209" s="1"/>
+    </row>
+    <row r="210" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B210" s="1"/>
+      <c r="C210" s="1"/>
+      <c r="D210" s="4"/>
+      <c r="E210" s="1"/>
+      <c r="F210" s="6"/>
+      <c r="G210" s="6"/>
+      <c r="H210" s="1"/>
+      <c r="I210" s="1"/>
+    </row>
+    <row r="211" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B211" s="1"/>
+      <c r="C211" s="1"/>
+      <c r="D211" s="4"/>
+      <c r="E211" s="1"/>
+      <c r="F211" s="6"/>
+      <c r="G211" s="6"/>
+      <c r="H211" s="1"/>
+      <c r="I211" s="1"/>
+    </row>
+    <row r="212" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B212" s="1"/>
+      <c r="C212" s="1"/>
+      <c r="D212" s="4"/>
+      <c r="E212" s="1"/>
+      <c r="F212" s="6"/>
+      <c r="G212" s="6"/>
+      <c r="H212" s="1"/>
+      <c r="I212" s="1"/>
+    </row>
+    <row r="213" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B213" s="1"/>
+      <c r="C213" s="1"/>
+      <c r="D213" s="4"/>
+      <c r="E213" s="1"/>
+      <c r="F213" s="6"/>
+      <c r="G213" s="6"/>
+      <c r="H213" s="1"/>
+      <c r="I213" s="1"/>
+    </row>
+    <row r="214" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B214" s="1"/>
+      <c r="C214" s="1"/>
+      <c r="D214" s="4"/>
+      <c r="E214" s="1"/>
+      <c r="F214" s="6"/>
+      <c r="G214" s="6"/>
+      <c r="H214" s="1"/>
+      <c r="I214" s="1"/>
+    </row>
+    <row r="215" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B215" s="1"/>
+      <c r="C215" s="1"/>
+      <c r="D215" s="4"/>
+      <c r="E215" s="1"/>
+      <c r="F215" s="6"/>
+      <c r="G215" s="6"/>
+      <c r="H215" s="1"/>
+      <c r="I215" s="1"/>
+    </row>
+    <row r="216" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B216" s="1"/>
+      <c r="C216" s="1"/>
+      <c r="D216" s="4"/>
+      <c r="E216" s="1"/>
+      <c r="F216" s="6"/>
+      <c r="G216" s="6"/>
+      <c r="H216" s="1"/>
+      <c r="I216" s="1"/>
+    </row>
+    <row r="217" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B217" s="1"/>
+      <c r="C217" s="1"/>
+      <c r="D217" s="4"/>
+      <c r="E217" s="1"/>
+      <c r="F217" s="6"/>
+      <c r="G217" s="6"/>
+      <c r="H217" s="1"/>
+      <c r="I217" s="1"/>
+    </row>
+    <row r="218" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B218" s="1"/>
+      <c r="C218" s="1"/>
+      <c r="D218" s="4"/>
+      <c r="E218" s="1"/>
+      <c r="F218" s="6"/>
+      <c r="G218" s="6"/>
+      <c r="H218" s="1"/>
+      <c r="I218" s="1"/>
+    </row>
+    <row r="219" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B219" s="1"/>
+      <c r="C219" s="1"/>
+      <c r="D219" s="4"/>
+      <c r="E219" s="1"/>
+      <c r="F219" s="6"/>
+      <c r="G219" s="6"/>
+      <c r="H219" s="1"/>
+      <c r="I219" s="1"/>
+    </row>
+    <row r="220" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B220" s="1"/>
+      <c r="C220" s="1"/>
+      <c r="D220" s="4"/>
+      <c r="E220" s="1"/>
+      <c r="F220" s="6"/>
+      <c r="G220" s="6"/>
+      <c r="H220" s="1"/>
+      <c r="I220" s="1"/>
+    </row>
+    <row r="221" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B221" s="1"/>
+      <c r="C221" s="1"/>
+      <c r="D221" s="4"/>
+      <c r="E221" s="1"/>
+      <c r="F221" s="6"/>
+      <c r="G221" s="6"/>
+      <c r="H221" s="1"/>
+      <c r="I221" s="1"/>
+    </row>
+    <row r="222" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B222" s="1"/>
+      <c r="C222" s="1"/>
+      <c r="D222" s="4"/>
+      <c r="E222" s="1"/>
+      <c r="F222" s="6"/>
+      <c r="G222" s="6"/>
+      <c r="H222" s="1"/>
+      <c r="I222" s="1"/>
+    </row>
+    <row r="223" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
+      <c r="D223" s="4"/>
+      <c r="E223" s="1"/>
+      <c r="F223" s="6"/>
+      <c r="G223" s="6"/>
+      <c r="H223" s="1"/>
+      <c r="I223" s="1"/>
+    </row>
+    <row r="224" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B224" s="1"/>
+      <c r="C224" s="1"/>
+      <c r="D224" s="4"/>
+      <c r="E224" s="1"/>
+      <c r="F224" s="6"/>
+      <c r="G224" s="6"/>
+      <c r="H224" s="1"/>
+      <c r="I224" s="1"/>
+    </row>
+    <row r="225" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B225" s="1"/>
+      <c r="C225" s="1"/>
+      <c r="D225" s="4"/>
+      <c r="E225" s="1"/>
+      <c r="F225" s="6"/>
+      <c r="G225" s="6"/>
+      <c r="H225" s="1"/>
+      <c r="I225" s="1"/>
+    </row>
+    <row r="226" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B226" s="1"/>
+      <c r="C226" s="1"/>
+      <c r="D226" s="4"/>
+      <c r="E226" s="1"/>
+      <c r="F226" s="6"/>
+      <c r="G226" s="6"/>
+      <c r="H226" s="1"/>
+      <c r="I226" s="1"/>
+    </row>
+    <row r="227" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B227" s="1"/>
+      <c r="C227" s="1"/>
+      <c r="D227" s="4"/>
+      <c r="E227" s="1"/>
+      <c r="F227" s="6"/>
+      <c r="G227" s="6"/>
+      <c r="H227" s="1"/>
+      <c r="I227" s="1"/>
+    </row>
+    <row r="228" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B228" s="1"/>
+      <c r="C228" s="1"/>
+      <c r="D228" s="4"/>
+      <c r="E228" s="1"/>
+      <c r="F228" s="6"/>
+      <c r="G228" s="6"/>
+      <c r="H228" s="1"/>
+      <c r="I228" s="1"/>
+    </row>
+    <row r="229" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B229" s="1"/>
+      <c r="C229" s="1"/>
+      <c r="D229" s="4"/>
+      <c r="E229" s="1"/>
+      <c r="F229" s="6"/>
+      <c r="G229" s="6"/>
+      <c r="H229" s="1"/>
+      <c r="I229" s="1"/>
+    </row>
+    <row r="230" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B230" s="1"/>
+      <c r="C230" s="1"/>
+      <c r="D230" s="4"/>
+      <c r="E230" s="1"/>
+      <c r="F230" s="6"/>
+      <c r="G230" s="6"/>
+      <c r="H230" s="1"/>
+      <c r="I230" s="1"/>
+    </row>
+    <row r="231" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B231" s="1"/>
+      <c r="C231" s="1"/>
+      <c r="D231" s="4"/>
+      <c r="E231" s="1"/>
+      <c r="F231" s="6"/>
+      <c r="G231" s="6"/>
+      <c r="H231" s="1"/>
+      <c r="I231" s="1"/>
+    </row>
+    <row r="232" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B232" s="1"/>
+      <c r="C232" s="1"/>
+      <c r="D232" s="4"/>
+      <c r="E232" s="1"/>
+      <c r="F232" s="6"/>
+      <c r="G232" s="6"/>
+      <c r="H232" s="1"/>
+      <c r="I232" s="1"/>
+    </row>
+    <row r="233" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B233" s="1"/>
+      <c r="C233" s="1"/>
+      <c r="D233" s="4"/>
+      <c r="E233" s="1"/>
+      <c r="F233" s="6"/>
+      <c r="G233" s="6"/>
+      <c r="H233" s="1"/>
+      <c r="I233" s="1"/>
+    </row>
+    <row r="234" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B234" s="1"/>
+      <c r="C234" s="1"/>
+      <c r="D234" s="4"/>
+      <c r="E234" s="1"/>
+      <c r="F234" s="6"/>
+      <c r="G234" s="6"/>
+      <c r="H234" s="1"/>
+      <c r="I234" s="1"/>
+    </row>
+    <row r="235" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B235" s="1"/>
+      <c r="C235" s="1"/>
+      <c r="D235" s="4"/>
+      <c r="E235" s="1"/>
+      <c r="F235" s="6"/>
+      <c r="G235" s="6"/>
+      <c r="H235" s="1"/>
+      <c r="I235" s="1"/>
+    </row>
+    <row r="236" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B236" s="1"/>
+      <c r="C236" s="1"/>
+      <c r="D236" s="4"/>
+      <c r="E236" s="1"/>
+      <c r="F236" s="6"/>
+      <c r="G236" s="6"/>
+      <c r="H236" s="1"/>
+      <c r="I236" s="1"/>
+    </row>
+    <row r="237" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B237" s="1"/>
+      <c r="C237" s="1"/>
+      <c r="D237" s="4"/>
+      <c r="E237" s="1"/>
+      <c r="F237" s="6"/>
+      <c r="G237" s="6"/>
+      <c r="H237" s="1"/>
+      <c r="I237" s="1"/>
+    </row>
+    <row r="238" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B238" s="1"/>
+      <c r="C238" s="1"/>
+      <c r="D238" s="4"/>
+      <c r="E238" s="1"/>
+      <c r="F238" s="6"/>
+      <c r="G238" s="6"/>
+      <c r="H238" s="1"/>
+      <c r="I238" s="1"/>
+    </row>
+    <row r="239" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B239" s="1"/>
+      <c r="C239" s="1"/>
+      <c r="D239" s="4"/>
+      <c r="E239" s="1"/>
+      <c r="F239" s="6"/>
+      <c r="G239" s="6"/>
+      <c r="H239" s="1"/>
+      <c r="I239" s="1"/>
+    </row>
+    <row r="240" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B240" s="1"/>
+      <c r="C240" s="1"/>
+      <c r="D240" s="4"/>
+      <c r="E240" s="1"/>
+      <c r="F240" s="6"/>
+      <c r="G240" s="6"/>
+      <c r="H240" s="1"/>
+      <c r="I240" s="1"/>
+    </row>
+    <row r="241" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B241" s="1"/>
+      <c r="C241" s="1"/>
+      <c r="D241" s="4"/>
+      <c r="E241" s="1"/>
+      <c r="F241" s="6"/>
+      <c r="G241" s="6"/>
+      <c r="H241" s="1"/>
+      <c r="I241" s="1"/>
+    </row>
+    <row r="242" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B242" s="1"/>
+      <c r="C242" s="1"/>
+      <c r="D242" s="4"/>
+      <c r="E242" s="1"/>
+      <c r="F242" s="6"/>
+      <c r="G242" s="6"/>
+      <c r="H242" s="1"/>
+      <c r="I242" s="1"/>
+    </row>
+    <row r="243" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B243" s="1"/>
+      <c r="C243" s="1"/>
+      <c r="D243" s="4"/>
+      <c r="E243" s="1"/>
+      <c r="F243" s="6"/>
+      <c r="G243" s="6"/>
+      <c r="H243" s="1"/>
+      <c r="I243" s="1"/>
+    </row>
+    <row r="244" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B244" s="1"/>
+      <c r="C244" s="1"/>
+      <c r="D244" s="4"/>
+      <c r="E244" s="1"/>
+      <c r="F244" s="6"/>
+      <c r="G244" s="6"/>
+      <c r="H244" s="1"/>
+      <c r="I244" s="1"/>
+    </row>
+    <row r="245" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
+      <c r="D245" s="4"/>
+      <c r="E245" s="1"/>
+      <c r="F245" s="6"/>
+      <c r="G245" s="6"/>
+      <c r="H245" s="1"/>
+      <c r="I245" s="1"/>
+    </row>
+    <row r="246" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B246" s="1"/>
+      <c r="C246" s="1"/>
+      <c r="D246" s="4"/>
+      <c r="E246" s="1"/>
+      <c r="F246" s="6"/>
+      <c r="G246" s="6"/>
+      <c r="H246" s="1"/>
+      <c r="I246" s="1"/>
+    </row>
+    <row r="247" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B247" s="1"/>
+      <c r="C247" s="1"/>
+      <c r="D247" s="4"/>
+      <c r="E247" s="1"/>
+      <c r="F247" s="6"/>
+      <c r="G247" s="6"/>
+      <c r="H247" s="1"/>
+      <c r="I247" s="1"/>
+    </row>
+    <row r="248" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="4"/>
+      <c r="E248" s="1"/>
+      <c r="F248" s="6"/>
+      <c r="G248" s="6"/>
+      <c r="H248" s="1"/>
+      <c r="I248" s="1"/>
+    </row>
+    <row r="249" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="4"/>
+      <c r="E249" s="1"/>
+      <c r="F249" s="6"/>
+      <c r="G249" s="6"/>
+      <c r="H249" s="1"/>
+      <c r="I249" s="1"/>
+    </row>
+    <row r="250" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B250" s="1"/>
+      <c r="C250" s="1"/>
+      <c r="D250" s="4"/>
+      <c r="E250" s="1"/>
+      <c r="F250" s="6"/>
+      <c r="G250" s="6"/>
+      <c r="H250" s="1"/>
+      <c r="I250" s="1"/>
+    </row>
+    <row r="251" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B251" s="1"/>
+      <c r="C251" s="1"/>
+      <c r="D251" s="4"/>
+      <c r="E251" s="1"/>
+      <c r="F251" s="6"/>
+      <c r="G251" s="6"/>
+      <c r="H251" s="1"/>
+      <c r="I251" s="1"/>
+    </row>
+    <row r="252" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B252" s="1"/>
+      <c r="C252" s="1"/>
+      <c r="D252" s="4"/>
+      <c r="E252" s="1"/>
+      <c r="F252" s="6"/>
+      <c r="G252" s="6"/>
+      <c r="H252" s="1"/>
+      <c r="I252" s="1"/>
+    </row>
+    <row r="253" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B253" s="1"/>
+      <c r="C253" s="1"/>
+      <c r="D253" s="4"/>
+      <c r="E253" s="1"/>
+      <c r="F253" s="6"/>
+      <c r="G253" s="6"/>
+      <c r="H253" s="1"/>
+      <c r="I253" s="1"/>
+    </row>
+    <row r="254" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B254" s="1"/>
+      <c r="C254" s="1"/>
+      <c r="D254" s="4"/>
+      <c r="E254" s="1"/>
+      <c r="F254" s="6"/>
+      <c r="G254" s="6"/>
+      <c r="H254" s="1"/>
+      <c r="I254" s="1"/>
+    </row>
+    <row r="255" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B255" s="1"/>
+      <c r="C255" s="1"/>
+      <c r="D255" s="4"/>
+      <c r="E255" s="1"/>
+      <c r="F255" s="6"/>
+      <c r="G255" s="6"/>
+      <c r="H255" s="1"/>
+      <c r="I255" s="1"/>
+    </row>
+    <row r="256" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B256" s="1"/>
+      <c r="C256" s="1"/>
+      <c r="D256" s="4"/>
+      <c r="E256" s="1"/>
+      <c r="F256" s="6"/>
+      <c r="G256" s="6"/>
+      <c r="H256" s="1"/>
+      <c r="I256" s="1"/>
+    </row>
+    <row r="257" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B257" s="1"/>
+      <c r="C257" s="1"/>
+      <c r="D257" s="4"/>
+      <c r="E257" s="1"/>
+      <c r="F257" s="6"/>
+      <c r="G257" s="6"/>
+      <c r="H257" s="1"/>
+      <c r="I257" s="1"/>
+    </row>
+    <row r="258" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B258" s="1"/>
+      <c r="C258" s="1"/>
+      <c r="D258" s="4"/>
+      <c r="E258" s="1"/>
+      <c r="F258" s="6"/>
+      <c r="G258" s="6"/>
+      <c r="H258" s="1"/>
+      <c r="I258" s="1"/>
+    </row>
+    <row r="259" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B259" s="1"/>
+      <c r="C259" s="1"/>
+      <c r="D259" s="4"/>
+      <c r="E259" s="1"/>
+      <c r="F259" s="6"/>
+      <c r="G259" s="6"/>
+      <c r="H259" s="1"/>
+      <c r="I259" s="1"/>
+    </row>
+    <row r="260" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B260" s="1"/>
+      <c r="C260" s="1"/>
+      <c r="D260" s="4"/>
+      <c r="E260" s="1"/>
+      <c r="F260" s="6"/>
+      <c r="G260" s="6"/>
+      <c r="H260" s="1"/>
+      <c r="I260" s="1"/>
+    </row>
+    <row r="261" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B261" s="1"/>
+      <c r="C261" s="1"/>
+      <c r="D261" s="4"/>
+      <c r="E261" s="1"/>
+      <c r="F261" s="6"/>
+      <c r="G261" s="6"/>
+      <c r="H261" s="1"/>
+      <c r="I261" s="1"/>
+    </row>
+    <row r="262" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B262" s="1"/>
+      <c r="C262" s="1"/>
+      <c r="D262" s="4"/>
+      <c r="E262" s="1"/>
+      <c r="F262" s="6"/>
+      <c r="G262" s="6"/>
+      <c r="H262" s="1"/>
+      <c r="I262" s="1"/>
+    </row>
+    <row r="263" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B263" s="1"/>
+      <c r="C263" s="1"/>
+      <c r="D263" s="4"/>
+      <c r="E263" s="1"/>
+      <c r="F263" s="6"/>
+      <c r="G263" s="6"/>
+      <c r="H263" s="1"/>
+      <c r="I263" s="1"/>
+    </row>
+    <row r="264" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B264" s="1"/>
+      <c r="C264" s="1"/>
+      <c r="D264" s="4"/>
+      <c r="E264" s="1"/>
+      <c r="F264" s="6"/>
+      <c r="G264" s="6"/>
+      <c r="H264" s="1"/>
+      <c r="I264" s="1"/>
+    </row>
+    <row r="265" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B265" s="1"/>
+      <c r="C265" s="1"/>
+      <c r="D265" s="4"/>
+      <c r="E265" s="1"/>
+      <c r="F265" s="6"/>
+      <c r="G265" s="6"/>
+      <c r="H265" s="1"/>
+      <c r="I265" s="1"/>
+    </row>
+    <row r="266" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B266" s="1"/>
+      <c r="C266" s="1"/>
+      <c r="D266" s="4"/>
+      <c r="E266" s="1"/>
+      <c r="F266" s="6"/>
+      <c r="G266" s="6"/>
+      <c r="H266" s="1"/>
+      <c r="I266" s="1"/>
+    </row>
+    <row r="267" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B267" s="1"/>
+      <c r="C267" s="1"/>
+      <c r="D267" s="4"/>
+      <c r="E267" s="1"/>
+      <c r="F267" s="6"/>
+      <c r="G267" s="6"/>
+      <c r="H267" s="1"/>
+      <c r="I267" s="1"/>
+    </row>
+    <row r="268" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B268" s="1"/>
+      <c r="C268" s="1"/>
+      <c r="D268" s="4"/>
+      <c r="E268" s="1"/>
+      <c r="F268" s="6"/>
+      <c r="G268" s="6"/>
+      <c r="H268" s="1"/>
+      <c r="I268" s="1"/>
+    </row>
+    <row r="269" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B269" s="1"/>
+      <c r="C269" s="1"/>
+      <c r="D269" s="4"/>
+      <c r="E269" s="1"/>
+      <c r="F269" s="6"/>
+      <c r="G269" s="6"/>
+      <c r="H269" s="1"/>
+      <c r="I269" s="1"/>
+    </row>
+    <row r="270" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B270" s="1"/>
+      <c r="C270" s="1"/>
+      <c r="D270" s="4"/>
+      <c r="E270" s="1"/>
+      <c r="F270" s="6"/>
+      <c r="G270" s="6"/>
+      <c r="H270" s="1"/>
+      <c r="I270" s="1"/>
+    </row>
+    <row r="271" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B271" s="1"/>
+      <c r="C271" s="1"/>
+      <c r="D271" s="4"/>
+      <c r="E271" s="1"/>
+      <c r="F271" s="6"/>
+      <c r="G271" s="6"/>
+      <c r="H271" s="1"/>
+      <c r="I271" s="1"/>
+    </row>
+    <row r="272" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B272" s="1"/>
+      <c r="C272" s="1"/>
+      <c r="D272" s="4"/>
+      <c r="E272" s="1"/>
+      <c r="F272" s="6"/>
+      <c r="G272" s="6"/>
+      <c r="H272" s="1"/>
+      <c r="I272" s="1"/>
+    </row>
+    <row r="273" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B273" s="1"/>
+      <c r="C273" s="1"/>
+      <c r="D273" s="4"/>
+      <c r="E273" s="1"/>
+      <c r="F273" s="6"/>
+      <c r="G273" s="6"/>
+      <c r="H273" s="1"/>
+      <c r="I273" s="1"/>
+    </row>
+    <row r="274" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B274" s="1"/>
+      <c r="C274" s="1"/>
+      <c r="D274" s="4"/>
+      <c r="E274" s="1"/>
+      <c r="F274" s="6"/>
+      <c r="G274" s="6"/>
+      <c r="H274" s="1"/>
+      <c r="I274" s="1"/>
+    </row>
+    <row r="275" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B275" s="1"/>
+      <c r="C275" s="1"/>
+      <c r="D275" s="4"/>
+      <c r="E275" s="1"/>
+      <c r="F275" s="6"/>
+      <c r="G275" s="6"/>
+      <c r="H275" s="1"/>
+      <c r="I275" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
GD and TTD 26/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="181">
   <si>
     <t>Date</t>
   </si>
@@ -473,19 +473,109 @@
   </si>
   <si>
     <t xml:space="preserve">First round </t>
+  </si>
+  <si>
+    <t>22/07/2020</t>
+  </si>
+  <si>
+    <t>1.6.5.1</t>
+  </si>
+  <si>
+    <t>1.00.02</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=muDPB_WlRUY</t>
+  </si>
+  <si>
+    <t>1.6.6.1</t>
+  </si>
+  <si>
+    <t>Speech</t>
+  </si>
+  <si>
+    <t>1.6.7.1</t>
+  </si>
+  <si>
+    <t>1.6.8.1</t>
+  </si>
+  <si>
+    <t>1.6.9.1</t>
+  </si>
+  <si>
+    <t>23/07/2020</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MBWldLzIEq4</t>
+  </si>
+  <si>
+    <t>1.6.9.2</t>
+  </si>
+  <si>
+    <t>1.6.10.1</t>
+  </si>
+  <si>
+    <t>1.6.11.5</t>
+  </si>
+  <si>
+    <t>24/07/2020</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hXiQbjWFzLM</t>
+  </si>
+  <si>
+    <t>1.6.11.6</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ghDems5CmHo</t>
+  </si>
+  <si>
+    <t>1.6.12.1</t>
+  </si>
+  <si>
+    <t>25/07/2020</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6H33Rf5PGE8</t>
+  </si>
+  <si>
+    <t>1.7.1.1</t>
+  </si>
+  <si>
+    <t>1.7.2.1</t>
+  </si>
+  <si>
+    <t>1.7.2.2</t>
+  </si>
+  <si>
+    <t>1.7.3.1</t>
+  </si>
+  <si>
+    <t>1.7.4.1</t>
+  </si>
+  <si>
+    <t>26/07/2020</t>
+  </si>
+  <si>
+    <t>1.7.4.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -533,25 +623,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,24 +950,24 @@
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="E148" sqref="E148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="42.33203125" customWidth="1"/>
+    <col min="9" max="9" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -903,7 +994,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -930,7 +1021,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -961,7 +1052,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="4">
@@ -983,7 +1074,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="4">
@@ -1005,7 +1096,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="4">
@@ -1027,7 +1118,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="4">
@@ -1053,7 +1144,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="4"/>
@@ -1067,7 +1158,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -1098,7 +1189,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="4">
@@ -1120,7 +1211,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="4">
@@ -1142,7 +1233,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="4">
@@ -1164,7 +1255,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="4">
@@ -1185,7 +1276,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="4">
@@ -1207,7 +1298,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="4"/>
@@ -1221,7 +1312,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -1252,7 +1343,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="4">
@@ -1274,7 +1365,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="4">
@@ -1299,7 +1390,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="4">
@@ -1322,7 +1413,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="4">
@@ -1345,7 +1436,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="4">
@@ -1370,7 +1461,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="4"/>
@@ -1384,7 +1475,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -1413,7 +1504,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="4">
@@ -1437,7 +1528,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="4">
@@ -1461,7 +1552,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="4">
@@ -1487,7 +1578,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="4">
@@ -1509,7 +1600,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="4">
@@ -1533,7 +1624,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="4">
@@ -1557,7 +1648,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="4">
@@ -1581,7 +1672,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="4"/>
@@ -1595,7 +1686,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -1626,7 +1717,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="4">
@@ -1650,7 +1741,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="4">
@@ -1674,7 +1765,7 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="4">
@@ -1698,7 +1789,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="4"/>
@@ -1712,7 +1803,7 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>5</v>
       </c>
@@ -1743,7 +1834,7 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="4">
@@ -1767,7 +1858,7 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="4">
@@ -1791,7 +1882,7 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="4">
@@ -1815,7 +1906,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="4">
@@ -1839,7 +1930,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="4">
@@ -1863,7 +1954,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="4">
@@ -1887,7 +1978,7 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="4">
@@ -1911,7 +2002,7 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="4"/>
@@ -1925,7 +2016,7 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>6</v>
       </c>
@@ -1956,7 +2047,7 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="4">
@@ -1980,7 +2071,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="4">
@@ -2004,7 +2095,7 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="4">
@@ -2028,7 +2119,7 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="4">
@@ -2052,7 +2143,7 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="4">
@@ -2076,7 +2167,7 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="4">
@@ -2102,7 +2193,7 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="4"/>
@@ -2116,7 +2207,7 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>7</v>
       </c>
@@ -2147,7 +2238,7 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="4">
@@ -2171,7 +2262,7 @@
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="4">
@@ -2195,7 +2286,7 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="4">
@@ -2219,7 +2310,7 @@
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="4">
@@ -2243,7 +2334,7 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="4">
@@ -2267,7 +2358,7 @@
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="4">
@@ -2291,7 +2382,7 @@
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="4">
@@ -2315,7 +2406,7 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="4">
@@ -2339,7 +2430,7 @@
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="4">
@@ -2363,7 +2454,7 @@
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="4">
@@ -2387,7 +2478,7 @@
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="4">
@@ -2411,7 +2502,7 @@
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="4"/>
@@ -2425,7 +2516,7 @@
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>6</v>
       </c>
@@ -2456,7 +2547,7 @@
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="4">
@@ -2480,7 +2571,7 @@
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="4">
@@ -2504,7 +2595,7 @@
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="4">
@@ -2528,7 +2619,7 @@
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="4">
@@ -2552,7 +2643,7 @@
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="4">
@@ -2576,7 +2667,7 @@
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="4">
@@ -2600,7 +2691,7 @@
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="4">
@@ -2624,7 +2715,7 @@
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="4">
@@ -2648,7 +2739,7 @@
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="4">
@@ -2672,7 +2763,7 @@
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="4">
@@ -2696,7 +2787,7 @@
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="4">
@@ -2720,7 +2811,7 @@
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="4">
@@ -2744,7 +2835,7 @@
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="4">
@@ -2768,7 +2859,7 @@
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
     </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D85" s="4">
         <f t="shared" si="11"/>
         <v>15</v>
@@ -2784,7 +2875,7 @@
         <v>32.44</v>
       </c>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D86" s="4">
         <f t="shared" si="11"/>
         <v>16</v>
@@ -2800,7 +2891,7 @@
         <v>34.42</v>
       </c>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D87" s="4">
         <f t="shared" si="11"/>
         <v>17</v>
@@ -2816,7 +2907,7 @@
         <v>37.020000000000003</v>
       </c>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D88" s="4">
         <f t="shared" si="11"/>
         <v>18</v>
@@ -2832,7 +2923,7 @@
         <v>38.24</v>
       </c>
     </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D89" s="4">
         <f t="shared" si="11"/>
         <v>19</v>
@@ -2848,7 +2939,7 @@
         <v>39.479999999999997</v>
       </c>
     </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D90" s="4">
         <f t="shared" si="11"/>
         <v>20</v>
@@ -2864,7 +2955,7 @@
         <v>41.14</v>
       </c>
     </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D91" s="4">
         <f t="shared" si="11"/>
         <v>21</v>
@@ -2880,7 +2971,7 @@
         <v>41.49</v>
       </c>
     </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D92" s="4">
         <f t="shared" si="11"/>
         <v>22</v>
@@ -2896,7 +2987,7 @@
         <v>43.08</v>
       </c>
     </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D93" s="4">
         <f t="shared" si="11"/>
         <v>23</v>
@@ -2912,7 +3003,7 @@
         <v>46.09</v>
       </c>
     </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D94" s="4">
         <f t="shared" si="11"/>
         <v>24</v>
@@ -2928,7 +3019,7 @@
         <v>48.37</v>
       </c>
     </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D95" s="4">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -2944,7 +3035,7 @@
         <v>50.39</v>
       </c>
     </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D96" s="4">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -2960,7 +3051,7 @@
         <v>52.16</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="4"/>
@@ -2970,7 +3061,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>7</v>
       </c>
@@ -2999,7 +3090,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="4">
@@ -3019,7 +3110,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="4">
@@ -3039,7 +3130,7 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="4">
@@ -3059,7 +3150,7 @@
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="4">
@@ -3079,7 +3170,7 @@
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="4">
@@ -3099,7 +3190,7 @@
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="4">
@@ -3119,7 +3210,7 @@
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="4">
@@ -3139,7 +3230,7 @@
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="4">
@@ -3159,7 +3250,7 @@
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="4"/>
@@ -3169,7 +3260,7 @@
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>8</v>
       </c>
@@ -3196,7 +3287,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="4">
@@ -3216,7 +3307,7 @@
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="4">
@@ -3236,7 +3327,7 @@
       <c r="H110" s="1"/>
       <c r="I110" s="1"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="4">
@@ -3256,7 +3347,7 @@
       <c r="H111" s="1"/>
       <c r="I111" s="1"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="4"/>
@@ -3266,7 +3357,7 @@
       <c r="H112" s="1"/>
       <c r="I112" s="1"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>9</v>
       </c>
@@ -3291,7 +3382,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="4">
@@ -3311,7 +3402,7 @@
       <c r="H114" s="1"/>
       <c r="I114" s="1"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="4">
@@ -3331,7 +3422,7 @@
       <c r="H115" s="1"/>
       <c r="I115" s="1"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="4">
@@ -3353,7 +3444,7 @@
       </c>
       <c r="I116" s="1"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="4"/>
@@ -3363,7 +3454,7 @@
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>10</v>
       </c>
@@ -3388,7 +3479,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="4">
@@ -3410,7 +3501,7 @@
       </c>
       <c r="I119" s="1"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="4">
@@ -3429,7 +3520,7 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="4">
@@ -3451,7 +3542,7 @@
       </c>
       <c r="I121" s="1"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="4"/>
@@ -3461,7 +3552,7 @@
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>11</v>
       </c>
@@ -3482,9 +3573,11 @@
         <v>5.59</v>
       </c>
       <c r="H123" s="1"/>
-      <c r="I123" s="1"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I123" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="4">
@@ -3504,7 +3597,7 @@
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="4">
@@ -3524,7 +3617,7 @@
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="4">
@@ -3544,7 +3637,7 @@
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="4">
@@ -3564,7 +3657,7 @@
       <c r="H127" s="1"/>
       <c r="I127" s="1"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="4"/>
@@ -3574,57 +3667,115 @@
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B129" s="1"/>
-      <c r="C129" s="1"/>
-      <c r="D129" s="4"/>
-      <c r="E129" s="1"/>
-      <c r="F129" s="6"/>
-      <c r="G129" s="6"/>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>12</v>
+      </c>
+      <c r="B129" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C129" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D129" s="4">
+        <v>1</v>
+      </c>
+      <c r="E129" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F129" s="6">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="G129" s="6">
+        <v>13.13</v>
+      </c>
       <c r="H129" s="1"/>
-      <c r="I129" s="1"/>
-    </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I129" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
-      <c r="D130" s="4"/>
-      <c r="E130" s="1"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="6"/>
-      <c r="H130" s="1"/>
+      <c r="D130" s="4">
+        <f t="shared" ref="D130:D133" si="20">+D129+1</f>
+        <v>2</v>
+      </c>
+      <c r="E130" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F130" s="6">
+        <f>+G129</f>
+        <v>13.13</v>
+      </c>
+      <c r="G130" s="6">
+        <v>25</v>
+      </c>
+      <c r="H130" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="I130" s="1"/>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
-      <c r="D131" s="4"/>
-      <c r="E131" s="1"/>
-      <c r="F131" s="6"/>
-      <c r="G131" s="6"/>
+      <c r="D131" s="4">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="E131" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F131" s="6">
+        <v>29</v>
+      </c>
+      <c r="G131" s="6">
+        <v>42.37</v>
+      </c>
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
-      <c r="D132" s="4"/>
-      <c r="E132" s="1"/>
-      <c r="F132" s="6"/>
-      <c r="G132" s="6"/>
+      <c r="D132" s="4">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="E132" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F132" s="6">
+        <f t="shared" ref="F131:F133" si="21">+G131</f>
+        <v>42.37</v>
+      </c>
+      <c r="G132" s="6">
+        <v>55.03</v>
+      </c>
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
-      <c r="D133" s="4"/>
-      <c r="E133" s="1"/>
-      <c r="F133" s="6"/>
-      <c r="G133" s="6"/>
+      <c r="D133" s="4">
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="E133" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F133" s="6">
+        <f t="shared" si="21"/>
+        <v>55.03</v>
+      </c>
+      <c r="G133" s="6">
+        <v>59.01</v>
+      </c>
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="4"/>
@@ -3634,37 +3785,73 @@
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B135" s="1"/>
-      <c r="C135" s="1"/>
-      <c r="D135" s="4"/>
-      <c r="E135" s="1"/>
-      <c r="F135" s="6"/>
-      <c r="G135" s="6"/>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>13</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C135" s="1">
+        <v>55.29</v>
+      </c>
+      <c r="D135" s="4">
+        <v>1</v>
+      </c>
+      <c r="E135" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F135" s="6">
+        <v>1.03</v>
+      </c>
+      <c r="G135" s="6">
+        <v>12.19</v>
+      </c>
       <c r="H135" s="1"/>
-      <c r="I135" s="1"/>
-    </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I135" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
-      <c r="D136" s="4"/>
-      <c r="E136" s="1"/>
-      <c r="F136" s="6"/>
-      <c r="G136" s="6"/>
+      <c r="D136" s="4">
+        <f t="shared" ref="D136:D141" si="22">+D135+1</f>
+        <v>2</v>
+      </c>
+      <c r="E136" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F136" s="6">
+        <f>+G135</f>
+        <v>12.19</v>
+      </c>
+      <c r="G136" s="6">
+        <v>33.57</v>
+      </c>
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
-      <c r="D137" s="4"/>
-      <c r="E137" s="1"/>
-      <c r="F137" s="6"/>
-      <c r="G137" s="6"/>
+      <c r="D137" s="4">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="E137" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F137" s="6">
+        <v>37.549999999999997</v>
+      </c>
+      <c r="G137" s="6">
+        <v>54.17</v>
+      </c>
       <c r="H137" s="1"/>
       <c r="I137" s="1"/>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="4"/>
@@ -3674,47 +3861,94 @@
       <c r="H138" s="1"/>
       <c r="I138" s="1"/>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B139" s="1"/>
-      <c r="C139" s="1"/>
-      <c r="D139" s="4"/>
-      <c r="E139" s="1"/>
-      <c r="F139" s="6"/>
-      <c r="G139" s="6"/>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>14</v>
+      </c>
+      <c r="B139" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C139" s="1">
+        <v>52.45</v>
+      </c>
+      <c r="D139" s="4">
+        <v>1</v>
+      </c>
+      <c r="E139" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="F139" s="6">
+        <v>1.05</v>
+      </c>
+      <c r="G139" s="6">
+        <v>8.07</v>
+      </c>
       <c r="H139" s="1"/>
-      <c r="I139" s="1"/>
-    </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I139" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
-      <c r="D140" s="4"/>
-      <c r="E140" s="1"/>
-      <c r="F140" s="6"/>
-      <c r="G140" s="6"/>
-      <c r="H140" s="1"/>
+      <c r="D140" s="4">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="E140" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F140" s="6">
+        <f>+G139</f>
+        <v>8.07</v>
+      </c>
+      <c r="G140" s="6">
+        <v>26.55</v>
+      </c>
+      <c r="H140" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="I140" s="1"/>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
-      <c r="D141" s="4"/>
-      <c r="E141" s="1"/>
-      <c r="F141" s="6"/>
-      <c r="G141" s="6"/>
+      <c r="D141" s="4">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="E141" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F141" s="6">
+        <v>28.53</v>
+      </c>
+      <c r="G141" s="6">
+        <v>48.25</v>
+      </c>
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
-      <c r="D142" s="4"/>
-      <c r="E142" s="1"/>
-      <c r="F142" s="6"/>
-      <c r="G142" s="6"/>
+      <c r="D142" s="4">
+        <v>4</v>
+      </c>
+      <c r="E142" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F142" s="6">
+        <f t="shared" ref="F141:F142" si="23">+G141</f>
+        <v>48.25</v>
+      </c>
+      <c r="G142" s="6">
+        <v>51.34</v>
+      </c>
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="4"/>
@@ -3724,37 +3958,73 @@
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B144" s="1"/>
-      <c r="C144" s="1"/>
-      <c r="D144" s="4"/>
-      <c r="E144" s="1"/>
-      <c r="F144" s="6"/>
-      <c r="G144" s="6"/>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>15</v>
+      </c>
+      <c r="B144" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C144" s="1">
+        <v>59.01</v>
+      </c>
+      <c r="D144" s="4">
+        <v>1</v>
+      </c>
+      <c r="E144" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F144" s="6">
+        <v>6.1</v>
+      </c>
+      <c r="G144" s="6">
+        <v>18.02</v>
+      </c>
       <c r="H144" s="1"/>
-      <c r="I144" s="1"/>
-    </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I144" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
-      <c r="D145" s="4"/>
-      <c r="E145" s="1"/>
-      <c r="F145" s="6"/>
-      <c r="G145" s="6"/>
+      <c r="D145" s="4">
+        <f t="shared" ref="D145" si="24">+D144+1</f>
+        <v>2</v>
+      </c>
+      <c r="E145" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F145" s="6">
+        <f>+G144</f>
+        <v>18.02</v>
+      </c>
+      <c r="G145" s="6">
+        <v>36.36</v>
+      </c>
       <c r="H145" s="1"/>
       <c r="I145" s="1"/>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
-      <c r="D146" s="4"/>
-      <c r="E146" s="1"/>
-      <c r="F146" s="6"/>
-      <c r="G146" s="6"/>
+      <c r="D146" s="4">
+        <v>3</v>
+      </c>
+      <c r="E146" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F146" s="6">
+        <f>+G145</f>
+        <v>36.36</v>
+      </c>
+      <c r="G146" s="6">
+        <v>57.03</v>
+      </c>
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="4"/>
@@ -3764,17 +4034,26 @@
       <c r="H147" s="1"/>
       <c r="I147" s="1"/>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B148" s="1"/>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>16</v>
+      </c>
+      <c r="B148" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="C148" s="1"/>
-      <c r="D148" s="4"/>
-      <c r="E148" s="1"/>
+      <c r="D148" s="4">
+        <v>1</v>
+      </c>
+      <c r="E148" s="12" t="s">
+        <v>180</v>
+      </c>
       <c r="F148" s="6"/>
       <c r="G148" s="6"/>
       <c r="H148" s="1"/>
       <c r="I148" s="1"/>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="4"/>
@@ -3784,7 +4063,7 @@
       <c r="H149" s="1"/>
       <c r="I149" s="1"/>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="4"/>
@@ -3794,7 +4073,7 @@
       <c r="H150" s="1"/>
       <c r="I150" s="1"/>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="4"/>
@@ -3804,7 +4083,7 @@
       <c r="H151" s="1"/>
       <c r="I151" s="1"/>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="4"/>
@@ -3814,7 +4093,7 @@
       <c r="H152" s="1"/>
       <c r="I152" s="1"/>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="4"/>
@@ -3824,7 +4103,7 @@
       <c r="H153" s="1"/>
       <c r="I153" s="1"/>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="4"/>
@@ -3834,7 +4113,7 @@
       <c r="H154" s="1"/>
       <c r="I154" s="1"/>
     </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="4"/>
@@ -3844,7 +4123,7 @@
       <c r="H155" s="1"/>
       <c r="I155" s="1"/>
     </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="4"/>
@@ -3854,7 +4133,7 @@
       <c r="H156" s="1"/>
       <c r="I156" s="1"/>
     </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="4"/>
@@ -3864,7 +4143,7 @@
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
     </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="4"/>
@@ -3874,7 +4153,7 @@
       <c r="H158" s="1"/>
       <c r="I158" s="1"/>
     </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="4"/>
@@ -3884,7 +4163,7 @@
       <c r="H159" s="1"/>
       <c r="I159" s="1"/>
     </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="4"/>
@@ -3894,7 +4173,7 @@
       <c r="H160" s="1"/>
       <c r="I160" s="1"/>
     </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="4"/>
@@ -3904,7 +4183,7 @@
       <c r="H161" s="1"/>
       <c r="I161" s="1"/>
     </row>
-    <row r="162" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="4"/>
@@ -3914,7 +4193,7 @@
       <c r="H162" s="1"/>
       <c r="I162" s="1"/>
     </row>
-    <row r="163" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="4"/>
@@ -3924,7 +4203,7 @@
       <c r="H163" s="1"/>
       <c r="I163" s="1"/>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="4"/>
@@ -3934,7 +4213,7 @@
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
     </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="4"/>
@@ -3944,7 +4223,7 @@
       <c r="H165" s="1"/>
       <c r="I165" s="1"/>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="4"/>
@@ -3954,7 +4233,7 @@
       <c r="H166" s="1"/>
       <c r="I166" s="1"/>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="4"/>
@@ -3964,7 +4243,7 @@
       <c r="H167" s="1"/>
       <c r="I167" s="1"/>
     </row>
-    <row r="168" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="4"/>
@@ -3974,7 +4253,7 @@
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
     </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="4"/>
@@ -3984,7 +4263,7 @@
       <c r="H169" s="1"/>
       <c r="I169" s="1"/>
     </row>
-    <row r="170" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="4"/>
@@ -3994,7 +4273,7 @@
       <c r="H170" s="1"/>
       <c r="I170" s="1"/>
     </row>
-    <row r="171" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="4"/>
@@ -4004,7 +4283,7 @@
       <c r="H171" s="1"/>
       <c r="I171" s="1"/>
     </row>
-    <row r="172" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="4"/>
@@ -4014,7 +4293,7 @@
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
     </row>
-    <row r="173" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="4"/>
@@ -4024,7 +4303,7 @@
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
     </row>
-    <row r="174" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="4"/>
@@ -4034,7 +4313,7 @@
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
     </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="4"/>
@@ -4044,7 +4323,7 @@
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
     </row>
-    <row r="176" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="4"/>
@@ -4054,7 +4333,7 @@
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="4"/>
@@ -4064,7 +4343,7 @@
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="4"/>
@@ -4074,7 +4353,7 @@
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="4"/>
@@ -4084,7 +4363,7 @@
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="4"/>
@@ -4094,7 +4373,7 @@
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="4"/>
@@ -4104,7 +4383,7 @@
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="4"/>
@@ -4114,7 +4393,7 @@
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="4"/>
@@ -4124,7 +4403,7 @@
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="4"/>
@@ -4134,7 +4413,7 @@
       <c r="H184" s="1"/>
       <c r="I184" s="1"/>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="4"/>
@@ -4144,7 +4423,7 @@
       <c r="H185" s="1"/>
       <c r="I185" s="1"/>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="4"/>
@@ -4154,7 +4433,7 @@
       <c r="H186" s="1"/>
       <c r="I186" s="1"/>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="4"/>
@@ -4164,7 +4443,7 @@
       <c r="H187" s="1"/>
       <c r="I187" s="1"/>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="4"/>
@@ -4174,7 +4453,7 @@
       <c r="H188" s="1"/>
       <c r="I188" s="1"/>
     </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="4"/>
@@ -4184,7 +4463,7 @@
       <c r="H189" s="1"/>
       <c r="I189" s="1"/>
     </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="4"/>
@@ -4194,7 +4473,7 @@
       <c r="H190" s="1"/>
       <c r="I190" s="1"/>
     </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="4"/>
@@ -4204,7 +4483,7 @@
       <c r="H191" s="1"/>
       <c r="I191" s="1"/>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="4"/>
@@ -4214,7 +4493,7 @@
       <c r="H192" s="1"/>
       <c r="I192" s="1"/>
     </row>
-    <row r="193" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="4"/>
@@ -4224,7 +4503,7 @@
       <c r="H193" s="1"/>
       <c r="I193" s="1"/>
     </row>
-    <row r="194" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="4"/>
@@ -4234,7 +4513,7 @@
       <c r="H194" s="1"/>
       <c r="I194" s="1"/>
     </row>
-    <row r="195" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="4"/>
@@ -4244,7 +4523,7 @@
       <c r="H195" s="1"/>
       <c r="I195" s="1"/>
     </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="4"/>
@@ -4254,7 +4533,7 @@
       <c r="H196" s="1"/>
       <c r="I196" s="1"/>
     </row>
-    <row r="197" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="4"/>
@@ -4264,7 +4543,7 @@
       <c r="H197" s="1"/>
       <c r="I197" s="1"/>
     </row>
-    <row r="198" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="4"/>
@@ -4274,7 +4553,7 @@
       <c r="H198" s="1"/>
       <c r="I198" s="1"/>
     </row>
-    <row r="199" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="4"/>
@@ -4284,7 +4563,7 @@
       <c r="H199" s="1"/>
       <c r="I199" s="1"/>
     </row>
-    <row r="200" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="4"/>
@@ -4294,7 +4573,7 @@
       <c r="H200" s="1"/>
       <c r="I200" s="1"/>
     </row>
-    <row r="201" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="4"/>
@@ -4304,7 +4583,7 @@
       <c r="H201" s="1"/>
       <c r="I201" s="1"/>
     </row>
-    <row r="202" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="4"/>
@@ -4314,7 +4593,7 @@
       <c r="H202" s="1"/>
       <c r="I202" s="1"/>
     </row>
-    <row r="203" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="4"/>
@@ -4324,7 +4603,7 @@
       <c r="H203" s="1"/>
       <c r="I203" s="1"/>
     </row>
-    <row r="204" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="4"/>
@@ -4334,7 +4613,7 @@
       <c r="H204" s="1"/>
       <c r="I204" s="1"/>
     </row>
-    <row r="205" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="4"/>
@@ -4344,7 +4623,7 @@
       <c r="H205" s="1"/>
       <c r="I205" s="1"/>
     </row>
-    <row r="206" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="4"/>
@@ -4354,7 +4633,7 @@
       <c r="H206" s="1"/>
       <c r="I206" s="1"/>
     </row>
-    <row r="207" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="4"/>
@@ -4364,7 +4643,7 @@
       <c r="H207" s="1"/>
       <c r="I207" s="1"/>
     </row>
-    <row r="208" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="4"/>
@@ -4374,7 +4653,7 @@
       <c r="H208" s="1"/>
       <c r="I208" s="1"/>
     </row>
-    <row r="209" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="4"/>
@@ -4384,7 +4663,7 @@
       <c r="H209" s="1"/>
       <c r="I209" s="1"/>
     </row>
-    <row r="210" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="4"/>
@@ -4394,7 +4673,7 @@
       <c r="H210" s="1"/>
       <c r="I210" s="1"/>
     </row>
-    <row r="211" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="4"/>
@@ -4404,7 +4683,7 @@
       <c r="H211" s="1"/>
       <c r="I211" s="1"/>
     </row>
-    <row r="212" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="4"/>
@@ -4414,7 +4693,7 @@
       <c r="H212" s="1"/>
       <c r="I212" s="1"/>
     </row>
-    <row r="213" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="4"/>
@@ -4424,7 +4703,7 @@
       <c r="H213" s="1"/>
       <c r="I213" s="1"/>
     </row>
-    <row r="214" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="4"/>
@@ -4434,7 +4713,7 @@
       <c r="H214" s="1"/>
       <c r="I214" s="1"/>
     </row>
-    <row r="215" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="4"/>
@@ -4444,7 +4723,7 @@
       <c r="H215" s="1"/>
       <c r="I215" s="1"/>
     </row>
-    <row r="216" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="4"/>
@@ -4454,7 +4733,7 @@
       <c r="H216" s="1"/>
       <c r="I216" s="1"/>
     </row>
-    <row r="217" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="4"/>
@@ -4464,7 +4743,7 @@
       <c r="H217" s="1"/>
       <c r="I217" s="1"/>
     </row>
-    <row r="218" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="4"/>
@@ -4474,7 +4753,7 @@
       <c r="H218" s="1"/>
       <c r="I218" s="1"/>
     </row>
-    <row r="219" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
       <c r="D219" s="4"/>
@@ -4484,7 +4763,7 @@
       <c r="H219" s="1"/>
       <c r="I219" s="1"/>
     </row>
-    <row r="220" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="4"/>
@@ -4494,7 +4773,7 @@
       <c r="H220" s="1"/>
       <c r="I220" s="1"/>
     </row>
-    <row r="221" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="4"/>
@@ -4504,7 +4783,7 @@
       <c r="H221" s="1"/>
       <c r="I221" s="1"/>
     </row>
-    <row r="222" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="4"/>
@@ -4514,7 +4793,7 @@
       <c r="H222" s="1"/>
       <c r="I222" s="1"/>
     </row>
-    <row r="223" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="4"/>
@@ -4524,7 +4803,7 @@
       <c r="H223" s="1"/>
       <c r="I223" s="1"/>
     </row>
-    <row r="224" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="4"/>
@@ -4534,7 +4813,7 @@
       <c r="H224" s="1"/>
       <c r="I224" s="1"/>
     </row>
-    <row r="225" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="4"/>
@@ -4544,7 +4823,7 @@
       <c r="H225" s="1"/>
       <c r="I225" s="1"/>
     </row>
-    <row r="226" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
       <c r="D226" s="4"/>
@@ -4554,7 +4833,7 @@
       <c r="H226" s="1"/>
       <c r="I226" s="1"/>
     </row>
-    <row r="227" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
       <c r="D227" s="4"/>
@@ -4564,7 +4843,7 @@
       <c r="H227" s="1"/>
       <c r="I227" s="1"/>
     </row>
-    <row r="228" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="4"/>
@@ -4574,7 +4853,7 @@
       <c r="H228" s="1"/>
       <c r="I228" s="1"/>
     </row>
-    <row r="229" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
       <c r="D229" s="4"/>
@@ -4584,7 +4863,7 @@
       <c r="H229" s="1"/>
       <c r="I229" s="1"/>
     </row>
-    <row r="230" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
       <c r="D230" s="4"/>
@@ -4594,7 +4873,7 @@
       <c r="H230" s="1"/>
       <c r="I230" s="1"/>
     </row>
-    <row r="231" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
       <c r="D231" s="4"/>
@@ -4604,7 +4883,7 @@
       <c r="H231" s="1"/>
       <c r="I231" s="1"/>
     </row>
-    <row r="232" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
       <c r="D232" s="4"/>
@@ -4614,7 +4893,7 @@
       <c r="H232" s="1"/>
       <c r="I232" s="1"/>
     </row>
-    <row r="233" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
       <c r="D233" s="4"/>
@@ -4624,7 +4903,7 @@
       <c r="H233" s="1"/>
       <c r="I233" s="1"/>
     </row>
-    <row r="234" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
       <c r="D234" s="4"/>
@@ -4634,7 +4913,7 @@
       <c r="H234" s="1"/>
       <c r="I234" s="1"/>
     </row>
-    <row r="235" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
       <c r="D235" s="4"/>
@@ -4644,7 +4923,7 @@
       <c r="H235" s="1"/>
       <c r="I235" s="1"/>
     </row>
-    <row r="236" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
       <c r="D236" s="4"/>
@@ -4654,7 +4933,7 @@
       <c r="H236" s="1"/>
       <c r="I236" s="1"/>
     </row>
-    <row r="237" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
       <c r="D237" s="4"/>
@@ -4664,7 +4943,7 @@
       <c r="H237" s="1"/>
       <c r="I237" s="1"/>
     </row>
-    <row r="238" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
       <c r="D238" s="4"/>
@@ -4674,7 +4953,7 @@
       <c r="H238" s="1"/>
       <c r="I238" s="1"/>
     </row>
-    <row r="239" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="4"/>
@@ -4684,7 +4963,7 @@
       <c r="H239" s="1"/>
       <c r="I239" s="1"/>
     </row>
-    <row r="240" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
       <c r="D240" s="4"/>
@@ -4694,7 +4973,7 @@
       <c r="H240" s="1"/>
       <c r="I240" s="1"/>
     </row>
-    <row r="241" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
       <c r="D241" s="4"/>
@@ -4704,7 +4983,7 @@
       <c r="H241" s="1"/>
       <c r="I241" s="1"/>
     </row>
-    <row r="242" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
       <c r="D242" s="4"/>
@@ -4714,7 +4993,7 @@
       <c r="H242" s="1"/>
       <c r="I242" s="1"/>
     </row>
-    <row r="243" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
       <c r="D243" s="4"/>
@@ -4724,7 +5003,7 @@
       <c r="H243" s="1"/>
       <c r="I243" s="1"/>
     </row>
-    <row r="244" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
       <c r="D244" s="4"/>
@@ -4734,7 +5013,7 @@
       <c r="H244" s="1"/>
       <c r="I244" s="1"/>
     </row>
-    <row r="245" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
       <c r="D245" s="4"/>
@@ -4744,7 +5023,7 @@
       <c r="H245" s="1"/>
       <c r="I245" s="1"/>
     </row>
-    <row r="246" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
       <c r="D246" s="4"/>
@@ -4754,7 +5033,7 @@
       <c r="H246" s="1"/>
       <c r="I246" s="1"/>
     </row>
-    <row r="247" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="4"/>
@@ -4764,7 +5043,7 @@
       <c r="H247" s="1"/>
       <c r="I247" s="1"/>
     </row>
-    <row r="248" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="4"/>
@@ -4774,7 +5053,7 @@
       <c r="H248" s="1"/>
       <c r="I248" s="1"/>
     </row>
-    <row r="249" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
       <c r="D249" s="4"/>
@@ -4784,7 +5063,7 @@
       <c r="H249" s="1"/>
       <c r="I249" s="1"/>
     </row>
-    <row r="250" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="4"/>
@@ -4794,7 +5073,7 @@
       <c r="H250" s="1"/>
       <c r="I250" s="1"/>
     </row>
-    <row r="251" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="4"/>
@@ -4804,7 +5083,7 @@
       <c r="H251" s="1"/>
       <c r="I251" s="1"/>
     </row>
-    <row r="252" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
       <c r="D252" s="4"/>
@@ -4814,7 +5093,7 @@
       <c r="H252" s="1"/>
       <c r="I252" s="1"/>
     </row>
-    <row r="253" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
       <c r="D253" s="4"/>
@@ -4824,7 +5103,7 @@
       <c r="H253" s="1"/>
       <c r="I253" s="1"/>
     </row>
-    <row r="254" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
       <c r="D254" s="4"/>
@@ -4834,7 +5113,7 @@
       <c r="H254" s="1"/>
       <c r="I254" s="1"/>
     </row>
-    <row r="255" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
       <c r="D255" s="4"/>
@@ -4844,7 +5123,7 @@
       <c r="H255" s="1"/>
       <c r="I255" s="1"/>
     </row>
-    <row r="256" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
       <c r="D256" s="4"/>
@@ -4854,7 +5133,7 @@
       <c r="H256" s="1"/>
       <c r="I256" s="1"/>
     </row>
-    <row r="257" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
       <c r="D257" s="4"/>
@@ -4864,7 +5143,7 @@
       <c r="H257" s="1"/>
       <c r="I257" s="1"/>
     </row>
-    <row r="258" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B258" s="1"/>
       <c r="C258" s="1"/>
       <c r="D258" s="4"/>
@@ -4874,7 +5153,7 @@
       <c r="H258" s="1"/>
       <c r="I258" s="1"/>
     </row>
-    <row r="259" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B259" s="1"/>
       <c r="C259" s="1"/>
       <c r="D259" s="4"/>
@@ -4884,7 +5163,7 @@
       <c r="H259" s="1"/>
       <c r="I259" s="1"/>
     </row>
-    <row r="260" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
       <c r="D260" s="4"/>
@@ -4894,7 +5173,7 @@
       <c r="H260" s="1"/>
       <c r="I260" s="1"/>
     </row>
-    <row r="261" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B261" s="1"/>
       <c r="C261" s="1"/>
       <c r="D261" s="4"/>
@@ -4904,7 +5183,7 @@
       <c r="H261" s="1"/>
       <c r="I261" s="1"/>
     </row>
-    <row r="262" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
       <c r="D262" s="4"/>
@@ -4914,7 +5193,7 @@
       <c r="H262" s="1"/>
       <c r="I262" s="1"/>
     </row>
-    <row r="263" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
       <c r="D263" s="4"/>
@@ -4924,7 +5203,7 @@
       <c r="H263" s="1"/>
       <c r="I263" s="1"/>
     </row>
-    <row r="264" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
       <c r="D264" s="4"/>
@@ -4934,7 +5213,7 @@
       <c r="H264" s="1"/>
       <c r="I264" s="1"/>
     </row>
-    <row r="265" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>
       <c r="D265" s="4"/>
@@ -4944,7 +5223,7 @@
       <c r="H265" s="1"/>
       <c r="I265" s="1"/>
     </row>
-    <row r="266" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
       <c r="D266" s="4"/>
@@ -4954,7 +5233,7 @@
       <c r="H266" s="1"/>
       <c r="I266" s="1"/>
     </row>
-    <row r="267" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B267" s="1"/>
       <c r="C267" s="1"/>
       <c r="D267" s="4"/>
@@ -4964,7 +5243,7 @@
       <c r="H267" s="1"/>
       <c r="I267" s="1"/>
     </row>
-    <row r="268" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
       <c r="D268" s="4"/>
@@ -4974,7 +5253,7 @@
       <c r="H268" s="1"/>
       <c r="I268" s="1"/>
     </row>
-    <row r="269" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B269" s="1"/>
       <c r="C269" s="1"/>
       <c r="D269" s="4"/>
@@ -4984,7 +5263,7 @@
       <c r="H269" s="1"/>
       <c r="I269" s="1"/>
     </row>
-    <row r="270" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="270" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
       <c r="D270" s="4"/>
@@ -4994,7 +5273,7 @@
       <c r="H270" s="1"/>
       <c r="I270" s="1"/>
     </row>
-    <row r="271" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="271" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B271" s="1"/>
       <c r="C271" s="1"/>
       <c r="D271" s="4"/>
@@ -5004,7 +5283,7 @@
       <c r="H271" s="1"/>
       <c r="I271" s="1"/>
     </row>
-    <row r="272" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B272" s="1"/>
       <c r="C272" s="1"/>
       <c r="D272" s="4"/>
@@ -5014,7 +5293,7 @@
       <c r="H272" s="1"/>
       <c r="I272" s="1"/>
     </row>
-    <row r="273" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B273" s="1"/>
       <c r="C273" s="1"/>
       <c r="D273" s="4"/>
@@ -5024,7 +5303,7 @@
       <c r="H273" s="1"/>
       <c r="I273" s="1"/>
     </row>
-    <row r="274" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B274" s="1"/>
       <c r="C274" s="1"/>
       <c r="D274" s="4"/>
@@ -5034,7 +5313,7 @@
       <c r="H274" s="1"/>
       <c r="I274" s="1"/>
     </row>
-    <row r="275" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
       <c r="D275" s="4"/>

</xml_diff>

<commit_message>
TTD, Ghana DarpaNam and padam w/o swaram 30/07
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="221">
   <si>
     <t>Date</t>
   </si>
@@ -103,9 +103,6 @@
     <t>1.2.3.1</t>
   </si>
   <si>
-    <t>Panchati 6</t>
-  </si>
-  <si>
     <t>1.2.3.2</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
     <t>1.3.14.1</t>
   </si>
   <si>
-    <t>upto 1.3.14.4</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=hPGh9CKobF8</t>
   </si>
   <si>
@@ -427,9 +421,6 @@
     <t>1.5.8.1</t>
   </si>
   <si>
-    <t>upto P33</t>
-  </si>
-  <si>
     <t>20/07/2020</t>
   </si>
   <si>
@@ -451,9 +442,6 @@
     <t>talk</t>
   </si>
   <si>
-    <t>upto P 50</t>
-  </si>
-  <si>
     <t>21/07/2020</t>
   </si>
   <si>
@@ -650,19 +638,70 @@
   </si>
   <si>
     <t>18.12.2</t>
+  </si>
+  <si>
+    <t>1.7.13.2</t>
+  </si>
+  <si>
+    <t>1.6.11.1</t>
+  </si>
+  <si>
+    <t>1.5.11.4</t>
+  </si>
+  <si>
+    <t>1.5.8.3</t>
+  </si>
+  <si>
+    <t>1.3.14.4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2aerAxZ9ZeE</t>
+  </si>
+  <si>
+    <t>1.8.12.3</t>
+  </si>
+  <si>
+    <t>1.8.13.1</t>
+  </si>
+  <si>
+    <t>1.8.14.1</t>
+  </si>
+  <si>
+    <t>1.8.15.1</t>
+  </si>
+  <si>
+    <t>1.8.16.1</t>
+  </si>
+  <si>
+    <t>1.8.17.1</t>
+  </si>
+  <si>
+    <t>1.8.18.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -722,25 +761,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1050,15 +1091,15 @@
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="H174" sqref="H174"/>
+      <selection pane="bottomLeft" activeCell="E183" sqref="E183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
@@ -1077,7 +1118,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>3</v>
@@ -1126,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="2">
-        <v>44050</v>
+        <v>44020</v>
       </c>
       <c r="C7" s="1">
         <v>34.270000000000003</v>
@@ -1145,7 +1186,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1234,10 +1275,10 @@
         <v>33.380000000000003</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1263,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="2">
-        <v>44081</v>
+        <v>44021</v>
       </c>
       <c r="C13" s="1">
         <v>56.45</v>
@@ -1282,7 +1323,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1417,7 +1458,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="2">
-        <v>44111</v>
+        <v>44022</v>
       </c>
       <c r="C20" s="1">
         <v>50.05</v>
@@ -1436,7 +1477,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1482,7 +1523,7 @@
         <v>29.49</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1552,8 +1593,8 @@
       <c r="G25" s="6">
         <v>49.18</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>29</v>
+      <c r="H25" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1580,14 +1621,14 @@
         <v>3</v>
       </c>
       <c r="B27" s="2">
-        <v>44142</v>
+        <v>44023</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="4">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F27" s="6">
         <v>5</v>
@@ -1597,7 +1638,7 @@
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1612,7 +1653,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" s="6">
         <f>+G27</f>
@@ -1636,7 +1677,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F29" s="6">
         <f t="shared" ref="F29:F34" si="2">+G28</f>
@@ -1660,7 +1701,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30" s="6">
         <f t="shared" si="2"/>
@@ -1670,7 +1711,7 @@
         <v>27.34</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1686,7 +1727,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31" s="6">
         <v>28.52</v>
@@ -1708,7 +1749,7 @@
         <v>6</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F32" s="6">
         <f t="shared" si="2"/>
@@ -1732,7 +1773,7 @@
         <v>7</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F33" s="6">
         <f t="shared" si="2"/>
@@ -1756,7 +1797,7 @@
         <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F34" s="6">
         <f t="shared" si="2"/>
@@ -1791,7 +1832,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="2">
-        <v>44172</v>
+        <v>44024</v>
       </c>
       <c r="C36" s="1">
         <v>55.25</v>
@@ -1800,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" s="6">
         <v>7.33</v>
@@ -1810,7 +1851,7 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -1825,7 +1866,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F37" s="6">
         <f>+G36</f>
@@ -1849,7 +1890,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F38" s="6">
         <f t="shared" ref="F38:F39" si="4">+G37</f>
@@ -1873,7 +1914,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F39" s="6">
         <f t="shared" si="4"/>
@@ -1907,8 +1948,8 @@
       <c r="A41" s="1">
         <v>5</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>48</v>
+      <c r="B41" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C41" s="1">
         <v>58.07</v>
@@ -1917,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F41" s="6">
         <v>4.1100000000000003</v>
@@ -1927,7 +1968,7 @@
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -1942,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F42" s="6">
         <f>+G41</f>
@@ -1966,7 +2007,7 @@
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F43" s="6">
         <f t="shared" ref="F43:F48" si="6">+G42</f>
@@ -1990,7 +2031,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F44" s="6">
         <f t="shared" si="6"/>
@@ -2014,7 +2055,7 @@
         <v>5</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F45" s="6">
         <f t="shared" si="6"/>
@@ -2038,7 +2079,7 @@
         <v>6</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F46" s="6">
         <f t="shared" si="6"/>
@@ -2062,7 +2103,7 @@
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F47" s="6">
         <f t="shared" si="6"/>
@@ -2086,7 +2127,7 @@
         <v>8</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F48" s="6">
         <f t="shared" si="6"/>
@@ -2121,7 +2162,7 @@
         <v>6</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C50" s="1">
         <v>56.28</v>
@@ -2130,7 +2171,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F50" s="6">
         <v>4.3600000000000003</v>
@@ -2140,7 +2181,7 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -2155,7 +2196,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F51" s="6">
         <f t="shared" ref="F51:F56" si="7">+G50</f>
@@ -2179,7 +2220,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F52" s="6">
         <f t="shared" si="7"/>
@@ -2203,7 +2244,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F53" s="6">
         <f t="shared" si="7"/>
@@ -2227,7 +2268,7 @@
         <v>5</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F54" s="6">
         <f t="shared" si="7"/>
@@ -2251,7 +2292,7 @@
         <v>6</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F55" s="6">
         <f t="shared" si="7"/>
@@ -2275,7 +2316,7 @@
         <v>7</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F56" s="6">
         <f t="shared" si="7"/>
@@ -2284,8 +2325,8 @@
       <c r="G56" s="6">
         <v>50.43</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>65</v>
+      <c r="H56" s="14" t="s">
+        <v>212</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -2312,7 +2353,7 @@
         <v>7</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C58" s="1">
         <v>55.31</v>
@@ -2321,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F58" s="6">
         <v>5.05</v>
@@ -2331,7 +2372,7 @@
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
@@ -2346,7 +2387,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F59" s="6">
         <f>+G58</f>
@@ -2370,7 +2411,7 @@
         <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F60" s="6">
         <f t="shared" ref="F60:F69" si="10">+G59</f>
@@ -2394,7 +2435,7 @@
         <v>4</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F61" s="6">
         <f t="shared" si="10"/>
@@ -2418,7 +2459,7 @@
         <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F62" s="6">
         <f t="shared" si="10"/>
@@ -2442,7 +2483,7 @@
         <v>6</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F63" s="6">
         <f t="shared" si="10"/>
@@ -2466,7 +2507,7 @@
         <v>7</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F64" s="6">
         <f t="shared" si="10"/>
@@ -2490,7 +2531,7 @@
         <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F65" s="6">
         <f t="shared" si="10"/>
@@ -2514,7 +2555,7 @@
         <v>9</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F66" s="6">
         <f t="shared" si="10"/>
@@ -2538,7 +2579,7 @@
         <v>10</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F67" s="6">
         <f t="shared" si="10"/>
@@ -2562,7 +2603,7 @@
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F68" s="6">
         <f t="shared" si="10"/>
@@ -2586,7 +2627,7 @@
         <v>12</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F69" s="6">
         <f t="shared" si="10"/>
@@ -2621,7 +2662,7 @@
         <v>6</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C71" s="1">
         <v>56.28</v>
@@ -2630,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F71" s="6">
         <v>4.2300000000000004</v>
@@ -2640,7 +2681,7 @@
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
@@ -2655,7 +2696,7 @@
         <v>2</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F72" s="6">
         <f>+G71</f>
@@ -2679,7 +2720,7 @@
         <v>3</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F73" s="6">
         <f t="shared" ref="F73:F106" si="12">+G72</f>
@@ -2703,7 +2744,7 @@
         <v>4</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F74" s="6">
         <f t="shared" si="12"/>
@@ -2727,7 +2768,7 @@
         <v>5</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F75" s="6">
         <f t="shared" si="12"/>
@@ -2751,7 +2792,7 @@
         <v>6</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F76" s="6">
         <f t="shared" si="12"/>
@@ -2775,7 +2816,7 @@
         <v>7</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F77" s="6">
         <f t="shared" si="12"/>
@@ -2799,7 +2840,7 @@
         <v>8</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F78" s="6">
         <f t="shared" si="12"/>
@@ -2823,7 +2864,7 @@
         <v>9</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F79" s="6">
         <f t="shared" si="12"/>
@@ -2847,7 +2888,7 @@
         <v>10</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F80" s="6">
         <f t="shared" si="12"/>
@@ -2871,7 +2912,7 @@
         <v>11</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F81" s="6">
         <f t="shared" si="12"/>
@@ -2895,7 +2936,7 @@
         <v>12</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F82" s="6">
         <f t="shared" si="12"/>
@@ -2919,7 +2960,7 @@
         <v>13</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F83" s="6">
         <f t="shared" si="12"/>
@@ -2943,7 +2984,7 @@
         <v>14</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F84" s="6">
         <f t="shared" si="12"/>
@@ -2965,7 +3006,7 @@
         <v>15</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F85" s="6">
         <f t="shared" si="12"/>
@@ -2981,7 +3022,7 @@
         <v>16</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F86" s="6">
         <f t="shared" si="12"/>
@@ -2997,7 +3038,7 @@
         <v>17</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F87" s="6">
         <f t="shared" si="12"/>
@@ -3013,7 +3054,7 @@
         <v>18</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F88" s="6">
         <f t="shared" si="12"/>
@@ -3029,7 +3070,7 @@
         <v>19</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F89" s="6">
         <f t="shared" si="12"/>
@@ -3045,7 +3086,7 @@
         <v>20</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F90" s="6">
         <f t="shared" si="12"/>
@@ -3061,7 +3102,7 @@
         <v>21</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F91" s="6">
         <f t="shared" si="12"/>
@@ -3077,7 +3118,7 @@
         <v>22</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F92" s="6">
         <f t="shared" si="12"/>
@@ -3093,7 +3134,7 @@
         <v>23</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F93" s="6">
         <f t="shared" si="12"/>
@@ -3109,7 +3150,7 @@
         <v>24</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F94" s="6">
         <f t="shared" si="12"/>
@@ -3125,7 +3166,7 @@
         <v>25</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F95" s="6">
         <f t="shared" si="12"/>
@@ -3141,7 +3182,7 @@
         <v>26</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F96" s="6">
         <f t="shared" si="12"/>
@@ -3166,7 +3207,7 @@
         <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C98" s="1">
         <v>50.24</v>
@@ -3175,7 +3216,7 @@
         <v>1</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F98" s="6">
         <v>0.28999999999999998</v>
@@ -3184,10 +3225,10 @@
         <v>2.0699999999999998</v>
       </c>
       <c r="H98" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I98" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -3198,7 +3239,7 @@
         <v>2</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F99" s="6">
         <f t="shared" si="12"/>
@@ -3218,7 +3259,7 @@
         <v>3</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F100" s="6">
         <f t="shared" si="12"/>
@@ -3238,7 +3279,7 @@
         <v>4</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F101" s="6">
         <f t="shared" si="12"/>
@@ -3258,7 +3299,7 @@
         <v>5</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F102" s="6">
         <f t="shared" si="12"/>
@@ -3278,7 +3319,7 @@
         <v>6</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F103" s="6">
         <f t="shared" si="12"/>
@@ -3298,7 +3339,7 @@
         <v>7</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F104" s="6">
         <f t="shared" si="12"/>
@@ -3318,7 +3359,7 @@
         <v>8</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F105" s="6">
         <f t="shared" si="12"/>
@@ -3338,7 +3379,7 @@
         <v>9</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F106" s="6">
         <f t="shared" si="12"/>
@@ -3365,7 +3406,7 @@
         <v>8</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C108" s="1">
         <v>53.53</v>
@@ -3374,7 +3415,7 @@
         <v>1</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F108" s="6">
         <v>1.46</v>
@@ -3384,7 +3425,7 @@
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -3395,7 +3436,7 @@
         <v>2</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F109" s="6">
         <f>+G108</f>
@@ -3415,7 +3456,7 @@
         <v>3</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F110" s="6">
         <f t="shared" ref="F110:F111" si="14">+G109</f>
@@ -3435,7 +3476,7 @@
         <v>4</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F111" s="6">
         <f t="shared" si="14"/>
@@ -3462,14 +3503,14 @@
         <v>9</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="4">
         <v>1</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F113" s="6">
         <v>1.25</v>
@@ -3479,7 +3520,7 @@
       </c>
       <c r="H113" s="1"/>
       <c r="I113" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -3490,7 +3531,7 @@
         <v>2</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F114" s="6">
         <f>+G113</f>
@@ -3510,7 +3551,7 @@
         <v>3</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F115" s="6">
         <f t="shared" ref="F115:F116" si="15">+G114</f>
@@ -3530,7 +3571,7 @@
         <v>4</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F116" s="6">
         <f t="shared" si="15"/>
@@ -3539,8 +3580,8 @@
       <c r="G116" s="6">
         <v>55.39</v>
       </c>
-      <c r="H116" s="1" t="s">
-        <v>137</v>
+      <c r="H116" s="14" t="s">
+        <v>211</v>
       </c>
       <c r="I116" s="1"/>
     </row>
@@ -3559,14 +3600,14 @@
         <v>10</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="4">
         <v>1</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F118" s="6">
         <v>1.07</v>
@@ -3576,7 +3617,7 @@
       </c>
       <c r="H118" s="1"/>
       <c r="I118" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -3587,7 +3628,7 @@
         <v>2</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F119" s="6">
         <f>+G118</f>
@@ -3597,7 +3638,7 @@
         <v>31.36</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I119" s="1"/>
     </row>
@@ -3609,7 +3650,7 @@
         <v>3</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F120" s="6">
         <v>35.130000000000003</v>
@@ -3628,7 +3669,7 @@
         <v>4</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F121" s="6">
         <f t="shared" ref="F121" si="17">+G120</f>
@@ -3637,8 +3678,8 @@
       <c r="G121" s="6">
         <v>59.38</v>
       </c>
-      <c r="H121" s="1" t="s">
-        <v>145</v>
+      <c r="H121" s="14" t="s">
+        <v>210</v>
       </c>
       <c r="I121" s="1"/>
     </row>
@@ -3657,14 +3698,14 @@
         <v>11</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="4">
         <v>1</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F123" s="6">
         <v>1.07</v>
@@ -3674,7 +3715,7 @@
       </c>
       <c r="H123" s="1"/>
       <c r="I123" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -3685,7 +3726,7 @@
         <v>2</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F124" s="6">
         <f>+G123</f>
@@ -3705,7 +3746,7 @@
         <v>3</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F125" s="6">
         <f t="shared" ref="F125:F127" si="19">+G124</f>
@@ -3725,7 +3766,7 @@
         <v>4</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F126" s="6">
         <f t="shared" si="19"/>
@@ -3745,7 +3786,7 @@
         <v>5</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F127" s="6">
         <f t="shared" si="19"/>
@@ -3772,16 +3813,16 @@
         <v>12</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D129" s="4">
         <v>1</v>
       </c>
       <c r="E129" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F129" s="6">
         <v>4.1900000000000004</v>
@@ -3791,7 +3832,7 @@
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -3802,7 +3843,7 @@
         <v>2</v>
       </c>
       <c r="E130" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F130" s="6">
         <f>+G129</f>
@@ -3812,7 +3853,7 @@
         <v>25</v>
       </c>
       <c r="H130" s="12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I130" s="1"/>
     </row>
@@ -3824,7 +3865,7 @@
         <v>3</v>
       </c>
       <c r="E131" s="12" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F131" s="6">
         <v>29</v>
@@ -3843,7 +3884,7 @@
         <v>4</v>
       </c>
       <c r="E132" s="12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F132" s="6">
         <f t="shared" ref="F132:F133" si="21">+G131</f>
@@ -3863,7 +3904,7 @@
         <v>5</v>
       </c>
       <c r="E133" s="12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F133" s="6">
         <f t="shared" si="21"/>
@@ -3872,7 +3913,9 @@
       <c r="G133" s="6">
         <v>59.01</v>
       </c>
-      <c r="H133" s="1"/>
+      <c r="H133" s="14" t="s">
+        <v>157</v>
+      </c>
       <c r="I133" s="1"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -3890,7 +3933,7 @@
         <v>13</v>
       </c>
       <c r="B135" s="12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C135" s="1">
         <v>55.29</v>
@@ -3899,7 +3942,7 @@
         <v>1</v>
       </c>
       <c r="E135" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F135" s="6">
         <v>1.03</v>
@@ -3909,7 +3952,7 @@
       </c>
       <c r="H135" s="1"/>
       <c r="I135" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -3920,7 +3963,7 @@
         <v>2</v>
       </c>
       <c r="E136" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F136" s="6">
         <f>+G135</f>
@@ -3939,8 +3982,8 @@
         <f t="shared" si="22"/>
         <v>3</v>
       </c>
-      <c r="E137" s="12" t="s">
-        <v>166</v>
+      <c r="E137" s="14" t="s">
+        <v>209</v>
       </c>
       <c r="F137" s="6">
         <v>37.549999999999997</v>
@@ -3948,7 +3991,9 @@
       <c r="G137" s="6">
         <v>54.17</v>
       </c>
-      <c r="H137" s="1"/>
+      <c r="H137" s="14" t="s">
+        <v>162</v>
+      </c>
       <c r="I137" s="1"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -3966,7 +4011,7 @@
         <v>14</v>
       </c>
       <c r="B139" s="12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C139" s="1">
         <v>52.45</v>
@@ -3975,7 +4020,7 @@
         <v>1</v>
       </c>
       <c r="E139" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F139" s="6">
         <v>1.05</v>
@@ -3985,7 +4030,7 @@
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -3996,7 +4041,7 @@
         <v>2</v>
       </c>
       <c r="E140" s="12" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F140" s="6">
         <f>+G139</f>
@@ -4006,7 +4051,7 @@
         <v>26.55</v>
       </c>
       <c r="H140" s="12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I140" s="1"/>
     </row>
@@ -4018,7 +4063,7 @@
         <v>3</v>
       </c>
       <c r="E141" s="12" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F141" s="6">
         <v>28.53</v>
@@ -4036,7 +4081,7 @@
         <v>4</v>
       </c>
       <c r="E142" s="12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F142" s="6">
         <f t="shared" ref="F142" si="23">+G141</f>
@@ -4045,7 +4090,9 @@
       <c r="G142" s="6">
         <v>51.34</v>
       </c>
-      <c r="H142" s="1"/>
+      <c r="H142" s="14" t="s">
+        <v>171</v>
+      </c>
       <c r="I142" s="1"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -4063,7 +4110,7 @@
         <v>15</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C144" s="1">
         <v>59.01</v>
@@ -4072,7 +4119,7 @@
         <v>1</v>
       </c>
       <c r="E144" s="12" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F144" s="6">
         <v>6.1</v>
@@ -4082,7 +4129,7 @@
       </c>
       <c r="H144" s="1"/>
       <c r="I144" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -4093,7 +4140,7 @@
         <v>2</v>
       </c>
       <c r="E145" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F145" s="6">
         <f>+G144</f>
@@ -4112,7 +4159,7 @@
         <v>3</v>
       </c>
       <c r="E146" s="12" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F146" s="6">
         <f>+G145</f>
@@ -4139,7 +4186,7 @@
         <v>16</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C148" s="1">
         <v>57.51</v>
@@ -4148,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="E148" s="12" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F148" s="6">
         <v>4.5</v>
@@ -4158,7 +4205,7 @@
       </c>
       <c r="H148" s="1"/>
       <c r="I148" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -4169,7 +4216,7 @@
         <v>2</v>
       </c>
       <c r="E149" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F149" s="6">
         <f>+G148</f>
@@ -4189,7 +4236,7 @@
         <v>3</v>
       </c>
       <c r="E150" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F150" s="6">
         <f t="shared" ref="F150:F152" si="26">+G149</f>
@@ -4209,7 +4256,7 @@
         <v>4</v>
       </c>
       <c r="E151" s="13" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F151" s="6">
         <f t="shared" si="26"/>
@@ -4229,7 +4276,7 @@
         <v>5</v>
       </c>
       <c r="E152" s="13" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F152" s="6">
         <f t="shared" si="26"/>
@@ -4238,7 +4285,9 @@
       <c r="G152" s="6">
         <v>55.39</v>
       </c>
-      <c r="H152" s="1"/>
+      <c r="H152" s="14" t="s">
+        <v>180</v>
+      </c>
       <c r="I152" s="1"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -4256,7 +4305,7 @@
         <v>17</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C154" s="1">
         <v>54.58</v>
@@ -4265,7 +4314,7 @@
         <v>1</v>
       </c>
       <c r="E154" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F154" s="6">
         <v>4.45</v>
@@ -4275,7 +4324,7 @@
       </c>
       <c r="H154" s="1"/>
       <c r="I154" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -4286,7 +4335,7 @@
         <v>2</v>
       </c>
       <c r="E155" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F155" s="6">
         <f>+G154</f>
@@ -4306,7 +4355,7 @@
         <v>3</v>
       </c>
       <c r="E156" s="13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F156" s="6">
         <f t="shared" ref="F156:F159" si="28">+G155</f>
@@ -4326,7 +4375,7 @@
         <v>4</v>
       </c>
       <c r="E157" s="13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F157" s="6">
         <f t="shared" si="28"/>
@@ -4346,7 +4395,7 @@
         <v>5</v>
       </c>
       <c r="E158" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F158" s="6">
         <f t="shared" si="28"/>
@@ -4366,7 +4415,7 @@
         <v>6</v>
       </c>
       <c r="E159" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F159" s="6">
         <f t="shared" si="28"/>
@@ -4375,7 +4424,9 @@
       <c r="G159" s="6">
         <v>53.04</v>
       </c>
-      <c r="H159" s="1"/>
+      <c r="H159" s="14" t="s">
+        <v>208</v>
+      </c>
       <c r="I159" s="1"/>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -4393,7 +4444,7 @@
         <v>18</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C161" s="1">
         <v>53.44</v>
@@ -4402,7 +4453,7 @@
         <v>1</v>
       </c>
       <c r="E161" s="13" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F161" s="6">
         <v>5.18</v>
@@ -4412,7 +4463,7 @@
       </c>
       <c r="H161" s="1"/>
       <c r="I161" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -4423,7 +4474,7 @@
         <v>2</v>
       </c>
       <c r="E162" s="13" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F162" s="6">
         <f>+G161</f>
@@ -4443,7 +4494,7 @@
         <v>3</v>
       </c>
       <c r="E163" s="13" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F163" s="6">
         <f t="shared" ref="F163:F167" si="30">+G162</f>
@@ -4463,7 +4514,7 @@
         <v>4</v>
       </c>
       <c r="E164" s="13" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F164" s="6">
         <f t="shared" si="30"/>
@@ -4483,7 +4534,7 @@
         <v>5</v>
       </c>
       <c r="E165" s="13" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F165" s="6">
         <f t="shared" si="30"/>
@@ -4503,7 +4554,7 @@
         <v>6</v>
       </c>
       <c r="E166" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F166" s="6">
         <f t="shared" si="30"/>
@@ -4523,7 +4574,7 @@
         <v>7</v>
       </c>
       <c r="E167" s="13" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F167" s="6">
         <f t="shared" si="30"/>
@@ -4550,7 +4601,7 @@
         <v>19</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C169" s="6">
         <v>58.4</v>
@@ -4559,7 +4610,7 @@
         <v>1</v>
       </c>
       <c r="E169" s="13" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F169" s="6">
         <v>6.21</v>
@@ -4569,7 +4620,7 @@
       </c>
       <c r="H169" s="1"/>
       <c r="I169" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -4580,7 +4631,7 @@
         <v>2</v>
       </c>
       <c r="E170" s="13" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F170" s="6">
         <f>+G169</f>
@@ -4600,7 +4651,7 @@
         <v>3</v>
       </c>
       <c r="E171" s="13" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F171" s="6">
         <f t="shared" ref="F171:F174" si="32">+G170</f>
@@ -4620,7 +4671,7 @@
         <v>4</v>
       </c>
       <c r="E172" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F172" s="6">
         <f t="shared" si="32"/>
@@ -4640,7 +4691,7 @@
         <v>5</v>
       </c>
       <c r="E173" s="13" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F173" s="6">
         <f t="shared" si="32"/>
@@ -4660,7 +4711,7 @@
         <v>6</v>
       </c>
       <c r="E174" s="13" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F174" s="6">
         <f t="shared" si="32"/>
@@ -4670,7 +4721,7 @@
         <v>55.13</v>
       </c>
       <c r="H174" s="13" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I174" s="1"/>
     </row>
@@ -4685,72 +4736,149 @@
       <c r="I175" s="1"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B176" s="1"/>
-      <c r="C176" s="1"/>
-      <c r="D176" s="4"/>
-      <c r="E176" s="1"/>
-      <c r="F176" s="6"/>
-      <c r="G176" s="6"/>
+      <c r="A176" s="1">
+        <v>20</v>
+      </c>
+      <c r="B176" s="2">
+        <v>44042</v>
+      </c>
+      <c r="C176" s="1">
+        <v>57.06</v>
+      </c>
+      <c r="D176" s="4">
+        <v>1</v>
+      </c>
+      <c r="E176" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="F176" s="6">
+        <v>7.48</v>
+      </c>
+      <c r="G176" s="6">
+        <v>11.1</v>
+      </c>
       <c r="H176" s="1"/>
-      <c r="I176" s="1"/>
+      <c r="I176" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
-      <c r="D177" s="4"/>
-      <c r="E177" s="1"/>
-      <c r="F177" s="6"/>
-      <c r="G177" s="6"/>
+      <c r="D177" s="4">
+        <f>+D176+1</f>
+        <v>2</v>
+      </c>
+      <c r="E177" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="F177" s="6">
+        <f>+G176</f>
+        <v>11.1</v>
+      </c>
+      <c r="G177" s="6">
+        <v>22.42</v>
+      </c>
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
-      <c r="D178" s="4"/>
-      <c r="E178" s="1"/>
-      <c r="F178" s="6"/>
-      <c r="G178" s="6"/>
+      <c r="D178" s="4">
+        <f t="shared" ref="D178:D182" si="33">+D177+1</f>
+        <v>3</v>
+      </c>
+      <c r="E178" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="F178" s="6">
+        <f t="shared" ref="F178:F182" si="34">+G177</f>
+        <v>22.42</v>
+      </c>
+      <c r="G178" s="6">
+        <v>29.52</v>
+      </c>
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
-      <c r="D179" s="4"/>
-      <c r="E179" s="1"/>
-      <c r="F179" s="6"/>
-      <c r="G179" s="6"/>
+      <c r="D179" s="4">
+        <f t="shared" si="33"/>
+        <v>4</v>
+      </c>
+      <c r="E179" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F179" s="6">
+        <f t="shared" si="34"/>
+        <v>29.52</v>
+      </c>
+      <c r="G179" s="6">
+        <v>37.020000000000003</v>
+      </c>
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
     </row>
     <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
-      <c r="D180" s="4"/>
-      <c r="E180" s="1"/>
-      <c r="F180" s="6"/>
-      <c r="G180" s="6"/>
+      <c r="D180" s="4">
+        <f t="shared" si="33"/>
+        <v>5</v>
+      </c>
+      <c r="E180" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="F180" s="6">
+        <f t="shared" si="34"/>
+        <v>37.020000000000003</v>
+      </c>
+      <c r="G180" s="6">
+        <v>45.22</v>
+      </c>
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
     </row>
     <row r="181" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
-      <c r="D181" s="4"/>
-      <c r="E181" s="1"/>
-      <c r="F181" s="6"/>
-      <c r="G181" s="6"/>
+      <c r="D181" s="4">
+        <f t="shared" si="33"/>
+        <v>6</v>
+      </c>
+      <c r="E181" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="F181" s="6">
+        <f t="shared" si="34"/>
+        <v>45.22</v>
+      </c>
+      <c r="G181" s="6">
+        <v>48.55</v>
+      </c>
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
-      <c r="D182" s="4"/>
-      <c r="E182" s="1"/>
-      <c r="F182" s="6"/>
-      <c r="G182" s="6"/>
+      <c r="D182" s="4">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="E182" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="F182" s="6">
+        <f t="shared" si="34"/>
+        <v>48.55</v>
+      </c>
+      <c r="G182" s="6">
+        <v>54.4</v>
+      </c>
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
     </row>

</xml_diff>

<commit_message>
TS Jatai working with TS 1.1 template 02/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
+    <sheet name="Kandam2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="229">
   <si>
     <t>Date</t>
   </si>
@@ -457,9 +458,6 @@
     <t>1.6.4.1</t>
   </si>
   <si>
-    <t xml:space="preserve">First round </t>
-  </si>
-  <si>
     <t>22/07/2020</t>
   </si>
   <si>
@@ -677,19 +675,52 @@
   </si>
   <si>
     <t>H2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Dvb7hq_Z4ng</t>
+  </si>
+  <si>
+    <t>1.8.19.1</t>
+  </si>
+  <si>
+    <t>1.8.20.1</t>
+  </si>
+  <si>
+    <t>1.8.21.1</t>
+  </si>
+  <si>
+    <t>1.8.22.1</t>
+  </si>
+  <si>
+    <t>2.1.1.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fwQugM1P_7c</t>
+  </si>
+  <si>
+    <t>2.1.2.1</t>
+  </si>
+  <si>
+    <t>2.1.3.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -741,7 +772,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -751,12 +782,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,31 +810,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1116,10 +1142,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1300,8 +1326,8 @@
       <c r="G11" s="6">
         <v>33.380000000000003</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>220</v>
+      <c r="H11" s="15" t="s">
+        <v>219</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>67</v>
@@ -1415,8 +1441,8 @@
       <c r="G16" s="6">
         <v>30.56</v>
       </c>
-      <c r="H16" s="17" t="s">
-        <v>220</v>
+      <c r="H16" s="16" t="s">
+        <v>219</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1460,7 +1486,7 @@
       <c r="G18" s="6">
         <v>52.12</v>
       </c>
-      <c r="H18" s="11"/>
+      <c r="H18" s="10"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1550,8 +1576,8 @@
       <c r="G22" s="6">
         <v>29.49</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>147</v>
+      <c r="H22" s="16" t="s">
+        <v>219</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1621,7 +1647,7 @@
       <c r="G25" s="6">
         <v>49.18</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="13" t="s">
         <v>28</v>
       </c>
       <c r="I25" s="1"/>
@@ -2353,8 +2379,8 @@
       <c r="G56" s="6">
         <v>50.43</v>
       </c>
-      <c r="H56" s="14" t="s">
-        <v>211</v>
+      <c r="H56" s="13" t="s">
+        <v>210</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -3608,8 +3634,8 @@
       <c r="G116" s="6">
         <v>55.39</v>
       </c>
-      <c r="H116" s="14" t="s">
-        <v>210</v>
+      <c r="H116" s="13" t="s">
+        <v>209</v>
       </c>
       <c r="I116" s="1"/>
     </row>
@@ -3706,8 +3732,8 @@
       <c r="G121" s="6">
         <v>59.38</v>
       </c>
-      <c r="H121" s="14" t="s">
-        <v>209</v>
+      <c r="H121" s="13" t="s">
+        <v>208</v>
       </c>
       <c r="I121" s="1"/>
     </row>
@@ -3743,7 +3769,7 @@
       </c>
       <c r="H123" s="1"/>
       <c r="I123" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -3840,17 +3866,17 @@
       <c r="A129" s="1">
         <v>12</v>
       </c>
-      <c r="B129" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C129" s="12" t="s">
-        <v>150</v>
+      <c r="B129" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C129" s="11" t="s">
+        <v>149</v>
       </c>
       <c r="D129" s="4">
         <v>1</v>
       </c>
-      <c r="E129" s="12" t="s">
-        <v>149</v>
+      <c r="E129" s="11" t="s">
+        <v>148</v>
       </c>
       <c r="F129" s="6">
         <v>4.1900000000000004</v>
@@ -3860,7 +3886,7 @@
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -3870,8 +3896,8 @@
         <f t="shared" ref="D130:D133" si="20">+D129+1</f>
         <v>2</v>
       </c>
-      <c r="E130" s="12" t="s">
-        <v>152</v>
+      <c r="E130" s="11" t="s">
+        <v>151</v>
       </c>
       <c r="F130" s="6">
         <f>+G129</f>
@@ -3880,8 +3906,8 @@
       <c r="G130" s="6">
         <v>25</v>
       </c>
-      <c r="H130" s="12" t="s">
-        <v>153</v>
+      <c r="H130" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="I130" s="1"/>
     </row>
@@ -3892,8 +3918,8 @@
         <f t="shared" si="20"/>
         <v>3</v>
       </c>
-      <c r="E131" s="12" t="s">
-        <v>154</v>
+      <c r="E131" s="11" t="s">
+        <v>153</v>
       </c>
       <c r="F131" s="6">
         <v>29</v>
@@ -3911,8 +3937,8 @@
         <f t="shared" si="20"/>
         <v>4</v>
       </c>
-      <c r="E132" s="12" t="s">
-        <v>155</v>
+      <c r="E132" s="11" t="s">
+        <v>154</v>
       </c>
       <c r="F132" s="6">
         <f t="shared" ref="F132:F133" si="21">+G131</f>
@@ -3931,8 +3957,8 @@
         <f t="shared" si="20"/>
         <v>5</v>
       </c>
-      <c r="E133" s="12" t="s">
-        <v>156</v>
+      <c r="E133" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="F133" s="6">
         <f t="shared" si="21"/>
@@ -3941,8 +3967,8 @@
       <c r="G133" s="6">
         <v>59.01</v>
       </c>
-      <c r="H133" s="14" t="s">
-        <v>156</v>
+      <c r="H133" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="I133" s="1"/>
     </row>
@@ -3960,8 +3986,8 @@
       <c r="A135" s="1">
         <v>13</v>
       </c>
-      <c r="B135" s="12" t="s">
-        <v>157</v>
+      <c r="B135" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="C135" s="1">
         <v>55.29</v>
@@ -3969,8 +3995,8 @@
       <c r="D135" s="4">
         <v>1</v>
       </c>
-      <c r="E135" s="12" t="s">
-        <v>159</v>
+      <c r="E135" s="11" t="s">
+        <v>158</v>
       </c>
       <c r="F135" s="6">
         <v>1.03</v>
@@ -3980,7 +4006,7 @@
       </c>
       <c r="H135" s="1"/>
       <c r="I135" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -3990,8 +4016,8 @@
         <f t="shared" ref="D136:D141" si="22">+D135+1</f>
         <v>2</v>
       </c>
-      <c r="E136" s="12" t="s">
-        <v>160</v>
+      <c r="E136" s="11" t="s">
+        <v>159</v>
       </c>
       <c r="F136" s="6">
         <f>+G135</f>
@@ -4010,8 +4036,8 @@
         <f t="shared" si="22"/>
         <v>3</v>
       </c>
-      <c r="E137" s="14" t="s">
-        <v>208</v>
+      <c r="E137" s="13" t="s">
+        <v>207</v>
       </c>
       <c r="F137" s="6">
         <v>37.549999999999997</v>
@@ -4019,8 +4045,8 @@
       <c r="G137" s="6">
         <v>54.17</v>
       </c>
-      <c r="H137" s="14" t="s">
-        <v>161</v>
+      <c r="H137" s="13" t="s">
+        <v>160</v>
       </c>
       <c r="I137" s="1"/>
     </row>
@@ -4038,8 +4064,8 @@
       <c r="A139" s="1">
         <v>14</v>
       </c>
-      <c r="B139" s="12" t="s">
-        <v>162</v>
+      <c r="B139" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="C139" s="1">
         <v>52.45</v>
@@ -4047,8 +4073,8 @@
       <c r="D139" s="4">
         <v>1</v>
       </c>
-      <c r="E139" s="12" t="s">
-        <v>164</v>
+      <c r="E139" s="11" t="s">
+        <v>163</v>
       </c>
       <c r="F139" s="6">
         <v>1.05</v>
@@ -4058,7 +4084,7 @@
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -4068,8 +4094,8 @@
         <f t="shared" si="22"/>
         <v>2</v>
       </c>
-      <c r="E140" s="12" t="s">
-        <v>166</v>
+      <c r="E140" s="11" t="s">
+        <v>165</v>
       </c>
       <c r="F140" s="6">
         <f>+G139</f>
@@ -4078,8 +4104,8 @@
       <c r="G140" s="6">
         <v>26.55</v>
       </c>
-      <c r="H140" s="12" t="s">
-        <v>153</v>
+      <c r="H140" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="I140" s="1"/>
     </row>
@@ -4090,8 +4116,8 @@
         <f t="shared" si="22"/>
         <v>3</v>
       </c>
-      <c r="E141" s="12" t="s">
-        <v>169</v>
+      <c r="E141" s="11" t="s">
+        <v>168</v>
       </c>
       <c r="F141" s="6">
         <v>28.53</v>
@@ -4108,8 +4134,8 @@
       <c r="D142" s="4">
         <v>4</v>
       </c>
-      <c r="E142" s="12" t="s">
-        <v>170</v>
+      <c r="E142" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="F142" s="6">
         <f t="shared" ref="F142" si="23">+G141</f>
@@ -4118,8 +4144,8 @@
       <c r="G142" s="6">
         <v>51.34</v>
       </c>
-      <c r="H142" s="14" t="s">
-        <v>170</v>
+      <c r="H142" s="13" t="s">
+        <v>169</v>
       </c>
       <c r="I142" s="1"/>
     </row>
@@ -4137,8 +4163,8 @@
       <c r="A144" s="1">
         <v>15</v>
       </c>
-      <c r="B144" s="12" t="s">
-        <v>167</v>
+      <c r="B144" s="11" t="s">
+        <v>166</v>
       </c>
       <c r="C144" s="1">
         <v>59.01</v>
@@ -4146,8 +4172,8 @@
       <c r="D144" s="4">
         <v>1</v>
       </c>
-      <c r="E144" s="12" t="s">
-        <v>171</v>
+      <c r="E144" s="11" t="s">
+        <v>170</v>
       </c>
       <c r="F144" s="6">
         <v>6.1</v>
@@ -4157,7 +4183,7 @@
       </c>
       <c r="H144" s="1"/>
       <c r="I144" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -4167,8 +4193,8 @@
         <f t="shared" ref="D145" si="24">+D144+1</f>
         <v>2</v>
       </c>
-      <c r="E145" s="12" t="s">
-        <v>172</v>
+      <c r="E145" s="11" t="s">
+        <v>171</v>
       </c>
       <c r="F145" s="6">
         <f>+G144</f>
@@ -4186,8 +4212,8 @@
       <c r="D146" s="4">
         <v>3</v>
       </c>
-      <c r="E146" s="12" t="s">
-        <v>173</v>
+      <c r="E146" s="11" t="s">
+        <v>172</v>
       </c>
       <c r="F146" s="6">
         <f>+G145</f>
@@ -4213,8 +4239,8 @@
       <c r="A148" s="1">
         <v>16</v>
       </c>
-      <c r="B148" s="12" t="s">
-        <v>174</v>
+      <c r="B148" s="11" t="s">
+        <v>173</v>
       </c>
       <c r="C148" s="1">
         <v>57.51</v>
@@ -4222,8 +4248,8 @@
       <c r="D148" s="4">
         <v>1</v>
       </c>
-      <c r="E148" s="12" t="s">
-        <v>175</v>
+      <c r="E148" s="11" t="s">
+        <v>174</v>
       </c>
       <c r="F148" s="6">
         <v>4.5</v>
@@ -4233,7 +4259,7 @@
       </c>
       <c r="H148" s="1"/>
       <c r="I148" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -4243,8 +4269,8 @@
         <f t="shared" ref="D149:D152" si="25">+D148+1</f>
         <v>2</v>
       </c>
-      <c r="E149" s="13" t="s">
-        <v>176</v>
+      <c r="E149" s="12" t="s">
+        <v>175</v>
       </c>
       <c r="F149" s="6">
         <f>+G148</f>
@@ -4263,8 +4289,8 @@
         <f t="shared" si="25"/>
         <v>3</v>
       </c>
-      <c r="E150" s="13" t="s">
-        <v>177</v>
+      <c r="E150" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="F150" s="6">
         <f t="shared" ref="F150:F152" si="26">+G149</f>
@@ -4283,8 +4309,8 @@
         <f t="shared" si="25"/>
         <v>4</v>
       </c>
-      <c r="E151" s="13" t="s">
-        <v>178</v>
+      <c r="E151" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="F151" s="6">
         <f t="shared" si="26"/>
@@ -4303,8 +4329,8 @@
         <f t="shared" si="25"/>
         <v>5</v>
       </c>
-      <c r="E152" s="13" t="s">
-        <v>179</v>
+      <c r="E152" s="12" t="s">
+        <v>178</v>
       </c>
       <c r="F152" s="6">
         <f t="shared" si="26"/>
@@ -4313,8 +4339,8 @@
       <c r="G152" s="6">
         <v>55.39</v>
       </c>
-      <c r="H152" s="14" t="s">
-        <v>179</v>
+      <c r="H152" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="I152" s="1"/>
     </row>
@@ -4332,8 +4358,8 @@
       <c r="A154" s="1">
         <v>17</v>
       </c>
-      <c r="B154" s="13" t="s">
-        <v>181</v>
+      <c r="B154" s="12" t="s">
+        <v>180</v>
       </c>
       <c r="C154" s="1">
         <v>54.58</v>
@@ -4341,8 +4367,8 @@
       <c r="D154" s="4">
         <v>1</v>
       </c>
-      <c r="E154" s="13" t="s">
-        <v>182</v>
+      <c r="E154" s="12" t="s">
+        <v>181</v>
       </c>
       <c r="F154" s="6">
         <v>4.45</v>
@@ -4352,7 +4378,7 @@
       </c>
       <c r="H154" s="1"/>
       <c r="I154" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -4362,8 +4388,8 @@
         <f>+D154+1</f>
         <v>2</v>
       </c>
-      <c r="E155" s="13" t="s">
-        <v>183</v>
+      <c r="E155" s="12" t="s">
+        <v>182</v>
       </c>
       <c r="F155" s="6">
         <f>+G154</f>
@@ -4382,8 +4408,8 @@
         <f t="shared" ref="D156:D159" si="27">+D155+1</f>
         <v>3</v>
       </c>
-      <c r="E156" s="13" t="s">
-        <v>184</v>
+      <c r="E156" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="F156" s="6">
         <f t="shared" ref="F156:F159" si="28">+G155</f>
@@ -4402,8 +4428,8 @@
         <f t="shared" si="27"/>
         <v>4</v>
       </c>
-      <c r="E157" s="13" t="s">
-        <v>185</v>
+      <c r="E157" s="12" t="s">
+        <v>184</v>
       </c>
       <c r="F157" s="6">
         <f t="shared" si="28"/>
@@ -4422,8 +4448,8 @@
         <f t="shared" si="27"/>
         <v>5</v>
       </c>
-      <c r="E158" s="13" t="s">
-        <v>186</v>
+      <c r="E158" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="F158" s="6">
         <f t="shared" si="28"/>
@@ -4442,8 +4468,8 @@
         <f t="shared" si="27"/>
         <v>6</v>
       </c>
-      <c r="E159" s="13" t="s">
-        <v>187</v>
+      <c r="E159" s="12" t="s">
+        <v>186</v>
       </c>
       <c r="F159" s="6">
         <f t="shared" si="28"/>
@@ -4452,8 +4478,8 @@
       <c r="G159" s="6">
         <v>53.04</v>
       </c>
-      <c r="H159" s="14" t="s">
-        <v>207</v>
+      <c r="H159" s="13" t="s">
+        <v>206</v>
       </c>
       <c r="I159" s="1"/>
     </row>
@@ -4471,8 +4497,8 @@
       <c r="A161" s="1">
         <v>18</v>
       </c>
-      <c r="B161" s="13" t="s">
-        <v>189</v>
+      <c r="B161" s="12" t="s">
+        <v>188</v>
       </c>
       <c r="C161" s="1">
         <v>53.44</v>
@@ -4480,8 +4506,8 @@
       <c r="D161" s="4">
         <v>1</v>
       </c>
-      <c r="E161" s="13" t="s">
-        <v>190</v>
+      <c r="E161" s="12" t="s">
+        <v>189</v>
       </c>
       <c r="F161" s="6">
         <v>5.18</v>
@@ -4491,7 +4517,7 @@
       </c>
       <c r="H161" s="1"/>
       <c r="I161" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -4501,8 +4527,8 @@
         <f>+D161+1</f>
         <v>2</v>
       </c>
-      <c r="E162" s="13" t="s">
-        <v>192</v>
+      <c r="E162" s="12" t="s">
+        <v>191</v>
       </c>
       <c r="F162" s="6">
         <f>+G161</f>
@@ -4521,8 +4547,8 @@
         <f t="shared" ref="D163:D167" si="29">+D162+1</f>
         <v>3</v>
       </c>
-      <c r="E163" s="13" t="s">
-        <v>193</v>
+      <c r="E163" s="12" t="s">
+        <v>192</v>
       </c>
       <c r="F163" s="6">
         <f t="shared" ref="F163:F167" si="30">+G162</f>
@@ -4541,8 +4567,8 @@
         <f t="shared" si="29"/>
         <v>4</v>
       </c>
-      <c r="E164" s="13" t="s">
-        <v>194</v>
+      <c r="E164" s="12" t="s">
+        <v>193</v>
       </c>
       <c r="F164" s="6">
         <f t="shared" si="30"/>
@@ -4561,8 +4587,8 @@
         <f t="shared" si="29"/>
         <v>5</v>
       </c>
-      <c r="E165" s="13" t="s">
-        <v>195</v>
+      <c r="E165" s="12" t="s">
+        <v>194</v>
       </c>
       <c r="F165" s="6">
         <f t="shared" si="30"/>
@@ -4581,8 +4607,8 @@
         <f t="shared" si="29"/>
         <v>6</v>
       </c>
-      <c r="E166" s="13" t="s">
-        <v>196</v>
+      <c r="E166" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="F166" s="6">
         <f t="shared" si="30"/>
@@ -4601,8 +4627,8 @@
         <f t="shared" si="29"/>
         <v>7</v>
       </c>
-      <c r="E167" s="13" t="s">
-        <v>197</v>
+      <c r="E167" s="12" t="s">
+        <v>196</v>
       </c>
       <c r="F167" s="6">
         <f t="shared" si="30"/>
@@ -4628,8 +4654,8 @@
       <c r="A169" s="1">
         <v>19</v>
       </c>
-      <c r="B169" s="13" t="s">
-        <v>198</v>
+      <c r="B169" s="12" t="s">
+        <v>197</v>
       </c>
       <c r="C169" s="6">
         <v>58.4</v>
@@ -4637,8 +4663,8 @@
       <c r="D169" s="4">
         <v>1</v>
       </c>
-      <c r="E169" s="13" t="s">
-        <v>200</v>
+      <c r="E169" s="12" t="s">
+        <v>199</v>
       </c>
       <c r="F169" s="6">
         <v>6.21</v>
@@ -4648,7 +4674,7 @@
       </c>
       <c r="H169" s="1"/>
       <c r="I169" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -4658,8 +4684,8 @@
         <f>+D169+1</f>
         <v>2</v>
       </c>
-      <c r="E170" s="13" t="s">
-        <v>201</v>
+      <c r="E170" s="12" t="s">
+        <v>200</v>
       </c>
       <c r="F170" s="6">
         <f>+G169</f>
@@ -4678,8 +4704,8 @@
         <f t="shared" ref="D171:D174" si="31">+D170+1</f>
         <v>3</v>
       </c>
-      <c r="E171" s="13" t="s">
-        <v>202</v>
+      <c r="E171" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="F171" s="6">
         <f t="shared" ref="F171:F174" si="32">+G170</f>
@@ -4698,8 +4724,8 @@
         <f t="shared" si="31"/>
         <v>4</v>
       </c>
-      <c r="E172" s="13" t="s">
-        <v>203</v>
+      <c r="E172" s="12" t="s">
+        <v>202</v>
       </c>
       <c r="F172" s="6">
         <f t="shared" si="32"/>
@@ -4718,8 +4744,8 @@
         <f t="shared" si="31"/>
         <v>5</v>
       </c>
-      <c r="E173" s="13" t="s">
-        <v>204</v>
+      <c r="E173" s="12" t="s">
+        <v>203</v>
       </c>
       <c r="F173" s="6">
         <f t="shared" si="32"/>
@@ -4738,8 +4764,8 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="E174" s="13" t="s">
-        <v>205</v>
+      <c r="E174" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="F174" s="6">
         <f t="shared" si="32"/>
@@ -4748,8 +4774,8 @@
       <c r="G174" s="6">
         <v>55.13</v>
       </c>
-      <c r="H174" s="13" t="s">
-        <v>206</v>
+      <c r="H174" s="12" t="s">
+        <v>205</v>
       </c>
       <c r="I174" s="1"/>
     </row>
@@ -4776,8 +4802,8 @@
       <c r="D176" s="4">
         <v>1</v>
       </c>
-      <c r="E176" s="15" t="s">
-        <v>213</v>
+      <c r="E176" s="14" t="s">
+        <v>212</v>
       </c>
       <c r="F176" s="6">
         <v>7.48</v>
@@ -4787,18 +4813,18 @@
       </c>
       <c r="H176" s="1"/>
       <c r="I176" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="4">
         <f>+D176+1</f>
         <v>2</v>
       </c>
-      <c r="E177" s="15" t="s">
-        <v>214</v>
+      <c r="E177" s="14" t="s">
+        <v>213</v>
       </c>
       <c r="F177" s="6">
         <f>+G176</f>
@@ -4810,15 +4836,15 @@
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="4">
         <f t="shared" ref="D178:D182" si="33">+D177+1</f>
         <v>3</v>
       </c>
-      <c r="E178" s="15" t="s">
-        <v>215</v>
+      <c r="E178" s="14" t="s">
+        <v>214</v>
       </c>
       <c r="F178" s="6">
         <f t="shared" ref="F178:F182" si="34">+G177</f>
@@ -4830,15 +4856,15 @@
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="4">
         <f t="shared" si="33"/>
         <v>4</v>
       </c>
-      <c r="E179" s="15" t="s">
-        <v>216</v>
+      <c r="E179" s="14" t="s">
+        <v>215</v>
       </c>
       <c r="F179" s="6">
         <f t="shared" si="34"/>
@@ -4850,15 +4876,15 @@
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="4">
         <f t="shared" si="33"/>
         <v>5</v>
       </c>
-      <c r="E180" s="15" t="s">
-        <v>217</v>
+      <c r="E180" s="14" t="s">
+        <v>216</v>
       </c>
       <c r="F180" s="6">
         <f t="shared" si="34"/>
@@ -4870,15 +4896,15 @@
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="4">
         <f t="shared" si="33"/>
         <v>6</v>
       </c>
-      <c r="E181" s="15" t="s">
-        <v>218</v>
+      <c r="E181" s="14" t="s">
+        <v>217</v>
       </c>
       <c r="F181" s="6">
         <f t="shared" si="34"/>
@@ -4890,15 +4916,15 @@
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="4">
         <f t="shared" si="33"/>
         <v>7</v>
       </c>
-      <c r="E182" s="15" t="s">
-        <v>219</v>
+      <c r="E182" s="14" t="s">
+        <v>218</v>
       </c>
       <c r="F182" s="6">
         <f t="shared" si="34"/>
@@ -4910,7 +4936,7 @@
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="4"/>
@@ -4920,57 +4946,100 @@
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B184" s="1"/>
-      <c r="C184" s="1"/>
-      <c r="D184" s="4"/>
-      <c r="E184" s="1"/>
-      <c r="F184" s="6"/>
-      <c r="G184" s="6"/>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>21</v>
+      </c>
+      <c r="B184" s="2">
+        <v>44043</v>
+      </c>
+      <c r="C184" s="1">
+        <v>39.44</v>
+      </c>
+      <c r="D184" s="4">
+        <v>1</v>
+      </c>
+      <c r="E184" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="F184" s="6">
+        <v>2.04</v>
+      </c>
+      <c r="G184" s="6">
+        <v>6.33</v>
+      </c>
       <c r="H184" s="1"/>
-      <c r="I184" s="1"/>
-    </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I184" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
-      <c r="D185" s="4"/>
-      <c r="E185" s="1"/>
-      <c r="F185" s="6"/>
-      <c r="G185" s="6"/>
+      <c r="D185" s="4">
+        <f>+D184+1</f>
+        <v>2</v>
+      </c>
+      <c r="E185" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F185" s="6">
+        <f>+G184</f>
+        <v>6.33</v>
+      </c>
+      <c r="G185" s="6">
+        <v>9.34</v>
+      </c>
       <c r="H185" s="1"/>
       <c r="I185" s="1"/>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
-      <c r="D186" s="4"/>
-      <c r="E186" s="1"/>
-      <c r="F186" s="6"/>
+      <c r="D186" s="4">
+        <f t="shared" ref="D186:D188" si="35">+D185+1</f>
+        <v>3</v>
+      </c>
+      <c r="E186" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F186" s="6">
+        <f t="shared" ref="F186:F187" si="36">+G185</f>
+        <v>9.34</v>
+      </c>
       <c r="G186" s="6"/>
       <c r="H186" s="1"/>
       <c r="I186" s="1"/>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
-      <c r="D187" s="4"/>
-      <c r="E187" s="1"/>
-      <c r="F187" s="6"/>
+      <c r="D187" s="4">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
+      <c r="E187" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="F187" s="6">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
       <c r="G187" s="6"/>
       <c r="H187" s="1"/>
       <c r="I187" s="1"/>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="4"/>
-      <c r="E188" s="1"/>
+      <c r="E188" s="17"/>
       <c r="F188" s="6"/>
       <c r="G188" s="6"/>
       <c r="H188" s="1"/>
       <c r="I188" s="1"/>
     </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="4"/>
@@ -4980,7 +5049,7 @@
       <c r="H189" s="1"/>
       <c r="I189" s="1"/>
     </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="4"/>
@@ -4990,7 +5059,7 @@
       <c r="H190" s="1"/>
       <c r="I190" s="1"/>
     </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="4"/>
@@ -5000,7 +5069,7 @@
       <c r="H191" s="1"/>
       <c r="I191" s="1"/>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="4"/>
@@ -5844,4 +5913,524 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="D3" s="7"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44044</v>
+      </c>
+      <c r="C4" s="1">
+        <v>57.23</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="18">
+        <v>22.28</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="4">
+        <f>+D4+1</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" s="6">
+        <f>+G4</f>
+        <v>22.28</v>
+      </c>
+      <c r="G5" s="18">
+        <v>53.37</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="4">
+        <f>+D5+1</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="6">
+        <f>+G5</f>
+        <v>53.37</v>
+      </c>
+      <c r="G6" s="18">
+        <v>56.43</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TS 2 and Chamaka Ghanam 04/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="238">
   <si>
     <t>Date</t>
   </si>
@@ -702,19 +702,58 @@
   </si>
   <si>
     <t>2.1.3.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hwx-JaRX2Yk</t>
+  </si>
+  <si>
+    <t>2.1.3.2</t>
+  </si>
+  <si>
+    <t>2.1.4.1</t>
+  </si>
+  <si>
+    <t>2.1.5.1</t>
+  </si>
+  <si>
+    <t>2.1.5.4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RJ0rC1roGYE</t>
+  </si>
+  <si>
+    <t>2.1.5.5</t>
+  </si>
+  <si>
+    <t>2.1.6.1</t>
+  </si>
+  <si>
+    <t>2.1.7.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -810,32 +849,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,7 +1186,7 @@
     <sheetView topLeftCell="A4" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="G186" sqref="G186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4997,7 +5038,7 @@
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="4">
-        <f t="shared" ref="D186:D188" si="35">+D185+1</f>
+        <f t="shared" ref="D186:D187" si="35">+D185+1</f>
         <v>3</v>
       </c>
       <c r="E186" s="17" t="s">
@@ -5920,7 +5961,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6078,36 +6119,75 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="18"/>
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44045</v>
+      </c>
+      <c r="C8" s="1">
+        <v>59.23</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="G8" s="18">
+        <v>16.13</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="1"/>
+      <c r="D9" s="4">
+        <f>+D8+1</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="F9" s="6">
+        <f>+G8</f>
+        <v>16.13</v>
+      </c>
+      <c r="G9" s="18">
+        <v>43.12</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>152</v>
+      </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="1"/>
+      <c r="D10" s="4">
+        <f>+D9+1</f>
+        <v>3</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="F10" s="6">
+        <v>45.55</v>
+      </c>
+      <c r="G10" s="18">
+        <v>58.23</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>233</v>
+      </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.25">
@@ -6122,24 +6202,50 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="18"/>
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>44046</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44.33</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="F12" s="6">
+        <v>3.22</v>
+      </c>
+      <c r="G12" s="18">
+        <v>13.19</v>
+      </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="4">
+        <f>+D12+1</f>
+        <v>2</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="6">
+        <f>+G12</f>
+        <v>13.19</v>
+      </c>
+      <c r="G13" s="18">
+        <v>30.39</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
@@ -6147,10 +6253,20 @@
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="4">
+        <f>+D13+1</f>
+        <v>3</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="F14" s="6">
+        <f>+G13</f>
+        <v>30.39</v>
+      </c>
+      <c r="G14" s="18">
+        <v>43.54</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>

</xml_diff>

<commit_message>
TS 4.7 PP template and TTD
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="249">
   <si>
     <t>Date</t>
   </si>
@@ -729,19 +729,58 @@
   </si>
   <si>
     <t>2.1.7.1</t>
+  </si>
+  <si>
+    <t>1.02.20</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=mIeanN8xfH4</t>
+  </si>
+  <si>
+    <t>2.1.7.4</t>
+  </si>
+  <si>
+    <t>2.1.7.5</t>
+  </si>
+  <si>
+    <t>2.1.8.1</t>
+  </si>
+  <si>
+    <t>2.1.9.1</t>
+  </si>
+  <si>
+    <t>2.1.10.1</t>
+  </si>
+  <si>
+    <t>2.1.11.1</t>
+  </si>
+  <si>
+    <t>1.01.14</t>
+  </si>
+  <si>
+    <t>2.1.11.3</t>
+  </si>
+  <si>
+    <t>middle of panchati 63</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -849,34 +888,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1183,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="G186" sqref="G186"/>
@@ -5960,13 +6001,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -6267,7 +6309,9 @@
       <c r="G14" s="18">
         <v>43.54</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="21" t="s">
+        <v>240</v>
+      </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
@@ -6282,24 +6326,50 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="18"/>
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2">
+        <v>44047</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1.45</v>
+      </c>
+      <c r="G16" s="18">
+        <v>12.42</v>
+      </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="4">
+        <f>+D16+1</f>
+        <v>2</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F17" s="6">
+        <f>+G16</f>
+        <v>12.42</v>
+      </c>
+      <c r="G17" s="18">
+        <v>28.52</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
@@ -6307,10 +6377,20 @@
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="4">
+        <f>+D17+1</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" ref="F18:F20" si="0">+G17</f>
+        <v>28.52</v>
+      </c>
+      <c r="G18" s="18">
+        <v>40.450000000000003</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
@@ -6318,10 +6398,20 @@
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="4">
+        <f t="shared" ref="D19:D20" si="1">+D18+1</f>
+        <v>4</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="0"/>
+        <v>40.450000000000003</v>
+      </c>
+      <c r="G19" s="18">
+        <v>50.25</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
@@ -6329,12 +6419,26 @@
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="D20" s="4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" si="0"/>
+        <v>50.25</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>

</xml_diff>

<commit_message>
TS 2 and TS PP 2.4 Corrections TTD 12/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="293">
   <si>
     <t>Date</t>
   </si>
@@ -891,6 +891,9 @@
   </si>
   <si>
     <t>2.3.10.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XUXikdynlU8</t>
   </si>
 </sst>
 </file>
@@ -6173,7 +6176,7 @@
   <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7282,17 +7285,25 @@
       <c r="B54" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="C54" s="15"/>
+      <c r="C54" s="15">
+        <v>54.34</v>
+      </c>
       <c r="D54" s="4">
         <v>1</v>
       </c>
       <c r="E54" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
+      <c r="F54" s="16">
+        <v>5.37</v>
+      </c>
+      <c r="G54" s="16">
+        <v>9.48</v>
+      </c>
       <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
+      <c r="I54" s="15" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
@@ -7305,8 +7316,13 @@
       <c r="E55" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
+      <c r="F55" s="16">
+        <f>+G54</f>
+        <v>9.48</v>
+      </c>
+      <c r="G55" s="16">
+        <v>18.27</v>
+      </c>
       <c r="H55" s="15"/>
       <c r="I55" s="15"/>
     </row>
@@ -7321,8 +7337,13 @@
       <c r="E56" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
+      <c r="F56" s="16">
+        <f t="shared" ref="F56:F59" si="10">+G55</f>
+        <v>18.27</v>
+      </c>
+      <c r="G56" s="16">
+        <v>29.45</v>
+      </c>
       <c r="H56" s="15"/>
       <c r="I56" s="15"/>
     </row>
@@ -7337,8 +7358,13 @@
       <c r="E57" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
+      <c r="F57" s="16">
+        <f t="shared" si="10"/>
+        <v>29.45</v>
+      </c>
+      <c r="G57" s="16">
+        <v>37.47</v>
+      </c>
       <c r="H57" s="15"/>
       <c r="I57" s="15"/>
     </row>
@@ -7353,8 +7379,13 @@
       <c r="E58" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
+      <c r="F58" s="16">
+        <f t="shared" si="10"/>
+        <v>37.47</v>
+      </c>
+      <c r="G58" s="16">
+        <v>47.54</v>
+      </c>
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
     </row>
@@ -7369,8 +7400,13 @@
       <c r="E59" s="31" t="s">
         <v>291</v>
       </c>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
+      <c r="F59" s="16">
+        <f t="shared" si="10"/>
+        <v>47.54</v>
+      </c>
+      <c r="G59" s="16">
+        <v>53.35</v>
+      </c>
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
     </row>

</xml_diff>

<commit_message>
Corrections to PP files incl Sans corr 13/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="302">
   <si>
     <t>Date</t>
   </si>
@@ -894,19 +894,52 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=XUXikdynlU8</t>
+  </si>
+  <si>
+    <t>1.00.40</t>
+  </si>
+  <si>
+    <t>2.3.10.2</t>
+  </si>
+  <si>
+    <t>2.3.10.3</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Hccmfk_D_Zg</t>
+  </si>
+  <si>
+    <t>2.3.11.1</t>
+  </si>
+  <si>
+    <t>2.3.12.1</t>
+  </si>
+  <si>
+    <t>2.3.13.1</t>
+  </si>
+  <si>
+    <t>2.3.14.1</t>
+  </si>
+  <si>
+    <t>2.3.14.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1056,46 +1089,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1403,9 +1438,9 @@
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6175,8 +6210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7407,7 +7442,9 @@
       <c r="G59" s="16">
         <v>53.35</v>
       </c>
-      <c r="H59" s="15"/>
+      <c r="H59" s="33" t="s">
+        <v>294</v>
+      </c>
       <c r="I59" s="15"/>
     </row>
     <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -7433,24 +7470,50 @@
       <c r="I61" s="15"/>
     </row>
     <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
+      <c r="A62" s="15">
+        <v>13</v>
+      </c>
+      <c r="B62" s="22">
+        <v>44056</v>
+      </c>
+      <c r="C62" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="D62" s="4">
+        <v>1</v>
+      </c>
+      <c r="E62" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="F62" s="34">
+        <v>2.21</v>
+      </c>
+      <c r="G62" s="16">
+        <v>7.19</v>
+      </c>
       <c r="H62" s="15"/>
-      <c r="I62" s="15"/>
+      <c r="I62" s="15" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="B63" s="22"/>
       <c r="C63" s="15"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
+      <c r="D63" s="4">
+        <f>+D62+1</f>
+        <v>2</v>
+      </c>
+      <c r="E63" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="F63" s="16">
+        <f>+G62</f>
+        <v>7.19</v>
+      </c>
+      <c r="G63" s="16">
+        <v>24.12</v>
+      </c>
       <c r="H63" s="15"/>
       <c r="I63" s="15"/>
     </row>
@@ -7458,21 +7521,42 @@
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="15"/>
+      <c r="D64" s="4">
+        <f t="shared" ref="D64:D66" si="11">+D63+1</f>
+        <v>3</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="F64" s="16">
+        <f>+G63</f>
+        <v>24.12</v>
+      </c>
+      <c r="G64" s="16">
+        <v>31.36</v>
+      </c>
+      <c r="H64" s="33" t="s">
+        <v>152</v>
+      </c>
       <c r="I64" s="15"/>
     </row>
     <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
+      <c r="D65" s="4">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="E65" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="F65" s="16">
+        <v>36.520000000000003</v>
+      </c>
+      <c r="G65" s="16">
+        <v>47.54</v>
+      </c>
       <c r="H65" s="15"/>
       <c r="I65" s="15"/>
     </row>
@@ -7480,11 +7564,23 @@
       <c r="A66" s="15"/>
       <c r="B66" s="22"/>
       <c r="C66" s="15"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="15"/>
+      <c r="D66" s="4">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="E66" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="F66" s="16">
+        <f>+G65</f>
+        <v>47.54</v>
+      </c>
+      <c r="G66" s="16">
+        <v>59.36</v>
+      </c>
+      <c r="H66" s="33" t="s">
+        <v>301</v>
+      </c>
       <c r="I66" s="15"/>
     </row>
     <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TS 5 Corrections Upplili 16/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="318">
   <si>
     <t>Date</t>
   </si>
@@ -957,19 +957,37 @@
   </si>
   <si>
     <t>2.4.9.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kIcQlCFRm98</t>
+  </si>
+  <si>
+    <t>2.4.10.1</t>
+  </si>
+  <si>
+    <t>2.4.11.1</t>
+  </si>
+  <si>
+    <t>2.4.12.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1137,48 +1155,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1488,9 +1507,9 @@
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6258,10 +6277,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7890,37 +7909,80 @@
       <c r="I79" s="15"/>
     </row>
     <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="16"/>
+      <c r="A80" s="15">
+        <v>16</v>
+      </c>
+      <c r="B80" s="22">
+        <v>44059</v>
+      </c>
+      <c r="C80" s="15">
+        <v>55.44</v>
+      </c>
+      <c r="D80" s="4">
+        <v>1</v>
+      </c>
+      <c r="E80" s="37" t="s">
+        <v>315</v>
+      </c>
+      <c r="F80" s="16">
+        <v>2.33</v>
+      </c>
+      <c r="G80" s="16">
+        <v>14.46</v>
+      </c>
       <c r="H80" s="15"/>
-      <c r="I80" s="15"/>
+      <c r="I80" s="15" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="15"/>
       <c r="B81" s="22"/>
       <c r="C81" s="15"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="16"/>
-      <c r="G81" s="16"/>
-      <c r="H81" s="15"/>
+      <c r="D81" s="4">
+        <f>+D80+1</f>
+        <v>2</v>
+      </c>
+      <c r="E81" s="37" t="s">
+        <v>316</v>
+      </c>
+      <c r="F81" s="16">
+        <f>+G80</f>
+        <v>14.46</v>
+      </c>
+      <c r="G81" s="16">
+        <v>33.590000000000003</v>
+      </c>
+      <c r="H81" s="37" t="s">
+        <v>152</v>
+      </c>
       <c r="I81" s="15"/>
     </row>
     <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="15"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="16"/>
+      <c r="D82" s="4">
+        <f t="shared" ref="D82:D84" si="15">+D81+1</f>
+        <v>3</v>
+      </c>
+      <c r="E82" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="F82" s="16">
+        <v>40.1</v>
+      </c>
+      <c r="G82" s="16">
+        <v>54.37</v>
+      </c>
       <c r="H82" s="15"/>
       <c r="I82" s="15"/>
+    </row>
+    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="D83" s="4"/>
+    </row>
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="D84" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Editing for Articles -20/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="341">
   <si>
     <t>Date</t>
   </si>
@@ -987,19 +987,88 @@
   </si>
   <si>
     <t>2.5.1.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sz5MVQljUUI</t>
+  </si>
+  <si>
+    <t>2.5.1.5</t>
+  </si>
+  <si>
+    <t>2.5.1.6</t>
+  </si>
+  <si>
+    <t>2.5.2.1</t>
+  </si>
+  <si>
+    <t>audio disc</t>
+  </si>
+  <si>
+    <t>2.5.3.1</t>
+  </si>
+  <si>
+    <t>There is a skip of 20/30 padams start end of anuvaakam not known</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LZAyORBWHkc&amp;frags=pl%2Cwn</t>
+  </si>
+  <si>
+    <t>2.5.3.5</t>
+  </si>
+  <si>
+    <t>2.5.3.6</t>
+  </si>
+  <si>
+    <t>2.5.4.1</t>
+  </si>
+  <si>
+    <t>2.5.5.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=msMS_nQsy_g</t>
+  </si>
+  <si>
+    <t>2.5.6.1</t>
+  </si>
+  <si>
+    <t>2.5.7.1</t>
+  </si>
+  <si>
+    <t>2.5.8.1</t>
+  </si>
+  <si>
+    <t>2.5.8.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1179,54 +1248,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6306,8 +6378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8096,7 +8168,9 @@
       <c r="G87" s="40">
         <v>57.05</v>
       </c>
-      <c r="H87" s="38"/>
+      <c r="H87" s="41" t="s">
+        <v>325</v>
+      </c>
       <c r="I87" s="38"/>
     </row>
     <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -8111,43 +8185,80 @@
       <c r="I88" s="38"/>
     </row>
     <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A89" s="38"/>
-      <c r="B89" s="38"/>
-      <c r="C89" s="38"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="38"/>
-      <c r="F89" s="40"/>
-      <c r="G89" s="40"/>
+      <c r="A89" s="38">
+        <v>18</v>
+      </c>
+      <c r="B89" s="39">
+        <v>44061</v>
+      </c>
+      <c r="C89" s="38">
+        <v>52.48</v>
+      </c>
+      <c r="D89" s="4">
+        <v>1</v>
+      </c>
+      <c r="E89" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="F89" s="40">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="G89" s="40">
+        <v>12.32</v>
+      </c>
       <c r="H89" s="38"/>
-      <c r="I89" s="38"/>
+      <c r="I89" s="38" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="38"/>
       <c r="B90" s="38"/>
       <c r="C90" s="38"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="F90" s="40"/>
+      <c r="D90" s="4">
+        <f>+D89+1</f>
+        <v>2</v>
+      </c>
+      <c r="E90" s="41" t="s">
+        <v>327</v>
+      </c>
+      <c r="F90" s="40">
+        <f>+G89</f>
+        <v>12.32</v>
+      </c>
       <c r="G90" s="40"/>
-      <c r="H90" s="38"/>
-      <c r="I90" s="38"/>
+      <c r="H90" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="I90" s="41" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="38"/>
       <c r="B91" s="38"/>
       <c r="C91" s="38"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="38"/>
+      <c r="D91" s="4">
+        <f t="shared" ref="D91" si="17">+D90+1</f>
+        <v>3</v>
+      </c>
+      <c r="E91" s="41" t="s">
+        <v>329</v>
+      </c>
       <c r="F91" s="40"/>
-      <c r="G91" s="40"/>
-      <c r="H91" s="38"/>
+      <c r="G91" s="40">
+        <v>48.37</v>
+      </c>
+      <c r="H91" s="42" t="s">
+        <v>332</v>
+      </c>
       <c r="I91" s="38"/>
     </row>
     <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="38"/>
       <c r="B92" s="38"/>
       <c r="C92" s="38"/>
-      <c r="D92" s="38"/>
+      <c r="D92" s="4"/>
       <c r="E92" s="38"/>
       <c r="F92" s="40"/>
       <c r="G92" s="40"/>
@@ -8155,35 +8266,72 @@
       <c r="I92" s="38"/>
     </row>
     <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A93" s="38"/>
-      <c r="B93" s="38"/>
-      <c r="C93" s="38"/>
-      <c r="D93" s="38"/>
-      <c r="E93" s="38"/>
-      <c r="F93" s="40"/>
-      <c r="G93" s="40"/>
+      <c r="A93" s="38">
+        <v>19</v>
+      </c>
+      <c r="B93" s="39">
+        <v>44062</v>
+      </c>
+      <c r="C93" s="38">
+        <v>56.12</v>
+      </c>
+      <c r="D93" s="4">
+        <v>1</v>
+      </c>
+      <c r="E93" s="42" t="s">
+        <v>333</v>
+      </c>
+      <c r="F93" s="40">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G93" s="40">
+        <v>9.5299999999999994</v>
+      </c>
       <c r="H93" s="38"/>
-      <c r="I93" s="38"/>
+      <c r="I93" s="38" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="38"/>
       <c r="B94" s="38"/>
       <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="38"/>
-      <c r="F94" s="40"/>
-      <c r="G94" s="40"/>
-      <c r="H94" s="38"/>
+      <c r="D94" s="4">
+        <f>+D93+1</f>
+        <v>2</v>
+      </c>
+      <c r="E94" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="F94" s="40">
+        <f>+G93</f>
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="G94" s="40">
+        <v>28.06</v>
+      </c>
+      <c r="H94" s="42" t="s">
+        <v>152</v>
+      </c>
       <c r="I94" s="38"/>
     </row>
     <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="38"/>
       <c r="B95" s="38"/>
       <c r="C95" s="38"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="38"/>
-      <c r="F95" s="40"/>
-      <c r="G95" s="40"/>
+      <c r="D95" s="4">
+        <f t="shared" ref="D95" si="18">+D94+1</f>
+        <v>3</v>
+      </c>
+      <c r="E95" s="42" t="s">
+        <v>335</v>
+      </c>
+      <c r="F95" s="40">
+        <v>32.32</v>
+      </c>
+      <c r="G95" s="40">
+        <v>55.12</v>
+      </c>
       <c r="H95" s="38"/>
       <c r="I95" s="38"/>
     </row>
@@ -8199,23 +8347,47 @@
       <c r="I96" s="38"/>
     </row>
     <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A97" s="38"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="38"/>
-      <c r="F97" s="40"/>
-      <c r="G97" s="40"/>
+      <c r="A97" s="38">
+        <v>20</v>
+      </c>
+      <c r="B97" s="39">
+        <v>44063</v>
+      </c>
+      <c r="C97" s="38">
+        <v>51.29</v>
+      </c>
+      <c r="D97" s="4">
+        <v>1</v>
+      </c>
+      <c r="E97" s="43" t="s">
+        <v>337</v>
+      </c>
+      <c r="F97" s="40">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="G97" s="40">
+        <v>29.18</v>
+      </c>
       <c r="H97" s="38"/>
-      <c r="I97" s="38"/>
+      <c r="I97" s="38" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="38"/>
       <c r="B98" s="38"/>
       <c r="C98" s="38"/>
-      <c r="D98" s="38"/>
-      <c r="E98" s="38"/>
-      <c r="F98" s="40"/>
+      <c r="D98" s="4">
+        <f>+D97+1</f>
+        <v>2</v>
+      </c>
+      <c r="E98" s="43" t="s">
+        <v>338</v>
+      </c>
+      <c r="F98" s="40">
+        <f>+G97</f>
+        <v>29.18</v>
+      </c>
       <c r="G98" s="40"/>
       <c r="H98" s="38"/>
       <c r="I98" s="38"/>
@@ -8224,11 +8396,20 @@
       <c r="A99" s="38"/>
       <c r="B99" s="38"/>
       <c r="C99" s="38"/>
-      <c r="D99" s="38"/>
-      <c r="E99" s="38"/>
+      <c r="D99" s="4">
+        <f t="shared" ref="D99" si="19">+D98+1</f>
+        <v>3</v>
+      </c>
+      <c r="E99" s="43" t="s">
+        <v>339</v>
+      </c>
       <c r="F99" s="40"/>
-      <c r="G99" s="40"/>
-      <c r="H99" s="38"/>
+      <c r="G99" s="40">
+        <v>46.32</v>
+      </c>
+      <c r="H99" s="43" t="s">
+        <v>340</v>
+      </c>
       <c r="I99" s="38"/>
     </row>
     <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TS Jatai woring Directory organised 21/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="346">
   <si>
     <t>Date</t>
   </si>
@@ -1038,19 +1038,40 @@
   </si>
   <si>
     <t>2.5.8.2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wcnTT6usKm8</t>
+  </si>
+  <si>
+    <t>2.5.8.3</t>
+  </si>
+  <si>
+    <t>2.5.9.1</t>
+  </si>
+  <si>
+    <t>2.5.10.1</t>
+  </si>
+  <si>
+    <t>2.5.10.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1248,54 +1269,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6378,8 +6400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="H100" sqref="H100"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8424,24 +8446,51 @@
       <c r="I100" s="38"/>
     </row>
     <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A101" s="38"/>
-      <c r="B101" s="38"/>
-      <c r="C101" s="38"/>
-      <c r="D101" s="38"/>
-      <c r="E101" s="38"/>
-      <c r="F101" s="40"/>
-      <c r="G101" s="40"/>
-      <c r="H101" s="38"/>
-      <c r="I101" s="38"/>
+      <c r="A101" s="38">
+        <v>21</v>
+      </c>
+      <c r="B101" s="39">
+        <v>44064</v>
+      </c>
+      <c r="C101" s="38">
+        <v>56.03</v>
+      </c>
+      <c r="D101" s="4">
+        <v>1</v>
+      </c>
+      <c r="E101" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="F101" s="40">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="G101" s="40">
+        <v>19.13</v>
+      </c>
+      <c r="H101" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="I101" s="38" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="102" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
       <c r="C102" s="38"/>
-      <c r="D102" s="38"/>
-      <c r="E102" s="38"/>
-      <c r="F102" s="40"/>
-      <c r="G102" s="40"/>
+      <c r="D102" s="4">
+        <f>+D101+1</f>
+        <v>2</v>
+      </c>
+      <c r="E102" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="F102" s="40">
+        <v>23.57</v>
+      </c>
+      <c r="G102" s="40">
+        <v>43.14</v>
+      </c>
       <c r="H102" s="38"/>
       <c r="I102" s="38"/>
     </row>
@@ -8449,11 +8498,23 @@
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
       <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
-      <c r="E103" s="38"/>
-      <c r="F103" s="40"/>
-      <c r="G103" s="40"/>
-      <c r="H103" s="38"/>
+      <c r="D103" s="4">
+        <f t="shared" ref="D103" si="20">+D102+1</f>
+        <v>3</v>
+      </c>
+      <c r="E103" s="44" t="s">
+        <v>344</v>
+      </c>
+      <c r="F103" s="40">
+        <f>+G102</f>
+        <v>43.14</v>
+      </c>
+      <c r="G103" s="40">
+        <v>55.02</v>
+      </c>
+      <c r="H103" s="44" t="s">
+        <v>345</v>
+      </c>
       <c r="I103" s="38"/>
     </row>
     <row r="104" spans="1:9" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edits during Articles and SJ 27/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="372">
   <si>
     <t>Date</t>
   </si>
@@ -1083,19 +1083,85 @@
   </si>
   <si>
     <t>2.6.3.2</t>
+  </si>
+  <si>
+    <t>2.6.3.3</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vwzr-rmCAIg</t>
+  </si>
+  <si>
+    <t>2.6.4.1</t>
+  </si>
+  <si>
+    <t>2.6.5.1</t>
+  </si>
+  <si>
+    <t>2.6.6.1</t>
+  </si>
+  <si>
+    <t>1.01.07</t>
+  </si>
+  <si>
+    <t>2.6.6.2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UZn5nE2O5Xo</t>
+  </si>
+  <si>
+    <t>2.6.7.1</t>
+  </si>
+  <si>
+    <t>2.6.8.1</t>
+  </si>
+  <si>
+    <t>2.6.8.4</t>
+  </si>
+  <si>
+    <t>2.6.8.5</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cfB9lHK5E3w</t>
+  </si>
+  <si>
+    <t>mess rec.</t>
+  </si>
+  <si>
+    <t>2.6.9.1</t>
+  </si>
+  <si>
+    <t>2.9.10.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1317,61 +1383,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="32" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="35" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -6452,8 +6522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8735,7 +8805,7 @@
       <c r="B112" s="38"/>
       <c r="C112" s="38"/>
       <c r="D112" s="4">
-        <f t="shared" ref="D112:D113" si="22">+D111+1</f>
+        <f t="shared" ref="D112" si="22">+D111+1</f>
         <v>3</v>
       </c>
       <c r="E112" s="47" t="s">
@@ -8765,24 +8835,50 @@
       <c r="I113" s="38"/>
     </row>
     <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A114" s="38"/>
-      <c r="B114" s="38"/>
-      <c r="C114" s="38"/>
-      <c r="D114" s="38"/>
-      <c r="E114" s="38"/>
-      <c r="F114" s="40"/>
-      <c r="G114" s="40"/>
+      <c r="A114" s="38">
+        <v>24</v>
+      </c>
+      <c r="B114" s="39">
+        <v>44067</v>
+      </c>
+      <c r="C114" s="38">
+        <v>57.04</v>
+      </c>
+      <c r="D114" s="4">
+        <v>1</v>
+      </c>
+      <c r="E114" s="49" t="s">
+        <v>356</v>
+      </c>
+      <c r="F114" s="40">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="G114" s="40">
+        <v>18.22</v>
+      </c>
       <c r="H114" s="38"/>
-      <c r="I114" s="38"/>
+      <c r="I114" s="38" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="115" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="38"/>
       <c r="B115" s="38"/>
       <c r="C115" s="38"/>
-      <c r="D115" s="38"/>
-      <c r="E115" s="38"/>
-      <c r="F115" s="40"/>
-      <c r="G115" s="40"/>
+      <c r="D115" s="4">
+        <f>+D114+1</f>
+        <v>2</v>
+      </c>
+      <c r="E115" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="F115" s="40">
+        <f>+G114</f>
+        <v>18.22</v>
+      </c>
+      <c r="G115" s="40">
+        <v>31.04</v>
+      </c>
       <c r="H115" s="38"/>
       <c r="I115" s="38"/>
     </row>
@@ -8790,10 +8886,20 @@
       <c r="A116" s="38"/>
       <c r="B116" s="38"/>
       <c r="C116" s="38"/>
-      <c r="D116" s="38"/>
-      <c r="E116" s="38"/>
-      <c r="F116" s="40"/>
-      <c r="G116" s="40"/>
+      <c r="D116" s="4">
+        <f t="shared" ref="D116:D117" si="23">+D115+1</f>
+        <v>3</v>
+      </c>
+      <c r="E116" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="F116" s="40">
+        <f>+G115</f>
+        <v>31.04</v>
+      </c>
+      <c r="G116" s="40">
+        <v>52.48</v>
+      </c>
       <c r="H116" s="38"/>
       <c r="I116" s="38"/>
     </row>
@@ -8801,11 +8907,23 @@
       <c r="A117" s="38"/>
       <c r="B117" s="38"/>
       <c r="C117" s="38"/>
-      <c r="D117" s="38"/>
-      <c r="E117" s="38"/>
-      <c r="F117" s="40"/>
-      <c r="G117" s="40"/>
-      <c r="H117" s="38"/>
+      <c r="D117" s="4">
+        <f t="shared" si="23"/>
+        <v>4</v>
+      </c>
+      <c r="E117" s="49" t="s">
+        <v>360</v>
+      </c>
+      <c r="F117" s="40">
+        <f>+G116</f>
+        <v>52.48</v>
+      </c>
+      <c r="G117" s="40">
+        <v>55.5</v>
+      </c>
+      <c r="H117" s="50" t="s">
+        <v>360</v>
+      </c>
       <c r="I117" s="38"/>
     </row>
     <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -8820,43 +8938,82 @@
       <c r="I118" s="38"/>
     </row>
     <row r="119" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A119" s="38"/>
-      <c r="B119" s="38"/>
-      <c r="C119" s="38"/>
-      <c r="D119" s="38"/>
-      <c r="E119" s="38"/>
-      <c r="F119" s="40"/>
-      <c r="G119" s="40"/>
+      <c r="A119" s="38">
+        <v>25</v>
+      </c>
+      <c r="B119" s="39">
+        <v>44068</v>
+      </c>
+      <c r="C119" s="50" t="s">
+        <v>361</v>
+      </c>
+      <c r="D119" s="4">
+        <v>1</v>
+      </c>
+      <c r="E119" s="50" t="s">
+        <v>362</v>
+      </c>
+      <c r="F119" s="40">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="G119" s="40">
+        <v>20.29</v>
+      </c>
       <c r="H119" s="38"/>
-      <c r="I119" s="38"/>
+      <c r="I119" s="38" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="38"/>
       <c r="B120" s="38"/>
       <c r="C120" s="38"/>
-      <c r="D120" s="38"/>
-      <c r="E120" s="38"/>
-      <c r="F120" s="40"/>
-      <c r="G120" s="40"/>
-      <c r="H120" s="38"/>
+      <c r="D120" s="4">
+        <f>+D119+1</f>
+        <v>2</v>
+      </c>
+      <c r="E120" s="50" t="s">
+        <v>364</v>
+      </c>
+      <c r="F120" s="40">
+        <f>+G119</f>
+        <v>20.29</v>
+      </c>
+      <c r="G120" s="40">
+        <v>40.130000000000003</v>
+      </c>
+      <c r="H120" s="50" t="s">
+        <v>152</v>
+      </c>
       <c r="I120" s="38"/>
     </row>
     <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="38"/>
       <c r="B121" s="38"/>
       <c r="C121" s="38"/>
-      <c r="D121" s="38"/>
-      <c r="E121" s="38"/>
-      <c r="F121" s="40"/>
-      <c r="G121" s="40"/>
-      <c r="H121" s="38"/>
+      <c r="D121" s="4">
+        <f t="shared" ref="D121" si="24">+D120+1</f>
+        <v>3</v>
+      </c>
+      <c r="E121" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="F121" s="40">
+        <v>47.44</v>
+      </c>
+      <c r="G121" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="H121" s="52" t="s">
+        <v>366</v>
+      </c>
       <c r="I121" s="38"/>
     </row>
     <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="38"/>
       <c r="B122" s="38"/>
       <c r="C122" s="38"/>
-      <c r="D122" s="38"/>
+      <c r="D122" s="4"/>
       <c r="E122" s="38"/>
       <c r="F122" s="40"/>
       <c r="G122" s="40"/>
@@ -8864,24 +9021,47 @@
       <c r="I122" s="38"/>
     </row>
     <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A123" s="38"/>
-      <c r="B123" s="38"/>
-      <c r="C123" s="38"/>
-      <c r="D123" s="38"/>
-      <c r="E123" s="38"/>
-      <c r="F123" s="40"/>
+      <c r="A123" s="38">
+        <v>26</v>
+      </c>
+      <c r="B123" s="39">
+        <v>44069</v>
+      </c>
+      <c r="C123" s="38">
+        <v>46.57</v>
+      </c>
+      <c r="D123" s="4">
+        <v>1</v>
+      </c>
+      <c r="E123" s="52" t="s">
+        <v>367</v>
+      </c>
+      <c r="F123" s="40">
+        <v>7.29</v>
+      </c>
       <c r="G123" s="40"/>
-      <c r="H123" s="38"/>
-      <c r="I123" s="38"/>
+      <c r="H123" s="52" t="s">
+        <v>369</v>
+      </c>
+      <c r="I123" s="38" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="38"/>
       <c r="B124" s="38"/>
       <c r="C124" s="38"/>
-      <c r="D124" s="38"/>
-      <c r="E124" s="38"/>
+      <c r="D124" s="4">
+        <f>+D123+1</f>
+        <v>2</v>
+      </c>
+      <c r="E124" s="52" t="s">
+        <v>370</v>
+      </c>
       <c r="F124" s="40"/>
-      <c r="G124" s="40"/>
+      <c r="G124" s="40">
+        <v>32.42</v>
+      </c>
       <c r="H124" s="38"/>
       <c r="I124" s="38"/>
     </row>
@@ -8889,10 +9069,20 @@
       <c r="A125" s="38"/>
       <c r="B125" s="38"/>
       <c r="C125" s="38"/>
-      <c r="D125" s="38"/>
-      <c r="E125" s="38"/>
-      <c r="F125" s="40"/>
-      <c r="G125" s="40"/>
+      <c r="D125" s="4">
+        <f t="shared" ref="D125" si="25">+D124+1</f>
+        <v>3</v>
+      </c>
+      <c r="E125" s="52" t="s">
+        <v>371</v>
+      </c>
+      <c r="F125" s="40">
+        <f>+G124</f>
+        <v>32.42</v>
+      </c>
+      <c r="G125" s="40">
+        <v>45.4</v>
+      </c>
       <c r="H125" s="38"/>
       <c r="I125" s="38"/>
     </row>

</xml_diff>

<commit_message>
Article Edit changes 29/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
     <sheet name="Kandam2" sheetId="2" r:id="rId2"/>
+    <sheet name="Kandam3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="383">
   <si>
     <t>Date</t>
   </si>
@@ -1130,14 +1131,47 @@
     <t>2.6.9.1</t>
   </si>
   <si>
-    <t>2.9.10.1</t>
+    <t>https://www.youtube.com/watch?v=j05_OKe5feo</t>
+  </si>
+  <si>
+    <t>2.6.10.1</t>
+  </si>
+  <si>
+    <t>2.6.11.1</t>
+  </si>
+  <si>
+    <t>2.6.12.1</t>
+  </si>
+  <si>
+    <t>3.1.1.1</t>
+  </si>
+  <si>
+    <t>3.1.2.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9oWeD-kx6EM</t>
+  </si>
+  <si>
+    <t>3.1.2.2</t>
+  </si>
+  <si>
+    <t>3.1.3.1</t>
+  </si>
+  <si>
+    <t>3.1.4.1</t>
+  </si>
+  <si>
+    <t>3.1.5.1</t>
+  </si>
+  <si>
+    <t>3.1.6.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1350,14 +1384,37 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1367,6 +1424,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1383,66 +1446,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="35" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="37" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="38" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6522,8 +6597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="I132" sqref="I132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9073,8 +9148,8 @@
         <f t="shared" ref="D125" si="25">+D124+1</f>
         <v>3</v>
       </c>
-      <c r="E125" s="52" t="s">
-        <v>371</v>
+      <c r="E125" s="53" t="s">
+        <v>372</v>
       </c>
       <c r="F125" s="40">
         <f>+G124</f>
@@ -9098,35 +9173,72 @@
       <c r="I126" s="38"/>
     </row>
     <row r="127" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A127" s="38"/>
-      <c r="B127" s="38"/>
-      <c r="C127" s="38"/>
-      <c r="D127" s="38"/>
-      <c r="E127" s="38"/>
-      <c r="F127" s="40"/>
-      <c r="G127" s="40"/>
+      <c r="A127" s="38">
+        <v>27</v>
+      </c>
+      <c r="B127" s="39">
+        <v>44070</v>
+      </c>
+      <c r="C127" s="38">
+        <v>56.05</v>
+      </c>
+      <c r="D127" s="4">
+        <v>1</v>
+      </c>
+      <c r="E127" s="53" t="s">
+        <v>373</v>
+      </c>
+      <c r="F127" s="40">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G127" s="40">
+        <v>14.09</v>
+      </c>
       <c r="H127" s="38"/>
-      <c r="I127" s="38"/>
+      <c r="I127" s="38" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="128" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="38"/>
       <c r="B128" s="38"/>
       <c r="C128" s="38"/>
-      <c r="D128" s="38"/>
-      <c r="E128" s="38"/>
-      <c r="F128" s="40"/>
-      <c r="G128" s="40"/>
-      <c r="H128" s="38"/>
+      <c r="D128" s="4">
+        <f>+D127+1</f>
+        <v>2</v>
+      </c>
+      <c r="E128" s="53" t="s">
+        <v>374</v>
+      </c>
+      <c r="F128" s="40">
+        <f>+G127</f>
+        <v>14.09</v>
+      </c>
+      <c r="G128" s="40">
+        <v>33.25</v>
+      </c>
+      <c r="H128" s="53" t="s">
+        <v>152</v>
+      </c>
       <c r="I128" s="38"/>
     </row>
     <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="38"/>
       <c r="B129" s="38"/>
       <c r="C129" s="38"/>
-      <c r="D129" s="38"/>
-      <c r="E129" s="38"/>
-      <c r="F129" s="40"/>
-      <c r="G129" s="40"/>
+      <c r="D129" s="4">
+        <f t="shared" ref="D129:D130" si="26">+D128+1</f>
+        <v>3</v>
+      </c>
+      <c r="E129" s="53" t="s">
+        <v>375</v>
+      </c>
+      <c r="F129" s="40">
+        <v>37.36</v>
+      </c>
+      <c r="G129" s="40">
+        <v>51.24</v>
+      </c>
       <c r="H129" s="38"/>
       <c r="I129" s="38"/>
     </row>
@@ -9134,11 +9246,23 @@
       <c r="A130" s="38"/>
       <c r="B130" s="38"/>
       <c r="C130" s="38"/>
-      <c r="D130" s="38"/>
-      <c r="E130" s="38"/>
-      <c r="F130" s="40"/>
-      <c r="G130" s="40"/>
-      <c r="H130" s="38"/>
+      <c r="D130" s="4">
+        <f t="shared" si="26"/>
+        <v>4</v>
+      </c>
+      <c r="E130" s="53" t="s">
+        <v>376</v>
+      </c>
+      <c r="F130" s="40">
+        <f>+G129</f>
+        <v>51.24</v>
+      </c>
+      <c r="G130" s="40">
+        <v>55.04</v>
+      </c>
+      <c r="H130" s="53" t="s">
+        <v>376</v>
+      </c>
       <c r="I130" s="38"/>
     </row>
     <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -9178,4 +9302,1039 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="38">
+        <v>1</v>
+      </c>
+      <c r="B4" s="39">
+        <v>44070</v>
+      </c>
+      <c r="C4" s="38">
+        <v>56.05</v>
+      </c>
+      <c r="D4" s="54">
+        <v>1</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>373</v>
+      </c>
+      <c r="F4" s="56">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G4" s="56">
+        <v>14.09</v>
+      </c>
+      <c r="H4" s="55"/>
+      <c r="I4" s="38" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="54">
+        <f>+D4+1</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>374</v>
+      </c>
+      <c r="F5" s="56">
+        <f>+G4</f>
+        <v>14.09</v>
+      </c>
+      <c r="G5" s="56">
+        <v>33.25</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="I5" s="38"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="4">
+        <f t="shared" ref="D6:D7" si="0">+D5+1</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>375</v>
+      </c>
+      <c r="F6" s="40">
+        <v>37.36</v>
+      </c>
+      <c r="G6" s="40">
+        <v>51.24</v>
+      </c>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+    </row>
+    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>376</v>
+      </c>
+      <c r="F7" s="40">
+        <f>+G6</f>
+        <v>51.24</v>
+      </c>
+      <c r="G7" s="40">
+        <v>55.04</v>
+      </c>
+      <c r="H7" s="53" t="s">
+        <v>376</v>
+      </c>
+      <c r="I7" s="38"/>
+    </row>
+    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="57">
+        <v>2</v>
+      </c>
+      <c r="B9" s="58">
+        <v>44071</v>
+      </c>
+      <c r="C9" s="57">
+        <v>56.08</v>
+      </c>
+      <c r="D9" s="59">
+        <v>1</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>378</v>
+      </c>
+      <c r="F9" s="57">
+        <v>7.42</v>
+      </c>
+      <c r="G9" s="57">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57" t="s">
+        <v>377</v>
+      </c>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+    </row>
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="57"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="59">
+        <f>+D9+1</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>379</v>
+      </c>
+      <c r="F10" s="57">
+        <f>+G9</f>
+        <v>20.079999999999998</v>
+      </c>
+      <c r="G10" s="60">
+        <v>29.1</v>
+      </c>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+    </row>
+    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="59">
+        <f t="shared" ref="D11:D13" si="1">+D10+1</f>
+        <v>3</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>380</v>
+      </c>
+      <c r="F11" s="60">
+        <f>+G10</f>
+        <v>29.1</v>
+      </c>
+      <c r="G11" s="57">
+        <v>43.21</v>
+      </c>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+    </row>
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="59">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>381</v>
+      </c>
+      <c r="F12" s="57">
+        <f>+G11</f>
+        <v>43.21</v>
+      </c>
+      <c r="G12" s="57">
+        <v>51.09</v>
+      </c>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+    </row>
+    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="59">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>382</v>
+      </c>
+      <c r="F13" s="57">
+        <f>+G12</f>
+        <v>51.09</v>
+      </c>
+      <c r="G13" s="57">
+        <v>54.55</v>
+      </c>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+    </row>
+    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+    </row>
+    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+    </row>
+    <row r="16" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+    </row>
+    <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+    </row>
+    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="57"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+    </row>
+    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="57"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+    </row>
+    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="57"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+    </row>
+    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="57"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="57"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+    </row>
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="57"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+    </row>
+    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="57"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+    </row>
+    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="57"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+    </row>
+    <row r="26" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+    </row>
+    <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="57"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="57"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="57"/>
+    </row>
+    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="57"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="57"/>
+    </row>
+    <row r="29" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="57"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="57"/>
+    </row>
+    <row r="30" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="57"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
+    </row>
+    <row r="31" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="57"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+    </row>
+    <row r="32" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="57"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="57"/>
+      <c r="M32" s="57"/>
+    </row>
+    <row r="33" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="57"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="57"/>
+      <c r="M33" s="57"/>
+    </row>
+    <row r="34" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="57"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="57"/>
+    </row>
+    <row r="35" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="57"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="57"/>
+      <c r="M35" s="57"/>
+    </row>
+    <row r="36" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="57"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="57"/>
+    </row>
+    <row r="37" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A37" s="57"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="57"/>
+    </row>
+    <row r="38" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="57"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+    </row>
+    <row r="39" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="57"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
+      <c r="J39" s="57"/>
+      <c r="K39" s="57"/>
+      <c r="L39" s="57"/>
+      <c r="M39" s="57"/>
+    </row>
+    <row r="40" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A40" s="57"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="57"/>
+      <c r="J40" s="57"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="57"/>
+      <c r="M40" s="57"/>
+    </row>
+    <row r="41" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A41" s="57"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="57"/>
+      <c r="M41" s="57"/>
+    </row>
+    <row r="42" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" s="57"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="57"/>
+      <c r="M42" s="57"/>
+    </row>
+    <row r="43" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" s="57"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="57"/>
+      <c r="M43" s="57"/>
+    </row>
+    <row r="44" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A44" s="57"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+      <c r="K44" s="57"/>
+      <c r="L44" s="57"/>
+      <c r="M44" s="57"/>
+    </row>
+    <row r="45" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A45" s="57"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="57"/>
+      <c r="K45" s="57"/>
+      <c r="L45" s="57"/>
+      <c r="M45" s="57"/>
+    </row>
+    <row r="46" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="57"/>
+    </row>
+    <row r="47" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A47" s="57"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="57"/>
+    </row>
+    <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A48" s="57"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="57"/>
+      <c r="J48" s="57"/>
+      <c r="K48" s="57"/>
+      <c r="L48" s="57"/>
+      <c r="M48" s="57"/>
+    </row>
+    <row r="49" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A49" s="57"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="57"/>
+      <c r="M49" s="57"/>
+    </row>
+    <row r="50" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A50" s="57"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="57"/>
+      <c r="M50" s="57"/>
+    </row>
+    <row r="51" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A51" s="57"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="57"/>
+      <c r="M51" s="57"/>
+    </row>
+    <row r="52" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A52" s="57"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="57"/>
+    </row>
+    <row r="53" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A53" s="57"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="57"/>
+      <c r="J53" s="57"/>
+      <c r="K53" s="57"/>
+      <c r="L53" s="57"/>
+      <c r="M53" s="57"/>
+    </row>
+    <row r="54" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A54" s="57"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="57"/>
+      <c r="H54" s="57"/>
+      <c r="I54" s="57"/>
+      <c r="J54" s="57"/>
+      <c r="K54" s="57"/>
+      <c r="L54" s="57"/>
+      <c r="M54" s="57"/>
+    </row>
+    <row r="55" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A55" s="57"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="57"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="57"/>
+      <c r="J55" s="57"/>
+      <c r="K55" s="57"/>
+      <c r="L55" s="57"/>
+      <c r="M55" s="57"/>
+    </row>
+    <row r="56" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A56" s="57"/>
+      <c r="B56" s="57"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="57"/>
+      <c r="E56" s="57"/>
+      <c r="F56" s="57"/>
+      <c r="G56" s="57"/>
+      <c r="H56" s="57"/>
+      <c r="I56" s="57"/>
+      <c r="J56" s="57"/>
+      <c r="K56" s="57"/>
+      <c r="L56" s="57"/>
+      <c r="M56" s="57"/>
+    </row>
+    <row r="57" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A57" s="57"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="57"/>
+      <c r="F57" s="57"/>
+      <c r="G57" s="57"/>
+      <c r="H57" s="57"/>
+      <c r="I57" s="57"/>
+      <c r="J57" s="57"/>
+      <c r="K57" s="57"/>
+      <c r="L57" s="57"/>
+      <c r="M57" s="57"/>
+    </row>
+    <row r="58" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A58" s="57"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="57"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="57"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="57"/>
+      <c r="L58" s="57"/>
+      <c r="M58" s="57"/>
+    </row>
+    <row r="59" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A59" s="57"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="57"/>
+      <c r="F59" s="57"/>
+      <c r="G59" s="57"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="57"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="57"/>
+      <c r="L59" s="57"/>
+      <c r="M59" s="57"/>
+    </row>
+    <row r="60" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A60" s="57"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="57"/>
+      <c r="G60" s="57"/>
+      <c r="H60" s="57"/>
+      <c r="I60" s="57"/>
+      <c r="J60" s="57"/>
+      <c r="K60" s="57"/>
+      <c r="L60" s="57"/>
+      <c r="M60" s="57"/>
+    </row>
+    <row r="61" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A61" s="57"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="57"/>
+      <c r="G61" s="57"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="57"/>
+      <c r="J61" s="57"/>
+      <c r="K61" s="57"/>
+      <c r="L61" s="57"/>
+      <c r="M61" s="57"/>
+    </row>
+    <row r="62" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A62" s="57"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="57"/>
+      <c r="G62" s="57"/>
+      <c r="H62" s="57"/>
+      <c r="I62" s="57"/>
+      <c r="J62" s="57"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="57"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Jatai Working files 31/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="393">
   <si>
     <t>Date</t>
   </si>
@@ -1165,19 +1165,61 @@
   </si>
   <si>
     <t>3.1.6.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZsRDpCQIw00</t>
+  </si>
+  <si>
+    <t>3.1.6.2</t>
+  </si>
+  <si>
+    <t>3.1.7.1</t>
+  </si>
+  <si>
+    <t>3.1.8.1</t>
+  </si>
+  <si>
+    <t>3.1.9.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=WZ6IdDRXNzc</t>
+  </si>
+  <si>
+    <t>3.1.10.1</t>
+  </si>
+  <si>
+    <t>3.1.11.1</t>
+  </si>
+  <si>
+    <t>3.2.1.1</t>
+  </si>
+  <si>
+    <t>3.2.2.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1446,78 +1488,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="37" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="39" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="38" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="40" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9308,8 +9352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9321,7 +9365,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.85546875" customWidth="1"/>
+    <col min="9" max="9" width="63.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.25">
@@ -9614,15 +9658,31 @@
       <c r="M14" s="57"/>
     </row>
     <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
+      <c r="A15" s="57">
+        <v>3</v>
+      </c>
+      <c r="B15" s="58">
+        <v>44072</v>
+      </c>
+      <c r="C15" s="57">
+        <v>57.42</v>
+      </c>
+      <c r="D15" s="59">
+        <v>1</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>384</v>
+      </c>
+      <c r="F15" s="60">
+        <v>3.1</v>
+      </c>
+      <c r="G15" s="57">
+        <v>9.39</v>
+      </c>
       <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
+      <c r="I15" s="57" t="s">
+        <v>383</v>
+      </c>
       <c r="J15" s="57"/>
       <c r="K15" s="57"/>
       <c r="L15" s="57"/>
@@ -9632,10 +9692,20 @@
       <c r="A16" s="57"/>
       <c r="B16" s="57"/>
       <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
+      <c r="D16" s="59">
+        <f>+D15+1</f>
+        <v>2</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>385</v>
+      </c>
+      <c r="F16" s="57">
+        <f>+G15</f>
+        <v>9.39</v>
+      </c>
+      <c r="G16" s="57">
+        <v>24.02</v>
+      </c>
       <c r="H16" s="57"/>
       <c r="I16" s="57"/>
       <c r="J16" s="57"/>
@@ -9647,10 +9717,20 @@
       <c r="A17" s="57"/>
       <c r="B17" s="57"/>
       <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
+      <c r="D17" s="59">
+        <f t="shared" ref="D17:D18" si="2">+D16+1</f>
+        <v>3</v>
+      </c>
+      <c r="E17" s="61" t="s">
+        <v>386</v>
+      </c>
+      <c r="F17" s="57">
+        <f t="shared" ref="F17:F18" si="3">+G16</f>
+        <v>24.02</v>
+      </c>
+      <c r="G17" s="57">
+        <v>34.520000000000003</v>
+      </c>
       <c r="H17" s="57"/>
       <c r="I17" s="57"/>
       <c r="J17" s="57"/>
@@ -9662,10 +9742,20 @@
       <c r="A18" s="57"/>
       <c r="B18" s="57"/>
       <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
+      <c r="D18" s="59">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>387</v>
+      </c>
+      <c r="F18" s="57">
+        <f t="shared" si="3"/>
+        <v>34.520000000000003</v>
+      </c>
+      <c r="G18" s="57">
+        <v>56.32</v>
+      </c>
       <c r="H18" s="57"/>
       <c r="I18" s="57"/>
       <c r="J18" s="57"/>
@@ -9677,7 +9767,7 @@
       <c r="A19" s="57"/>
       <c r="B19" s="57"/>
       <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
+      <c r="D19" s="59"/>
       <c r="E19" s="57"/>
       <c r="F19" s="57"/>
       <c r="G19" s="57"/>
@@ -9689,15 +9779,31 @@
       <c r="M19" s="57"/>
     </row>
     <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="57"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
+      <c r="A20" s="57">
+        <v>4</v>
+      </c>
+      <c r="B20" s="58">
+        <v>44073</v>
+      </c>
+      <c r="C20" s="57">
+        <v>59.56</v>
+      </c>
+      <c r="D20" s="59">
+        <v>1</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>389</v>
+      </c>
+      <c r="F20" s="57">
+        <v>5.05</v>
+      </c>
+      <c r="G20" s="57">
+        <v>14.51</v>
+      </c>
       <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
+      <c r="I20" s="57" t="s">
+        <v>388</v>
+      </c>
       <c r="J20" s="57"/>
       <c r="K20" s="57"/>
       <c r="L20" s="57"/>
@@ -9707,11 +9813,23 @@
       <c r="A21" s="57"/>
       <c r="B21" s="57"/>
       <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
+      <c r="D21" s="59">
+        <f>+D20+1</f>
+        <v>2</v>
+      </c>
+      <c r="E21" s="62" t="s">
+        <v>390</v>
+      </c>
+      <c r="F21" s="57">
+        <f>+G20</f>
+        <v>14.51</v>
+      </c>
+      <c r="G21" s="57">
+        <v>37.14</v>
+      </c>
+      <c r="H21" s="62" t="s">
+        <v>152</v>
+      </c>
       <c r="I21" s="57"/>
       <c r="J21" s="57"/>
       <c r="K21" s="57"/>
@@ -9722,10 +9840,19 @@
       <c r="A22" s="57"/>
       <c r="B22" s="57"/>
       <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
+      <c r="D22" s="59">
+        <f t="shared" ref="D22:D23" si="4">+D21+1</f>
+        <v>3</v>
+      </c>
+      <c r="E22" s="62" t="s">
+        <v>391</v>
+      </c>
+      <c r="F22" s="60">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="G22" s="57">
+        <v>48.35</v>
+      </c>
       <c r="H22" s="57"/>
       <c r="I22" s="57"/>
       <c r="J22" s="57"/>
@@ -9737,10 +9864,20 @@
       <c r="A23" s="57"/>
       <c r="B23" s="57"/>
       <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
+      <c r="D23" s="59">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E23" s="62" t="s">
+        <v>392</v>
+      </c>
+      <c r="F23" s="57">
+        <f t="shared" ref="F22:F23" si="5">+G22</f>
+        <v>48.35</v>
+      </c>
+      <c r="G23" s="57">
+        <v>58.58</v>
+      </c>
       <c r="H23" s="57"/>
       <c r="I23" s="57"/>
       <c r="J23" s="57"/>

</xml_diff>

<commit_message>
TB 3.7 Corrections Venkat AAK 01/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="398">
   <si>
     <t>Date</t>
   </si>
@@ -1195,19 +1195,40 @@
   </si>
   <si>
     <t>3.2.2.1</t>
+  </si>
+  <si>
+    <t>31-08-202</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=U1CFFnO7dqs</t>
+  </si>
+  <si>
+    <t>3.2.3.1</t>
+  </si>
+  <si>
+    <t>3.2.4.1</t>
+  </si>
+  <si>
+    <t>3.2.5.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1488,78 +1509,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="39" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="40" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="40" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="41" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -9352,8 +9374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9872,7 +9894,7 @@
         <v>392</v>
       </c>
       <c r="F23" s="57">
-        <f t="shared" ref="F22:F23" si="5">+G22</f>
+        <f t="shared" ref="F23" si="5">+G22</f>
         <v>48.35</v>
       </c>
       <c r="G23" s="57">
@@ -9901,15 +9923,31 @@
       <c r="M24" s="57"/>
     </row>
     <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
+      <c r="A25" s="57">
+        <v>5</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="C25" s="57">
+        <v>59.38</v>
+      </c>
+      <c r="D25" s="59">
+        <v>1</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>395</v>
+      </c>
+      <c r="F25" s="57">
+        <v>5.56</v>
+      </c>
+      <c r="G25" s="57">
+        <v>19.55</v>
+      </c>
       <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
+      <c r="I25" s="57" t="s">
+        <v>394</v>
+      </c>
       <c r="J25" s="57"/>
       <c r="K25" s="57"/>
       <c r="L25" s="57"/>
@@ -9919,10 +9957,20 @@
       <c r="A26" s="57"/>
       <c r="B26" s="57"/>
       <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
+      <c r="D26" s="59">
+        <f>+D25+1</f>
+        <v>2</v>
+      </c>
+      <c r="E26" s="63" t="s">
+        <v>396</v>
+      </c>
+      <c r="F26" s="57">
+        <f>+G25</f>
+        <v>19.55</v>
+      </c>
+      <c r="G26" s="57">
+        <v>35.03</v>
+      </c>
       <c r="H26" s="57"/>
       <c r="I26" s="57"/>
       <c r="J26" s="57"/>
@@ -9934,10 +9982,20 @@
       <c r="A27" s="57"/>
       <c r="B27" s="57"/>
       <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
+      <c r="D27" s="59">
+        <f t="shared" ref="D27:D28" si="6">+D26+1</f>
+        <v>3</v>
+      </c>
+      <c r="E27" s="63" t="s">
+        <v>397</v>
+      </c>
+      <c r="F27" s="57">
+        <f t="shared" ref="F27:F28" si="7">+G26</f>
+        <v>35.03</v>
+      </c>
+      <c r="G27" s="57">
+        <v>58.45</v>
+      </c>
       <c r="H27" s="57"/>
       <c r="I27" s="57"/>
       <c r="J27" s="57"/>
@@ -9949,7 +10007,7 @@
       <c r="A28" s="57"/>
       <c r="B28" s="57"/>
       <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
+      <c r="D28" s="59"/>
       <c r="E28" s="57"/>
       <c r="F28" s="57"/>
       <c r="G28" s="57"/>
@@ -10472,6 +10530,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrections, Baraha files of TS, Latin Jatai 07/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="435">
   <si>
     <t>Date</t>
   </si>
@@ -1252,19 +1252,112 @@
   </si>
   <si>
     <t>3.3.4.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ShJvFs1yvBA</t>
+  </si>
+  <si>
+    <t>3.3.4.2</t>
+  </si>
+  <si>
+    <t>3.3.5.1</t>
+  </si>
+  <si>
+    <t>3.3.6.1</t>
+  </si>
+  <si>
+    <t>3.3.7.1</t>
+  </si>
+  <si>
+    <t>3.3.8.1</t>
+  </si>
+  <si>
+    <t>3.3.9.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RejlWzQfyd8</t>
+  </si>
+  <si>
+    <t>3.3.10.1</t>
+  </si>
+  <si>
+    <t>3.3.11.1</t>
+  </si>
+  <si>
+    <t>3.4.1.1</t>
+  </si>
+  <si>
+    <t>3.4.1.2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=tVH8-yDUq30</t>
+  </si>
+  <si>
+    <t>3.4.5.1</t>
+  </si>
+  <si>
+    <t>3.4.6.1</t>
+  </si>
+  <si>
+    <t>3.4.7.1</t>
+  </si>
+  <si>
+    <t>3.4.8.1</t>
+  </si>
+  <si>
+    <t>3.4.9.1</t>
+  </si>
+  <si>
+    <t>3.4.2.1</t>
+  </si>
+  <si>
+    <t>3.4.3.1</t>
+  </si>
+  <si>
+    <t>3.4.4.1</t>
+  </si>
+  <si>
+    <t>3.4.6.2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Zj43zg9-3ug</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1563,55 +1656,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="42" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="46" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1619,27 +1717,27 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="47" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="43" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9428,10 +9526,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10371,7 +10469,9 @@
       <c r="G40" s="57">
         <v>53.46</v>
       </c>
-      <c r="H40" s="57"/>
+      <c r="H40" s="66" t="s">
+        <v>411</v>
+      </c>
       <c r="I40" s="57"/>
       <c r="J40" s="57"/>
       <c r="K40" s="57"/>
@@ -10394,15 +10494,31 @@
       <c r="M41" s="57"/>
     </row>
     <row r="42" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="57"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="57"/>
+      <c r="A42" s="57">
+        <v>8</v>
+      </c>
+      <c r="B42" s="58">
+        <v>44077</v>
+      </c>
+      <c r="C42" s="57">
+        <v>58.26</v>
+      </c>
+      <c r="D42" s="59">
+        <v>1</v>
+      </c>
+      <c r="E42" s="66" t="s">
+        <v>413</v>
+      </c>
+      <c r="F42" s="57">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="G42" s="60">
+        <v>10.199999999999999</v>
+      </c>
       <c r="H42" s="57"/>
-      <c r="I42" s="57"/>
+      <c r="I42" s="57" t="s">
+        <v>412</v>
+      </c>
       <c r="J42" s="57"/>
       <c r="K42" s="57"/>
       <c r="L42" s="57"/>
@@ -10412,10 +10528,20 @@
       <c r="A43" s="57"/>
       <c r="B43" s="57"/>
       <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
-      <c r="G43" s="57"/>
+      <c r="D43" s="59">
+        <f>+D42+1</f>
+        <v>2</v>
+      </c>
+      <c r="E43" s="66" t="s">
+        <v>414</v>
+      </c>
+      <c r="F43" s="60">
+        <f>+G42</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G43" s="57">
+        <v>23.34</v>
+      </c>
       <c r="H43" s="57"/>
       <c r="I43" s="57"/>
       <c r="J43" s="57"/>
@@ -10427,10 +10553,20 @@
       <c r="A44" s="57"/>
       <c r="B44" s="57"/>
       <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
+      <c r="D44" s="59">
+        <f t="shared" ref="D44:D46" si="11">+D43+1</f>
+        <v>3</v>
+      </c>
+      <c r="E44" s="66" t="s">
+        <v>415</v>
+      </c>
+      <c r="F44" s="60">
+        <f t="shared" ref="F44:F46" si="12">+G43</f>
+        <v>23.34</v>
+      </c>
+      <c r="G44" s="57">
+        <v>32.47</v>
+      </c>
       <c r="H44" s="57"/>
       <c r="I44" s="57"/>
       <c r="J44" s="57"/>
@@ -10442,10 +10578,20 @@
       <c r="A45" s="57"/>
       <c r="B45" s="57"/>
       <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
+      <c r="D45" s="59">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="E45" s="66" t="s">
+        <v>416</v>
+      </c>
+      <c r="F45" s="60">
+        <f t="shared" si="12"/>
+        <v>32.47</v>
+      </c>
+      <c r="G45" s="57">
+        <v>41.09</v>
+      </c>
       <c r="H45" s="57"/>
       <c r="I45" s="57"/>
       <c r="J45" s="57"/>
@@ -10457,10 +10603,20 @@
       <c r="A46" s="57"/>
       <c r="B46" s="57"/>
       <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
+      <c r="D46" s="59">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="E46" s="66" t="s">
+        <v>417</v>
+      </c>
+      <c r="F46" s="60">
+        <f t="shared" si="12"/>
+        <v>41.09</v>
+      </c>
+      <c r="G46" s="57">
+        <v>57.44</v>
+      </c>
       <c r="H46" s="57"/>
       <c r="I46" s="57"/>
       <c r="J46" s="57"/>
@@ -10484,15 +10640,31 @@
       <c r="M47" s="57"/>
     </row>
     <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="57"/>
+      <c r="A48" s="57">
+        <v>9</v>
+      </c>
+      <c r="B48" s="58">
+        <v>44078</v>
+      </c>
+      <c r="C48" s="57">
+        <v>34.06</v>
+      </c>
+      <c r="D48" s="59">
+        <v>1</v>
+      </c>
+      <c r="E48" s="67" t="s">
+        <v>418</v>
+      </c>
+      <c r="F48" s="60">
+        <v>1.2</v>
+      </c>
+      <c r="G48" s="57">
+        <v>7.46</v>
+      </c>
       <c r="H48" s="57"/>
-      <c r="I48" s="57"/>
+      <c r="I48" s="57" t="s">
+        <v>419</v>
+      </c>
       <c r="J48" s="57"/>
       <c r="K48" s="57"/>
       <c r="L48" s="57"/>
@@ -10502,10 +10674,20 @@
       <c r="A49" s="57"/>
       <c r="B49" s="57"/>
       <c r="C49" s="57"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="57"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="57"/>
+      <c r="D49" s="59">
+        <f>+D48+1</f>
+        <v>2</v>
+      </c>
+      <c r="E49" s="67" t="s">
+        <v>420</v>
+      </c>
+      <c r="F49" s="57">
+        <f>+G48</f>
+        <v>7.46</v>
+      </c>
+      <c r="G49" s="57">
+        <v>13.22</v>
+      </c>
       <c r="H49" s="57"/>
       <c r="I49" s="57"/>
       <c r="J49" s="57"/>
@@ -10517,10 +10699,20 @@
       <c r="A50" s="57"/>
       <c r="B50" s="57"/>
       <c r="C50" s="57"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
+      <c r="D50" s="59">
+        <f t="shared" ref="D50:D51" si="13">+D49+1</f>
+        <v>3</v>
+      </c>
+      <c r="E50" s="67" t="s">
+        <v>421</v>
+      </c>
+      <c r="F50" s="57">
+        <f>+G49</f>
+        <v>13.22</v>
+      </c>
+      <c r="G50" s="57">
+        <v>30.11</v>
+      </c>
       <c r="H50" s="57"/>
       <c r="I50" s="57"/>
       <c r="J50" s="57"/>
@@ -10532,12 +10724,23 @@
       <c r="A51" s="57"/>
       <c r="B51" s="57"/>
       <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
+      <c r="D51" s="59">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="E51" s="67" t="s">
+        <v>422</v>
+      </c>
+      <c r="F51" s="57">
+        <f>+G50</f>
+        <v>30.11</v>
+      </c>
+      <c r="G51" s="57">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="H51" s="68" t="s">
+        <v>422</v>
+      </c>
       <c r="J51" s="57"/>
       <c r="K51" s="57"/>
       <c r="L51" s="57"/>
@@ -10559,15 +10762,31 @@
       <c r="M52" s="57"/>
     </row>
     <row r="53" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="57"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="57"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="57"/>
+      <c r="A53" s="57">
+        <v>10</v>
+      </c>
+      <c r="B53" s="58">
+        <v>44079</v>
+      </c>
+      <c r="C53" s="57">
+        <v>57.57</v>
+      </c>
+      <c r="D53" s="59">
+        <v>1</v>
+      </c>
+      <c r="E53" s="68" t="s">
+        <v>423</v>
+      </c>
+      <c r="F53" s="57">
+        <v>5.18</v>
+      </c>
+      <c r="G53" s="57">
+        <v>15.38</v>
+      </c>
       <c r="H53" s="57"/>
-      <c r="I53" s="57"/>
+      <c r="I53" s="57" t="s">
+        <v>424</v>
+      </c>
       <c r="J53" s="57"/>
       <c r="K53" s="57"/>
       <c r="L53" s="57"/>
@@ -10577,10 +10796,20 @@
       <c r="A54" s="57"/>
       <c r="B54" s="57"/>
       <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="57"/>
+      <c r="D54" s="59">
+        <f>+D53+1</f>
+        <v>2</v>
+      </c>
+      <c r="E54" s="69" t="s">
+        <v>430</v>
+      </c>
+      <c r="F54" s="57">
+        <f>+G53</f>
+        <v>15.38</v>
+      </c>
+      <c r="G54" s="57">
+        <v>22.19</v>
+      </c>
       <c r="H54" s="57"/>
       <c r="I54" s="57"/>
       <c r="J54" s="57"/>
@@ -10592,10 +10821,20 @@
       <c r="A55" s="57"/>
       <c r="B55" s="57"/>
       <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="57"/>
+      <c r="D55" s="59">
+        <f t="shared" ref="D55:D58" si="14">+D54+1</f>
+        <v>3</v>
+      </c>
+      <c r="E55" s="69" t="s">
+        <v>431</v>
+      </c>
+      <c r="F55" s="57">
+        <f t="shared" ref="F55:F57" si="15">+G54</f>
+        <v>22.19</v>
+      </c>
+      <c r="G55" s="57">
+        <v>46.27</v>
+      </c>
       <c r="H55" s="57"/>
       <c r="I55" s="57"/>
       <c r="J55" s="57"/>
@@ -10607,10 +10846,20 @@
       <c r="A56" s="57"/>
       <c r="B56" s="57"/>
       <c r="C56" s="57"/>
-      <c r="D56" s="57"/>
-      <c r="E56" s="57"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="57"/>
+      <c r="D56" s="59">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="E56" s="69" t="s">
+        <v>432</v>
+      </c>
+      <c r="F56" s="57">
+        <f t="shared" si="15"/>
+        <v>46.27</v>
+      </c>
+      <c r="G56" s="57">
+        <v>50.19</v>
+      </c>
       <c r="H56" s="57"/>
       <c r="I56" s="57"/>
       <c r="J56" s="57"/>
@@ -10622,10 +10871,20 @@
       <c r="A57" s="57"/>
       <c r="B57" s="57"/>
       <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="57"/>
-      <c r="F57" s="57"/>
-      <c r="G57" s="57"/>
+      <c r="D57" s="59">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="E57" s="69" t="s">
+        <v>425</v>
+      </c>
+      <c r="F57" s="57">
+        <f t="shared" si="15"/>
+        <v>50.19</v>
+      </c>
+      <c r="G57" s="57">
+        <v>54.25</v>
+      </c>
       <c r="H57" s="57"/>
       <c r="I57" s="57"/>
       <c r="J57" s="57"/>
@@ -10637,11 +10896,23 @@
       <c r="A58" s="57"/>
       <c r="B58" s="57"/>
       <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="57"/>
-      <c r="F58" s="57"/>
-      <c r="G58" s="57"/>
-      <c r="H58" s="57"/>
+      <c r="D58" s="59">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="E58" s="69" t="s">
+        <v>426</v>
+      </c>
+      <c r="F58" s="57">
+        <f>+G57</f>
+        <v>54.25</v>
+      </c>
+      <c r="G58" s="57">
+        <v>57.19</v>
+      </c>
+      <c r="H58" s="69" t="s">
+        <v>426</v>
+      </c>
       <c r="I58" s="57"/>
       <c r="J58" s="57"/>
       <c r="K58" s="57"/>
@@ -10664,15 +10935,31 @@
       <c r="M59" s="57"/>
     </row>
     <row r="60" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A60" s="57"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="57"/>
+      <c r="A60" s="57">
+        <v>11</v>
+      </c>
+      <c r="B60" s="58">
+        <v>44080</v>
+      </c>
+      <c r="C60" s="57">
+        <v>56.02</v>
+      </c>
+      <c r="D60" s="59">
+        <v>1</v>
+      </c>
+      <c r="E60" s="69" t="s">
+        <v>433</v>
+      </c>
+      <c r="F60" s="57">
+        <v>8.09</v>
+      </c>
+      <c r="G60" s="57">
+        <v>13.55</v>
+      </c>
       <c r="H60" s="57"/>
-      <c r="I60" s="57"/>
+      <c r="I60" s="57" t="s">
+        <v>434</v>
+      </c>
       <c r="J60" s="57"/>
       <c r="K60" s="57"/>
       <c r="L60" s="57"/>
@@ -10682,10 +10969,20 @@
       <c r="A61" s="57"/>
       <c r="B61" s="57"/>
       <c r="C61" s="57"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="57"/>
-      <c r="F61" s="57"/>
-      <c r="G61" s="57"/>
+      <c r="D61" s="59">
+        <f>+D60+1</f>
+        <v>2</v>
+      </c>
+      <c r="E61" s="69" t="s">
+        <v>427</v>
+      </c>
+      <c r="F61" s="57">
+        <f>+G60</f>
+        <v>13.55</v>
+      </c>
+      <c r="G61" s="57">
+        <v>24.12</v>
+      </c>
       <c r="H61" s="57"/>
       <c r="I61" s="57"/>
       <c r="J61" s="57"/>
@@ -10697,10 +10994,20 @@
       <c r="A62" s="57"/>
       <c r="B62" s="57"/>
       <c r="C62" s="57"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="57"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="57"/>
+      <c r="D62" s="59">
+        <f t="shared" ref="D62:D63" si="16">+D61+1</f>
+        <v>3</v>
+      </c>
+      <c r="E62" s="69" t="s">
+        <v>428</v>
+      </c>
+      <c r="F62" s="57">
+        <f t="shared" ref="F62:F63" si="17">+G61</f>
+        <v>24.12</v>
+      </c>
+      <c r="G62" s="57">
+        <v>48.37</v>
+      </c>
       <c r="H62" s="57"/>
       <c r="I62" s="57"/>
       <c r="J62" s="57"/>
@@ -10708,6 +11015,22 @@
       <c r="L62" s="57"/>
       <c r="M62" s="57"/>
     </row>
+    <row r="63" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="D63" s="59">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="E63" s="69" t="s">
+        <v>429</v>
+      </c>
+      <c r="F63" s="57">
+        <f t="shared" si="17"/>
+        <v>48.37</v>
+      </c>
+      <c r="G63" s="70">
+        <v>54.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Ghanam and TB 3.7 edits 07/08 Sept
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="441">
   <si>
     <t>Date</t>
   </si>
@@ -1321,19 +1321,43 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=Zj43zg9-3ug</t>
+  </si>
+  <si>
+    <t>3.4.9.2</t>
+  </si>
+  <si>
+    <t>3.4.9.3</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=EDh8TaLUDZo</t>
+  </si>
+  <si>
+    <t>3.4.10.1</t>
+  </si>
+  <si>
+    <t>3.4.11.1</t>
+  </si>
+  <si>
+    <t>3.5.1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1656,78 +1680,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="46" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="47" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="47" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="48" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1736,8 +1761,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9526,10 +9552,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11030,6 +11056,451 @@
       <c r="G63" s="70">
         <v>54.5</v>
       </c>
+      <c r="H63" s="69" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A64" s="71"/>
+      <c r="B64" s="71"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="71"/>
+      <c r="F64" s="71"/>
+      <c r="G64" s="71"/>
+      <c r="H64" s="71"/>
+      <c r="I64" s="71"/>
+    </row>
+    <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A65" s="71">
+        <v>12</v>
+      </c>
+      <c r="B65" s="72">
+        <v>44081</v>
+      </c>
+      <c r="C65" s="71">
+        <v>57.23</v>
+      </c>
+      <c r="D65" s="59">
+        <v>1</v>
+      </c>
+      <c r="E65" s="71" t="s">
+        <v>436</v>
+      </c>
+      <c r="F65" s="71">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="G65" s="71">
+        <v>20.57</v>
+      </c>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A66" s="71"/>
+      <c r="B66" s="71"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="59">
+        <f>+D65+1</f>
+        <v>2</v>
+      </c>
+      <c r="E66" s="71" t="s">
+        <v>438</v>
+      </c>
+      <c r="F66" s="71">
+        <f>+G65</f>
+        <v>20.57</v>
+      </c>
+      <c r="G66" s="71">
+        <v>37.14</v>
+      </c>
+      <c r="H66" s="71"/>
+      <c r="I66" s="71"/>
+    </row>
+    <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A67" s="71"/>
+      <c r="B67" s="71"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="59">
+        <f t="shared" ref="D67:D68" si="18">+D66+1</f>
+        <v>3</v>
+      </c>
+      <c r="E67" s="71" t="s">
+        <v>439</v>
+      </c>
+      <c r="F67" s="71">
+        <f>+G66</f>
+        <v>37.14</v>
+      </c>
+      <c r="G67" s="71">
+        <v>53.42</v>
+      </c>
+      <c r="H67" s="71"/>
+      <c r="I67" s="71"/>
+    </row>
+    <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A68" s="71"/>
+      <c r="B68" s="71"/>
+      <c r="C68" s="71"/>
+      <c r="D68" s="59">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+      <c r="E68" s="71" t="s">
+        <v>440</v>
+      </c>
+      <c r="F68" s="71">
+        <f>+G67</f>
+        <v>53.42</v>
+      </c>
+      <c r="G68" s="71">
+        <v>56.51</v>
+      </c>
+      <c r="H68" s="71"/>
+      <c r="I68" s="71"/>
+    </row>
+    <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A69" s="71"/>
+      <c r="B69" s="71"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="71"/>
+      <c r="E69" s="71"/>
+      <c r="F69" s="71"/>
+      <c r="G69" s="71"/>
+      <c r="H69" s="71"/>
+      <c r="I69" s="71"/>
+    </row>
+    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A70" s="71"/>
+      <c r="B70" s="71"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="71"/>
+      <c r="E70" s="71"/>
+      <c r="F70" s="71"/>
+      <c r="G70" s="71"/>
+      <c r="H70" s="71"/>
+      <c r="I70" s="71"/>
+    </row>
+    <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A71" s="71"/>
+      <c r="B71" s="71"/>
+      <c r="C71" s="71"/>
+      <c r="D71" s="71"/>
+      <c r="E71" s="71"/>
+      <c r="F71" s="71"/>
+      <c r="G71" s="71"/>
+      <c r="H71" s="71"/>
+      <c r="I71" s="71"/>
+    </row>
+    <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A72" s="71"/>
+      <c r="B72" s="71"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="71"/>
+      <c r="F72" s="71"/>
+      <c r="G72" s="71"/>
+      <c r="H72" s="71"/>
+      <c r="I72" s="71"/>
+    </row>
+    <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A73" s="71"/>
+      <c r="B73" s="71"/>
+      <c r="C73" s="71"/>
+      <c r="D73" s="71"/>
+      <c r="E73" s="71"/>
+      <c r="F73" s="71"/>
+      <c r="G73" s="71"/>
+      <c r="H73" s="71"/>
+      <c r="I73" s="71"/>
+    </row>
+    <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A74" s="71"/>
+      <c r="B74" s="71"/>
+      <c r="C74" s="71"/>
+      <c r="D74" s="71"/>
+      <c r="E74" s="71"/>
+      <c r="F74" s="71"/>
+      <c r="G74" s="71"/>
+      <c r="H74" s="71"/>
+      <c r="I74" s="71"/>
+    </row>
+    <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A75" s="71"/>
+      <c r="B75" s="71"/>
+      <c r="C75" s="71"/>
+      <c r="D75" s="71"/>
+      <c r="E75" s="71"/>
+      <c r="F75" s="71"/>
+      <c r="G75" s="71"/>
+      <c r="H75" s="71"/>
+      <c r="I75" s="71"/>
+    </row>
+    <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A76" s="71"/>
+      <c r="B76" s="71"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="71"/>
+      <c r="E76" s="71"/>
+      <c r="F76" s="71"/>
+      <c r="G76" s="71"/>
+      <c r="H76" s="71"/>
+      <c r="I76" s="71"/>
+    </row>
+    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A77" s="71"/>
+      <c r="B77" s="71"/>
+      <c r="C77" s="71"/>
+      <c r="D77" s="71"/>
+      <c r="E77" s="71"/>
+      <c r="F77" s="71"/>
+      <c r="G77" s="71"/>
+      <c r="H77" s="71"/>
+      <c r="I77" s="71"/>
+    </row>
+    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A78" s="71"/>
+      <c r="B78" s="71"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="71"/>
+      <c r="E78" s="71"/>
+      <c r="F78" s="71"/>
+      <c r="G78" s="71"/>
+      <c r="H78" s="71"/>
+      <c r="I78" s="71"/>
+    </row>
+    <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A79" s="71"/>
+      <c r="B79" s="71"/>
+      <c r="C79" s="71"/>
+      <c r="D79" s="71"/>
+      <c r="E79" s="71"/>
+      <c r="F79" s="71"/>
+      <c r="G79" s="71"/>
+      <c r="H79" s="71"/>
+      <c r="I79" s="71"/>
+    </row>
+    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A80" s="71"/>
+      <c r="B80" s="71"/>
+      <c r="C80" s="71"/>
+      <c r="D80" s="71"/>
+      <c r="E80" s="71"/>
+      <c r="F80" s="71"/>
+      <c r="G80" s="71"/>
+      <c r="H80" s="71"/>
+      <c r="I80" s="71"/>
+    </row>
+    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A81" s="71"/>
+      <c r="B81" s="71"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="71"/>
+      <c r="E81" s="71"/>
+      <c r="F81" s="71"/>
+      <c r="G81" s="71"/>
+      <c r="H81" s="71"/>
+      <c r="I81" s="71"/>
+    </row>
+    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A82" s="71"/>
+      <c r="B82" s="71"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="71"/>
+      <c r="E82" s="71"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="71"/>
+      <c r="H82" s="71"/>
+      <c r="I82" s="71"/>
+    </row>
+    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A83" s="71"/>
+      <c r="B83" s="71"/>
+      <c r="C83" s="71"/>
+      <c r="D83" s="71"/>
+      <c r="E83" s="71"/>
+      <c r="F83" s="71"/>
+      <c r="G83" s="71"/>
+      <c r="H83" s="71"/>
+      <c r="I83" s="71"/>
+    </row>
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A84" s="71"/>
+      <c r="B84" s="71"/>
+      <c r="C84" s="71"/>
+      <c r="D84" s="71"/>
+      <c r="E84" s="71"/>
+      <c r="F84" s="71"/>
+      <c r="G84" s="71"/>
+      <c r="H84" s="71"/>
+      <c r="I84" s="71"/>
+    </row>
+    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A85" s="71"/>
+      <c r="B85" s="71"/>
+      <c r="C85" s="71"/>
+      <c r="D85" s="71"/>
+      <c r="E85" s="71"/>
+      <c r="F85" s="71"/>
+      <c r="G85" s="71"/>
+      <c r="H85" s="71"/>
+      <c r="I85" s="71"/>
+    </row>
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A86" s="71"/>
+      <c r="B86" s="71"/>
+      <c r="C86" s="71"/>
+      <c r="D86" s="71"/>
+      <c r="E86" s="71"/>
+      <c r="F86" s="71"/>
+      <c r="G86" s="71"/>
+      <c r="H86" s="71"/>
+      <c r="I86" s="71"/>
+    </row>
+    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A87" s="71"/>
+      <c r="B87" s="71"/>
+      <c r="C87" s="71"/>
+      <c r="D87" s="71"/>
+      <c r="E87" s="71"/>
+      <c r="F87" s="71"/>
+      <c r="G87" s="71"/>
+      <c r="H87" s="71"/>
+      <c r="I87" s="71"/>
+    </row>
+    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A88" s="71"/>
+      <c r="B88" s="71"/>
+      <c r="C88" s="71"/>
+      <c r="D88" s="71"/>
+      <c r="E88" s="71"/>
+      <c r="F88" s="71"/>
+      <c r="G88" s="71"/>
+      <c r="H88" s="71"/>
+      <c r="I88" s="71"/>
+    </row>
+    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A89" s="71"/>
+      <c r="B89" s="71"/>
+      <c r="C89" s="71"/>
+      <c r="D89" s="71"/>
+      <c r="E89" s="71"/>
+      <c r="F89" s="71"/>
+      <c r="G89" s="71"/>
+      <c r="H89" s="71"/>
+      <c r="I89" s="71"/>
+    </row>
+    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A90" s="71"/>
+      <c r="B90" s="71"/>
+      <c r="C90" s="71"/>
+      <c r="D90" s="71"/>
+      <c r="E90" s="71"/>
+      <c r="F90" s="71"/>
+      <c r="G90" s="71"/>
+      <c r="H90" s="71"/>
+      <c r="I90" s="71"/>
+    </row>
+    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A91" s="71"/>
+      <c r="B91" s="71"/>
+      <c r="C91" s="71"/>
+      <c r="D91" s="71"/>
+      <c r="E91" s="71"/>
+      <c r="F91" s="71"/>
+      <c r="G91" s="71"/>
+      <c r="H91" s="71"/>
+      <c r="I91" s="71"/>
+    </row>
+    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A92" s="71"/>
+      <c r="B92" s="71"/>
+      <c r="C92" s="71"/>
+      <c r="D92" s="71"/>
+      <c r="E92" s="71"/>
+      <c r="F92" s="71"/>
+      <c r="G92" s="71"/>
+      <c r="H92" s="71"/>
+      <c r="I92" s="71"/>
+    </row>
+    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A93" s="71"/>
+      <c r="B93" s="71"/>
+      <c r="C93" s="71"/>
+      <c r="D93" s="71"/>
+      <c r="E93" s="71"/>
+      <c r="F93" s="71"/>
+      <c r="G93" s="71"/>
+      <c r="H93" s="71"/>
+      <c r="I93" s="71"/>
+    </row>
+    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A94" s="71"/>
+      <c r="B94" s="71"/>
+      <c r="C94" s="71"/>
+      <c r="D94" s="71"/>
+      <c r="E94" s="71"/>
+      <c r="F94" s="71"/>
+      <c r="G94" s="71"/>
+      <c r="H94" s="71"/>
+      <c r="I94" s="71"/>
+    </row>
+    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A95" s="71"/>
+      <c r="B95" s="71"/>
+      <c r="C95" s="71"/>
+      <c r="D95" s="71"/>
+      <c r="E95" s="71"/>
+      <c r="F95" s="71"/>
+      <c r="G95" s="71"/>
+      <c r="H95" s="71"/>
+      <c r="I95" s="71"/>
+    </row>
+    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A96" s="71"/>
+      <c r="B96" s="71"/>
+      <c r="C96" s="71"/>
+      <c r="D96" s="71"/>
+      <c r="E96" s="71"/>
+      <c r="F96" s="71"/>
+      <c r="G96" s="71"/>
+      <c r="H96" s="71"/>
+      <c r="I96" s="71"/>
+    </row>
+    <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A97" s="71"/>
+      <c r="B97" s="71"/>
+      <c r="C97" s="71"/>
+      <c r="D97" s="71"/>
+      <c r="E97" s="71"/>
+      <c r="F97" s="71"/>
+      <c r="G97" s="71"/>
+      <c r="H97" s="71"/>
+      <c r="I97" s="71"/>
+    </row>
+    <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A98" s="71"/>
+      <c r="B98" s="71"/>
+      <c r="C98" s="71"/>
+      <c r="D98" s="71"/>
+      <c r="E98" s="71"/>
+      <c r="F98" s="71"/>
+      <c r="G98" s="71"/>
+      <c r="H98" s="71"/>
+      <c r="I98" s="71"/>
+    </row>
+    <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A99" s="71"/>
+      <c r="B99" s="71"/>
+      <c r="C99" s="71"/>
+      <c r="D99" s="71"/>
+      <c r="E99" s="71"/>
+      <c r="F99" s="71"/>
+      <c r="G99" s="71"/>
+      <c r="H99" s="71"/>
+      <c r="I99" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TB 3.7-12, Latin docx TTD 09/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Kandam3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="453">
   <si>
     <t>Date</t>
   </si>
@@ -1339,19 +1340,67 @@
   </si>
   <si>
     <t>3.5.1.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QvaBB09CHDI</t>
+  </si>
+  <si>
+    <t>3.5.1.2</t>
+  </si>
+  <si>
+    <t>3.5.2.1</t>
+  </si>
+  <si>
+    <t>3.5.3.1</t>
+  </si>
+  <si>
+    <t>3.5.4.1</t>
+  </si>
+  <si>
+    <t>3.5.5.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dSgPzo3S_94</t>
+  </si>
+  <si>
+    <t>3.5.6.1</t>
+  </si>
+  <si>
+    <t>3.5.7.1</t>
+  </si>
+  <si>
+    <t>3.5.8.1</t>
+  </si>
+  <si>
+    <t>3.5.9.1</t>
+  </si>
+  <si>
+    <t>3.5.10.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="52" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1680,78 +1729,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="47" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="49" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="48" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="50" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1759,11 +1810,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2496,7 +2547,7 @@
         <v>25</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" ref="F22:F25" si="0">+G21</f>
+        <f>+G21</f>
         <v>16.29</v>
       </c>
       <c r="G22" s="6">
@@ -2519,7 +2570,7 @@
         <v>26</v>
       </c>
       <c r="F23" s="6">
-        <f t="shared" si="0"/>
+        <f>+G22</f>
         <v>29.49</v>
       </c>
       <c r="G23" s="6">
@@ -2542,7 +2593,7 @@
         <v>27</v>
       </c>
       <c r="F24" s="6">
-        <f t="shared" si="0"/>
+        <f>+G23</f>
         <v>36.57</v>
       </c>
       <c r="G24" s="6">
@@ -2565,7 +2616,7 @@
         <v>28</v>
       </c>
       <c r="F25" s="6">
-        <f t="shared" si="0"/>
+        <f>+G24</f>
         <v>45.53</v>
       </c>
       <c r="G25" s="6">
@@ -2651,14 +2702,14 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="4">
-        <f t="shared" ref="D29:D34" si="1">+D28+1</f>
+        <f t="shared" ref="D29:D34" si="0">+D28+1</f>
         <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F29" s="6">
-        <f t="shared" ref="F29:F34" si="2">+G28</f>
+        <f t="shared" ref="F29:F34" si="1">+G28</f>
         <v>18.510000000000002</v>
       </c>
       <c r="G29" s="6">
@@ -2675,14 +2726,14 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>23.47</v>
       </c>
       <c r="G30" s="6">
@@ -2701,7 +2752,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -2723,14 +2774,14 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>34.01</v>
       </c>
       <c r="G32" s="6">
@@ -2754,7 +2805,7 @@
         <v>36</v>
       </c>
       <c r="F33" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>39.36</v>
       </c>
       <c r="G33" s="6">
@@ -2771,14 +2822,14 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F34" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44.39</v>
       </c>
       <c r="G34" s="6">
@@ -2864,14 +2915,14 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="4">
-        <f t="shared" ref="D38:D39" si="3">+D37+1</f>
+        <f>+D37+1</f>
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F38" s="6">
-        <f t="shared" ref="F38:F39" si="4">+G37</f>
+        <f>+G37</f>
         <v>23.04</v>
       </c>
       <c r="G38" s="6">
@@ -2888,14 +2939,14 @@
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="4">
-        <f t="shared" si="3"/>
+        <f>+D38+1</f>
         <v>4</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>46</v>
       </c>
       <c r="F39" s="6">
-        <f t="shared" si="4"/>
+        <f>+G38</f>
         <v>32.42</v>
       </c>
       <c r="G39" s="6">
@@ -2981,14 +3032,14 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="4">
-        <f t="shared" ref="D43:D48" si="5">+D42+1</f>
+        <f t="shared" ref="D43:D48" si="2">+D42+1</f>
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F43" s="6">
-        <f t="shared" ref="F43:F48" si="6">+G42</f>
+        <f t="shared" ref="F43:F48" si="3">+G42</f>
         <v>15.42</v>
       </c>
       <c r="G43" s="6">
@@ -3005,14 +3056,14 @@
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>51</v>
       </c>
       <c r="F44" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>24.17</v>
       </c>
       <c r="G44" s="6">
@@ -3029,14 +3080,14 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F45" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>27.47</v>
       </c>
       <c r="G45" s="6">
@@ -3053,14 +3104,14 @@
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>37.08</v>
       </c>
       <c r="G46" s="6">
@@ -3077,14 +3128,14 @@
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F47" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>41.1</v>
       </c>
       <c r="G47" s="6">
@@ -3101,14 +3152,14 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F48" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>49.11</v>
       </c>
       <c r="G48" s="6">
@@ -3170,14 +3221,14 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="4">
-        <f>+D50+1</f>
+        <f t="shared" ref="D51:D56" si="4">+D50+1</f>
         <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F51" s="6">
-        <f t="shared" ref="F51:F56" si="7">+G50</f>
+        <f t="shared" ref="F51:F56" si="5">+G50</f>
         <v>11.48</v>
       </c>
       <c r="G51" s="6">
@@ -3194,14 +3245,14 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="4">
-        <f t="shared" ref="D52:D56" si="8">+D51+1</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F52" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>18.12</v>
       </c>
       <c r="G52" s="6">
@@ -3218,14 +3269,14 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>60</v>
       </c>
       <c r="F53" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>24.08</v>
       </c>
       <c r="G53" s="6">
@@ -3242,14 +3293,14 @@
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F54" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>29.13</v>
       </c>
       <c r="G54" s="6">
@@ -3266,14 +3317,14 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F55" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>32.14</v>
       </c>
       <c r="G55" s="6">
@@ -3290,14 +3341,14 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>63</v>
       </c>
       <c r="F56" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.090000000000003</v>
       </c>
       <c r="G56" s="6">
@@ -3361,7 +3412,7 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="4">
-        <f t="shared" ref="D59:D69" si="9">+D58+1</f>
+        <f t="shared" ref="D59:D69" si="6">+D58+1</f>
         <v>2</v>
       </c>
       <c r="E59" s="1" t="s">
@@ -3385,14 +3436,14 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F60" s="6">
-        <f t="shared" ref="F60:F69" si="10">+G59</f>
+        <f t="shared" ref="F60:F69" si="7">+G59</f>
         <v>28.14</v>
       </c>
       <c r="G60" s="6">
@@ -3409,14 +3460,14 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F61" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>31.45</v>
       </c>
       <c r="G61" s="6">
@@ -3433,14 +3484,14 @@
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F62" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>36.06</v>
       </c>
       <c r="G62" s="6">
@@ -3457,14 +3508,14 @@
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F63" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>39.119999999999997</v>
       </c>
       <c r="G63" s="6">
@@ -3481,14 +3532,14 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F64" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>40.42</v>
       </c>
       <c r="G64" s="6">
@@ -3505,14 +3556,14 @@
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>76</v>
       </c>
       <c r="F65" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>42.04</v>
       </c>
       <c r="G65" s="6">
@@ -3529,14 +3580,14 @@
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>77</v>
       </c>
       <c r="F66" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>43.23</v>
       </c>
       <c r="G66" s="6">
@@ -3553,14 +3604,14 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F67" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>45.19</v>
       </c>
       <c r="G67" s="6">
@@ -3577,14 +3628,14 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F68" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>47.22</v>
       </c>
       <c r="G68" s="6">
@@ -3601,14 +3652,14 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F69" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>50.19</v>
       </c>
       <c r="G69" s="6">
@@ -3694,14 +3745,14 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="4">
-        <f t="shared" ref="D73:D106" si="11">+D72+1</f>
+        <f t="shared" ref="D73:D106" si="8">+D72+1</f>
         <v>3</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F73" s="6">
-        <f t="shared" ref="F73:F106" si="12">+G72</f>
+        <f t="shared" ref="F73:F106" si="9">+G72</f>
         <v>9.0399999999999991</v>
       </c>
       <c r="G73" s="6">
@@ -3718,14 +3769,14 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F74" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>10.5</v>
       </c>
       <c r="G74" s="6">
@@ -3742,14 +3793,14 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>87</v>
       </c>
       <c r="F75" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>12.28</v>
       </c>
       <c r="G75" s="6">
@@ -3766,14 +3817,14 @@
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>88</v>
       </c>
       <c r="F76" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>14.01</v>
       </c>
       <c r="G76" s="6">
@@ -3790,14 +3841,14 @@
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>90</v>
       </c>
       <c r="F77" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>15.53</v>
       </c>
       <c r="G77" s="6">
@@ -3814,14 +3865,14 @@
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F78" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>17.46</v>
       </c>
       <c r="G78" s="6">
@@ -3838,14 +3889,14 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>92</v>
       </c>
       <c r="F79" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>19.41</v>
       </c>
       <c r="G79" s="6">
@@ -3862,14 +3913,14 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F80" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>21.08</v>
       </c>
       <c r="G80" s="6">
@@ -3886,14 +3937,14 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F81" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>23.18</v>
       </c>
       <c r="G81" s="6">
@@ -3910,14 +3961,14 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F82" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>27.5</v>
       </c>
       <c r="G82" s="6">
@@ -3934,14 +3985,14 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F83" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>29.24</v>
       </c>
       <c r="G83" s="6">
@@ -3958,14 +4009,14 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F84" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>30.55</v>
       </c>
       <c r="G84" s="6">
@@ -3980,14 +4031,14 @@
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D85" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>98</v>
       </c>
       <c r="F85" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>31.52</v>
       </c>
       <c r="G85" s="6">
@@ -3996,14 +4047,14 @@
     </row>
     <row r="86" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D86" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>99</v>
       </c>
       <c r="F86" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>32.44</v>
       </c>
       <c r="G86" s="6">
@@ -4012,14 +4063,14 @@
     </row>
     <row r="87" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D87" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>100</v>
       </c>
       <c r="F87" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>34.42</v>
       </c>
       <c r="G87" s="6">
@@ -4028,14 +4079,14 @@
     </row>
     <row r="88" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D88" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F88" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>37.020000000000003</v>
       </c>
       <c r="G88" s="6">
@@ -4044,14 +4095,14 @@
     </row>
     <row r="89" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D89" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>102</v>
       </c>
       <c r="F89" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>38.24</v>
       </c>
       <c r="G89" s="6">
@@ -4060,14 +4111,14 @@
     </row>
     <row r="90" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D90" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>103</v>
       </c>
       <c r="F90" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>39.479999999999997</v>
       </c>
       <c r="G90" s="6">
@@ -4076,14 +4127,14 @@
     </row>
     <row r="91" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D91" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>104</v>
       </c>
       <c r="F91" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>41.14</v>
       </c>
       <c r="G91" s="6">
@@ -4092,14 +4143,14 @@
     </row>
     <row r="92" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D92" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>105</v>
       </c>
       <c r="F92" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>41.49</v>
       </c>
       <c r="G92" s="6">
@@ -4108,14 +4159,14 @@
     </row>
     <row r="93" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D93" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F93" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>43.08</v>
       </c>
       <c r="G93" s="6">
@@ -4124,14 +4175,14 @@
     </row>
     <row r="94" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D94" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>107</v>
       </c>
       <c r="F94" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>46.09</v>
       </c>
       <c r="G94" s="6">
@@ -4140,14 +4191,14 @@
     </row>
     <row r="95" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D95" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>108</v>
       </c>
       <c r="F95" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>48.37</v>
       </c>
       <c r="G95" s="6">
@@ -4156,14 +4207,14 @@
     </row>
     <row r="96" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D96" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>109</v>
       </c>
       <c r="F96" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>50.39</v>
       </c>
       <c r="G96" s="6">
@@ -4213,14 +4264,14 @@
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>111</v>
       </c>
       <c r="F99" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>2.0699999999999998</v>
       </c>
       <c r="G99" s="6">
@@ -4233,14 +4284,14 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>113</v>
       </c>
       <c r="F100" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>3.52</v>
       </c>
       <c r="G100" s="6">
@@ -4253,14 +4304,14 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>114</v>
       </c>
       <c r="F101" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>5.56</v>
       </c>
       <c r="G101" s="6">
@@ -4273,14 +4324,14 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>115</v>
       </c>
       <c r="F102" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>7.56</v>
       </c>
       <c r="G102" s="6">
@@ -4293,14 +4344,14 @@
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>116</v>
       </c>
       <c r="F103" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>10.06</v>
       </c>
       <c r="G103" s="6">
@@ -4313,14 +4364,14 @@
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F104" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>18.149999999999999</v>
       </c>
       <c r="G104" s="6">
@@ -4333,14 +4384,14 @@
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>118</v>
       </c>
       <c r="F105" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>27.26</v>
       </c>
       <c r="G105" s="6">
@@ -4353,14 +4404,14 @@
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>119</v>
       </c>
       <c r="F106" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>37.22</v>
       </c>
       <c r="G106" s="6">
@@ -4410,7 +4461,7 @@
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="4">
-        <f t="shared" ref="D109:D116" si="13">+D108+1</f>
+        <f t="shared" ref="D109:D116" si="10">+D108+1</f>
         <v>2</v>
       </c>
       <c r="E109" s="1" t="s">
@@ -4430,14 +4481,14 @@
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>128</v>
       </c>
       <c r="F110" s="6">
-        <f t="shared" ref="F110:F111" si="14">+G109</f>
+        <f>+G109</f>
         <v>31.32</v>
       </c>
       <c r="G110" s="6">
@@ -4450,14 +4501,14 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>129</v>
       </c>
       <c r="F111" s="6">
-        <f t="shared" si="14"/>
+        <f>+G110</f>
         <v>40.15</v>
       </c>
       <c r="G111" s="6">
@@ -4505,7 +4556,7 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="E114" s="1" t="s">
@@ -4525,14 +4576,14 @@
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>132</v>
       </c>
       <c r="F115" s="6">
-        <f t="shared" ref="F115:F116" si="15">+G114</f>
+        <f>+G114</f>
         <v>28.29</v>
       </c>
       <c r="G115" s="6">
@@ -4545,14 +4596,14 @@
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>133</v>
       </c>
       <c r="F116" s="6">
-        <f t="shared" si="15"/>
+        <f>+G115</f>
         <v>47.08</v>
       </c>
       <c r="G116" s="6">
@@ -4602,7 +4653,7 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="4">
-        <f t="shared" ref="D119:D121" si="16">+D118+1</f>
+        <f>+D118+1</f>
         <v>2</v>
       </c>
       <c r="E119" s="1" t="s">
@@ -4624,7 +4675,7 @@
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="4">
-        <f t="shared" si="16"/>
+        <f>+D119+1</f>
         <v>3</v>
       </c>
       <c r="E120" s="1" t="s">
@@ -4643,14 +4694,14 @@
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="4">
-        <f t="shared" si="16"/>
+        <f>+D120+1</f>
         <v>4</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>139</v>
       </c>
       <c r="F121" s="6">
-        <f t="shared" ref="F121" si="17">+G120</f>
+        <f>+G120</f>
         <v>47.24</v>
       </c>
       <c r="G121" s="6">
@@ -4700,7 +4751,7 @@
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="4">
-        <f t="shared" ref="D124:D127" si="18">+D123+1</f>
+        <f>+D123+1</f>
         <v>2</v>
       </c>
       <c r="E124" s="1" t="s">
@@ -4720,14 +4771,14 @@
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="4">
-        <f t="shared" si="18"/>
+        <f>+D124+1</f>
         <v>3</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>144</v>
       </c>
       <c r="F125" s="6">
-        <f t="shared" ref="F125:F127" si="19">+G124</f>
+        <f>+G124</f>
         <v>15.35</v>
       </c>
       <c r="G125" s="6">
@@ -4740,14 +4791,14 @@
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="4">
-        <f t="shared" si="18"/>
+        <f>+D125+1</f>
         <v>4</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>145</v>
       </c>
       <c r="F126" s="6">
-        <f t="shared" si="19"/>
+        <f>+G125</f>
         <v>34.299999999999997</v>
       </c>
       <c r="G126" s="6">
@@ -4760,14 +4811,14 @@
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="4">
-        <f t="shared" si="18"/>
+        <f>+D126+1</f>
         <v>5</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F127" s="6">
-        <f t="shared" si="19"/>
+        <f>+G126</f>
         <v>43.32</v>
       </c>
       <c r="G127" s="6">
@@ -4817,7 +4868,7 @@
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="4">
-        <f t="shared" ref="D130:D133" si="20">+D129+1</f>
+        <f>+D129+1</f>
         <v>2</v>
       </c>
       <c r="E130" s="11" t="s">
@@ -4839,7 +4890,7 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="4">
-        <f t="shared" si="20"/>
+        <f>+D130+1</f>
         <v>3</v>
       </c>
       <c r="E131" s="11" t="s">
@@ -4858,14 +4909,14 @@
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="4">
-        <f t="shared" si="20"/>
+        <f>+D131+1</f>
         <v>4</v>
       </c>
       <c r="E132" s="11" t="s">
         <v>154</v>
       </c>
       <c r="F132" s="6">
-        <f t="shared" ref="F132:F133" si="21">+G131</f>
+        <f>+G131</f>
         <v>42.37</v>
       </c>
       <c r="G132" s="6">
@@ -4878,14 +4929,14 @@
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="4">
-        <f t="shared" si="20"/>
+        <f>+D132+1</f>
         <v>5</v>
       </c>
       <c r="E133" s="11" t="s">
         <v>155</v>
       </c>
       <c r="F133" s="6">
-        <f t="shared" si="21"/>
+        <f>+G132</f>
         <v>55.03</v>
       </c>
       <c r="G133" s="6">
@@ -4937,7 +4988,7 @@
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="4">
-        <f t="shared" ref="D136:D141" si="22">+D135+1</f>
+        <f t="shared" ref="D136:D141" si="11">+D135+1</f>
         <v>2</v>
       </c>
       <c r="E136" s="11" t="s">
@@ -4957,7 +5008,7 @@
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E137" s="13" t="s">
@@ -5015,7 +5066,7 @@
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="E140" s="11" t="s">
@@ -5037,7 +5088,7 @@
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E141" s="11" t="s">
@@ -5062,7 +5113,7 @@
         <v>169</v>
       </c>
       <c r="F142" s="6">
-        <f t="shared" ref="F142" si="23">+G141</f>
+        <f>+G141</f>
         <v>48.25</v>
       </c>
       <c r="G142" s="6">
@@ -5114,7 +5165,7 @@
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="4">
-        <f t="shared" ref="D145" si="24">+D144+1</f>
+        <f>+D144+1</f>
         <v>2</v>
       </c>
       <c r="E145" s="11" t="s">
@@ -5190,7 +5241,7 @@
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="4">
-        <f t="shared" ref="D149:D152" si="25">+D148+1</f>
+        <f>+D148+1</f>
         <v>2</v>
       </c>
       <c r="E149" s="12" t="s">
@@ -5210,14 +5261,14 @@
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="4">
-        <f t="shared" si="25"/>
+        <f>+D149+1</f>
         <v>3</v>
       </c>
       <c r="E150" s="12" t="s">
         <v>176</v>
       </c>
       <c r="F150" s="6">
-        <f t="shared" ref="F150:F152" si="26">+G149</f>
+        <f>+G149</f>
         <v>22.09</v>
       </c>
       <c r="G150" s="6">
@@ -5230,14 +5281,14 @@
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="4">
-        <f t="shared" si="25"/>
+        <f>+D150+1</f>
         <v>4</v>
       </c>
       <c r="E151" s="12" t="s">
         <v>177</v>
       </c>
       <c r="F151" s="6">
-        <f t="shared" si="26"/>
+        <f>+G150</f>
         <v>45.27</v>
       </c>
       <c r="G151" s="6">
@@ -5250,14 +5301,14 @@
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="4">
-        <f t="shared" si="25"/>
+        <f>+D151+1</f>
         <v>5</v>
       </c>
       <c r="E152" s="12" t="s">
         <v>178</v>
       </c>
       <c r="F152" s="6">
-        <f t="shared" si="26"/>
+        <f>+G151</f>
         <v>52.3</v>
       </c>
       <c r="G152" s="6">
@@ -5329,14 +5380,14 @@
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="4">
-        <f t="shared" ref="D156:D159" si="27">+D155+1</f>
+        <f>+D155+1</f>
         <v>3</v>
       </c>
       <c r="E156" s="12" t="s">
         <v>183</v>
       </c>
       <c r="F156" s="6">
-        <f t="shared" ref="F156:F159" si="28">+G155</f>
+        <f>+G155</f>
         <v>22.28</v>
       </c>
       <c r="G156" s="6">
@@ -5349,14 +5400,14 @@
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="4">
-        <f t="shared" si="27"/>
+        <f>+D156+1</f>
         <v>4</v>
       </c>
       <c r="E157" s="12" t="s">
         <v>184</v>
       </c>
       <c r="F157" s="6">
-        <f t="shared" si="28"/>
+        <f>+G156</f>
         <v>31.35</v>
       </c>
       <c r="G157" s="6">
@@ -5369,14 +5420,14 @@
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="4">
-        <f t="shared" si="27"/>
+        <f>+D157+1</f>
         <v>5</v>
       </c>
       <c r="E158" s="12" t="s">
         <v>185</v>
       </c>
       <c r="F158" s="6">
-        <f t="shared" si="28"/>
+        <f>+G157</f>
         <v>39.4</v>
       </c>
       <c r="G158" s="6">
@@ -5389,14 +5440,14 @@
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="4">
-        <f t="shared" si="27"/>
+        <f>+D158+1</f>
         <v>6</v>
       </c>
       <c r="E159" s="12" t="s">
         <v>186</v>
       </c>
       <c r="F159" s="6">
-        <f t="shared" si="28"/>
+        <f>+G158</f>
         <v>47.26</v>
       </c>
       <c r="G159" s="6">
@@ -5448,14 +5499,14 @@
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="4">
-        <f>+D161+1</f>
+        <f t="shared" ref="D162:D167" si="12">+D161+1</f>
         <v>2</v>
       </c>
       <c r="E162" s="12" t="s">
         <v>191</v>
       </c>
       <c r="F162" s="6">
-        <f>+G161</f>
+        <f t="shared" ref="F162:F167" si="13">+G161</f>
         <v>15.05</v>
       </c>
       <c r="G162" s="6">
@@ -5468,14 +5519,14 @@
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="4">
-        <f t="shared" ref="D163:D167" si="29">+D162+1</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="E163" s="12" t="s">
         <v>192</v>
       </c>
       <c r="F163" s="6">
-        <f t="shared" ref="F163:F167" si="30">+G162</f>
+        <f t="shared" si="13"/>
         <v>21.48</v>
       </c>
       <c r="G163" s="6">
@@ -5488,14 +5539,14 @@
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="E164" s="12" t="s">
         <v>193</v>
       </c>
       <c r="F164" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="13"/>
         <v>23.36</v>
       </c>
       <c r="G164" s="6">
@@ -5508,14 +5559,14 @@
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="E165" s="12" t="s">
         <v>194</v>
       </c>
       <c r="F165" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="13"/>
         <v>28.1</v>
       </c>
       <c r="G165" s="6">
@@ -5528,14 +5579,14 @@
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="E166" s="12" t="s">
         <v>195</v>
       </c>
       <c r="F166" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="13"/>
         <v>34.01</v>
       </c>
       <c r="G166" s="6">
@@ -5548,14 +5599,14 @@
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="E167" s="12" t="s">
         <v>196</v>
       </c>
       <c r="F167" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="13"/>
         <v>42.59</v>
       </c>
       <c r="G167" s="6">
@@ -5625,14 +5676,14 @@
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="4">
-        <f t="shared" ref="D171:D174" si="31">+D170+1</f>
+        <f>+D170+1</f>
         <v>3</v>
       </c>
       <c r="E171" s="12" t="s">
         <v>201</v>
       </c>
       <c r="F171" s="6">
-        <f t="shared" ref="F171:F174" si="32">+G170</f>
+        <f>+G170</f>
         <v>20.38</v>
       </c>
       <c r="G171" s="6">
@@ -5645,14 +5696,14 @@
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="4">
-        <f t="shared" si="31"/>
+        <f>+D171+1</f>
         <v>4</v>
       </c>
       <c r="E172" s="12" t="s">
         <v>202</v>
       </c>
       <c r="F172" s="6">
-        <f t="shared" si="32"/>
+        <f>+G171</f>
         <v>32.21</v>
       </c>
       <c r="G172" s="6">
@@ -5665,14 +5716,14 @@
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="4">
-        <f t="shared" si="31"/>
+        <f>+D172+1</f>
         <v>5</v>
       </c>
       <c r="E173" s="12" t="s">
         <v>203</v>
       </c>
       <c r="F173" s="6">
-        <f t="shared" si="32"/>
+        <f>+G172</f>
         <v>42.34</v>
       </c>
       <c r="G173" s="6">
@@ -5685,14 +5736,14 @@
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="4">
-        <f t="shared" si="31"/>
+        <f>+D173+1</f>
         <v>6</v>
       </c>
       <c r="E174" s="12" t="s">
         <v>204</v>
       </c>
       <c r="F174" s="6">
-        <f t="shared" si="32"/>
+        <f>+G173</f>
         <v>47.05</v>
       </c>
       <c r="G174" s="6">
@@ -5744,14 +5795,14 @@
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="4">
-        <f>+D176+1</f>
+        <f t="shared" ref="D177:D182" si="14">+D176+1</f>
         <v>2</v>
       </c>
       <c r="E177" s="14" t="s">
         <v>213</v>
       </c>
       <c r="F177" s="6">
-        <f>+G176</f>
+        <f t="shared" ref="F177:F182" si="15">+G176</f>
         <v>11.1</v>
       </c>
       <c r="G177" s="6">
@@ -5764,14 +5815,14 @@
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="4">
-        <f t="shared" ref="D178:D182" si="33">+D177+1</f>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E178" s="14" t="s">
         <v>214</v>
       </c>
       <c r="F178" s="6">
-        <f t="shared" ref="F178:F182" si="34">+G177</f>
+        <f t="shared" si="15"/>
         <v>22.42</v>
       </c>
       <c r="G178" s="6">
@@ -5784,14 +5835,14 @@
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E179" s="14" t="s">
         <v>215</v>
       </c>
       <c r="F179" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="15"/>
         <v>29.52</v>
       </c>
       <c r="G179" s="6">
@@ -5804,14 +5855,14 @@
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E180" s="14" t="s">
         <v>216</v>
       </c>
       <c r="F180" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="15"/>
         <v>37.020000000000003</v>
       </c>
       <c r="G180" s="6">
@@ -5824,14 +5875,14 @@
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="E181" s="14" t="s">
         <v>217</v>
       </c>
       <c r="F181" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="15"/>
         <v>45.22</v>
       </c>
       <c r="G181" s="6">
@@ -5844,14 +5895,14 @@
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="E182" s="14" t="s">
         <v>218</v>
       </c>
       <c r="F182" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="15"/>
         <v>48.55</v>
       </c>
       <c r="G182" s="6">
@@ -5921,14 +5972,14 @@
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="4">
-        <f t="shared" ref="D186:D187" si="35">+D185+1</f>
+        <f>+D185+1</f>
         <v>3</v>
       </c>
       <c r="E186" s="15" t="s">
         <v>222</v>
       </c>
       <c r="F186" s="6">
-        <f t="shared" ref="F186:F187" si="36">+G185</f>
+        <f>+G185</f>
         <v>9.34</v>
       </c>
       <c r="G186" s="6"/>
@@ -5939,14 +5990,14 @@
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="4">
-        <f t="shared" si="35"/>
+        <f>+D186+1</f>
         <v>4</v>
       </c>
       <c r="E187" s="15" t="s">
         <v>223</v>
       </c>
       <c r="F187" s="6">
-        <f t="shared" si="36"/>
+        <f>+G186</f>
         <v>0</v>
       </c>
       <c r="G187" s="6"/>
@@ -7225,7 +7276,7 @@
         <v>242</v>
       </c>
       <c r="F18" s="6">
-        <f t="shared" ref="F18:F20" si="0">+G17</f>
+        <f>+G17</f>
         <v>28.52</v>
       </c>
       <c r="G18" s="16">
@@ -7239,14 +7290,14 @@
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="4">
-        <f t="shared" ref="D19:D20" si="1">+D18+1</f>
+        <f>+D18+1</f>
         <v>4</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>243</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" si="0"/>
+        <f>+G18</f>
         <v>40.450000000000003</v>
       </c>
       <c r="G19" s="16">
@@ -7260,14 +7311,14 @@
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="4">
-        <f t="shared" si="1"/>
+        <f>+D19+1</f>
         <v>5</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>244</v>
       </c>
       <c r="F20" s="6">
-        <f t="shared" si="0"/>
+        <f>+G19</f>
         <v>50.25</v>
       </c>
       <c r="G20" s="20" t="s">
@@ -7427,7 +7478,7 @@
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="4">
-        <f t="shared" ref="D28:D29" si="2">+D27+1</f>
+        <f>+D27+1</f>
         <v>3</v>
       </c>
       <c r="E28" s="23" t="s">
@@ -7450,7 +7501,7 @@
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="4">
-        <f t="shared" si="2"/>
+        <f>+D28+1</f>
         <v>4</v>
       </c>
       <c r="E29" s="23" t="s">
@@ -7532,7 +7583,7 @@
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="4">
-        <f t="shared" ref="D33:D34" si="3">+D32+1</f>
+        <f>+D32+1</f>
         <v>3</v>
       </c>
       <c r="E33" s="24" t="s">
@@ -7555,7 +7606,7 @@
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="4">
-        <f t="shared" si="3"/>
+        <f>+D33+1</f>
         <v>4</v>
       </c>
       <c r="E34" s="15"/>
@@ -7628,7 +7679,7 @@
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="4">
-        <f t="shared" ref="D38" si="4">+D37+1</f>
+        <f>+D37+1</f>
         <v>3</v>
       </c>
       <c r="E38" s="25" t="s">
@@ -7710,7 +7761,7 @@
       <c r="B42" s="22"/>
       <c r="C42" s="15"/>
       <c r="D42" s="4">
-        <f t="shared" ref="D42" si="5">+D41+1</f>
+        <f>+D41+1</f>
         <v>3</v>
       </c>
       <c r="E42" s="26" t="s">
@@ -7794,7 +7845,7 @@
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="4">
-        <f t="shared" ref="D46:D47" si="6">+D45+1</f>
+        <f>+D45+1</f>
         <v>3</v>
       </c>
       <c r="E46" s="30" t="s">
@@ -7814,7 +7865,7 @@
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
       <c r="D47" s="4">
-        <f t="shared" si="6"/>
+        <f>+D46+1</f>
         <v>4</v>
       </c>
       <c r="E47" s="30" t="s">
@@ -7896,14 +7947,14 @@
       <c r="B51" s="22"/>
       <c r="C51" s="15"/>
       <c r="D51" s="4">
-        <f t="shared" ref="D51:D52" si="7">+D50+1</f>
+        <f>+D50+1</f>
         <v>3</v>
       </c>
       <c r="E51" s="31" t="s">
         <v>281</v>
       </c>
       <c r="F51" s="16">
-        <f t="shared" ref="F51:F52" si="8">+G50</f>
+        <f>+G50</f>
         <v>39.19</v>
       </c>
       <c r="G51" s="16">
@@ -7917,14 +7968,14 @@
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
       <c r="D52" s="4">
-        <f t="shared" si="7"/>
+        <f>+D51+1</f>
         <v>4</v>
       </c>
       <c r="E52" s="31" t="s">
         <v>283</v>
       </c>
       <c r="F52" s="16">
-        <f t="shared" si="8"/>
+        <f>+G51</f>
         <v>51.29</v>
       </c>
       <c r="G52" s="16">
@@ -7999,14 +8050,14 @@
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="4">
-        <f t="shared" ref="D56:D59" si="9">+D55+1</f>
+        <f>+D55+1</f>
         <v>3</v>
       </c>
       <c r="E56" s="31" t="s">
         <v>288</v>
       </c>
       <c r="F56" s="16">
-        <f t="shared" ref="F56:F59" si="10">+G55</f>
+        <f>+G55</f>
         <v>18.27</v>
       </c>
       <c r="G56" s="16">
@@ -8020,14 +8071,14 @@
       <c r="B57" s="22"/>
       <c r="C57" s="15"/>
       <c r="D57" s="4">
-        <f t="shared" si="9"/>
+        <f>+D56+1</f>
         <v>4</v>
       </c>
       <c r="E57" s="31" t="s">
         <v>289</v>
       </c>
       <c r="F57" s="16">
-        <f t="shared" si="10"/>
+        <f>+G56</f>
         <v>29.45</v>
       </c>
       <c r="G57" s="16">
@@ -8041,14 +8092,14 @@
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
       <c r="D58" s="4">
-        <f t="shared" si="9"/>
+        <f>+D57+1</f>
         <v>5</v>
       </c>
       <c r="E58" s="31" t="s">
         <v>290</v>
       </c>
       <c r="F58" s="16">
-        <f t="shared" si="10"/>
+        <f>+G57</f>
         <v>37.47</v>
       </c>
       <c r="G58" s="16">
@@ -8062,14 +8113,14 @@
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
       <c r="D59" s="4">
-        <f t="shared" si="9"/>
+        <f>+D58+1</f>
         <v>6</v>
       </c>
       <c r="E59" s="31" t="s">
         <v>291</v>
       </c>
       <c r="F59" s="16">
-        <f t="shared" si="10"/>
+        <f>+G58</f>
         <v>47.54</v>
       </c>
       <c r="G59" s="16">
@@ -8155,7 +8206,7 @@
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
       <c r="D64" s="4">
-        <f t="shared" ref="D64:D66" si="11">+D63+1</f>
+        <f>+D63+1</f>
         <v>3</v>
       </c>
       <c r="E64" s="33" t="s">
@@ -8178,7 +8229,7 @@
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
       <c r="D65" s="4">
-        <f t="shared" si="11"/>
+        <f>+D64+1</f>
         <v>4</v>
       </c>
       <c r="E65" s="33" t="s">
@@ -8198,7 +8249,7 @@
       <c r="B66" s="22"/>
       <c r="C66" s="15"/>
       <c r="D66" s="4">
-        <f t="shared" si="11"/>
+        <f>+D65+1</f>
         <v>5</v>
       </c>
       <c r="E66" s="33" t="s">
@@ -8281,7 +8332,7 @@
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
       <c r="D70" s="4">
-        <f t="shared" ref="D70:D71" si="12">+D69+1</f>
+        <f>+D69+1</f>
         <v>3</v>
       </c>
       <c r="E70" s="35" t="s">
@@ -8302,7 +8353,7 @@
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
       <c r="D71" s="4">
-        <f t="shared" si="12"/>
+        <f>+D70+1</f>
         <v>4</v>
       </c>
       <c r="E71" s="35" t="s">
@@ -8382,14 +8433,14 @@
       <c r="B75" s="22"/>
       <c r="C75" s="15"/>
       <c r="D75" s="4">
-        <f t="shared" ref="D75:D78" si="13">+D74+1</f>
+        <f>+D74+1</f>
         <v>3</v>
       </c>
       <c r="E75" s="36" t="s">
         <v>310</v>
       </c>
       <c r="F75" s="16">
-        <f t="shared" ref="F75:F78" si="14">+G74</f>
+        <f>+G74</f>
         <v>19.149999999999999</v>
       </c>
       <c r="G75" s="16">
@@ -8403,14 +8454,14 @@
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
       <c r="D76" s="4">
-        <f t="shared" si="13"/>
+        <f>+D75+1</f>
         <v>4</v>
       </c>
       <c r="E76" s="36" t="s">
         <v>311</v>
       </c>
       <c r="F76" s="16">
-        <f t="shared" si="14"/>
+        <f>+G75</f>
         <v>26.33</v>
       </c>
       <c r="G76" s="16">
@@ -8424,14 +8475,14 @@
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
       <c r="D77" s="4">
-        <f t="shared" si="13"/>
+        <f>+D76+1</f>
         <v>5</v>
       </c>
       <c r="E77" s="36" t="s">
         <v>312</v>
       </c>
       <c r="F77" s="16">
-        <f t="shared" si="14"/>
+        <f>+G76</f>
         <v>33.119999999999997</v>
       </c>
       <c r="G77" s="16">
@@ -8445,14 +8496,14 @@
       <c r="B78" s="22"/>
       <c r="C78" s="15"/>
       <c r="D78" s="4">
-        <f t="shared" si="13"/>
+        <f>+D77+1</f>
         <v>6</v>
       </c>
       <c r="E78" s="36" t="s">
         <v>313</v>
       </c>
       <c r="F78" s="16">
-        <f t="shared" si="14"/>
+        <f>+G77</f>
         <v>40.14</v>
       </c>
       <c r="G78" s="16">
@@ -8527,7 +8578,7 @@
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
       <c r="D82" s="4">
-        <f t="shared" ref="D82" si="15">+D81+1</f>
+        <f>+D81+1</f>
         <v>3</v>
       </c>
       <c r="E82" s="37" t="s">
@@ -8600,7 +8651,7 @@
       <c r="B86" s="38"/>
       <c r="C86" s="38"/>
       <c r="D86" s="4">
-        <f t="shared" ref="D86:D87" si="16">+D85+1</f>
+        <f>+D85+1</f>
         <v>3</v>
       </c>
       <c r="E86" s="38" t="s">
@@ -8621,7 +8672,7 @@
       <c r="B87" s="38"/>
       <c r="C87" s="38"/>
       <c r="D87" s="4">
-        <f t="shared" si="16"/>
+        <f>+D86+1</f>
         <v>4</v>
       </c>
       <c r="E87" s="38" t="s">
@@ -8704,7 +8755,7 @@
       <c r="B91" s="38"/>
       <c r="C91" s="38"/>
       <c r="D91" s="4">
-        <f t="shared" ref="D91" si="17">+D90+1</f>
+        <f>+D90+1</f>
         <v>3</v>
       </c>
       <c r="E91" s="41" t="s">
@@ -8785,7 +8836,7 @@
       <c r="B95" s="38"/>
       <c r="C95" s="38"/>
       <c r="D95" s="4">
-        <f t="shared" ref="D95" si="18">+D94+1</f>
+        <f>+D94+1</f>
         <v>3</v>
       </c>
       <c r="E95" s="42" t="s">
@@ -8862,7 +8913,7 @@
       <c r="B99" s="38"/>
       <c r="C99" s="38"/>
       <c r="D99" s="4">
-        <f t="shared" ref="D99" si="19">+D98+1</f>
+        <f>+D98+1</f>
         <v>3</v>
       </c>
       <c r="E99" s="43" t="s">
@@ -8942,7 +8993,7 @@
       <c r="B103" s="38"/>
       <c r="C103" s="38"/>
       <c r="D103" s="4">
-        <f t="shared" ref="D103" si="20">+D102+1</f>
+        <f>+D102+1</f>
         <v>3</v>
       </c>
       <c r="E103" s="44" t="s">
@@ -9022,7 +9073,7 @@
       <c r="B107" s="38"/>
       <c r="C107" s="38"/>
       <c r="D107" s="4">
-        <f t="shared" ref="D107:D108" si="21">+D106+1</f>
+        <f>+D106+1</f>
         <v>3</v>
       </c>
       <c r="E107" s="45" t="s">
@@ -9045,7 +9096,7 @@
       <c r="B108" s="38"/>
       <c r="C108" s="38"/>
       <c r="D108" s="4">
-        <f t="shared" si="21"/>
+        <f>+D107+1</f>
         <v>4</v>
       </c>
       <c r="E108" s="45" t="s">
@@ -9126,7 +9177,7 @@
       <c r="B112" s="38"/>
       <c r="C112" s="38"/>
       <c r="D112" s="4">
-        <f t="shared" ref="D112" si="22">+D111+1</f>
+        <f>+D111+1</f>
         <v>3</v>
       </c>
       <c r="E112" s="47" t="s">
@@ -9208,7 +9259,7 @@
       <c r="B116" s="38"/>
       <c r="C116" s="38"/>
       <c r="D116" s="4">
-        <f t="shared" ref="D116:D117" si="23">+D115+1</f>
+        <f>+D115+1</f>
         <v>3</v>
       </c>
       <c r="E116" s="49" t="s">
@@ -9229,7 +9280,7 @@
       <c r="B117" s="38"/>
       <c r="C117" s="38"/>
       <c r="D117" s="4">
-        <f t="shared" si="23"/>
+        <f>+D116+1</f>
         <v>4</v>
       </c>
       <c r="E117" s="49" t="s">
@@ -9313,7 +9364,7 @@
       <c r="B121" s="38"/>
       <c r="C121" s="38"/>
       <c r="D121" s="4">
-        <f t="shared" ref="D121" si="24">+D120+1</f>
+        <f>+D120+1</f>
         <v>3</v>
       </c>
       <c r="E121" s="50" t="s">
@@ -9391,7 +9442,7 @@
       <c r="B125" s="38"/>
       <c r="C125" s="38"/>
       <c r="D125" s="4">
-        <f t="shared" ref="D125" si="25">+D124+1</f>
+        <f>+D124+1</f>
         <v>3</v>
       </c>
       <c r="E125" s="53" t="s">
@@ -9473,7 +9524,7 @@
       <c r="B129" s="38"/>
       <c r="C129" s="38"/>
       <c r="D129" s="4">
-        <f t="shared" ref="D129:D130" si="26">+D128+1</f>
+        <f>+D128+1</f>
         <v>3</v>
       </c>
       <c r="E129" s="53" t="s">
@@ -9493,7 +9544,7 @@
       <c r="B130" s="38"/>
       <c r="C130" s="38"/>
       <c r="D130" s="4">
-        <f t="shared" si="26"/>
+        <f>+D129+1</f>
         <v>4</v>
       </c>
       <c r="E130" s="53" t="s">
@@ -9554,8 +9605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9675,7 +9726,7 @@
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
       <c r="D6" s="4">
-        <f t="shared" ref="D6:D7" si="0">+D5+1</f>
+        <f>+D5+1</f>
         <v>3</v>
       </c>
       <c r="E6" s="53" t="s">
@@ -9695,7 +9746,7 @@
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
       <c r="D7" s="4">
-        <f t="shared" si="0"/>
+        <f>+D6+1</f>
         <v>4</v>
       </c>
       <c r="E7" s="53" t="s">
@@ -9774,7 +9825,7 @@
       <c r="B11" s="57"/>
       <c r="C11" s="57"/>
       <c r="D11" s="59">
-        <f t="shared" ref="D11:D13" si="1">+D10+1</f>
+        <f>+D10+1</f>
         <v>3</v>
       </c>
       <c r="E11" s="57" t="s">
@@ -9799,7 +9850,7 @@
       <c r="B12" s="57"/>
       <c r="C12" s="57"/>
       <c r="D12" s="59">
-        <f t="shared" si="1"/>
+        <f>+D11+1</f>
         <v>4</v>
       </c>
       <c r="E12" s="57" t="s">
@@ -9824,7 +9875,7 @@
       <c r="B13" s="57"/>
       <c r="C13" s="57"/>
       <c r="D13" s="59">
-        <f t="shared" si="1"/>
+        <f>+D12+1</f>
         <v>5</v>
       </c>
       <c r="E13" s="57" t="s">
@@ -9920,14 +9971,14 @@
       <c r="B17" s="57"/>
       <c r="C17" s="57"/>
       <c r="D17" s="59">
-        <f t="shared" ref="D17:D18" si="2">+D16+1</f>
+        <f>+D16+1</f>
         <v>3</v>
       </c>
       <c r="E17" s="61" t="s">
         <v>386</v>
       </c>
       <c r="F17" s="57">
-        <f t="shared" ref="F17:F18" si="3">+G16</f>
+        <f>+G16</f>
         <v>24.02</v>
       </c>
       <c r="G17" s="57">
@@ -9945,14 +9996,14 @@
       <c r="B18" s="57"/>
       <c r="C18" s="57"/>
       <c r="D18" s="59">
-        <f t="shared" si="2"/>
+        <f>+D17+1</f>
         <v>4</v>
       </c>
       <c r="E18" s="61" t="s">
         <v>387</v>
       </c>
       <c r="F18" s="57">
-        <f t="shared" si="3"/>
+        <f>+G17</f>
         <v>34.520000000000003</v>
       </c>
       <c r="G18" s="57">
@@ -10043,7 +10094,7 @@
       <c r="B22" s="57"/>
       <c r="C22" s="57"/>
       <c r="D22" s="59">
-        <f t="shared" ref="D22:D23" si="4">+D21+1</f>
+        <f>+D21+1</f>
         <v>3</v>
       </c>
       <c r="E22" s="62" t="s">
@@ -10067,14 +10118,14 @@
       <c r="B23" s="57"/>
       <c r="C23" s="57"/>
       <c r="D23" s="59">
-        <f t="shared" si="4"/>
+        <f>+D22+1</f>
         <v>4</v>
       </c>
       <c r="E23" s="62" t="s">
         <v>392</v>
       </c>
       <c r="F23" s="57">
-        <f t="shared" ref="F23" si="5">+G22</f>
+        <f>+G22</f>
         <v>48.35</v>
       </c>
       <c r="G23" s="57">
@@ -10163,14 +10214,14 @@
       <c r="B27" s="57"/>
       <c r="C27" s="57"/>
       <c r="D27" s="59">
-        <f t="shared" ref="D27" si="6">+D26+1</f>
+        <f>+D26+1</f>
         <v>3</v>
       </c>
       <c r="E27" s="63" t="s">
         <v>397</v>
       </c>
       <c r="F27" s="57">
-        <f t="shared" ref="F27" si="7">+G26</f>
+        <f>+G26</f>
         <v>35.03</v>
       </c>
       <c r="G27" s="57">
@@ -10259,7 +10310,7 @@
       <c r="B31" s="57"/>
       <c r="C31" s="57"/>
       <c r="D31" s="59">
-        <f t="shared" ref="D31:D32" si="8">+D30+1</f>
+        <f>+D30+1</f>
         <v>3</v>
       </c>
       <c r="E31" s="64" t="s">
@@ -10284,7 +10335,7 @@
       <c r="B32" s="57"/>
       <c r="C32" s="57"/>
       <c r="D32" s="59">
-        <f t="shared" si="8"/>
+        <f>+D31+1</f>
         <v>4</v>
       </c>
       <c r="E32" s="64" t="s">
@@ -10357,14 +10408,14 @@
       <c r="B35" s="57"/>
       <c r="C35" s="57"/>
       <c r="D35" s="59">
-        <f>+D34+1</f>
+        <f t="shared" ref="D35:D40" si="0">+D34+1</f>
         <v>2</v>
       </c>
       <c r="E35" s="65" t="s">
         <v>406</v>
       </c>
       <c r="F35" s="57">
-        <f>+G34</f>
+        <f t="shared" ref="F35:F40" si="1">+G34</f>
         <v>14.58</v>
       </c>
       <c r="G35" s="57">
@@ -10382,14 +10433,14 @@
       <c r="B36" s="57"/>
       <c r="C36" s="57"/>
       <c r="D36" s="59">
-        <f t="shared" ref="D36:D40" si="9">+D35+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E36" s="65" t="s">
         <v>407</v>
       </c>
       <c r="F36" s="57">
-        <f>+G35</f>
+        <f t="shared" si="1"/>
         <v>23.14</v>
       </c>
       <c r="G36" s="57">
@@ -10407,14 +10458,14 @@
       <c r="B37" s="57"/>
       <c r="C37" s="57"/>
       <c r="D37" s="59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E37" s="65" t="s">
         <v>408</v>
       </c>
       <c r="F37" s="57">
-        <f t="shared" ref="F37:F39" si="10">+G36</f>
+        <f t="shared" si="1"/>
         <v>31.34</v>
       </c>
       <c r="G37" s="57">
@@ -10432,14 +10483,14 @@
       <c r="B38" s="57"/>
       <c r="C38" s="57"/>
       <c r="D38" s="59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E38" s="65" t="s">
         <v>409</v>
       </c>
       <c r="F38" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>37.49</v>
       </c>
       <c r="G38" s="57">
@@ -10457,14 +10508,14 @@
       <c r="B39" s="57"/>
       <c r="C39" s="57"/>
       <c r="D39" s="59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E39" s="65" t="s">
         <v>410</v>
       </c>
       <c r="F39" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>42.54</v>
       </c>
       <c r="G39" s="57">
@@ -10482,14 +10533,14 @@
       <c r="B40" s="57"/>
       <c r="C40" s="57"/>
       <c r="D40" s="59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E40" s="65" t="s">
         <v>411</v>
       </c>
       <c r="F40" s="57">
-        <f>+G39</f>
+        <f t="shared" si="1"/>
         <v>51.23</v>
       </c>
       <c r="G40" s="57">
@@ -10580,14 +10631,14 @@
       <c r="B44" s="57"/>
       <c r="C44" s="57"/>
       <c r="D44" s="59">
-        <f t="shared" ref="D44:D46" si="11">+D43+1</f>
+        <f>+D43+1</f>
         <v>3</v>
       </c>
       <c r="E44" s="66" t="s">
         <v>415</v>
       </c>
       <c r="F44" s="60">
-        <f t="shared" ref="F44:F46" si="12">+G43</f>
+        <f>+G43</f>
         <v>23.34</v>
       </c>
       <c r="G44" s="57">
@@ -10605,14 +10656,14 @@
       <c r="B45" s="57"/>
       <c r="C45" s="57"/>
       <c r="D45" s="59">
-        <f t="shared" si="11"/>
+        <f>+D44+1</f>
         <v>4</v>
       </c>
       <c r="E45" s="66" t="s">
         <v>416</v>
       </c>
       <c r="F45" s="60">
-        <f t="shared" si="12"/>
+        <f>+G44</f>
         <v>32.47</v>
       </c>
       <c r="G45" s="57">
@@ -10630,14 +10681,14 @@
       <c r="B46" s="57"/>
       <c r="C46" s="57"/>
       <c r="D46" s="59">
-        <f t="shared" si="11"/>
+        <f>+D45+1</f>
         <v>5</v>
       </c>
       <c r="E46" s="66" t="s">
         <v>417</v>
       </c>
       <c r="F46" s="60">
-        <f t="shared" si="12"/>
+        <f>+G45</f>
         <v>41.09</v>
       </c>
       <c r="G46" s="57">
@@ -10726,7 +10777,7 @@
       <c r="B50" s="57"/>
       <c r="C50" s="57"/>
       <c r="D50" s="59">
-        <f t="shared" ref="D50:D51" si="13">+D49+1</f>
+        <f>+D49+1</f>
         <v>3</v>
       </c>
       <c r="E50" s="67" t="s">
@@ -10751,7 +10802,7 @@
       <c r="B51" s="57"/>
       <c r="C51" s="57"/>
       <c r="D51" s="59">
-        <f t="shared" si="13"/>
+        <f>+D50+1</f>
         <v>4</v>
       </c>
       <c r="E51" s="67" t="s">
@@ -10848,14 +10899,14 @@
       <c r="B55" s="57"/>
       <c r="C55" s="57"/>
       <c r="D55" s="59">
-        <f t="shared" ref="D55:D58" si="14">+D54+1</f>
+        <f>+D54+1</f>
         <v>3</v>
       </c>
       <c r="E55" s="69" t="s">
         <v>431</v>
       </c>
       <c r="F55" s="57">
-        <f t="shared" ref="F55:F57" si="15">+G54</f>
+        <f>+G54</f>
         <v>22.19</v>
       </c>
       <c r="G55" s="57">
@@ -10873,14 +10924,14 @@
       <c r="B56" s="57"/>
       <c r="C56" s="57"/>
       <c r="D56" s="59">
-        <f t="shared" si="14"/>
+        <f>+D55+1</f>
         <v>4</v>
       </c>
       <c r="E56" s="69" t="s">
         <v>432</v>
       </c>
       <c r="F56" s="57">
-        <f t="shared" si="15"/>
+        <f>+G55</f>
         <v>46.27</v>
       </c>
       <c r="G56" s="57">
@@ -10898,14 +10949,14 @@
       <c r="B57" s="57"/>
       <c r="C57" s="57"/>
       <c r="D57" s="59">
-        <f t="shared" si="14"/>
+        <f>+D56+1</f>
         <v>5</v>
       </c>
       <c r="E57" s="69" t="s">
         <v>425</v>
       </c>
       <c r="F57" s="57">
-        <f t="shared" si="15"/>
+        <f>+G56</f>
         <v>50.19</v>
       </c>
       <c r="G57" s="57">
@@ -10923,7 +10974,7 @@
       <c r="B58" s="57"/>
       <c r="C58" s="57"/>
       <c r="D58" s="59">
-        <f t="shared" si="14"/>
+        <f>+D57+1</f>
         <v>6</v>
       </c>
       <c r="E58" s="69" t="s">
@@ -11021,14 +11072,14 @@
       <c r="B62" s="57"/>
       <c r="C62" s="57"/>
       <c r="D62" s="59">
-        <f t="shared" ref="D62:D63" si="16">+D61+1</f>
+        <f>+D61+1</f>
         <v>3</v>
       </c>
       <c r="E62" s="69" t="s">
         <v>428</v>
       </c>
       <c r="F62" s="57">
-        <f t="shared" ref="F62:F63" si="17">+G61</f>
+        <f>+G61</f>
         <v>24.12</v>
       </c>
       <c r="G62" s="57">
@@ -11043,14 +11094,14 @@
     </row>
     <row r="63" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="D63" s="59">
-        <f t="shared" si="16"/>
+        <f>+D62+1</f>
         <v>4</v>
       </c>
       <c r="E63" s="69" t="s">
         <v>429</v>
       </c>
       <c r="F63" s="57">
-        <f t="shared" si="17"/>
+        <f>+G62</f>
         <v>48.37</v>
       </c>
       <c r="G63" s="70">
@@ -11124,7 +11175,7 @@
       <c r="B67" s="71"/>
       <c r="C67" s="71"/>
       <c r="D67" s="59">
-        <f t="shared" ref="D67:D68" si="18">+D66+1</f>
+        <f>+D66+1</f>
         <v>3</v>
       </c>
       <c r="E67" s="71" t="s">
@@ -11145,7 +11196,7 @@
       <c r="B68" s="71"/>
       <c r="C68" s="71"/>
       <c r="D68" s="59">
-        <f t="shared" si="18"/>
+        <f>+D67+1</f>
         <v>4</v>
       </c>
       <c r="E68" s="71" t="s">
@@ -11158,7 +11209,9 @@
       <c r="G68" s="71">
         <v>56.51</v>
       </c>
-      <c r="H68" s="71"/>
+      <c r="H68" s="73" t="s">
+        <v>440</v>
+      </c>
       <c r="I68" s="71"/>
     </row>
     <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -11173,24 +11226,50 @@
       <c r="I69" s="71"/>
     </row>
     <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A70" s="71"/>
-      <c r="B70" s="71"/>
-      <c r="C70" s="71"/>
-      <c r="D70" s="71"/>
-      <c r="E70" s="71"/>
-      <c r="F70" s="71"/>
-      <c r="G70" s="71"/>
+      <c r="A70" s="71">
+        <v>13</v>
+      </c>
+      <c r="B70" s="72">
+        <v>44082</v>
+      </c>
+      <c r="C70" s="71">
+        <v>57.25</v>
+      </c>
+      <c r="D70" s="59">
+        <v>1</v>
+      </c>
+      <c r="E70" s="73" t="s">
+        <v>442</v>
+      </c>
+      <c r="F70" s="71">
+        <v>5.35</v>
+      </c>
+      <c r="G70" s="71">
+        <v>20.28</v>
+      </c>
       <c r="H70" s="71"/>
-      <c r="I70" s="71"/>
+      <c r="I70" s="71" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="71"/>
       <c r="B71" s="71"/>
       <c r="C71" s="71"/>
-      <c r="D71" s="71"/>
-      <c r="E71" s="71"/>
-      <c r="F71" s="71"/>
-      <c r="G71" s="71"/>
+      <c r="D71" s="59">
+        <f>+D70+1</f>
+        <v>2</v>
+      </c>
+      <c r="E71" s="73" t="s">
+        <v>443</v>
+      </c>
+      <c r="F71" s="71">
+        <f>+G70</f>
+        <v>20.28</v>
+      </c>
+      <c r="G71" s="71">
+        <v>35.229999999999997</v>
+      </c>
       <c r="H71" s="71"/>
       <c r="I71" s="71"/>
     </row>
@@ -11198,10 +11277,20 @@
       <c r="A72" s="71"/>
       <c r="B72" s="71"/>
       <c r="C72" s="71"/>
-      <c r="D72" s="71"/>
-      <c r="E72" s="71"/>
-      <c r="F72" s="71"/>
-      <c r="G72" s="71"/>
+      <c r="D72" s="59">
+        <f>+D71+1</f>
+        <v>3</v>
+      </c>
+      <c r="E72" s="73" t="s">
+        <v>444</v>
+      </c>
+      <c r="F72" s="71">
+        <f>+G71</f>
+        <v>35.229999999999997</v>
+      </c>
+      <c r="G72" s="71">
+        <v>42.43</v>
+      </c>
       <c r="H72" s="71"/>
       <c r="I72" s="71"/>
     </row>
@@ -11209,10 +11298,20 @@
       <c r="A73" s="71"/>
       <c r="B73" s="71"/>
       <c r="C73" s="71"/>
-      <c r="D73" s="71"/>
-      <c r="E73" s="71"/>
-      <c r="F73" s="71"/>
-      <c r="G73" s="71"/>
+      <c r="D73" s="59">
+        <f>+D72+1</f>
+        <v>4</v>
+      </c>
+      <c r="E73" s="73" t="s">
+        <v>445</v>
+      </c>
+      <c r="F73" s="71">
+        <f>+G72</f>
+        <v>42.43</v>
+      </c>
+      <c r="G73" s="71">
+        <v>56.26</v>
+      </c>
       <c r="H73" s="71"/>
       <c r="I73" s="71"/>
     </row>
@@ -11228,24 +11327,50 @@
       <c r="I74" s="71"/>
     </row>
     <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="71"/>
-      <c r="B75" s="71"/>
-      <c r="C75" s="71"/>
-      <c r="D75" s="71"/>
-      <c r="E75" s="71"/>
-      <c r="F75" s="71"/>
-      <c r="G75" s="71"/>
+      <c r="A75" s="71">
+        <v>14</v>
+      </c>
+      <c r="B75" s="72">
+        <v>44083</v>
+      </c>
+      <c r="C75" s="71">
+        <v>55.46</v>
+      </c>
+      <c r="D75" s="59">
+        <v>1</v>
+      </c>
+      <c r="E75" s="74" t="s">
+        <v>446</v>
+      </c>
+      <c r="F75" s="71">
+        <v>4.03</v>
+      </c>
+      <c r="G75" s="71">
+        <v>13.21</v>
+      </c>
       <c r="H75" s="71"/>
-      <c r="I75" s="71"/>
+      <c r="I75" s="71" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="71"/>
       <c r="B76" s="71"/>
       <c r="C76" s="71"/>
-      <c r="D76" s="71"/>
-      <c r="E76" s="71"/>
-      <c r="F76" s="71"/>
-      <c r="G76" s="71"/>
+      <c r="D76" s="59">
+        <f>+D75+1</f>
+        <v>2</v>
+      </c>
+      <c r="E76" s="74" t="s">
+        <v>448</v>
+      </c>
+      <c r="F76" s="71">
+        <f>+G75</f>
+        <v>13.21</v>
+      </c>
+      <c r="G76" s="71">
+        <v>21.37</v>
+      </c>
       <c r="H76" s="71"/>
       <c r="I76" s="71"/>
     </row>
@@ -11253,10 +11378,20 @@
       <c r="A77" s="71"/>
       <c r="B77" s="71"/>
       <c r="C77" s="71"/>
-      <c r="D77" s="71"/>
-      <c r="E77" s="71"/>
-      <c r="F77" s="71"/>
-      <c r="G77" s="71"/>
+      <c r="D77" s="59">
+        <f>+D76+1</f>
+        <v>3</v>
+      </c>
+      <c r="E77" s="74" t="s">
+        <v>449</v>
+      </c>
+      <c r="F77" s="71">
+        <f>+G76</f>
+        <v>21.37</v>
+      </c>
+      <c r="G77" s="71">
+        <v>31.33</v>
+      </c>
       <c r="H77" s="71"/>
       <c r="I77" s="71"/>
     </row>
@@ -11264,10 +11399,20 @@
       <c r="A78" s="71"/>
       <c r="B78" s="71"/>
       <c r="C78" s="71"/>
-      <c r="D78" s="71"/>
-      <c r="E78" s="71"/>
-      <c r="F78" s="71"/>
-      <c r="G78" s="71"/>
+      <c r="D78" s="59">
+        <f>+D77+1</f>
+        <v>4</v>
+      </c>
+      <c r="E78" s="74" t="s">
+        <v>450</v>
+      </c>
+      <c r="F78" s="71">
+        <f>+G77</f>
+        <v>31.33</v>
+      </c>
+      <c r="G78" s="71">
+        <v>36.450000000000003</v>
+      </c>
       <c r="H78" s="71"/>
       <c r="I78" s="71"/>
     </row>
@@ -11275,10 +11420,20 @@
       <c r="A79" s="71"/>
       <c r="B79" s="71"/>
       <c r="C79" s="71"/>
-      <c r="D79" s="71"/>
-      <c r="E79" s="71"/>
-      <c r="F79" s="71"/>
-      <c r="G79" s="71"/>
+      <c r="D79" s="59">
+        <f>+D78+1</f>
+        <v>5</v>
+      </c>
+      <c r="E79" s="74" t="s">
+        <v>451</v>
+      </c>
+      <c r="F79" s="71">
+        <f>+G78</f>
+        <v>36.450000000000003</v>
+      </c>
+      <c r="G79" s="71">
+        <v>46.44</v>
+      </c>
       <c r="H79" s="71"/>
       <c r="I79" s="71"/>
     </row>
@@ -11286,10 +11441,20 @@
       <c r="A80" s="71"/>
       <c r="B80" s="71"/>
       <c r="C80" s="71"/>
-      <c r="D80" s="71"/>
-      <c r="E80" s="71"/>
-      <c r="F80" s="71"/>
-      <c r="G80" s="71"/>
+      <c r="D80" s="59">
+        <f>+D79+1</f>
+        <v>6</v>
+      </c>
+      <c r="E80" s="74" t="s">
+        <v>452</v>
+      </c>
+      <c r="F80" s="71">
+        <f>+G79</f>
+        <v>46.44</v>
+      </c>
+      <c r="G80" s="71">
+        <v>55.12</v>
+      </c>
       <c r="H80" s="71"/>
       <c r="I80" s="71"/>
     </row>

</xml_diff>

<commit_message>
AAK Separate PDFs BRH corr TTD as on 10/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
     <sheet name="Kandam2" sheetId="2" r:id="rId2"/>
     <sheet name="Kandam3" sheetId="3" r:id="rId3"/>
+    <sheet name="Kandam4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="457">
   <si>
     <t>Date</t>
   </si>
@@ -1376,19 +1376,37 @@
   </si>
   <si>
     <t>3.5.10.1</t>
+  </si>
+  <si>
+    <t>3.5.11.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ashEiCEpYPQ</t>
+  </si>
+  <si>
+    <t>4.1.1.1</t>
+  </si>
+  <si>
+    <t>4.1.2.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="52" x14ac:knownFonts="1">
+  <fonts count="53" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1729,78 +1747,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="49" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="50" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="50" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1809,10 +1828,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -9605,8 +9624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="G81" sqref="G81"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11470,21 +11489,40 @@
       <c r="I81" s="71"/>
     </row>
     <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A82" s="71"/>
-      <c r="B82" s="71"/>
-      <c r="C82" s="71"/>
-      <c r="D82" s="71"/>
-      <c r="E82" s="71"/>
-      <c r="F82" s="71"/>
-      <c r="G82" s="71"/>
+      <c r="A82" s="71">
+        <v>15</v>
+      </c>
+      <c r="B82" s="72">
+        <v>44084</v>
+      </c>
+      <c r="C82" s="71">
+        <v>55.27</v>
+      </c>
+      <c r="D82" s="59">
+        <v>1</v>
+      </c>
+      <c r="E82" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="F82" s="71">
+        <v>4.05</v>
+      </c>
+      <c r="G82" s="71">
+        <v>21.12</v>
+      </c>
       <c r="H82" s="71"/>
-      <c r="I82" s="71"/>
+      <c r="I82" s="71" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="71"/>
       <c r="B83" s="71"/>
       <c r="C83" s="71"/>
-      <c r="D83" s="71"/>
+      <c r="D83" s="59">
+        <f>+D82+1</f>
+        <v>2</v>
+      </c>
       <c r="E83" s="71"/>
       <c r="F83" s="71"/>
       <c r="G83" s="71"/>
@@ -11495,7 +11533,10 @@
       <c r="A84" s="71"/>
       <c r="B84" s="71"/>
       <c r="C84" s="71"/>
-      <c r="D84" s="71"/>
+      <c r="D84" s="59">
+        <f>+D83+1</f>
+        <v>3</v>
+      </c>
       <c r="E84" s="71"/>
       <c r="F84" s="71"/>
       <c r="G84" s="71"/>
@@ -11506,7 +11547,10 @@
       <c r="A85" s="71"/>
       <c r="B85" s="71"/>
       <c r="C85" s="71"/>
-      <c r="D85" s="71"/>
+      <c r="D85" s="59">
+        <f>+D84+1</f>
+        <v>4</v>
+      </c>
       <c r="E85" s="71"/>
       <c r="F85" s="71"/>
       <c r="G85" s="71"/>
@@ -11517,7 +11561,10 @@
       <c r="A86" s="71"/>
       <c r="B86" s="71"/>
       <c r="C86" s="71"/>
-      <c r="D86" s="71"/>
+      <c r="D86" s="59">
+        <f>+D85+1</f>
+        <v>5</v>
+      </c>
       <c r="E86" s="71"/>
       <c r="F86" s="71"/>
       <c r="G86" s="71"/>
@@ -11671,4 +11718,170 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="71">
+        <v>15</v>
+      </c>
+      <c r="B4" s="72">
+        <v>44084</v>
+      </c>
+      <c r="C4" s="71">
+        <v>55.27</v>
+      </c>
+      <c r="D4" s="54">
+        <v>1</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>453</v>
+      </c>
+      <c r="F4" s="55">
+        <v>4.05</v>
+      </c>
+      <c r="G4" s="55">
+        <v>21.12</v>
+      </c>
+      <c r="H4" s="75" t="s">
+        <v>152</v>
+      </c>
+      <c r="I4" s="71" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="71"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="59">
+        <f>+D4+1</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="75" t="s">
+        <v>455</v>
+      </c>
+      <c r="F5" s="71">
+        <v>27.12</v>
+      </c>
+      <c r="G5" s="71">
+        <v>40.380000000000003</v>
+      </c>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="71"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="59">
+        <f>+D5+1</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>456</v>
+      </c>
+      <c r="F6" s="71">
+        <f>+G5</f>
+        <v>40.380000000000003</v>
+      </c>
+      <c r="G6" s="71">
+        <v>54.28</v>
+      </c>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="71"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="71"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AbhiSravaNam corrections - 12/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="466">
   <si>
     <t>Date</t>
   </si>
@@ -1388,19 +1388,52 @@
   </si>
   <si>
     <t>4.1.2.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7mi0xnXWass</t>
+  </si>
+  <si>
+    <t>4.1.2.5</t>
+  </si>
+  <si>
+    <t>4.1.2.4</t>
+  </si>
+  <si>
+    <t>4.1.3.1</t>
+  </si>
+  <si>
+    <t>4.1.4.1</t>
+  </si>
+  <si>
+    <t>4.1.5.1</t>
+  </si>
+  <si>
+    <t>4.1.6.1</t>
+  </si>
+  <si>
+    <t>4.1.6.2</t>
+  </si>
+  <si>
+    <t>4.1.6.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1747,78 +1780,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="50" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="51" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="52" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1827,13 +1861,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11722,10 +11757,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11790,7 +11825,7 @@
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="71">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B4" s="72">
         <v>44084</v>
@@ -11855,7 +11890,9 @@
       <c r="G6" s="71">
         <v>54.28</v>
       </c>
-      <c r="H6" s="71"/>
+      <c r="H6" s="76" t="s">
+        <v>459</v>
+      </c>
       <c r="I6" s="71"/>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -11870,15 +11907,1828 @@
       <c r="I7" s="71"/>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="71">
+        <v>2</v>
+      </c>
+      <c r="B8" s="72">
+        <v>44085</v>
+      </c>
+      <c r="C8" s="71">
+        <v>47.46</v>
+      </c>
+      <c r="D8" s="59">
+        <v>1</v>
+      </c>
+      <c r="E8" s="76" t="s">
+        <v>458</v>
+      </c>
+      <c r="F8" s="71">
+        <v>3.14</v>
+      </c>
+      <c r="G8" s="71">
+        <v>7.38</v>
+      </c>
       <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
+      <c r="I8" s="71" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="59">
+        <f>+D8+1</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="76" t="s">
+        <v>460</v>
+      </c>
+      <c r="F9" s="76">
+        <f>+G8</f>
+        <v>7.38</v>
+      </c>
+      <c r="G9" s="76">
+        <v>18.04</v>
+      </c>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="59">
+        <f>+D9+1</f>
+        <v>3</v>
+      </c>
+      <c r="E10" s="76" t="s">
+        <v>461</v>
+      </c>
+      <c r="F10" s="76">
+        <f>+G9</f>
+        <v>18.04</v>
+      </c>
+      <c r="G10" s="76">
+        <v>28.02</v>
+      </c>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+    </row>
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="59">
+        <f t="shared" ref="D11:D12" si="0">+D10+1</f>
+        <v>4</v>
+      </c>
+      <c r="E11" s="76" t="s">
+        <v>462</v>
+      </c>
+      <c r="F11" s="76">
+        <f t="shared" ref="F11:F12" si="1">+G10</f>
+        <v>28.02</v>
+      </c>
+      <c r="G11" s="76">
+        <v>39.47</v>
+      </c>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="76"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="59">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E12" s="76" t="s">
+        <v>463</v>
+      </c>
+      <c r="F12" s="76">
+        <f t="shared" si="1"/>
+        <v>39.47</v>
+      </c>
+      <c r="G12" s="76">
+        <v>46.36</v>
+      </c>
+      <c r="H12" s="76" t="s">
+        <v>464</v>
+      </c>
+      <c r="I12" s="76"/>
+    </row>
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+    </row>
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="76">
+        <v>3</v>
+      </c>
+      <c r="B14" s="77">
+        <v>44086</v>
+      </c>
+      <c r="C14" s="76"/>
+      <c r="D14" s="59">
+        <v>1</v>
+      </c>
+      <c r="E14" s="76" t="s">
+        <v>465</v>
+      </c>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+    </row>
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="76"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="59">
+        <f>+D14+1</f>
+        <v>2</v>
+      </c>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+    </row>
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="76"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="59">
+        <f>+D15+1</f>
+        <v>3</v>
+      </c>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="76"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="59">
+        <f t="shared" ref="D17" si="2">+D16+1</f>
+        <v>4</v>
+      </c>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="76"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="76"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="76"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="76"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="76"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="76"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="76"/>
+    </row>
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="76"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="76"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="76"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
+    </row>
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="76"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="76"/>
+      <c r="I27" s="76"/>
+    </row>
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="76"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="76"/>
+    </row>
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="76"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="76"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="76"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="76"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="76"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="76"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="76"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="76"/>
+      <c r="H32" s="76"/>
+      <c r="I32" s="76"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="76"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="76"/>
+    </row>
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="76"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+    </row>
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="76"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="76"/>
+    </row>
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="76"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+    </row>
+    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A37" s="76"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="76"/>
+    </row>
+    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="76"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="76"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="76"/>
+    </row>
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="76"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
+    </row>
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A40" s="76"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="76"/>
+      <c r="I40" s="76"/>
+    </row>
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A41" s="76"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+    </row>
+    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" s="76"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" s="76"/>
+      <c r="B43" s="76"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="76"/>
+    </row>
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A44" s="76"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+    </row>
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A45" s="76"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
+    </row>
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A46" s="76"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
+      <c r="H46" s="76"/>
+      <c r="I46" s="76"/>
+    </row>
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A47" s="76"/>
+      <c r="B47" s="76"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+    </row>
+    <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A48" s="76"/>
+      <c r="B48" s="76"/>
+      <c r="C48" s="76"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="76"/>
+      <c r="G48" s="76"/>
+      <c r="H48" s="76"/>
+      <c r="I48" s="76"/>
+    </row>
+    <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A49" s="76"/>
+      <c r="B49" s="76"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
+    </row>
+    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A50" s="76"/>
+      <c r="B50" s="76"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="76"/>
+      <c r="G50" s="76"/>
+      <c r="H50" s="76"/>
+      <c r="I50" s="76"/>
+    </row>
+    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A51" s="76"/>
+      <c r="B51" s="76"/>
+      <c r="C51" s="76"/>
+      <c r="D51" s="76"/>
+      <c r="E51" s="76"/>
+      <c r="F51" s="76"/>
+      <c r="G51" s="76"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="76"/>
+    </row>
+    <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A52" s="76"/>
+      <c r="B52" s="76"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="76"/>
+    </row>
+    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A53" s="76"/>
+      <c r="B53" s="76"/>
+      <c r="C53" s="76"/>
+      <c r="D53" s="76"/>
+      <c r="E53" s="76"/>
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
+      <c r="H53" s="76"/>
+      <c r="I53" s="76"/>
+    </row>
+    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A54" s="76"/>
+      <c r="B54" s="76"/>
+      <c r="C54" s="76"/>
+      <c r="D54" s="76"/>
+      <c r="E54" s="76"/>
+      <c r="F54" s="76"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="76"/>
+      <c r="I54" s="76"/>
+    </row>
+    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A55" s="76"/>
+      <c r="B55" s="76"/>
+      <c r="C55" s="76"/>
+      <c r="D55" s="76"/>
+      <c r="E55" s="76"/>
+      <c r="F55" s="76"/>
+      <c r="G55" s="76"/>
+      <c r="H55" s="76"/>
+      <c r="I55" s="76"/>
+    </row>
+    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A56" s="76"/>
+      <c r="B56" s="76"/>
+      <c r="C56" s="76"/>
+      <c r="D56" s="76"/>
+      <c r="E56" s="76"/>
+      <c r="F56" s="76"/>
+      <c r="G56" s="76"/>
+      <c r="H56" s="76"/>
+      <c r="I56" s="76"/>
+    </row>
+    <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A57" s="76"/>
+      <c r="B57" s="76"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+    </row>
+    <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A58" s="76"/>
+      <c r="B58" s="76"/>
+      <c r="C58" s="76"/>
+      <c r="D58" s="76"/>
+      <c r="E58" s="76"/>
+      <c r="F58" s="76"/>
+      <c r="G58" s="76"/>
+      <c r="H58" s="76"/>
+      <c r="I58" s="76"/>
+    </row>
+    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A59" s="76"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="76"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="76"/>
+      <c r="G59" s="76"/>
+      <c r="H59" s="76"/>
+      <c r="I59" s="76"/>
+    </row>
+    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A60" s="76"/>
+      <c r="B60" s="76"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="76"/>
+      <c r="G60" s="76"/>
+      <c r="H60" s="76"/>
+      <c r="I60" s="76"/>
+    </row>
+    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A61" s="76"/>
+      <c r="B61" s="76"/>
+      <c r="C61" s="76"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="76"/>
+      <c r="G61" s="76"/>
+      <c r="H61" s="76"/>
+      <c r="I61" s="76"/>
+    </row>
+    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A62" s="76"/>
+      <c r="B62" s="76"/>
+      <c r="C62" s="76"/>
+      <c r="D62" s="76"/>
+      <c r="E62" s="76"/>
+      <c r="F62" s="76"/>
+      <c r="G62" s="76"/>
+      <c r="H62" s="76"/>
+      <c r="I62" s="76"/>
+    </row>
+    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A63" s="76"/>
+      <c r="B63" s="76"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="76"/>
+      <c r="G63" s="76"/>
+      <c r="H63" s="76"/>
+      <c r="I63" s="76"/>
+    </row>
+    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A64" s="76"/>
+      <c r="B64" s="76"/>
+      <c r="C64" s="76"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="76"/>
+      <c r="F64" s="76"/>
+      <c r="G64" s="76"/>
+      <c r="H64" s="76"/>
+      <c r="I64" s="76"/>
+    </row>
+    <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A65" s="76"/>
+      <c r="B65" s="76"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="76"/>
+      <c r="G65" s="76"/>
+      <c r="H65" s="76"/>
+      <c r="I65" s="76"/>
+    </row>
+    <row r="66" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A66" s="76"/>
+      <c r="B66" s="76"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="76"/>
+      <c r="E66" s="76"/>
+      <c r="F66" s="76"/>
+      <c r="G66" s="76"/>
+      <c r="H66" s="76"/>
+      <c r="I66" s="76"/>
+    </row>
+    <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A67" s="76"/>
+      <c r="B67" s="76"/>
+      <c r="C67" s="76"/>
+      <c r="D67" s="76"/>
+      <c r="E67" s="76"/>
+      <c r="F67" s="76"/>
+      <c r="G67" s="76"/>
+      <c r="H67" s="76"/>
+      <c r="I67" s="76"/>
+    </row>
+    <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A68" s="76"/>
+      <c r="B68" s="76"/>
+      <c r="C68" s="76"/>
+      <c r="D68" s="76"/>
+      <c r="E68" s="76"/>
+      <c r="F68" s="76"/>
+      <c r="G68" s="76"/>
+      <c r="H68" s="76"/>
+      <c r="I68" s="76"/>
+    </row>
+    <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A69" s="76"/>
+      <c r="B69" s="76"/>
+      <c r="C69" s="76"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="76"/>
+      <c r="G69" s="76"/>
+      <c r="H69" s="76"/>
+      <c r="I69" s="76"/>
+    </row>
+    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A70" s="76"/>
+      <c r="B70" s="76"/>
+      <c r="C70" s="76"/>
+      <c r="D70" s="76"/>
+      <c r="E70" s="76"/>
+      <c r="F70" s="76"/>
+      <c r="G70" s="76"/>
+      <c r="H70" s="76"/>
+      <c r="I70" s="76"/>
+    </row>
+    <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A71" s="76"/>
+      <c r="B71" s="76"/>
+      <c r="C71" s="76"/>
+      <c r="D71" s="76"/>
+      <c r="E71" s="76"/>
+      <c r="F71" s="76"/>
+      <c r="G71" s="76"/>
+      <c r="H71" s="76"/>
+      <c r="I71" s="76"/>
+    </row>
+    <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A72" s="76"/>
+      <c r="B72" s="76"/>
+      <c r="C72" s="76"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="76"/>
+      <c r="G72" s="76"/>
+      <c r="H72" s="76"/>
+      <c r="I72" s="76"/>
+    </row>
+    <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A73" s="76"/>
+      <c r="B73" s="76"/>
+      <c r="C73" s="76"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="76"/>
+      <c r="G73" s="76"/>
+      <c r="H73" s="76"/>
+      <c r="I73" s="76"/>
+    </row>
+    <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A74" s="76"/>
+      <c r="B74" s="76"/>
+      <c r="C74" s="76"/>
+      <c r="D74" s="76"/>
+      <c r="E74" s="76"/>
+      <c r="F74" s="76"/>
+      <c r="G74" s="76"/>
+      <c r="H74" s="76"/>
+      <c r="I74" s="76"/>
+    </row>
+    <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A75" s="76"/>
+      <c r="B75" s="76"/>
+      <c r="C75" s="76"/>
+      <c r="D75" s="76"/>
+      <c r="E75" s="76"/>
+      <c r="F75" s="76"/>
+      <c r="G75" s="76"/>
+      <c r="H75" s="76"/>
+      <c r="I75" s="76"/>
+    </row>
+    <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A76" s="76"/>
+      <c r="B76" s="76"/>
+      <c r="C76" s="76"/>
+      <c r="D76" s="76"/>
+      <c r="E76" s="76"/>
+      <c r="F76" s="76"/>
+      <c r="G76" s="76"/>
+      <c r="H76" s="76"/>
+      <c r="I76" s="76"/>
+    </row>
+    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A77" s="76"/>
+      <c r="B77" s="76"/>
+      <c r="C77" s="76"/>
+      <c r="D77" s="76"/>
+      <c r="E77" s="76"/>
+      <c r="F77" s="76"/>
+      <c r="G77" s="76"/>
+      <c r="H77" s="76"/>
+      <c r="I77" s="76"/>
+    </row>
+    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A78" s="76"/>
+      <c r="B78" s="76"/>
+      <c r="C78" s="76"/>
+      <c r="D78" s="76"/>
+      <c r="E78" s="76"/>
+      <c r="F78" s="76"/>
+      <c r="G78" s="76"/>
+      <c r="H78" s="76"/>
+      <c r="I78" s="76"/>
+    </row>
+    <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A79" s="76"/>
+      <c r="B79" s="76"/>
+      <c r="C79" s="76"/>
+      <c r="D79" s="76"/>
+      <c r="E79" s="76"/>
+      <c r="F79" s="76"/>
+      <c r="G79" s="76"/>
+      <c r="H79" s="76"/>
+      <c r="I79" s="76"/>
+    </row>
+    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A80" s="76"/>
+      <c r="B80" s="76"/>
+      <c r="C80" s="76"/>
+      <c r="D80" s="76"/>
+      <c r="E80" s="76"/>
+      <c r="F80" s="76"/>
+      <c r="G80" s="76"/>
+      <c r="H80" s="76"/>
+      <c r="I80" s="76"/>
+    </row>
+    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A81" s="76"/>
+      <c r="B81" s="76"/>
+      <c r="C81" s="76"/>
+      <c r="D81" s="76"/>
+      <c r="E81" s="76"/>
+      <c r="F81" s="76"/>
+      <c r="G81" s="76"/>
+      <c r="H81" s="76"/>
+      <c r="I81" s="76"/>
+    </row>
+    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A82" s="76"/>
+      <c r="B82" s="76"/>
+      <c r="C82" s="76"/>
+      <c r="D82" s="76"/>
+      <c r="E82" s="76"/>
+      <c r="F82" s="76"/>
+      <c r="G82" s="76"/>
+      <c r="H82" s="76"/>
+      <c r="I82" s="76"/>
+    </row>
+    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A83" s="76"/>
+      <c r="B83" s="76"/>
+      <c r="C83" s="76"/>
+      <c r="D83" s="76"/>
+      <c r="E83" s="76"/>
+      <c r="F83" s="76"/>
+      <c r="G83" s="76"/>
+      <c r="H83" s="76"/>
+      <c r="I83" s="76"/>
+    </row>
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A84" s="76"/>
+      <c r="B84" s="76"/>
+      <c r="C84" s="76"/>
+      <c r="D84" s="76"/>
+      <c r="E84" s="76"/>
+      <c r="F84" s="76"/>
+      <c r="G84" s="76"/>
+      <c r="H84" s="76"/>
+      <c r="I84" s="76"/>
+    </row>
+    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A85" s="76"/>
+      <c r="B85" s="76"/>
+      <c r="C85" s="76"/>
+      <c r="D85" s="76"/>
+      <c r="E85" s="76"/>
+      <c r="F85" s="76"/>
+      <c r="G85" s="76"/>
+      <c r="H85" s="76"/>
+      <c r="I85" s="76"/>
+    </row>
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A86" s="76"/>
+      <c r="B86" s="76"/>
+      <c r="C86" s="76"/>
+      <c r="D86" s="76"/>
+      <c r="E86" s="76"/>
+      <c r="F86" s="76"/>
+      <c r="G86" s="76"/>
+      <c r="H86" s="76"/>
+      <c r="I86" s="76"/>
+    </row>
+    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A87" s="76"/>
+      <c r="B87" s="76"/>
+      <c r="C87" s="76"/>
+      <c r="D87" s="76"/>
+      <c r="E87" s="76"/>
+      <c r="F87" s="76"/>
+      <c r="G87" s="76"/>
+      <c r="H87" s="76"/>
+      <c r="I87" s="76"/>
+    </row>
+    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A88" s="76"/>
+      <c r="B88" s="76"/>
+      <c r="C88" s="76"/>
+      <c r="D88" s="76"/>
+      <c r="E88" s="76"/>
+      <c r="F88" s="76"/>
+      <c r="G88" s="76"/>
+      <c r="H88" s="76"/>
+      <c r="I88" s="76"/>
+    </row>
+    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A89" s="76"/>
+      <c r="B89" s="76"/>
+      <c r="C89" s="76"/>
+      <c r="D89" s="76"/>
+      <c r="E89" s="76"/>
+      <c r="F89" s="76"/>
+      <c r="G89" s="76"/>
+      <c r="H89" s="76"/>
+      <c r="I89" s="76"/>
+    </row>
+    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A90" s="76"/>
+      <c r="B90" s="76"/>
+      <c r="C90" s="76"/>
+      <c r="D90" s="76"/>
+      <c r="E90" s="76"/>
+      <c r="F90" s="76"/>
+      <c r="G90" s="76"/>
+      <c r="H90" s="76"/>
+      <c r="I90" s="76"/>
+    </row>
+    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A91" s="76"/>
+      <c r="B91" s="76"/>
+      <c r="C91" s="76"/>
+      <c r="D91" s="76"/>
+      <c r="E91" s="76"/>
+      <c r="F91" s="76"/>
+      <c r="G91" s="76"/>
+      <c r="H91" s="76"/>
+      <c r="I91" s="76"/>
+    </row>
+    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A92" s="76"/>
+      <c r="B92" s="76"/>
+      <c r="C92" s="76"/>
+      <c r="D92" s="76"/>
+      <c r="E92" s="76"/>
+      <c r="F92" s="76"/>
+      <c r="G92" s="76"/>
+      <c r="H92" s="76"/>
+      <c r="I92" s="76"/>
+    </row>
+    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A93" s="76"/>
+      <c r="B93" s="76"/>
+      <c r="C93" s="76"/>
+      <c r="D93" s="76"/>
+      <c r="E93" s="76"/>
+      <c r="F93" s="76"/>
+      <c r="G93" s="76"/>
+      <c r="H93" s="76"/>
+      <c r="I93" s="76"/>
+    </row>
+    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A94" s="76"/>
+      <c r="B94" s="76"/>
+      <c r="C94" s="76"/>
+      <c r="D94" s="76"/>
+      <c r="E94" s="76"/>
+      <c r="F94" s="76"/>
+      <c r="G94" s="76"/>
+      <c r="H94" s="76"/>
+      <c r="I94" s="76"/>
+    </row>
+    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A95" s="76"/>
+      <c r="B95" s="76"/>
+      <c r="C95" s="76"/>
+      <c r="D95" s="76"/>
+      <c r="E95" s="76"/>
+      <c r="F95" s="76"/>
+      <c r="G95" s="76"/>
+      <c r="H95" s="76"/>
+      <c r="I95" s="76"/>
+    </row>
+    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A96" s="76"/>
+      <c r="B96" s="76"/>
+      <c r="C96" s="76"/>
+      <c r="D96" s="76"/>
+      <c r="E96" s="76"/>
+      <c r="F96" s="76"/>
+      <c r="G96" s="76"/>
+      <c r="H96" s="76"/>
+      <c r="I96" s="76"/>
+    </row>
+    <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A97" s="76"/>
+      <c r="B97" s="76"/>
+      <c r="C97" s="76"/>
+      <c r="D97" s="76"/>
+      <c r="E97" s="76"/>
+      <c r="F97" s="76"/>
+      <c r="G97" s="76"/>
+      <c r="H97" s="76"/>
+      <c r="I97" s="76"/>
+    </row>
+    <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A98" s="76"/>
+      <c r="B98" s="76"/>
+      <c r="C98" s="76"/>
+      <c r="D98" s="76"/>
+      <c r="E98" s="76"/>
+      <c r="F98" s="76"/>
+      <c r="G98" s="76"/>
+      <c r="H98" s="76"/>
+      <c r="I98" s="76"/>
+    </row>
+    <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A99" s="76"/>
+      <c r="B99" s="76"/>
+      <c r="C99" s="76"/>
+      <c r="D99" s="76"/>
+      <c r="E99" s="76"/>
+      <c r="F99" s="76"/>
+      <c r="G99" s="76"/>
+      <c r="H99" s="76"/>
+      <c r="I99" s="76"/>
+    </row>
+    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A100" s="76"/>
+      <c r="B100" s="76"/>
+      <c r="C100" s="76"/>
+      <c r="D100" s="76"/>
+      <c r="E100" s="76"/>
+      <c r="F100" s="76"/>
+      <c r="G100" s="76"/>
+      <c r="H100" s="76"/>
+      <c r="I100" s="76"/>
+    </row>
+    <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A101" s="76"/>
+      <c r="B101" s="76"/>
+      <c r="C101" s="76"/>
+      <c r="D101" s="76"/>
+      <c r="E101" s="76"/>
+      <c r="F101" s="76"/>
+      <c r="G101" s="76"/>
+      <c r="H101" s="76"/>
+      <c r="I101" s="76"/>
+    </row>
+    <row r="102" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A102" s="76"/>
+      <c r="B102" s="76"/>
+      <c r="C102" s="76"/>
+      <c r="D102" s="76"/>
+      <c r="E102" s="76"/>
+      <c r="F102" s="76"/>
+      <c r="G102" s="76"/>
+      <c r="H102" s="76"/>
+      <c r="I102" s="76"/>
+    </row>
+    <row r="103" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A103" s="76"/>
+      <c r="B103" s="76"/>
+      <c r="C103" s="76"/>
+      <c r="D103" s="76"/>
+      <c r="E103" s="76"/>
+      <c r="F103" s="76"/>
+      <c r="G103" s="76"/>
+      <c r="H103" s="76"/>
+      <c r="I103" s="76"/>
+    </row>
+    <row r="104" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A104" s="76"/>
+      <c r="B104" s="76"/>
+      <c r="C104" s="76"/>
+      <c r="D104" s="76"/>
+      <c r="E104" s="76"/>
+      <c r="F104" s="76"/>
+      <c r="G104" s="76"/>
+      <c r="H104" s="76"/>
+      <c r="I104" s="76"/>
+    </row>
+    <row r="105" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A105" s="76"/>
+      <c r="B105" s="76"/>
+      <c r="C105" s="76"/>
+      <c r="D105" s="76"/>
+      <c r="E105" s="76"/>
+      <c r="F105" s="76"/>
+      <c r="G105" s="76"/>
+      <c r="H105" s="76"/>
+      <c r="I105" s="76"/>
+    </row>
+    <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A106" s="76"/>
+      <c r="B106" s="76"/>
+      <c r="C106" s="76"/>
+      <c r="D106" s="76"/>
+      <c r="E106" s="76"/>
+      <c r="F106" s="76"/>
+      <c r="G106" s="76"/>
+      <c r="H106" s="76"/>
+      <c r="I106" s="76"/>
+    </row>
+    <row r="107" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A107" s="76"/>
+      <c r="B107" s="76"/>
+      <c r="C107" s="76"/>
+      <c r="D107" s="76"/>
+      <c r="E107" s="76"/>
+      <c r="F107" s="76"/>
+      <c r="G107" s="76"/>
+      <c r="H107" s="76"/>
+      <c r="I107" s="76"/>
+    </row>
+    <row r="108" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A108" s="76"/>
+      <c r="B108" s="76"/>
+      <c r="C108" s="76"/>
+      <c r="D108" s="76"/>
+      <c r="E108" s="76"/>
+      <c r="F108" s="76"/>
+      <c r="G108" s="76"/>
+      <c r="H108" s="76"/>
+      <c r="I108" s="76"/>
+    </row>
+    <row r="109" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A109" s="76"/>
+      <c r="B109" s="76"/>
+      <c r="C109" s="76"/>
+      <c r="D109" s="76"/>
+      <c r="E109" s="76"/>
+      <c r="F109" s="76"/>
+      <c r="G109" s="76"/>
+      <c r="H109" s="76"/>
+      <c r="I109" s="76"/>
+    </row>
+    <row r="110" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A110" s="76"/>
+      <c r="B110" s="76"/>
+      <c r="C110" s="76"/>
+      <c r="D110" s="76"/>
+      <c r="E110" s="76"/>
+      <c r="F110" s="76"/>
+      <c r="G110" s="76"/>
+      <c r="H110" s="76"/>
+      <c r="I110" s="76"/>
+    </row>
+    <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A111" s="76"/>
+      <c r="B111" s="76"/>
+      <c r="C111" s="76"/>
+      <c r="D111" s="76"/>
+      <c r="E111" s="76"/>
+      <c r="F111" s="76"/>
+      <c r="G111" s="76"/>
+      <c r="H111" s="76"/>
+      <c r="I111" s="76"/>
+    </row>
+    <row r="112" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A112" s="76"/>
+      <c r="B112" s="76"/>
+      <c r="C112" s="76"/>
+      <c r="D112" s="76"/>
+      <c r="E112" s="76"/>
+      <c r="F112" s="76"/>
+      <c r="G112" s="76"/>
+      <c r="H112" s="76"/>
+      <c r="I112" s="76"/>
+    </row>
+    <row r="113" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A113" s="76"/>
+      <c r="B113" s="76"/>
+      <c r="C113" s="76"/>
+      <c r="D113" s="76"/>
+      <c r="E113" s="76"/>
+      <c r="F113" s="76"/>
+      <c r="G113" s="76"/>
+      <c r="H113" s="76"/>
+      <c r="I113" s="76"/>
+    </row>
+    <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A114" s="76"/>
+      <c r="B114" s="76"/>
+      <c r="C114" s="76"/>
+      <c r="D114" s="76"/>
+      <c r="E114" s="76"/>
+      <c r="F114" s="76"/>
+      <c r="G114" s="76"/>
+      <c r="H114" s="76"/>
+      <c r="I114" s="76"/>
+    </row>
+    <row r="115" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A115" s="76"/>
+      <c r="B115" s="76"/>
+      <c r="C115" s="76"/>
+      <c r="D115" s="76"/>
+      <c r="E115" s="76"/>
+      <c r="F115" s="76"/>
+      <c r="G115" s="76"/>
+      <c r="H115" s="76"/>
+      <c r="I115" s="76"/>
+    </row>
+    <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A116" s="76"/>
+      <c r="B116" s="76"/>
+      <c r="C116" s="76"/>
+      <c r="D116" s="76"/>
+      <c r="E116" s="76"/>
+      <c r="F116" s="76"/>
+      <c r="G116" s="76"/>
+      <c r="H116" s="76"/>
+      <c r="I116" s="76"/>
+    </row>
+    <row r="117" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A117" s="76"/>
+      <c r="B117" s="76"/>
+      <c r="C117" s="76"/>
+      <c r="D117" s="76"/>
+      <c r="E117" s="76"/>
+      <c r="F117" s="76"/>
+      <c r="G117" s="76"/>
+      <c r="H117" s="76"/>
+      <c r="I117" s="76"/>
+    </row>
+    <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A118" s="76"/>
+      <c r="B118" s="76"/>
+      <c r="C118" s="76"/>
+      <c r="D118" s="76"/>
+      <c r="E118" s="76"/>
+      <c r="F118" s="76"/>
+      <c r="G118" s="76"/>
+      <c r="H118" s="76"/>
+      <c r="I118" s="76"/>
+    </row>
+    <row r="119" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A119" s="76"/>
+      <c r="B119" s="76"/>
+      <c r="C119" s="76"/>
+      <c r="D119" s="76"/>
+      <c r="E119" s="76"/>
+      <c r="F119" s="76"/>
+      <c r="G119" s="76"/>
+      <c r="H119" s="76"/>
+      <c r="I119" s="76"/>
+    </row>
+    <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A120" s="76"/>
+      <c r="B120" s="76"/>
+      <c r="C120" s="76"/>
+      <c r="D120" s="76"/>
+      <c r="E120" s="76"/>
+      <c r="F120" s="76"/>
+      <c r="G120" s="76"/>
+      <c r="H120" s="76"/>
+      <c r="I120" s="76"/>
+    </row>
+    <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A121" s="76"/>
+      <c r="B121" s="76"/>
+      <c r="C121" s="76"/>
+      <c r="D121" s="76"/>
+      <c r="E121" s="76"/>
+      <c r="F121" s="76"/>
+      <c r="G121" s="76"/>
+      <c r="H121" s="76"/>
+      <c r="I121" s="76"/>
+    </row>
+    <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A122" s="76"/>
+      <c r="B122" s="76"/>
+      <c r="C122" s="76"/>
+      <c r="D122" s="76"/>
+      <c r="E122" s="76"/>
+      <c r="F122" s="76"/>
+      <c r="G122" s="76"/>
+      <c r="H122" s="76"/>
+      <c r="I122" s="76"/>
+    </row>
+    <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A123" s="76"/>
+      <c r="B123" s="76"/>
+      <c r="C123" s="76"/>
+      <c r="D123" s="76"/>
+      <c r="E123" s="76"/>
+      <c r="F123" s="76"/>
+      <c r="G123" s="76"/>
+      <c r="H123" s="76"/>
+      <c r="I123" s="76"/>
+    </row>
+    <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A124" s="76"/>
+      <c r="B124" s="76"/>
+      <c r="C124" s="76"/>
+      <c r="D124" s="76"/>
+      <c r="E124" s="76"/>
+      <c r="F124" s="76"/>
+      <c r="G124" s="76"/>
+      <c r="H124" s="76"/>
+      <c r="I124" s="76"/>
+    </row>
+    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A125" s="76"/>
+      <c r="B125" s="76"/>
+      <c r="C125" s="76"/>
+      <c r="D125" s="76"/>
+      <c r="E125" s="76"/>
+      <c r="F125" s="76"/>
+      <c r="G125" s="76"/>
+      <c r="H125" s="76"/>
+      <c r="I125" s="76"/>
+    </row>
+    <row r="126" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A126" s="76"/>
+      <c r="B126" s="76"/>
+      <c r="C126" s="76"/>
+      <c r="D126" s="76"/>
+      <c r="E126" s="76"/>
+      <c r="F126" s="76"/>
+      <c r="G126" s="76"/>
+      <c r="H126" s="76"/>
+      <c r="I126" s="76"/>
+    </row>
+    <row r="127" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A127" s="76"/>
+      <c r="B127" s="76"/>
+      <c r="C127" s="76"/>
+      <c r="D127" s="76"/>
+      <c r="E127" s="76"/>
+      <c r="F127" s="76"/>
+      <c r="G127" s="76"/>
+      <c r="H127" s="76"/>
+      <c r="I127" s="76"/>
+    </row>
+    <row r="128" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A128" s="76"/>
+      <c r="B128" s="76"/>
+      <c r="C128" s="76"/>
+      <c r="D128" s="76"/>
+      <c r="E128" s="76"/>
+      <c r="F128" s="76"/>
+      <c r="G128" s="76"/>
+      <c r="H128" s="76"/>
+      <c r="I128" s="76"/>
+    </row>
+    <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A129" s="76"/>
+      <c r="B129" s="76"/>
+      <c r="C129" s="76"/>
+      <c r="D129" s="76"/>
+      <c r="E129" s="76"/>
+      <c r="F129" s="76"/>
+      <c r="G129" s="76"/>
+      <c r="H129" s="76"/>
+      <c r="I129" s="76"/>
+    </row>
+    <row r="130" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A130" s="76"/>
+      <c r="B130" s="76"/>
+      <c r="C130" s="76"/>
+      <c r="D130" s="76"/>
+      <c r="E130" s="76"/>
+      <c r="F130" s="76"/>
+      <c r="G130" s="76"/>
+      <c r="H130" s="76"/>
+      <c r="I130" s="76"/>
+    </row>
+    <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A131" s="76"/>
+      <c r="B131" s="76"/>
+      <c r="C131" s="76"/>
+      <c r="D131" s="76"/>
+      <c r="E131" s="76"/>
+      <c r="F131" s="76"/>
+      <c r="G131" s="76"/>
+      <c r="H131" s="76"/>
+      <c r="I131" s="76"/>
+    </row>
+    <row r="132" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A132" s="76"/>
+      <c r="B132" s="76"/>
+      <c r="C132" s="76"/>
+      <c r="D132" s="76"/>
+      <c r="E132" s="76"/>
+      <c r="F132" s="76"/>
+      <c r="G132" s="76"/>
+      <c r="H132" s="76"/>
+      <c r="I132" s="76"/>
+    </row>
+    <row r="133" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A133" s="76"/>
+      <c r="B133" s="76"/>
+      <c r="C133" s="76"/>
+      <c r="D133" s="76"/>
+      <c r="E133" s="76"/>
+      <c r="F133" s="76"/>
+      <c r="G133" s="76"/>
+      <c r="H133" s="76"/>
+      <c r="I133" s="76"/>
+    </row>
+    <row r="134" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A134" s="76"/>
+      <c r="B134" s="76"/>
+      <c r="C134" s="76"/>
+      <c r="D134" s="76"/>
+      <c r="E134" s="76"/>
+      <c r="F134" s="76"/>
+      <c r="G134" s="76"/>
+      <c r="H134" s="76"/>
+      <c r="I134" s="76"/>
+    </row>
+    <row r="135" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A135" s="76"/>
+      <c r="B135" s="76"/>
+      <c r="C135" s="76"/>
+      <c r="D135" s="76"/>
+      <c r="E135" s="76"/>
+      <c r="F135" s="76"/>
+      <c r="G135" s="76"/>
+      <c r="H135" s="76"/>
+      <c r="I135" s="76"/>
+    </row>
+    <row r="136" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A136" s="76"/>
+      <c r="B136" s="76"/>
+      <c r="C136" s="76"/>
+      <c r="D136" s="76"/>
+      <c r="E136" s="76"/>
+      <c r="F136" s="76"/>
+      <c r="G136" s="76"/>
+      <c r="H136" s="76"/>
+      <c r="I136" s="76"/>
+    </row>
+    <row r="137" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A137" s="76"/>
+      <c r="B137" s="76"/>
+      <c r="C137" s="76"/>
+      <c r="D137" s="76"/>
+      <c r="E137" s="76"/>
+      <c r="F137" s="76"/>
+      <c r="G137" s="76"/>
+      <c r="H137" s="76"/>
+      <c r="I137" s="76"/>
+    </row>
+    <row r="138" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A138" s="76"/>
+      <c r="B138" s="76"/>
+      <c r="C138" s="76"/>
+      <c r="D138" s="76"/>
+      <c r="E138" s="76"/>
+      <c r="F138" s="76"/>
+      <c r="G138" s="76"/>
+      <c r="H138" s="76"/>
+      <c r="I138" s="76"/>
+    </row>
+    <row r="139" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A139" s="76"/>
+      <c r="B139" s="76"/>
+      <c r="C139" s="76"/>
+      <c r="D139" s="76"/>
+      <c r="E139" s="76"/>
+      <c r="F139" s="76"/>
+      <c r="G139" s="76"/>
+      <c r="H139" s="76"/>
+      <c r="I139" s="76"/>
+    </row>
+    <row r="140" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A140" s="76"/>
+      <c r="B140" s="76"/>
+      <c r="C140" s="76"/>
+      <c r="D140" s="76"/>
+      <c r="E140" s="76"/>
+      <c r="F140" s="76"/>
+      <c r="G140" s="76"/>
+      <c r="H140" s="76"/>
+      <c r="I140" s="76"/>
+    </row>
+    <row r="141" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A141" s="76"/>
+      <c r="B141" s="76"/>
+      <c r="C141" s="76"/>
+      <c r="D141" s="76"/>
+      <c r="E141" s="76"/>
+      <c r="F141" s="76"/>
+      <c r="G141" s="76"/>
+      <c r="H141" s="76"/>
+      <c r="I141" s="76"/>
+    </row>
+    <row r="142" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A142" s="76"/>
+      <c r="B142" s="76"/>
+      <c r="C142" s="76"/>
+      <c r="D142" s="76"/>
+      <c r="E142" s="76"/>
+      <c r="F142" s="76"/>
+      <c r="G142" s="76"/>
+      <c r="H142" s="76"/>
+      <c r="I142" s="76"/>
+    </row>
+    <row r="143" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A143" s="76"/>
+      <c r="B143" s="76"/>
+      <c r="C143" s="76"/>
+      <c r="D143" s="76"/>
+      <c r="E143" s="76"/>
+      <c r="F143" s="76"/>
+      <c r="G143" s="76"/>
+      <c r="H143" s="76"/>
+      <c r="I143" s="76"/>
+    </row>
+    <row r="144" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A144" s="76"/>
+      <c r="B144" s="76"/>
+      <c r="C144" s="76"/>
+      <c r="D144" s="76"/>
+      <c r="E144" s="76"/>
+      <c r="F144" s="76"/>
+      <c r="G144" s="76"/>
+      <c r="H144" s="76"/>
+      <c r="I144" s="76"/>
+    </row>
+    <row r="145" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A145" s="76"/>
+      <c r="B145" s="76"/>
+      <c r="C145" s="76"/>
+      <c r="D145" s="76"/>
+      <c r="E145" s="76"/>
+      <c r="F145" s="76"/>
+      <c r="G145" s="76"/>
+      <c r="H145" s="76"/>
+      <c r="I145" s="76"/>
+    </row>
+    <row r="146" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A146" s="76"/>
+      <c r="B146" s="76"/>
+      <c r="C146" s="76"/>
+      <c r="D146" s="76"/>
+      <c r="E146" s="76"/>
+      <c r="F146" s="76"/>
+      <c r="G146" s="76"/>
+      <c r="H146" s="76"/>
+      <c r="I146" s="76"/>
+    </row>
+    <row r="147" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A147" s="76"/>
+      <c r="B147" s="76"/>
+      <c r="C147" s="76"/>
+      <c r="D147" s="76"/>
+      <c r="E147" s="76"/>
+      <c r="F147" s="76"/>
+      <c r="G147" s="76"/>
+      <c r="H147" s="76"/>
+      <c r="I147" s="76"/>
+    </row>
+    <row r="148" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A148" s="76"/>
+      <c r="B148" s="76"/>
+      <c r="C148" s="76"/>
+      <c r="D148" s="76"/>
+      <c r="E148" s="76"/>
+      <c r="F148" s="76"/>
+      <c r="G148" s="76"/>
+      <c r="H148" s="76"/>
+      <c r="I148" s="76"/>
+    </row>
+    <row r="149" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A149" s="76"/>
+      <c r="B149" s="76"/>
+      <c r="C149" s="76"/>
+      <c r="D149" s="76"/>
+      <c r="E149" s="76"/>
+      <c r="F149" s="76"/>
+      <c r="G149" s="76"/>
+      <c r="H149" s="76"/>
+      <c r="I149" s="76"/>
+    </row>
+    <row r="150" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A150" s="76"/>
+      <c r="B150" s="76"/>
+      <c r="C150" s="76"/>
+      <c r="D150" s="76"/>
+      <c r="E150" s="76"/>
+      <c r="F150" s="76"/>
+      <c r="G150" s="76"/>
+      <c r="H150" s="76"/>
+      <c r="I150" s="76"/>
+    </row>
+    <row r="151" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A151" s="76"/>
+      <c r="B151" s="76"/>
+      <c r="C151" s="76"/>
+      <c r="D151" s="76"/>
+      <c r="E151" s="76"/>
+      <c r="F151" s="76"/>
+      <c r="G151" s="76"/>
+      <c r="H151" s="76"/>
+      <c r="I151" s="76"/>
+    </row>
+    <row r="152" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A152" s="76"/>
+      <c r="B152" s="76"/>
+      <c r="C152" s="76"/>
+      <c r="D152" s="76"/>
+      <c r="E152" s="76"/>
+      <c r="F152" s="76"/>
+      <c r="G152" s="76"/>
+      <c r="H152" s="76"/>
+      <c r="I152" s="76"/>
+    </row>
+    <row r="153" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A153" s="76"/>
+      <c r="B153" s="76"/>
+      <c r="C153" s="76"/>
+      <c r="D153" s="76"/>
+      <c r="E153" s="76"/>
+      <c r="F153" s="76"/>
+      <c r="G153" s="76"/>
+      <c r="H153" s="76"/>
+      <c r="I153" s="76"/>
+    </row>
+    <row r="154" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A154" s="76"/>
+      <c r="B154" s="76"/>
+      <c r="C154" s="76"/>
+      <c r="D154" s="76"/>
+      <c r="E154" s="76"/>
+      <c r="F154" s="76"/>
+      <c r="G154" s="76"/>
+      <c r="H154" s="76"/>
+      <c r="I154" s="76"/>
+    </row>
+    <row r="155" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A155" s="76"/>
+      <c r="B155" s="76"/>
+      <c r="C155" s="76"/>
+      <c r="D155" s="76"/>
+      <c r="E155" s="76"/>
+      <c r="F155" s="76"/>
+      <c r="G155" s="76"/>
+      <c r="H155" s="76"/>
+      <c r="I155" s="76"/>
+    </row>
+    <row r="156" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A156" s="76"/>
+      <c r="B156" s="76"/>
+      <c r="C156" s="76"/>
+      <c r="D156" s="76"/>
+      <c r="E156" s="76"/>
+      <c r="F156" s="76"/>
+      <c r="G156" s="76"/>
+      <c r="H156" s="76"/>
+      <c r="I156" s="76"/>
+    </row>
+    <row r="157" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A157" s="76"/>
+      <c r="B157" s="76"/>
+      <c r="C157" s="76"/>
+      <c r="D157" s="76"/>
+      <c r="E157" s="76"/>
+      <c r="F157" s="76"/>
+      <c r="G157" s="76"/>
+      <c r="H157" s="76"/>
+      <c r="I157" s="76"/>
+    </row>
+    <row r="158" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A158" s="76"/>
+      <c r="B158" s="76"/>
+      <c r="C158" s="76"/>
+      <c r="D158" s="76"/>
+      <c r="E158" s="76"/>
+      <c r="F158" s="76"/>
+      <c r="G158" s="76"/>
+      <c r="H158" s="76"/>
+      <c r="I158" s="76"/>
+    </row>
+    <row r="159" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A159" s="76"/>
+      <c r="B159" s="76"/>
+      <c r="C159" s="76"/>
+      <c r="D159" s="76"/>
+      <c r="E159" s="76"/>
+      <c r="F159" s="76"/>
+      <c r="G159" s="76"/>
+      <c r="H159" s="76"/>
+      <c r="I159" s="76"/>
+    </row>
+    <row r="160" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A160" s="76"/>
+      <c r="B160" s="76"/>
+      <c r="C160" s="76"/>
+      <c r="D160" s="76"/>
+      <c r="E160" s="76"/>
+      <c r="F160" s="76"/>
+      <c r="G160" s="76"/>
+      <c r="H160" s="76"/>
+      <c r="I160" s="76"/>
+    </row>
+    <row r="161" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A161" s="76"/>
+      <c r="B161" s="76"/>
+      <c r="C161" s="76"/>
+      <c r="D161" s="76"/>
+      <c r="E161" s="76"/>
+      <c r="F161" s="76"/>
+      <c r="G161" s="76"/>
+      <c r="H161" s="76"/>
+      <c r="I161" s="76"/>
+    </row>
+    <row r="162" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A162" s="76"/>
+      <c r="B162" s="76"/>
+      <c r="C162" s="76"/>
+      <c r="D162" s="76"/>
+      <c r="E162" s="76"/>
+      <c r="F162" s="76"/>
+      <c r="G162" s="76"/>
+      <c r="H162" s="76"/>
+      <c r="I162" s="76"/>
+    </row>
+    <row r="163" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A163" s="76"/>
+      <c r="B163" s="76"/>
+      <c r="C163" s="76"/>
+      <c r="D163" s="76"/>
+      <c r="E163" s="76"/>
+      <c r="F163" s="76"/>
+      <c r="G163" s="76"/>
+      <c r="H163" s="76"/>
+      <c r="I163" s="76"/>
+    </row>
+    <row r="164" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A164" s="76"/>
+      <c r="B164" s="76"/>
+      <c r="C164" s="76"/>
+      <c r="D164" s="76"/>
+      <c r="E164" s="76"/>
+      <c r="F164" s="76"/>
+      <c r="G164" s="76"/>
+      <c r="H164" s="76"/>
+      <c r="I164" s="76"/>
+    </row>
+    <row r="165" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A165" s="76"/>
+      <c r="B165" s="76"/>
+      <c r="C165" s="76"/>
+      <c r="D165" s="76"/>
+      <c r="E165" s="76"/>
+      <c r="F165" s="76"/>
+      <c r="G165" s="76"/>
+      <c r="H165" s="76"/>
+      <c r="I165" s="76"/>
+    </row>
+    <row r="166" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A166" s="76"/>
+      <c r="B166" s="76"/>
+      <c r="C166" s="76"/>
+      <c r="D166" s="76"/>
+      <c r="E166" s="76"/>
+      <c r="F166" s="76"/>
+      <c r="G166" s="76"/>
+      <c r="H166" s="76"/>
+      <c r="I166" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TU Corrections Tamil 14/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="474">
   <si>
     <t>Date</t>
   </si>
@@ -1415,19 +1415,55 @@
   </si>
   <si>
     <t>4.1.6.3</t>
+  </si>
+  <si>
+    <t>4.1.7.1</t>
+  </si>
+  <si>
+    <t>4.1.8.1</t>
+  </si>
+  <si>
+    <t>4.1.9.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=JGI1kCHX_y4</t>
+  </si>
+  <si>
+    <t>4.1.10.1</t>
+  </si>
+  <si>
+    <t>4.1.11.1</t>
+  </si>
+  <si>
+    <t>4.2.1.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=H669N76DrwA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="54" x14ac:knownFonts="1">
+  <fonts count="56" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1780,78 +1816,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="53" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="51" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="53" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="52" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="54" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1859,16 +1897,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11759,8 +11798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12037,17 +12076,25 @@
       <c r="B14" s="77">
         <v>44086</v>
       </c>
-      <c r="C14" s="76"/>
+      <c r="C14" s="76">
+        <v>44.29</v>
+      </c>
       <c r="D14" s="59">
         <v>1</v>
       </c>
       <c r="E14" s="76" t="s">
         <v>465</v>
       </c>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
+      <c r="F14" s="76">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G14" s="79">
+        <v>7.2</v>
+      </c>
       <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
+      <c r="I14" s="76" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="76"/>
@@ -12057,11 +12104,17 @@
         <f>+D14+1</f>
         <v>2</v>
       </c>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
+      <c r="E15" s="78" t="s">
+        <v>466</v>
+      </c>
+      <c r="F15" s="79">
+        <f>+G14</f>
+        <v>7.2</v>
+      </c>
+      <c r="G15" s="76">
+        <v>18.23</v>
+      </c>
       <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="76"/>
@@ -12071,9 +12124,16 @@
         <f>+D15+1</f>
         <v>3</v>
       </c>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
+      <c r="E16" s="78" t="s">
+        <v>467</v>
+      </c>
+      <c r="F16" s="79">
+        <f>+G15</f>
+        <v>18.23</v>
+      </c>
+      <c r="G16" s="76">
+        <v>34.31</v>
+      </c>
       <c r="H16" s="76"/>
       <c r="I16" s="76"/>
     </row>
@@ -12085,9 +12145,16 @@
         <f t="shared" ref="D17" si="2">+D16+1</f>
         <v>4</v>
       </c>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
+      <c r="E17" s="78" t="s">
+        <v>468</v>
+      </c>
+      <c r="F17" s="76">
+        <f>+G16</f>
+        <v>34.31</v>
+      </c>
+      <c r="G17" s="76">
+        <v>43.54</v>
+      </c>
       <c r="H17" s="76"/>
       <c r="I17" s="76"/>
     </row>
@@ -12103,24 +12170,50 @@
       <c r="I18" s="76"/>
     </row>
     <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="76"/>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
+      <c r="A19" s="76">
+        <v>4</v>
+      </c>
+      <c r="B19" s="77">
+        <v>44087</v>
+      </c>
+      <c r="C19" s="76">
+        <v>39.380000000000003</v>
+      </c>
+      <c r="D19" s="59">
+        <v>1</v>
+      </c>
+      <c r="E19" s="80" t="s">
+        <v>470</v>
+      </c>
+      <c r="F19" s="76">
+        <v>5.21</v>
+      </c>
+      <c r="G19" s="76">
+        <v>20.350000000000001</v>
+      </c>
       <c r="H19" s="76"/>
-      <c r="I19" s="76"/>
+      <c r="I19" s="76" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="76"/>
       <c r="B20" s="76"/>
       <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
+      <c r="D20" s="59">
+        <f>+D19+1</f>
+        <v>2</v>
+      </c>
+      <c r="E20" s="80" t="s">
+        <v>471</v>
+      </c>
+      <c r="F20" s="76">
+        <f>+G19</f>
+        <v>20.350000000000001</v>
+      </c>
+      <c r="G20" s="76">
+        <v>33.03</v>
+      </c>
       <c r="H20" s="76"/>
       <c r="I20" s="76"/>
     </row>
@@ -12128,10 +12221,20 @@
       <c r="A21" s="76"/>
       <c r="B21" s="76"/>
       <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="76"/>
+      <c r="D21" s="59">
+        <f>+D20+1</f>
+        <v>3</v>
+      </c>
+      <c r="E21" s="80" t="s">
+        <v>472</v>
+      </c>
+      <c r="F21" s="76">
+        <f>+G20</f>
+        <v>33.03</v>
+      </c>
+      <c r="G21" s="76">
+        <v>38.47</v>
+      </c>
       <c r="H21" s="76"/>
       <c r="I21" s="76"/>
     </row>

</xml_diff>

<commit_message>
GS 1.1-1.8 Baraha file 15/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="488">
   <si>
     <t>Date</t>
   </si>
@@ -1460,19 +1460,46 @@
   </si>
   <si>
     <t>4.2.5.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=owACaHfnStk</t>
+  </si>
+  <si>
+    <t>4.2.6.1</t>
+  </si>
+  <si>
+    <t>4.2.7.1</t>
+  </si>
+  <si>
+    <t>4.2.8.1</t>
+  </si>
+  <si>
+    <t>4.2.9.1</t>
+  </si>
+  <si>
+    <t>4.2.10.1</t>
+  </si>
+  <si>
+    <t>4.2.11.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="57" x14ac:knownFonts="1">
+  <fonts count="58" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1843,78 +1870,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="54" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="54" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="55" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="55" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="56" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1923,17 +1951,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -11826,8 +11854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12339,7 +12367,7 @@
         <v>478</v>
       </c>
       <c r="F25" s="76">
-        <f t="shared" ref="F25:F27" si="3">+G24</f>
+        <f t="shared" ref="F25:F26" si="3">+G24</f>
         <v>28.58</v>
       </c>
       <c r="G25" s="79">
@@ -12387,17 +12415,25 @@
       <c r="B28" s="77">
         <v>44089</v>
       </c>
-      <c r="C28" s="76"/>
+      <c r="C28" s="76">
+        <v>50.19</v>
+      </c>
       <c r="D28" s="59">
         <v>1</v>
       </c>
       <c r="E28" s="81" t="s">
         <v>480</v>
       </c>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
+      <c r="F28" s="76">
+        <v>3.02</v>
+      </c>
+      <c r="G28" s="76">
+        <v>22.41</v>
+      </c>
       <c r="H28" s="76"/>
-      <c r="I28" s="76"/>
+      <c r="I28" s="76" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="76"/>
@@ -12407,9 +12443,16 @@
         <f>+D28+1</f>
         <v>2</v>
       </c>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
+      <c r="E29" s="82" t="s">
+        <v>482</v>
+      </c>
+      <c r="F29" s="76">
+        <f>+G28</f>
+        <v>22.41</v>
+      </c>
+      <c r="G29" s="76">
+        <v>38.14</v>
+      </c>
       <c r="H29" s="76"/>
       <c r="I29" s="76"/>
     </row>
@@ -12421,9 +12464,16 @@
         <f>+D29+1</f>
         <v>3</v>
       </c>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
+      <c r="E30" s="82" t="s">
+        <v>483</v>
+      </c>
+      <c r="F30" s="76">
+        <f>+G29</f>
+        <v>38.14</v>
+      </c>
+      <c r="G30" s="76">
+        <v>49.15</v>
+      </c>
       <c r="H30" s="76"/>
       <c r="I30" s="76"/>
     </row>
@@ -12431,10 +12481,7 @@
       <c r="A31" s="76"/>
       <c r="B31" s="76"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="59">
-        <f>+D30+1</f>
-        <v>4</v>
-      </c>
+      <c r="D31" s="59"/>
       <c r="E31" s="76"/>
       <c r="F31" s="76"/>
       <c r="G31" s="76"/>
@@ -12442,11 +12489,19 @@
       <c r="I31" s="76"/>
     </row>
     <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="76"/>
+      <c r="A32" s="76">
+        <v>7</v>
+      </c>
+      <c r="B32" s="77">
+        <v>44090</v>
+      </c>
       <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
+      <c r="D32" s="59">
+        <v>1</v>
+      </c>
+      <c r="E32" s="82" t="s">
+        <v>484</v>
+      </c>
       <c r="F32" s="76"/>
       <c r="G32" s="76"/>
       <c r="H32" s="76"/>
@@ -12456,8 +12511,13 @@
       <c r="A33" s="76"/>
       <c r="B33" s="76"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
+      <c r="D33" s="59">
+        <f>+D32+1</f>
+        <v>2</v>
+      </c>
+      <c r="E33" s="82" t="s">
+        <v>485</v>
+      </c>
       <c r="F33" s="76"/>
       <c r="G33" s="76"/>
       <c r="H33" s="76"/>
@@ -12467,8 +12527,13 @@
       <c r="A34" s="76"/>
       <c r="B34" s="76"/>
       <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
+      <c r="D34" s="59">
+        <f>+D33+1</f>
+        <v>3</v>
+      </c>
+      <c r="E34" s="82" t="s">
+        <v>486</v>
+      </c>
       <c r="F34" s="76"/>
       <c r="G34" s="76"/>
       <c r="H34" s="76"/>
@@ -12478,8 +12543,13 @@
       <c r="A35" s="76"/>
       <c r="B35" s="76"/>
       <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
+      <c r="D35" s="59">
+        <f>+D34+1</f>
+        <v>4</v>
+      </c>
+      <c r="E35" s="82" t="s">
+        <v>487</v>
+      </c>
       <c r="F35" s="76"/>
       <c r="G35" s="76"/>
       <c r="H35" s="76"/>

</xml_diff>

<commit_message>
Ghana Sandhi 1.1-1.8 as of 19/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -13,11 +13,12 @@
     <sheet name="Kandam4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="506">
   <si>
     <t>Date</t>
   </si>
@@ -1484,19 +1485,88 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=iG5Ds-XUhog</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4ymk1MR1PD4</t>
+  </si>
+  <si>
+    <t>4.3.1.1</t>
+  </si>
+  <si>
+    <t>4.3.2.1</t>
+  </si>
+  <si>
+    <t>4.3.3.1</t>
+  </si>
+  <si>
+    <t>4.3.4.1</t>
+  </si>
+  <si>
+    <t>4.3.5.1</t>
+  </si>
+  <si>
+    <t>4.3.6.1</t>
+  </si>
+  <si>
+    <t>4.3.7.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=02xxeSIBfuA</t>
+  </si>
+  <si>
+    <t>4.3.8.1</t>
+  </si>
+  <si>
+    <t>4.3.9.1</t>
+  </si>
+  <si>
+    <t>4.3.10.1</t>
+  </si>
+  <si>
+    <t>4.3.11.1</t>
+  </si>
+  <si>
+    <t>4.3.12.1</t>
+  </si>
+  <si>
+    <t>4.3.12.2</t>
+  </si>
+  <si>
+    <t>4.3.12.3</t>
+  </si>
+  <si>
+    <t>4.3.13.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="58" x14ac:knownFonts="1">
+  <fonts count="61" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1873,97 +1943,100 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="55" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="58" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="58" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="55" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="58" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="59" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="59" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="56" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -11857,8 +11930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12593,24 +12666,50 @@
       <c r="I36" s="76"/>
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="76"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
+      <c r="A37" s="76">
+        <v>8</v>
+      </c>
+      <c r="B37" s="77">
+        <v>44091</v>
+      </c>
+      <c r="C37" s="76">
+        <v>57.06</v>
+      </c>
+      <c r="D37" s="59">
+        <v>1</v>
+      </c>
+      <c r="E37" s="83" t="s">
+        <v>490</v>
+      </c>
+      <c r="F37" s="79">
+        <v>4.2</v>
+      </c>
+      <c r="G37" s="76">
+        <v>8.15</v>
+      </c>
       <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
+      <c r="I37" s="76" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="76"/>
       <c r="B38" s="76"/>
       <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="76"/>
+      <c r="D38" s="59">
+        <f t="shared" ref="D38:D43" si="4">+D37+1</f>
+        <v>2</v>
+      </c>
+      <c r="E38" s="83" t="s">
+        <v>491</v>
+      </c>
+      <c r="F38" s="79">
+        <f>+G37</f>
+        <v>8.15</v>
+      </c>
+      <c r="G38" s="76">
+        <v>19.440000000000001</v>
+      </c>
       <c r="H38" s="76"/>
       <c r="I38" s="76"/>
     </row>
@@ -12618,10 +12717,20 @@
       <c r="A39" s="76"/>
       <c r="B39" s="76"/>
       <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
+      <c r="D39" s="59">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E39" s="83" t="s">
+        <v>492</v>
+      </c>
+      <c r="F39" s="79">
+        <f t="shared" ref="F39:F43" si="5">+G38</f>
+        <v>19.440000000000001</v>
+      </c>
+      <c r="G39" s="76">
+        <v>28.39</v>
+      </c>
       <c r="H39" s="76"/>
       <c r="I39" s="76"/>
     </row>
@@ -12629,10 +12738,20 @@
       <c r="A40" s="76"/>
       <c r="B40" s="76"/>
       <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
+      <c r="D40" s="59">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E40" s="83" t="s">
+        <v>493</v>
+      </c>
+      <c r="F40" s="79">
+        <f t="shared" si="5"/>
+        <v>28.39</v>
+      </c>
+      <c r="G40" s="76">
+        <v>39.08</v>
+      </c>
       <c r="H40" s="76"/>
       <c r="I40" s="76"/>
     </row>
@@ -12640,10 +12759,20 @@
       <c r="A41" s="76"/>
       <c r="B41" s="76"/>
       <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
+      <c r="D41" s="59">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="E41" s="83" t="s">
+        <v>494</v>
+      </c>
+      <c r="F41" s="79">
+        <f t="shared" si="5"/>
+        <v>39.08</v>
+      </c>
+      <c r="G41" s="76">
+        <v>43.52</v>
+      </c>
       <c r="H41" s="76"/>
       <c r="I41" s="76"/>
     </row>
@@ -12651,10 +12780,20 @@
       <c r="A42" s="76"/>
       <c r="B42" s="76"/>
       <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
+      <c r="D42" s="59">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="E42" s="83" t="s">
+        <v>495</v>
+      </c>
+      <c r="F42" s="79">
+        <f t="shared" si="5"/>
+        <v>43.52</v>
+      </c>
+      <c r="G42" s="76">
+        <v>50.11</v>
+      </c>
       <c r="H42" s="76"/>
       <c r="I42" s="76"/>
     </row>
@@ -12662,10 +12801,20 @@
       <c r="A43" s="76"/>
       <c r="B43" s="76"/>
       <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
+      <c r="D43" s="59">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="E43" s="83" t="s">
+        <v>496</v>
+      </c>
+      <c r="F43" s="79">
+        <f t="shared" si="5"/>
+        <v>50.11</v>
+      </c>
+      <c r="G43" s="76">
+        <v>55.58</v>
+      </c>
       <c r="H43" s="76"/>
       <c r="I43" s="76"/>
     </row>
@@ -12681,24 +12830,50 @@
       <c r="I44" s="76"/>
     </row>
     <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="76"/>
-      <c r="B45" s="76"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="76"/>
-      <c r="F45" s="76"/>
-      <c r="G45" s="76"/>
+      <c r="A45" s="76">
+        <v>8</v>
+      </c>
+      <c r="B45" s="77">
+        <v>44092</v>
+      </c>
+      <c r="C45" s="76">
+        <v>57.27</v>
+      </c>
+      <c r="D45" s="59">
+        <v>1</v>
+      </c>
+      <c r="E45" s="84" t="s">
+        <v>498</v>
+      </c>
+      <c r="F45" s="84">
+        <v>5.53</v>
+      </c>
+      <c r="G45" s="76">
+        <v>10.23</v>
+      </c>
       <c r="H45" s="76"/>
-      <c r="I45" s="76"/>
+      <c r="I45" s="76" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="76"/>
       <c r="B46" s="76"/>
       <c r="C46" s="76"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76"/>
+      <c r="D46" s="59">
+        <f t="shared" ref="D46:D49" si="6">+D45+1</f>
+        <v>2</v>
+      </c>
+      <c r="E46" s="84" t="s">
+        <v>499</v>
+      </c>
+      <c r="F46" s="79">
+        <f>+G45</f>
+        <v>10.23</v>
+      </c>
+      <c r="G46" s="76">
+        <v>18.54</v>
+      </c>
       <c r="H46" s="76"/>
       <c r="I46" s="76"/>
     </row>
@@ -12706,10 +12881,20 @@
       <c r="A47" s="76"/>
       <c r="B47" s="76"/>
       <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
-      <c r="E47" s="76"/>
-      <c r="F47" s="76"/>
-      <c r="G47" s="76"/>
+      <c r="D47" s="59">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="E47" s="84" t="s">
+        <v>500</v>
+      </c>
+      <c r="F47" s="79">
+        <f>+G46</f>
+        <v>18.54</v>
+      </c>
+      <c r="G47" s="76">
+        <v>31.34</v>
+      </c>
       <c r="H47" s="76"/>
       <c r="I47" s="76"/>
     </row>
@@ -12717,10 +12902,20 @@
       <c r="A48" s="76"/>
       <c r="B48" s="76"/>
       <c r="C48" s="76"/>
-      <c r="D48" s="76"/>
-      <c r="E48" s="76"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="76"/>
+      <c r="D48" s="59">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E48" s="84" t="s">
+        <v>501</v>
+      </c>
+      <c r="F48" s="76">
+        <f>+G47</f>
+        <v>31.34</v>
+      </c>
+      <c r="G48" s="76">
+        <v>49.42</v>
+      </c>
       <c r="H48" s="76"/>
       <c r="I48" s="76"/>
     </row>
@@ -12728,11 +12923,23 @@
       <c r="A49" s="76"/>
       <c r="B49" s="76"/>
       <c r="C49" s="76"/>
-      <c r="D49" s="76"/>
-      <c r="E49" s="76"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="76"/>
-      <c r="H49" s="76"/>
+      <c r="D49" s="59">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="E49" s="85" t="s">
+        <v>502</v>
+      </c>
+      <c r="F49" s="76">
+        <f>+G48</f>
+        <v>49.42</v>
+      </c>
+      <c r="G49" s="76">
+        <v>56.29</v>
+      </c>
+      <c r="H49" s="85" t="s">
+        <v>503</v>
+      </c>
       <c r="I49" s="76"/>
     </row>
     <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -12747,11 +12954,19 @@
       <c r="I50" s="76"/>
     </row>
     <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="76"/>
-      <c r="B51" s="76"/>
+      <c r="A51" s="76">
+        <v>9</v>
+      </c>
+      <c r="B51" s="77">
+        <v>44093</v>
+      </c>
       <c r="C51" s="76"/>
-      <c r="D51" s="76"/>
-      <c r="E51" s="76"/>
+      <c r="D51" s="59">
+        <v>1</v>
+      </c>
+      <c r="E51" s="85" t="s">
+        <v>504</v>
+      </c>
       <c r="F51" s="76"/>
       <c r="G51" s="76"/>
       <c r="H51" s="76"/>
@@ -12761,8 +12976,13 @@
       <c r="A52" s="76"/>
       <c r="B52" s="76"/>
       <c r="C52" s="76"/>
-      <c r="D52" s="76"/>
-      <c r="E52" s="76"/>
+      <c r="D52" s="59">
+        <f t="shared" ref="D52:D54" si="7">+D51+1</f>
+        <v>2</v>
+      </c>
+      <c r="E52" s="85" t="s">
+        <v>505</v>
+      </c>
       <c r="F52" s="76"/>
       <c r="G52" s="76"/>
       <c r="H52" s="76"/>
@@ -12772,7 +12992,10 @@
       <c r="A53" s="76"/>
       <c r="B53" s="76"/>
       <c r="C53" s="76"/>
-      <c r="D53" s="76"/>
+      <c r="D53" s="59">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
       <c r="E53" s="76"/>
       <c r="F53" s="76"/>
       <c r="G53" s="76"/>
@@ -12783,7 +13006,10 @@
       <c r="A54" s="76"/>
       <c r="B54" s="76"/>
       <c r="C54" s="76"/>
-      <c r="D54" s="76"/>
+      <c r="D54" s="59">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
       <c r="E54" s="76"/>
       <c r="F54" s="76"/>
       <c r="G54" s="76"/>

</xml_diff>

<commit_message>
Move Padam Input Excel to Raja
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="512">
   <si>
     <t>Date</t>
   </si>
@@ -1541,19 +1541,37 @@
   </si>
   <si>
     <t>4.4.1.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7LBPenE9P8E</t>
+  </si>
+  <si>
+    <t>4.4.2.1</t>
+  </si>
+  <si>
+    <t>4.4.3.1</t>
+  </si>
+  <si>
+    <t>4.4.4.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="62" x14ac:knownFonts="1">
+  <fonts count="63" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1954,78 +1972,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="59" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="59" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="60" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="60" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="60" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="61" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2034,17 +2053,17 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2358,10 +2377,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -11942,8 +11961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13046,24 +13065,50 @@
       <c r="I54" s="76"/>
     </row>
     <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="76"/>
-      <c r="B55" s="76"/>
-      <c r="C55" s="76"/>
-      <c r="D55" s="76"/>
-      <c r="E55" s="76"/>
-      <c r="F55" s="76"/>
-      <c r="G55" s="76"/>
+      <c r="A55" s="76">
+        <v>10</v>
+      </c>
+      <c r="B55" s="77">
+        <v>44094</v>
+      </c>
+      <c r="C55" s="76">
+        <v>59.55</v>
+      </c>
+      <c r="D55" s="59">
+        <v>1</v>
+      </c>
+      <c r="E55" s="87" t="s">
+        <v>509</v>
+      </c>
+      <c r="F55" s="76">
+        <v>5.12</v>
+      </c>
+      <c r="G55" s="76">
+        <v>17.32</v>
+      </c>
       <c r="H55" s="76"/>
-      <c r="I55" s="76"/>
+      <c r="I55" s="76" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="76"/>
       <c r="B56" s="76"/>
       <c r="C56" s="76"/>
-      <c r="D56" s="76"/>
-      <c r="E56" s="76"/>
-      <c r="F56" s="76"/>
-      <c r="G56" s="76"/>
+      <c r="D56" s="59">
+        <f t="shared" ref="D56:D58" si="8">+D55+1</f>
+        <v>2</v>
+      </c>
+      <c r="E56" s="87" t="s">
+        <v>510</v>
+      </c>
+      <c r="F56" s="76">
+        <f>+G55</f>
+        <v>17.32</v>
+      </c>
+      <c r="G56" s="79">
+        <v>32.200000000000003</v>
+      </c>
       <c r="H56" s="76"/>
       <c r="I56" s="76"/>
     </row>
@@ -13071,10 +13116,20 @@
       <c r="A57" s="76"/>
       <c r="B57" s="76"/>
       <c r="C57" s="76"/>
-      <c r="D57" s="76"/>
-      <c r="E57" s="76"/>
-      <c r="F57" s="76"/>
-      <c r="G57" s="76"/>
+      <c r="D57" s="59">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="E57" s="87" t="s">
+        <v>511</v>
+      </c>
+      <c r="F57" s="79">
+        <f>+G56</f>
+        <v>32.200000000000003</v>
+      </c>
+      <c r="G57" s="76">
+        <v>59.12</v>
+      </c>
       <c r="H57" s="76"/>
       <c r="I57" s="76"/>
     </row>
@@ -13082,7 +13137,10 @@
       <c r="A58" s="76"/>
       <c r="B58" s="76"/>
       <c r="C58" s="76"/>
-      <c r="D58" s="76"/>
+      <c r="D58" s="59">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
       <c r="E58" s="76"/>
       <c r="F58" s="76"/>
       <c r="G58" s="76"/>

</xml_diff>

<commit_message>
Gana Maala revision and other editing 23/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="536">
   <si>
     <t>Date</t>
   </si>
@@ -1553,19 +1553,109 @@
   </si>
   <si>
     <t>4.4.4.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PT1uLnZ4mk8</t>
+  </si>
+  <si>
+    <t>4.4.5.1</t>
+  </si>
+  <si>
+    <t>4.4.6.1</t>
+  </si>
+  <si>
+    <t>4.4.7.1</t>
+  </si>
+  <si>
+    <t>4.4.8.1</t>
+  </si>
+  <si>
+    <t>4.4.9.1</t>
+  </si>
+  <si>
+    <t>4.4.10.1</t>
+  </si>
+  <si>
+    <t>4.4.11.1</t>
+  </si>
+  <si>
+    <t>4.4.12.1</t>
+  </si>
+  <si>
+    <t>4.4.12.2</t>
+  </si>
+  <si>
+    <t>4.5.1.1</t>
+  </si>
+  <si>
+    <t>4.5.2.1</t>
+  </si>
+  <si>
+    <t>4.5.3.1</t>
+  </si>
+  <si>
+    <t>4.5.4.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4nzwGKLpF1Y</t>
+  </si>
+  <si>
+    <t>4.5.5.1</t>
+  </si>
+  <si>
+    <t>4.5.6.1</t>
+  </si>
+  <si>
+    <t>4.5.7.1</t>
+  </si>
+  <si>
+    <t>4.5.8.1</t>
+  </si>
+  <si>
+    <t>4.5.9.1</t>
+  </si>
+  <si>
+    <t>4.5.10.1</t>
+  </si>
+  <si>
+    <t>4.5.11.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=KYCrgE57cIU</t>
+  </si>
+  <si>
+    <t>4.6.1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="63" x14ac:knownFonts="1">
+  <fonts count="66" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1972,97 +2062,100 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="60" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="63" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="60" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="63" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="64" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="64" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="61" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="61" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2378,9 +2471,9 @@
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -11961,8 +12054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13096,7 +13189,7 @@
       <c r="B56" s="76"/>
       <c r="C56" s="76"/>
       <c r="D56" s="59">
-        <f t="shared" ref="D56:D58" si="8">+D55+1</f>
+        <f t="shared" ref="D56:D66" si="8">+D55+1</f>
         <v>2</v>
       </c>
       <c r="E56" s="87" t="s">
@@ -13137,10 +13230,7 @@
       <c r="A58" s="76"/>
       <c r="B58" s="76"/>
       <c r="C58" s="76"/>
-      <c r="D58" s="59">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
+      <c r="D58" s="59"/>
       <c r="E58" s="76"/>
       <c r="F58" s="76"/>
       <c r="G58" s="76"/>
@@ -13148,24 +13238,50 @@
       <c r="I58" s="76"/>
     </row>
     <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="76"/>
-      <c r="B59" s="76"/>
-      <c r="C59" s="76"/>
-      <c r="D59" s="76"/>
-      <c r="E59" s="76"/>
-      <c r="F59" s="76"/>
-      <c r="G59" s="76"/>
+      <c r="A59" s="76">
+        <v>11</v>
+      </c>
+      <c r="B59" s="77">
+        <v>44095</v>
+      </c>
+      <c r="C59" s="76">
+        <v>58.32</v>
+      </c>
+      <c r="D59" s="59">
+        <v>1</v>
+      </c>
+      <c r="E59" s="88" t="s">
+        <v>513</v>
+      </c>
+      <c r="F59" s="76">
+        <v>5.18</v>
+      </c>
+      <c r="G59" s="76">
+        <v>10.54</v>
+      </c>
       <c r="H59" s="76"/>
-      <c r="I59" s="76"/>
+      <c r="I59" s="76" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="76"/>
       <c r="B60" s="76"/>
       <c r="C60" s="76"/>
-      <c r="D60" s="76"/>
-      <c r="E60" s="76"/>
-      <c r="F60" s="76"/>
-      <c r="G60" s="76"/>
+      <c r="D60" s="59">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E60" s="88" t="s">
+        <v>514</v>
+      </c>
+      <c r="F60" s="76">
+        <f>+G59</f>
+        <v>10.54</v>
+      </c>
+      <c r="G60" s="79">
+        <v>19.3</v>
+      </c>
       <c r="H60" s="76"/>
       <c r="I60" s="76"/>
     </row>
@@ -13173,10 +13289,20 @@
       <c r="A61" s="76"/>
       <c r="B61" s="76"/>
       <c r="C61" s="76"/>
-      <c r="D61" s="76"/>
-      <c r="E61" s="76"/>
-      <c r="F61" s="76"/>
-      <c r="G61" s="76"/>
+      <c r="D61" s="59">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="E61" s="88" t="s">
+        <v>515</v>
+      </c>
+      <c r="F61" s="79">
+        <f t="shared" ref="F61:F64" si="9">+G60</f>
+        <v>19.3</v>
+      </c>
+      <c r="G61" s="79">
+        <v>24.1</v>
+      </c>
       <c r="H61" s="76"/>
       <c r="I61" s="76"/>
     </row>
@@ -13184,10 +13310,20 @@
       <c r="A62" s="76"/>
       <c r="B62" s="76"/>
       <c r="C62" s="76"/>
-      <c r="D62" s="76"/>
-      <c r="E62" s="76"/>
-      <c r="F62" s="76"/>
-      <c r="G62" s="76"/>
+      <c r="D62" s="59">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E62" s="88" t="s">
+        <v>516</v>
+      </c>
+      <c r="F62" s="79">
+        <f t="shared" si="9"/>
+        <v>24.1</v>
+      </c>
+      <c r="G62" s="76">
+        <v>28.01</v>
+      </c>
       <c r="H62" s="76"/>
       <c r="I62" s="76"/>
     </row>
@@ -13195,10 +13331,20 @@
       <c r="A63" s="76"/>
       <c r="B63" s="76"/>
       <c r="C63" s="76"/>
-      <c r="D63" s="76"/>
-      <c r="E63" s="76"/>
-      <c r="F63" s="76"/>
-      <c r="G63" s="76"/>
+      <c r="D63" s="59">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="E63" s="88" t="s">
+        <v>517</v>
+      </c>
+      <c r="F63" s="79">
+        <f t="shared" si="9"/>
+        <v>28.01</v>
+      </c>
+      <c r="G63" s="79">
+        <v>34.299999999999997</v>
+      </c>
       <c r="H63" s="76"/>
       <c r="I63" s="76"/>
     </row>
@@ -13206,10 +13352,20 @@
       <c r="A64" s="76"/>
       <c r="B64" s="76"/>
       <c r="C64" s="76"/>
-      <c r="D64" s="76"/>
-      <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
-      <c r="G64" s="76"/>
+      <c r="D64" s="59">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E64" s="88" t="s">
+        <v>518</v>
+      </c>
+      <c r="F64" s="79">
+        <f t="shared" si="9"/>
+        <v>34.299999999999997</v>
+      </c>
+      <c r="G64" s="79">
+        <v>43.16</v>
+      </c>
       <c r="H64" s="76"/>
       <c r="I64" s="76"/>
     </row>
@@ -13217,10 +13373,20 @@
       <c r="A65" s="76"/>
       <c r="B65" s="76"/>
       <c r="C65" s="76"/>
-      <c r="D65" s="76"/>
-      <c r="E65" s="76"/>
-      <c r="F65" s="76"/>
-      <c r="G65" s="76"/>
+      <c r="D65" s="59">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="E65" s="88" t="s">
+        <v>519</v>
+      </c>
+      <c r="F65" s="79">
+        <f>+G64</f>
+        <v>43.16</v>
+      </c>
+      <c r="G65" s="76">
+        <v>54.16</v>
+      </c>
       <c r="H65" s="76"/>
       <c r="I65" s="76"/>
     </row>
@@ -13228,11 +13394,23 @@
       <c r="A66" s="76"/>
       <c r="B66" s="76"/>
       <c r="C66" s="76"/>
-      <c r="D66" s="76"/>
-      <c r="E66" s="76"/>
-      <c r="F66" s="76"/>
-      <c r="G66" s="76"/>
-      <c r="H66" s="76"/>
+      <c r="D66" s="59">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="E66" s="88" t="s">
+        <v>520</v>
+      </c>
+      <c r="F66" s="76">
+        <f>+G65</f>
+        <v>54.16</v>
+      </c>
+      <c r="G66" s="76">
+        <v>57.33</v>
+      </c>
+      <c r="H66" s="88" t="s">
+        <v>520</v>
+      </c>
       <c r="I66" s="76"/>
     </row>
     <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -13247,24 +13425,51 @@
       <c r="I67" s="76"/>
     </row>
     <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="76"/>
-      <c r="B68" s="76"/>
-      <c r="C68" s="76"/>
-      <c r="D68" s="76"/>
-      <c r="E68" s="76"/>
-      <c r="F68" s="76"/>
-      <c r="G68" s="76"/>
-      <c r="H68" s="76"/>
-      <c r="I68" s="76"/>
+      <c r="A68" s="76">
+        <v>12</v>
+      </c>
+      <c r="B68" s="77">
+        <v>44096</v>
+      </c>
+      <c r="C68" s="89">
+        <v>54.01</v>
+      </c>
+      <c r="D68" s="59">
+        <v>1</v>
+      </c>
+      <c r="E68" s="88" t="s">
+        <v>521</v>
+      </c>
+      <c r="F68" s="76">
+        <v>5.08</v>
+      </c>
+      <c r="G68" s="76">
+        <v>20.53</v>
+      </c>
+      <c r="H68" s="89" t="s">
+        <v>152</v>
+      </c>
+      <c r="I68" s="76" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="76"/>
       <c r="B69" s="76"/>
       <c r="C69" s="76"/>
-      <c r="D69" s="76"/>
-      <c r="E69" s="76"/>
-      <c r="F69" s="76"/>
-      <c r="G69" s="76"/>
+      <c r="D69" s="59">
+        <f t="shared" ref="D69:D80" si="10">+D68+1</f>
+        <v>2</v>
+      </c>
+      <c r="E69" s="88" t="s">
+        <v>522</v>
+      </c>
+      <c r="F69" s="79">
+        <v>24.13</v>
+      </c>
+      <c r="G69" s="76">
+        <v>37.590000000000003</v>
+      </c>
       <c r="H69" s="76"/>
       <c r="I69" s="76"/>
     </row>
@@ -13272,10 +13477,20 @@
       <c r="A70" s="76"/>
       <c r="B70" s="76"/>
       <c r="C70" s="76"/>
-      <c r="D70" s="76"/>
-      <c r="E70" s="76"/>
-      <c r="F70" s="76"/>
-      <c r="G70" s="76"/>
+      <c r="D70" s="59">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="E70" s="88" t="s">
+        <v>523</v>
+      </c>
+      <c r="F70" s="79">
+        <f t="shared" ref="F70:F71" si="11">+G69</f>
+        <v>37.590000000000003</v>
+      </c>
+      <c r="G70" s="76">
+        <v>44.26</v>
+      </c>
       <c r="H70" s="76"/>
       <c r="I70" s="76"/>
     </row>
@@ -13283,10 +13498,20 @@
       <c r="A71" s="76"/>
       <c r="B71" s="76"/>
       <c r="C71" s="76"/>
-      <c r="D71" s="76"/>
-      <c r="E71" s="76"/>
-      <c r="F71" s="76"/>
-      <c r="G71" s="76"/>
+      <c r="D71" s="59">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="E71" s="88" t="s">
+        <v>524</v>
+      </c>
+      <c r="F71" s="79">
+        <f t="shared" si="11"/>
+        <v>44.26</v>
+      </c>
+      <c r="G71" s="76">
+        <v>52.35</v>
+      </c>
       <c r="H71" s="76"/>
       <c r="I71" s="76"/>
     </row>
@@ -13294,32 +13519,58 @@
       <c r="A72" s="76"/>
       <c r="B72" s="76"/>
       <c r="C72" s="76"/>
-      <c r="D72" s="76"/>
-      <c r="E72" s="76"/>
-      <c r="F72" s="76"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="88"/>
+      <c r="F72" s="79"/>
       <c r="G72" s="76"/>
       <c r="H72" s="76"/>
       <c r="I72" s="76"/>
     </row>
     <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A73" s="76"/>
-      <c r="B73" s="76"/>
-      <c r="C73" s="76"/>
-      <c r="D73" s="76"/>
-      <c r="E73" s="76"/>
-      <c r="F73" s="76"/>
-      <c r="G73" s="76"/>
+      <c r="A73" s="76">
+        <v>13</v>
+      </c>
+      <c r="B73" s="77">
+        <v>44097</v>
+      </c>
+      <c r="C73" s="76">
+        <v>58.18</v>
+      </c>
+      <c r="D73" s="59">
+        <v>1</v>
+      </c>
+      <c r="E73" s="89" t="s">
+        <v>525</v>
+      </c>
+      <c r="F73" s="76">
+        <v>2.34</v>
+      </c>
+      <c r="G73" s="76">
+        <v>8.57</v>
+      </c>
       <c r="H73" s="76"/>
-      <c r="I73" s="76"/>
+      <c r="I73" s="76" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="76"/>
       <c r="B74" s="76"/>
       <c r="C74" s="76"/>
-      <c r="D74" s="76"/>
-      <c r="E74" s="76"/>
-      <c r="F74" s="76"/>
-      <c r="G74" s="76"/>
+      <c r="D74" s="59">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="E74" s="89" t="s">
+        <v>527</v>
+      </c>
+      <c r="F74" s="79">
+        <f>+G73</f>
+        <v>8.57</v>
+      </c>
+      <c r="G74" s="76">
+        <v>13.01</v>
+      </c>
       <c r="H74" s="76"/>
       <c r="I74" s="76"/>
     </row>
@@ -13327,10 +13578,20 @@
       <c r="A75" s="76"/>
       <c r="B75" s="76"/>
       <c r="C75" s="76"/>
-      <c r="D75" s="76"/>
-      <c r="E75" s="76"/>
-      <c r="F75" s="76"/>
-      <c r="G75" s="76"/>
+      <c r="D75" s="59">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="E75" s="89" t="s">
+        <v>528</v>
+      </c>
+      <c r="F75" s="79">
+        <f t="shared" ref="F75:F81" si="12">+G74</f>
+        <v>13.01</v>
+      </c>
+      <c r="G75" s="76">
+        <v>17.09</v>
+      </c>
       <c r="H75" s="76"/>
       <c r="I75" s="76"/>
     </row>
@@ -13338,10 +13599,20 @@
       <c r="A76" s="76"/>
       <c r="B76" s="76"/>
       <c r="C76" s="76"/>
-      <c r="D76" s="76"/>
-      <c r="E76" s="76"/>
-      <c r="F76" s="76"/>
-      <c r="G76" s="76"/>
+      <c r="D76" s="59">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="E76" s="89" t="s">
+        <v>529</v>
+      </c>
+      <c r="F76" s="79">
+        <f t="shared" si="12"/>
+        <v>17.09</v>
+      </c>
+      <c r="G76" s="76">
+        <v>21.34</v>
+      </c>
       <c r="H76" s="76"/>
       <c r="I76" s="76"/>
     </row>
@@ -13349,10 +13620,20 @@
       <c r="A77" s="76"/>
       <c r="B77" s="76"/>
       <c r="C77" s="76"/>
-      <c r="D77" s="76"/>
-      <c r="E77" s="76"/>
-      <c r="F77" s="76"/>
-      <c r="G77" s="76"/>
+      <c r="D77" s="59">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="E77" s="89" t="s">
+        <v>530</v>
+      </c>
+      <c r="F77" s="79">
+        <f t="shared" si="12"/>
+        <v>21.34</v>
+      </c>
+      <c r="G77" s="76">
+        <v>26.23</v>
+      </c>
       <c r="H77" s="76"/>
       <c r="I77" s="76"/>
     </row>
@@ -13360,10 +13641,20 @@
       <c r="A78" s="76"/>
       <c r="B78" s="76"/>
       <c r="C78" s="76"/>
-      <c r="D78" s="76"/>
-      <c r="E78" s="76"/>
-      <c r="F78" s="76"/>
-      <c r="G78" s="76"/>
+      <c r="D78" s="59">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="E78" s="89" t="s">
+        <v>531</v>
+      </c>
+      <c r="F78" s="79">
+        <f t="shared" si="12"/>
+        <v>26.23</v>
+      </c>
+      <c r="G78" s="76">
+        <v>31.42</v>
+      </c>
       <c r="H78" s="76"/>
       <c r="I78" s="76"/>
     </row>
@@ -13371,10 +13662,20 @@
       <c r="A79" s="76"/>
       <c r="B79" s="76"/>
       <c r="C79" s="76"/>
-      <c r="D79" s="76"/>
-      <c r="E79" s="76"/>
-      <c r="F79" s="76"/>
-      <c r="G79" s="76"/>
+      <c r="D79" s="59">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="E79" s="89" t="s">
+        <v>532</v>
+      </c>
+      <c r="F79" s="79">
+        <f t="shared" si="12"/>
+        <v>31.42</v>
+      </c>
+      <c r="G79" s="76">
+        <v>43.02</v>
+      </c>
       <c r="H79" s="76"/>
       <c r="I79" s="76"/>
     </row>
@@ -13382,10 +13683,20 @@
       <c r="A80" s="76"/>
       <c r="B80" s="76"/>
       <c r="C80" s="76"/>
-      <c r="D80" s="76"/>
-      <c r="E80" s="76"/>
-      <c r="F80" s="76"/>
-      <c r="G80" s="76"/>
+      <c r="D80" s="59">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="E80" s="90" t="s">
+        <v>533</v>
+      </c>
+      <c r="F80" s="79">
+        <f t="shared" si="12"/>
+        <v>43.02</v>
+      </c>
+      <c r="G80" s="76">
+        <v>49.48</v>
+      </c>
       <c r="H80" s="76"/>
       <c r="I80" s="76"/>
     </row>
@@ -13393,10 +13704,19 @@
       <c r="A81" s="76"/>
       <c r="B81" s="76"/>
       <c r="C81" s="76"/>
-      <c r="D81" s="76"/>
-      <c r="E81" s="76"/>
-      <c r="F81" s="76"/>
-      <c r="G81" s="76"/>
+      <c r="D81" s="59">
+        <v>9</v>
+      </c>
+      <c r="E81" s="90" t="s">
+        <v>535</v>
+      </c>
+      <c r="F81" s="79">
+        <f t="shared" si="12"/>
+        <v>49.48</v>
+      </c>
+      <c r="G81" s="76">
+        <v>56.58</v>
+      </c>
       <c r="H81" s="76"/>
       <c r="I81" s="76"/>
     </row>

</xml_diff>

<commit_message>
Padam Input 4.7+Chamaka Red marks 02/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="588">
   <si>
     <t>Date</t>
   </si>
@@ -1780,19 +1780,28 @@
   </si>
   <si>
     <t>5.1.7.1</t>
+  </si>
+  <si>
+    <t>5.1.7.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="73" x14ac:knownFonts="1">
+  <fonts count="74" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -2259,78 +2268,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="70" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="70" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="71" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="71" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="70" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="70" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="71" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="53" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="71" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="72" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="71" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="72" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="72" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2339,17 +2349,17 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2364,19 +2374,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="70" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="71" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="71" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="72" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -15224,8 +15234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15557,11 +15567,19 @@
       <c r="I16" s="96"/>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
+      <c r="A17" s="96">
+        <v>3</v>
+      </c>
+      <c r="B17" s="99">
+        <v>44106</v>
+      </c>
+      <c r="C17" s="102"/>
+      <c r="D17" s="100">
+        <v>1</v>
+      </c>
+      <c r="E17" s="104" t="s">
+        <v>587</v>
+      </c>
       <c r="F17" s="96"/>
       <c r="G17" s="96"/>
       <c r="H17" s="96"/>
@@ -15571,7 +15589,10 @@
       <c r="A18" s="96"/>
       <c r="B18" s="96"/>
       <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
+      <c r="D18" s="100">
+        <f>+D17+1</f>
+        <v>2</v>
+      </c>
       <c r="E18" s="96"/>
       <c r="F18" s="96"/>
       <c r="G18" s="96"/>
@@ -15582,7 +15603,10 @@
       <c r="A19" s="96"/>
       <c r="B19" s="96"/>
       <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
+      <c r="D19" s="100">
+        <f>+D18+1</f>
+        <v>3</v>
+      </c>
       <c r="E19" s="96"/>
       <c r="F19" s="96"/>
       <c r="G19" s="96"/>

</xml_diff>

<commit_message>
TS Jatai working+Raja Sandhi Restriction Rule 03/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="597">
   <si>
     <t>Date</t>
   </si>
@@ -1783,19 +1783,58 @@
   </si>
   <si>
     <t>5.1.7.2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1Pon2uK7hqo</t>
+  </si>
+  <si>
+    <t>5.1.8.1</t>
+  </si>
+  <si>
+    <t>5.1.9.1</t>
+  </si>
+  <si>
+    <t>5.1.10.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=b4UIdTTT_Y0</t>
+  </si>
+  <si>
+    <t>5.1.10.3</t>
+  </si>
+  <si>
+    <t>5.1.10.4</t>
+  </si>
+  <si>
+    <t>5.1.11.1</t>
+  </si>
+  <si>
+    <t>5.2.1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="74" x14ac:knownFonts="1">
+  <fonts count="76" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -2268,78 +2307,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="70" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="71" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="73" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="73" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="70" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="71" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="73" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="54" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="72" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="74" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="72" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="72" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="74" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="74" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2347,18 +2388,18 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2372,20 +2413,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="71" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="73" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="72" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="74" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -15234,8 +15275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15573,17 +15614,25 @@
       <c r="B17" s="99">
         <v>44106</v>
       </c>
-      <c r="C17" s="102"/>
+      <c r="C17" s="102">
+        <v>55.53</v>
+      </c>
       <c r="D17" s="100">
         <v>1</v>
       </c>
       <c r="E17" s="104" t="s">
         <v>587</v>
       </c>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
+      <c r="F17" s="96">
+        <v>1.05</v>
+      </c>
+      <c r="G17" s="96">
+        <v>9.43</v>
+      </c>
       <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
+      <c r="I17" s="96" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="96"/>
@@ -15593,9 +15642,16 @@
         <f>+D17+1</f>
         <v>2</v>
       </c>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
+      <c r="E18" s="105" t="s">
+        <v>589</v>
+      </c>
+      <c r="F18" s="96">
+        <f>+G17</f>
+        <v>9.43</v>
+      </c>
+      <c r="G18" s="96">
+        <v>30.35</v>
+      </c>
       <c r="H18" s="96"/>
       <c r="I18" s="96"/>
     </row>
@@ -15607,9 +15663,16 @@
         <f>+D18+1</f>
         <v>3</v>
       </c>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
+      <c r="E19" s="105" t="s">
+        <v>590</v>
+      </c>
+      <c r="F19" s="96">
+        <f>+G18</f>
+        <v>30.35</v>
+      </c>
+      <c r="G19" s="96">
+        <v>46.27</v>
+      </c>
       <c r="H19" s="96"/>
       <c r="I19" s="96"/>
     </row>
@@ -15617,11 +15680,23 @@
       <c r="A20" s="96"/>
       <c r="B20" s="96"/>
       <c r="C20" s="96"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="96"/>
+      <c r="D20" s="100">
+        <f>+D19+1</f>
+        <v>4</v>
+      </c>
+      <c r="E20" s="105" t="s">
+        <v>591</v>
+      </c>
+      <c r="F20" s="96">
+        <f>+G19</f>
+        <v>46.27</v>
+      </c>
+      <c r="G20" s="96">
+        <v>55.17</v>
+      </c>
+      <c r="H20" s="106" t="s">
+        <v>593</v>
+      </c>
       <c r="I20" s="96"/>
     </row>
     <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15636,35 +15711,72 @@
       <c r="I21" s="96"/>
     </row>
     <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="96"/>
-      <c r="B22" s="96"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
+      <c r="A22" s="96">
+        <v>4</v>
+      </c>
+      <c r="B22" s="99">
+        <v>44107</v>
+      </c>
+      <c r="C22" s="102">
+        <v>55.4</v>
+      </c>
+      <c r="D22" s="100">
+        <v>1</v>
+      </c>
+      <c r="E22" s="106" t="s">
+        <v>594</v>
+      </c>
+      <c r="F22" s="96">
+        <v>1.45</v>
+      </c>
+      <c r="G22" s="96">
+        <v>11.36</v>
+      </c>
       <c r="H22" s="96"/>
-      <c r="I22" s="96"/>
+      <c r="I22" s="96" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="96"/>
       <c r="B23" s="96"/>
       <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
+      <c r="D23" s="100">
+        <f>+D22+1</f>
+        <v>2</v>
+      </c>
+      <c r="E23" s="106" t="s">
+        <v>595</v>
+      </c>
+      <c r="F23" s="96">
+        <f>+G22</f>
+        <v>11.36</v>
+      </c>
+      <c r="G23" s="96">
+        <v>25.53</v>
+      </c>
+      <c r="H23" s="106" t="s">
+        <v>152</v>
+      </c>
       <c r="I23" s="96"/>
     </row>
     <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="96"/>
       <c r="B24" s="96"/>
       <c r="C24" s="96"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="96"/>
-      <c r="G24" s="96"/>
+      <c r="D24" s="100">
+        <f>+D23+1</f>
+        <v>3</v>
+      </c>
+      <c r="E24" s="106" t="s">
+        <v>596</v>
+      </c>
+      <c r="F24" s="96">
+        <v>31.29</v>
+      </c>
+      <c r="G24" s="96">
+        <v>54.14</v>
+      </c>
       <c r="H24" s="96"/>
       <c r="I24" s="96"/>
     </row>
@@ -15672,7 +15784,10 @@
       <c r="A25" s="96"/>
       <c r="B25" s="96"/>
       <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
+      <c r="D25" s="100">
+        <f>+D24+1</f>
+        <v>4</v>
+      </c>
       <c r="E25" s="96"/>
       <c r="F25" s="96"/>
       <c r="G25" s="96"/>

</xml_diff>

<commit_message>
TS 1.3 Padam Template related corr 05/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="601">
   <si>
     <t>Date</t>
   </si>
@@ -1810,19 +1810,37 @@
   </si>
   <si>
     <t>5.2.1.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1Dbz9_iNRjQ</t>
+  </si>
+  <si>
+    <t>5.2.2.1</t>
+  </si>
+  <si>
+    <t>5.2.3.1</t>
+  </si>
+  <si>
+    <t>5.2.4.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="76" x14ac:knownFonts="1">
+  <fonts count="77" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -2307,78 +2325,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="73" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="74" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="74" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="73" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="74" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="74" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="75" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="74" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="74" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="75" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="75" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2387,17 +2406,17 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2412,19 +2431,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="73" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="74" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="74" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="75" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2736,9 +2755,9 @@
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F148" sqref="F148"/>
+      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -15275,8 +15294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15784,10 +15803,7 @@
       <c r="A25" s="96"/>
       <c r="B25" s="96"/>
       <c r="C25" s="96"/>
-      <c r="D25" s="100">
-        <f>+D24+1</f>
-        <v>4</v>
-      </c>
+      <c r="D25" s="100"/>
       <c r="E25" s="96"/>
       <c r="F25" s="96"/>
       <c r="G25" s="96"/>
@@ -15795,24 +15811,50 @@
       <c r="I25" s="96"/>
     </row>
     <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="96"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96"/>
-      <c r="E26" s="96"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="96"/>
+      <c r="A26" s="96">
+        <v>5</v>
+      </c>
+      <c r="B26" s="99">
+        <v>44108</v>
+      </c>
+      <c r="C26" s="96">
+        <v>58.24</v>
+      </c>
+      <c r="D26" s="100">
+        <v>1</v>
+      </c>
+      <c r="E26" s="107" t="s">
+        <v>598</v>
+      </c>
+      <c r="F26" s="96">
+        <v>9.35</v>
+      </c>
+      <c r="G26" s="96">
+        <v>27.26</v>
+      </c>
       <c r="H26" s="96"/>
-      <c r="I26" s="96"/>
+      <c r="I26" s="96" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="96"/>
       <c r="B27" s="96"/>
       <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="96"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="96"/>
+      <c r="D27" s="100">
+        <f>+D26+1</f>
+        <v>2</v>
+      </c>
+      <c r="E27" s="107" t="s">
+        <v>599</v>
+      </c>
+      <c r="F27" s="96">
+        <f>+G26</f>
+        <v>27.26</v>
+      </c>
+      <c r="G27" s="96">
+        <v>49.08</v>
+      </c>
       <c r="H27" s="96"/>
       <c r="I27" s="96"/>
     </row>
@@ -15820,10 +15862,20 @@
       <c r="A28" s="96"/>
       <c r="B28" s="96"/>
       <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="96"/>
+      <c r="D28" s="100">
+        <f>+D27+1</f>
+        <v>3</v>
+      </c>
+      <c r="E28" s="107" t="s">
+        <v>600</v>
+      </c>
+      <c r="F28" s="96">
+        <f>+G27</f>
+        <v>49.08</v>
+      </c>
+      <c r="G28" s="102">
+        <v>57.5</v>
+      </c>
       <c r="H28" s="96"/>
       <c r="I28" s="96"/>
     </row>
@@ -15831,7 +15883,10 @@
       <c r="A29" s="96"/>
       <c r="B29" s="96"/>
       <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
+      <c r="D29" s="100">
+        <f>+D28+1</f>
+        <v>4</v>
+      </c>
       <c r="E29" s="96"/>
       <c r="F29" s="96"/>
       <c r="G29" s="96"/>

</xml_diff>

<commit_message>
TS Padam Input related corr, Raja Vowel output 07/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -15,11 +15,12 @@
     <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="618">
   <si>
     <t>Date</t>
   </si>
@@ -1837,19 +1838,67 @@
   </si>
   <si>
     <t>5.2.7.1</t>
+  </si>
+  <si>
+    <t>1.00.32</t>
+  </si>
+  <si>
+    <t>5.2.7.2</t>
+  </si>
+  <si>
+    <t>5.2.8.1</t>
+  </si>
+  <si>
+    <t>5.2.9.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=soZ8A0NqrTQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7EnTCwBJZi4</t>
+  </si>
+  <si>
+    <t>5.2.10.1</t>
+  </si>
+  <si>
+    <t>5.2.10.2</t>
+  </si>
+  <si>
+    <t>5.2.10.3</t>
+  </si>
+  <si>
+    <t>5.2.11.1</t>
+  </si>
+  <si>
+    <t>5.2.12.1</t>
+  </si>
+  <si>
+    <t>5.3.1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="78" x14ac:knownFonts="1">
+  <fonts count="80" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -2346,78 +2395,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="75" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="77" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="75" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="77" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="75" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="77" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="58" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="78" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="76" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="76" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="78" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="78" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2425,18 +2476,18 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2450,20 +2501,20 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="75" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="77" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="76" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="78" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2776,10 +2827,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -15316,8 +15367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15937,7 +15988,9 @@
         <v>9.2899999999999991</v>
       </c>
       <c r="H30" s="96"/>
-      <c r="I30" s="96"/>
+      <c r="I30" s="96" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="96"/>
@@ -16014,24 +16067,50 @@
       <c r="I34" s="96"/>
     </row>
     <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="96"/>
-      <c r="B35" s="96"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
+      <c r="A35" s="96">
+        <v>7</v>
+      </c>
+      <c r="B35" s="99">
+        <v>44110</v>
+      </c>
+      <c r="C35" s="109" t="s">
+        <v>606</v>
+      </c>
+      <c r="D35" s="100">
+        <v>1</v>
+      </c>
+      <c r="E35" s="109" t="s">
+        <v>607</v>
+      </c>
+      <c r="F35" s="102">
+        <v>3</v>
+      </c>
+      <c r="G35" s="96">
+        <v>16.079999999999998</v>
+      </c>
       <c r="H35" s="96"/>
-      <c r="I35" s="96"/>
+      <c r="I35" s="96" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="96"/>
       <c r="B36" s="96"/>
       <c r="C36" s="96"/>
-      <c r="D36" s="96"/>
-      <c r="E36" s="96"/>
-      <c r="F36" s="96"/>
-      <c r="G36" s="96"/>
+      <c r="D36" s="100">
+        <f>+D35+1</f>
+        <v>2</v>
+      </c>
+      <c r="E36" s="109" t="s">
+        <v>608</v>
+      </c>
+      <c r="F36" s="96">
+        <f>+G35</f>
+        <v>16.079999999999998</v>
+      </c>
+      <c r="G36" s="102">
+        <v>38</v>
+      </c>
       <c r="H36" s="96"/>
       <c r="I36" s="96"/>
     </row>
@@ -16039,10 +16118,20 @@
       <c r="A37" s="96"/>
       <c r="B37" s="96"/>
       <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
+      <c r="D37" s="100">
+        <f>+D36+1</f>
+        <v>3</v>
+      </c>
+      <c r="E37" s="109" t="s">
+        <v>609</v>
+      </c>
+      <c r="F37" s="102">
+        <f>+G36</f>
+        <v>38</v>
+      </c>
+      <c r="G37" s="102">
+        <v>54.5</v>
+      </c>
       <c r="H37" s="96"/>
       <c r="I37" s="96"/>
     </row>
@@ -16050,11 +16139,23 @@
       <c r="A38" s="96"/>
       <c r="B38" s="96"/>
       <c r="C38" s="96"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="96"/>
-      <c r="F38" s="96"/>
-      <c r="G38" s="96"/>
-      <c r="H38" s="96"/>
+      <c r="D38" s="100">
+        <f>+D37+1</f>
+        <v>4</v>
+      </c>
+      <c r="E38" s="110" t="s">
+        <v>612</v>
+      </c>
+      <c r="F38" s="102">
+        <f>+G37</f>
+        <v>54.5</v>
+      </c>
+      <c r="G38" s="96">
+        <v>59.56</v>
+      </c>
+      <c r="H38" s="110" t="s">
+        <v>613</v>
+      </c>
       <c r="I38" s="96"/>
     </row>
     <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -16069,11 +16170,19 @@
       <c r="I39" s="96"/>
     </row>
     <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="96"/>
-      <c r="B40" s="96"/>
-      <c r="C40" s="96"/>
-      <c r="D40" s="96"/>
-      <c r="E40" s="96"/>
+      <c r="A40" s="96">
+        <v>8</v>
+      </c>
+      <c r="B40" s="99">
+        <v>44111</v>
+      </c>
+      <c r="C40" s="109"/>
+      <c r="D40" s="100">
+        <v>1</v>
+      </c>
+      <c r="E40" s="110" t="s">
+        <v>614</v>
+      </c>
       <c r="F40" s="96"/>
       <c r="G40" s="96"/>
       <c r="H40" s="96"/>
@@ -16083,8 +16192,13 @@
       <c r="A41" s="96"/>
       <c r="B41" s="96"/>
       <c r="C41" s="96"/>
-      <c r="D41" s="96"/>
-      <c r="E41" s="96"/>
+      <c r="D41" s="100">
+        <f>+D40+1</f>
+        <v>2</v>
+      </c>
+      <c r="E41" s="110" t="s">
+        <v>615</v>
+      </c>
       <c r="F41" s="96"/>
       <c r="G41" s="96"/>
       <c r="H41" s="96"/>
@@ -16094,8 +16208,13 @@
       <c r="A42" s="96"/>
       <c r="B42" s="96"/>
       <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="96"/>
+      <c r="D42" s="100">
+        <f>+D41+1</f>
+        <v>3</v>
+      </c>
+      <c r="E42" s="110" t="s">
+        <v>616</v>
+      </c>
       <c r="F42" s="96"/>
       <c r="G42" s="96"/>
       <c r="H42" s="96"/>
@@ -16105,8 +16224,13 @@
       <c r="A43" s="96"/>
       <c r="B43" s="96"/>
       <c r="C43" s="96"/>
-      <c r="D43" s="96"/>
-      <c r="E43" s="96"/>
+      <c r="D43" s="100">
+        <f>+D42+1</f>
+        <v>4</v>
+      </c>
+      <c r="E43" s="110" t="s">
+        <v>617</v>
+      </c>
       <c r="F43" s="96"/>
       <c r="G43" s="96"/>
       <c r="H43" s="96"/>

</xml_diff>

<commit_message>
Latest changes Jatai 17/10/2020 3 am
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="683">
   <si>
     <t>Date</t>
   </si>
@@ -2038,19 +2038,55 @@
   </si>
   <si>
     <t>H2</t>
+  </si>
+  <si>
+    <t>5.5.16.1</t>
+  </si>
+  <si>
+    <t>5.5.17.1</t>
+  </si>
+  <si>
+    <t>5.5.18.1</t>
+  </si>
+  <si>
+    <t>5.5.19.1</t>
+  </si>
+  <si>
+    <t>5.5.20.1</t>
+  </si>
+  <si>
+    <t>5.5.21.1</t>
+  </si>
+  <si>
+    <t>5.5.22.1</t>
+  </si>
+  <si>
+    <t>5.5.23.1</t>
+  </si>
+  <si>
+    <t>5.5.24.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=bUMIAvgMFwM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="95" x14ac:knownFonts="1">
+  <fonts count="96" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -2655,77 +2691,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="92" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="93" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="92" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="93" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="92" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="93" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="93" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="94" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="93" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="93" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="94" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="94" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2734,17 +2771,17 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2759,19 +2796,19 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="92" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="93" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="93" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="94" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2786,17 +2823,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10597,8 +10634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15653,8 +15690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17466,17 +17503,25 @@
       <c r="B89" s="98">
         <v>44120</v>
       </c>
-      <c r="C89" s="95"/>
+      <c r="C89" s="95">
+        <v>57.17</v>
+      </c>
       <c r="D89" s="99">
         <v>1</v>
       </c>
       <c r="E89" s="124" t="s">
         <v>665</v>
       </c>
-      <c r="F89" s="95"/>
-      <c r="G89" s="95"/>
+      <c r="F89" s="95">
+        <v>4.25</v>
+      </c>
+      <c r="G89" s="101">
+        <v>20.3</v>
+      </c>
       <c r="H89" s="95"/>
-      <c r="I89" s="95"/>
+      <c r="I89" s="95" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="95"/>
@@ -17489,8 +17534,13 @@
       <c r="E90" s="124" t="s">
         <v>666</v>
       </c>
-      <c r="F90" s="95"/>
-      <c r="G90" s="95"/>
+      <c r="F90" s="101">
+        <f>+G89</f>
+        <v>20.3</v>
+      </c>
+      <c r="G90" s="95">
+        <v>42.44</v>
+      </c>
       <c r="H90" s="95"/>
       <c r="I90" s="95"/>
     </row>
@@ -17505,8 +17555,13 @@
       <c r="E91" s="124" t="s">
         <v>667</v>
       </c>
-      <c r="F91" s="95"/>
-      <c r="G91" s="95"/>
+      <c r="F91" s="95">
+        <f t="shared" ref="F91:F100" si="12">+G90</f>
+        <v>42.44</v>
+      </c>
+      <c r="G91" s="95">
+        <v>45.12</v>
+      </c>
       <c r="H91" s="95"/>
       <c r="I91" s="95"/>
     </row>
@@ -17521,8 +17576,13 @@
       <c r="E92" s="124" t="s">
         <v>668</v>
       </c>
-      <c r="F92" s="95"/>
-      <c r="G92" s="95"/>
+      <c r="F92" s="95">
+        <f t="shared" si="12"/>
+        <v>45.12</v>
+      </c>
+      <c r="G92" s="95">
+        <v>47.05</v>
+      </c>
       <c r="H92" s="95"/>
       <c r="I92" s="95"/>
     </row>
@@ -17537,8 +17597,13 @@
       <c r="E93" s="124" t="s">
         <v>669</v>
       </c>
-      <c r="F93" s="95"/>
-      <c r="G93" s="95"/>
+      <c r="F93" s="95">
+        <f t="shared" si="12"/>
+        <v>47.05</v>
+      </c>
+      <c r="G93" s="95">
+        <v>48.34</v>
+      </c>
       <c r="H93" s="95"/>
       <c r="I93" s="95"/>
     </row>
@@ -17547,14 +17612,19 @@
       <c r="B94" s="95"/>
       <c r="C94" s="95"/>
       <c r="D94" s="99">
-        <f t="shared" ref="D94:D97" si="12">+D93+1</f>
+        <f t="shared" ref="D94:D100" si="13">+D93+1</f>
         <v>6</v>
       </c>
       <c r="E94" s="124" t="s">
         <v>670</v>
       </c>
-      <c r="F94" s="95"/>
-      <c r="G94" s="95"/>
+      <c r="F94" s="95">
+        <f t="shared" si="12"/>
+        <v>48.34</v>
+      </c>
+      <c r="G94" s="95">
+        <v>50.15</v>
+      </c>
       <c r="H94" s="95"/>
       <c r="I94" s="95"/>
     </row>
@@ -17563,14 +17633,19 @@
       <c r="B95" s="95"/>
       <c r="C95" s="95"/>
       <c r="D95" s="99">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="E95" s="124" t="s">
         <v>671</v>
       </c>
-      <c r="F95" s="95"/>
-      <c r="G95" s="95"/>
+      <c r="F95" s="95">
+        <f t="shared" si="12"/>
+        <v>50.15</v>
+      </c>
+      <c r="G95" s="95">
+        <v>51.48</v>
+      </c>
       <c r="H95" s="95"/>
       <c r="I95" s="95"/>
     </row>
@@ -17579,12 +17654,19 @@
       <c r="B96" s="95"/>
       <c r="C96" s="95"/>
       <c r="D96" s="99">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="E96" s="127" t="s">
+        <v>673</v>
+      </c>
+      <c r="F96" s="95">
         <f t="shared" si="12"/>
-        <v>8</v>
-      </c>
-      <c r="E96" s="95"/>
-      <c r="F96" s="95"/>
-      <c r="G96" s="95"/>
+        <v>51.48</v>
+      </c>
+      <c r="G96" s="95">
+        <v>53.13</v>
+      </c>
       <c r="H96" s="95"/>
       <c r="I96" s="95"/>
     </row>
@@ -17593,12 +17675,19 @@
       <c r="B97" s="95"/>
       <c r="C97" s="95"/>
       <c r="D97" s="99">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="E97" s="127" t="s">
+        <v>674</v>
+      </c>
+      <c r="F97" s="95">
         <f t="shared" si="12"/>
-        <v>9</v>
-      </c>
-      <c r="E97" s="95"/>
-      <c r="F97" s="95"/>
-      <c r="G97" s="95"/>
+        <v>53.13</v>
+      </c>
+      <c r="G97" s="95">
+        <v>54.54</v>
+      </c>
       <c r="H97" s="95"/>
       <c r="I97" s="95"/>
     </row>
@@ -17606,10 +17695,20 @@
       <c r="A98" s="95"/>
       <c r="B98" s="95"/>
       <c r="C98" s="95"/>
-      <c r="D98" s="95"/>
-      <c r="E98" s="95"/>
-      <c r="F98" s="95"/>
-      <c r="G98" s="95"/>
+      <c r="D98" s="99">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="E98" s="127" t="s">
+        <v>675</v>
+      </c>
+      <c r="F98" s="95">
+        <f t="shared" si="12"/>
+        <v>54.54</v>
+      </c>
+      <c r="G98" s="95">
+        <v>56.17</v>
+      </c>
       <c r="H98" s="95"/>
       <c r="I98" s="95"/>
     </row>
@@ -17617,7 +17716,7 @@
       <c r="A99" s="95"/>
       <c r="B99" s="95"/>
       <c r="C99" s="95"/>
-      <c r="D99" s="95"/>
+      <c r="D99" s="99"/>
       <c r="E99" s="95"/>
       <c r="F99" s="95"/>
       <c r="G99" s="95"/>
@@ -17625,11 +17724,19 @@
       <c r="I99" s="95"/>
     </row>
     <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A100" s="95"/>
-      <c r="B100" s="95"/>
+      <c r="A100" s="95">
+        <v>18</v>
+      </c>
+      <c r="B100" s="98">
+        <v>44121</v>
+      </c>
       <c r="C100" s="95"/>
-      <c r="D100" s="95"/>
-      <c r="E100" s="95"/>
+      <c r="D100" s="99">
+        <v>1</v>
+      </c>
+      <c r="E100" s="127" t="s">
+        <v>676</v>
+      </c>
       <c r="F100" s="95"/>
       <c r="G100" s="95"/>
       <c r="H100" s="95"/>
@@ -17639,8 +17746,13 @@
       <c r="A101" s="95"/>
       <c r="B101" s="95"/>
       <c r="C101" s="95"/>
-      <c r="D101" s="95"/>
-      <c r="E101" s="95"/>
+      <c r="D101" s="99">
+        <f>+D100+1</f>
+        <v>2</v>
+      </c>
+      <c r="E101" s="127" t="s">
+        <v>677</v>
+      </c>
       <c r="F101" s="95"/>
       <c r="G101" s="95"/>
       <c r="H101" s="95"/>
@@ -17650,8 +17762,13 @@
       <c r="A102" s="95"/>
       <c r="B102" s="95"/>
       <c r="C102" s="95"/>
-      <c r="D102" s="95"/>
-      <c r="E102" s="95"/>
+      <c r="D102" s="99">
+        <f>+D101+1</f>
+        <v>3</v>
+      </c>
+      <c r="E102" s="127" t="s">
+        <v>678</v>
+      </c>
       <c r="F102" s="95"/>
       <c r="G102" s="95"/>
       <c r="H102" s="95"/>
@@ -17661,8 +17778,13 @@
       <c r="A103" s="95"/>
       <c r="B103" s="95"/>
       <c r="C103" s="95"/>
-      <c r="D103" s="95"/>
-      <c r="E103" s="95"/>
+      <c r="D103" s="99">
+        <f>+D102+1</f>
+        <v>4</v>
+      </c>
+      <c r="E103" s="127" t="s">
+        <v>679</v>
+      </c>
       <c r="F103" s="95"/>
       <c r="G103" s="95"/>
       <c r="H103" s="95"/>
@@ -17672,8 +17794,13 @@
       <c r="A104" s="95"/>
       <c r="B104" s="95"/>
       <c r="C104" s="95"/>
-      <c r="D104" s="95"/>
-      <c r="E104" s="95"/>
+      <c r="D104" s="99">
+        <f>+D103+1</f>
+        <v>5</v>
+      </c>
+      <c r="E104" s="127" t="s">
+        <v>680</v>
+      </c>
       <c r="F104" s="95"/>
       <c r="G104" s="95"/>
       <c r="H104" s="95"/>
@@ -17683,8 +17810,13 @@
       <c r="A105" s="95"/>
       <c r="B105" s="95"/>
       <c r="C105" s="95"/>
-      <c r="D105" s="95"/>
-      <c r="E105" s="95"/>
+      <c r="D105" s="99">
+        <f t="shared" ref="D105" si="14">+D104+1</f>
+        <v>6</v>
+      </c>
+      <c r="E105" s="127" t="s">
+        <v>681</v>
+      </c>
       <c r="F105" s="95"/>
       <c r="G105" s="95"/>
       <c r="H105" s="95"/>

</xml_diff>

<commit_message>
TS Jatai changes 25/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="757">
   <si>
     <t>Date</t>
   </si>
@@ -2263,19 +2263,58 @@
   </si>
   <si>
     <t>6.1.2.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iIs3nEGIVz4</t>
+  </si>
+  <si>
+    <t>6.1.3.1</t>
+  </si>
+  <si>
+    <t>6.1.3.2</t>
+  </si>
+  <si>
+    <t>6.1.4.1</t>
+  </si>
+  <si>
+    <t>6.1.5.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Lxar3bTRTH4</t>
+  </si>
+  <si>
+    <t>6.1.4.8</t>
+  </si>
+  <si>
+    <t>6.1.4.7</t>
+  </si>
+  <si>
+    <t>6.1.6.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="103" x14ac:knownFonts="1">
+  <fonts count="105" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -2928,77 +2967,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="100" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="102" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="100" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="102" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="100" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="102" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="71" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="101" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="103" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="101" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="101" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="103" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="103" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3006,18 +3047,18 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3031,20 +3072,20 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="100" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="102" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="101" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="103" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3058,33 +3099,34 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18966,7 +19008,7 @@
         <v>729</v>
       </c>
       <c r="F147" s="101">
-        <f t="shared" ref="F147:G162" si="23">+G146</f>
+        <f t="shared" ref="F147:F162" si="23">+G146</f>
         <v>27.11</v>
       </c>
       <c r="G147" s="101">
@@ -20115,7 +20157,7 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20197,26 +20239,44 @@
       <c r="B4" s="137">
         <v>44127</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
+      <c r="C4" s="136">
+        <v>53.14</v>
+      </c>
+      <c r="D4" s="136">
+        <v>1</v>
+      </c>
       <c r="E4" s="136" t="s">
         <v>746</v>
       </c>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
+      <c r="F4" s="138">
+        <v>2.1</v>
+      </c>
+      <c r="G4" s="138">
+        <v>28.48</v>
+      </c>
       <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
+      <c r="I4" s="136" t="s">
+        <v>748</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="136"/>
       <c r="B5" s="136"/>
       <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
+      <c r="D5" s="136">
+        <f>+D4+1</f>
+        <v>2</v>
+      </c>
       <c r="E5" s="136" t="s">
         <v>747</v>
       </c>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
+      <c r="F5" s="138">
+        <f>+G4</f>
+        <v>28.48</v>
+      </c>
+      <c r="G5" s="138">
+        <v>49.26</v>
+      </c>
       <c r="H5" s="136"/>
       <c r="I5" s="136"/>
     </row>
@@ -20224,11 +20284,23 @@
       <c r="A6" s="136"/>
       <c r="B6" s="136"/>
       <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
+      <c r="D6" s="136">
+        <f>+D5+1</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="139" t="s">
+        <v>749</v>
+      </c>
+      <c r="F6" s="138">
+        <f>+G5</f>
+        <v>49.26</v>
+      </c>
+      <c r="G6" s="138">
+        <v>52.3</v>
+      </c>
+      <c r="H6" s="140" t="s">
+        <v>749</v>
+      </c>
       <c r="I6" s="136"/>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20237,31 +20309,59 @@
       <c r="C7" s="136"/>
       <c r="D7" s="136"/>
       <c r="E7" s="136"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="136"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
       <c r="H7" s="136"/>
       <c r="I7" s="136"/>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="136"/>
-      <c r="B8" s="136"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
+      <c r="A8" s="136">
+        <v>2</v>
+      </c>
+      <c r="B8" s="137">
+        <v>44128</v>
+      </c>
+      <c r="C8" s="136">
+        <v>51.28</v>
+      </c>
+      <c r="D8" s="136">
+        <v>1</v>
+      </c>
+      <c r="E8" s="140" t="s">
+        <v>750</v>
+      </c>
+      <c r="F8" s="138">
+        <v>4.08</v>
+      </c>
+      <c r="G8" s="138">
+        <v>28</v>
+      </c>
       <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
+      <c r="I8" s="136" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="136"/>
       <c r="B9" s="136"/>
       <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
-      <c r="F9" s="136"/>
-      <c r="G9" s="136"/>
-      <c r="H9" s="136"/>
+      <c r="D9" s="136">
+        <f>+D8+1</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="140" t="s">
+        <v>751</v>
+      </c>
+      <c r="F9" s="138">
+        <f>+G8</f>
+        <v>28</v>
+      </c>
+      <c r="G9" s="136">
+        <v>49.5</v>
+      </c>
+      <c r="H9" s="140" t="s">
+        <v>755</v>
+      </c>
       <c r="I9" s="136"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20269,18 +20369,25 @@
       <c r="B10" s="136"/>
       <c r="C10" s="136"/>
       <c r="D10" s="136"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="136"/>
+      <c r="F10" s="138"/>
       <c r="G10" s="136"/>
       <c r="H10" s="136"/>
       <c r="I10" s="136"/>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="136"/>
-      <c r="B11" s="136"/>
+      <c r="A11" s="136">
+        <v>2</v>
+      </c>
+      <c r="B11" s="137">
+        <v>44129</v>
+      </c>
       <c r="C11" s="136"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="136"/>
+      <c r="D11" s="136">
+        <v>1</v>
+      </c>
+      <c r="E11" s="140" t="s">
+        <v>754</v>
+      </c>
       <c r="F11" s="136"/>
       <c r="G11" s="136"/>
       <c r="H11" s="136"/>
@@ -20290,8 +20397,13 @@
       <c r="A12" s="136"/>
       <c r="B12" s="136"/>
       <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="136"/>
+      <c r="D12" s="136">
+        <f>+D11+1</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="140" t="s">
+        <v>752</v>
+      </c>
       <c r="F12" s="136"/>
       <c r="G12" s="136"/>
       <c r="H12" s="136"/>
@@ -20301,8 +20413,13 @@
       <c r="A13" s="136"/>
       <c r="B13" s="136"/>
       <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
+      <c r="D13" s="136">
+        <f>+D12+1</f>
+        <v>3</v>
+      </c>
+      <c r="E13" s="140" t="s">
+        <v>756</v>
+      </c>
       <c r="F13" s="136"/>
       <c r="G13" s="136"/>
       <c r="H13" s="136"/>

</xml_diff>

<commit_message>
Veda Lecutres +all edits Padams 27/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="770">
   <si>
     <t>Date</t>
   </si>
@@ -2323,19 +2323,31 @@
   </si>
   <si>
     <t>6.2.1.1</t>
+  </si>
+  <si>
+    <t>1.00.11</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=mcXc1D39dNE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="107" x14ac:knownFonts="1">
+  <fonts count="108" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3012,77 +3024,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="104" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="104" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="104" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="105" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="71" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="105" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="106" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="105" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="105" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="106" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="106" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3091,17 +3104,17 @@
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3116,19 +3129,19 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="104" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="105" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="105" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="106" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3143,40 +3156,40 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -20208,7 +20221,7 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20615,19 +20628,25 @@
       <c r="B20" s="136">
         <v>44131</v>
       </c>
-      <c r="C20" s="135"/>
+      <c r="C20" s="145" t="s">
+        <v>768</v>
+      </c>
       <c r="D20" s="141">
         <v>1</v>
       </c>
       <c r="E20" s="144" t="s">
         <v>765</v>
       </c>
-      <c r="F20" s="135"/>
+      <c r="F20" s="137">
+        <v>3.2</v>
+      </c>
       <c r="G20" s="137">
-        <v>0</v>
+        <v>19.18</v>
       </c>
       <c r="H20" s="135"/>
-      <c r="I20" s="135"/>
+      <c r="I20" s="135" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="135"/>
@@ -20642,9 +20661,11 @@
       </c>
       <c r="F21" s="137">
         <f>+G20</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="135"/>
+        <v>19.18</v>
+      </c>
+      <c r="G21" s="135">
+        <v>37.549999999999997</v>
+      </c>
       <c r="H21" s="135"/>
       <c r="I21" s="135"/>
     </row>
@@ -20661,9 +20682,11 @@
       </c>
       <c r="F22" s="137">
         <f>+G21</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="135"/>
+        <v>37.549999999999997</v>
+      </c>
+      <c r="G22" s="135">
+        <v>59.35</v>
+      </c>
       <c r="H22" s="135"/>
       <c r="I22" s="135"/>
     </row>

</xml_diff>

<commit_message>
TS 3.1 PP, GS change TTD etc. 01/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="804">
   <si>
     <t>Date</t>
   </si>
@@ -2398,19 +2398,58 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=bbQm9RvFTYw</t>
+  </si>
+  <si>
+    <t>1.00.06</t>
+  </si>
+  <si>
+    <t>6.3.2.4</t>
+  </si>
+  <si>
+    <t>6.3.2.5</t>
+  </si>
+  <si>
+    <t>6.3.3.1</t>
+  </si>
+  <si>
+    <t>6.3.4.1</t>
+  </si>
+  <si>
+    <t>6.3.4.8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-HSnXsFVpkk</t>
+  </si>
+  <si>
+    <t>6.3.4.9</t>
+  </si>
+  <si>
+    <t>6.3.5.1</t>
+  </si>
+  <si>
+    <t>6.3.6.1</t>
+  </si>
+  <si>
+    <t>6.3.7.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="112" x14ac:knownFonts="1">
+  <fonts count="113" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3117,77 +3156,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="108" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="109" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="110" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="109" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="110" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="108" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="109" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="110" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="110" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="111" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="110" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="110" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="111" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="111" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3196,17 +3236,17 @@
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3221,19 +3261,19 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="109" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="110" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="110" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="111" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3248,44 +3288,44 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -20318,8 +20358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21174,7 +21214,9 @@
       <c r="G41" s="134">
         <v>59.55</v>
       </c>
-      <c r="H41" s="134"/>
+      <c r="H41" s="151" t="s">
+        <v>794</v>
+      </c>
       <c r="I41" s="134"/>
     </row>
     <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -21189,24 +21231,50 @@
       <c r="I42" s="134"/>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="134"/>
-      <c r="B43" s="134"/>
-      <c r="C43" s="134"/>
-      <c r="D43" s="134"/>
-      <c r="E43" s="134"/>
-      <c r="F43" s="134"/>
-      <c r="G43" s="134"/>
+      <c r="A43" s="134">
+        <v>10</v>
+      </c>
+      <c r="B43" s="135">
+        <v>44136</v>
+      </c>
+      <c r="C43" s="151" t="s">
+        <v>793</v>
+      </c>
+      <c r="D43" s="140">
+        <v>1</v>
+      </c>
+      <c r="E43" s="151" t="s">
+        <v>795</v>
+      </c>
+      <c r="F43" s="134">
+        <v>3.12</v>
+      </c>
+      <c r="G43" s="134">
+        <v>10.16</v>
+      </c>
       <c r="H43" s="134"/>
-      <c r="I43" s="134"/>
+      <c r="I43" s="134" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="134"/>
       <c r="B44" s="134"/>
       <c r="C44" s="134"/>
-      <c r="D44" s="134"/>
-      <c r="E44" s="134"/>
-      <c r="F44" s="134"/>
-      <c r="G44" s="134"/>
+      <c r="D44" s="140">
+        <f>+D43+1</f>
+        <v>2</v>
+      </c>
+      <c r="E44" s="151" t="s">
+        <v>796</v>
+      </c>
+      <c r="F44" s="134">
+        <f>+G43</f>
+        <v>10.16</v>
+      </c>
+      <c r="G44" s="134">
+        <v>33.549999999999997</v>
+      </c>
       <c r="H44" s="134"/>
       <c r="I44" s="134"/>
     </row>
@@ -21214,18 +21282,30 @@
       <c r="A45" s="134"/>
       <c r="B45" s="134"/>
       <c r="C45" s="134"/>
-      <c r="D45" s="134"/>
-      <c r="E45" s="134"/>
-      <c r="F45" s="134"/>
-      <c r="G45" s="134"/>
-      <c r="H45" s="134"/>
+      <c r="D45" s="140">
+        <f>+D44+1</f>
+        <v>3</v>
+      </c>
+      <c r="E45" s="151" t="s">
+        <v>797</v>
+      </c>
+      <c r="F45" s="134">
+        <f t="shared" ref="F45:F46" si="3">+G44</f>
+        <v>33.549999999999997</v>
+      </c>
+      <c r="G45" s="134">
+        <v>59.05</v>
+      </c>
+      <c r="H45" s="151" t="s">
+        <v>798</v>
+      </c>
       <c r="I45" s="134"/>
     </row>
     <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="134"/>
       <c r="B46" s="134"/>
       <c r="C46" s="134"/>
-      <c r="D46" s="134"/>
+      <c r="D46" s="140"/>
       <c r="E46" s="134"/>
       <c r="F46" s="134"/>
       <c r="G46" s="134"/>
@@ -21233,11 +21313,19 @@
       <c r="I46" s="134"/>
     </row>
     <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="134"/>
-      <c r="B47" s="134"/>
+      <c r="A47" s="151">
+        <v>11</v>
+      </c>
+      <c r="B47" s="135">
+        <v>44137</v>
+      </c>
       <c r="C47" s="134"/>
-      <c r="D47" s="134"/>
-      <c r="E47" s="134"/>
+      <c r="D47" s="140">
+        <v>1</v>
+      </c>
+      <c r="E47" s="151" t="s">
+        <v>800</v>
+      </c>
       <c r="F47" s="134"/>
       <c r="G47" s="134"/>
       <c r="H47" s="134"/>
@@ -21247,8 +21335,13 @@
       <c r="A48" s="134"/>
       <c r="B48" s="134"/>
       <c r="C48" s="134"/>
-      <c r="D48" s="134"/>
-      <c r="E48" s="134"/>
+      <c r="D48" s="140">
+        <f>+D47+1</f>
+        <v>2</v>
+      </c>
+      <c r="E48" s="151" t="s">
+        <v>801</v>
+      </c>
       <c r="F48" s="134"/>
       <c r="G48" s="134"/>
       <c r="H48" s="134"/>
@@ -21258,8 +21351,13 @@
       <c r="A49" s="134"/>
       <c r="B49" s="134"/>
       <c r="C49" s="134"/>
-      <c r="D49" s="134"/>
-      <c r="E49" s="134"/>
+      <c r="D49" s="140">
+        <f>+D48+1</f>
+        <v>3</v>
+      </c>
+      <c r="E49" s="151" t="s">
+        <v>802</v>
+      </c>
       <c r="F49" s="134"/>
       <c r="G49" s="134"/>
       <c r="H49" s="134"/>
@@ -21269,8 +21367,13 @@
       <c r="A50" s="134"/>
       <c r="B50" s="134"/>
       <c r="C50" s="134"/>
-      <c r="D50" s="134"/>
-      <c r="E50" s="134"/>
+      <c r="D50" s="140">
+        <f>+D49+1</f>
+        <v>4</v>
+      </c>
+      <c r="E50" s="151" t="s">
+        <v>803</v>
+      </c>
       <c r="F50" s="134"/>
       <c r="G50" s="134"/>
       <c r="H50" s="134"/>

</xml_diff>

<commit_message>
TS 3.1 PP Tamil and Raja files 02/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="811">
   <si>
     <t>Date</t>
   </si>
@@ -2431,19 +2431,46 @@
   </si>
   <si>
     <t>6.3.7.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qpiYD5UnFa4</t>
+  </si>
+  <si>
+    <t>6.3.8.1</t>
+  </si>
+  <si>
+    <t>6.3.8.3</t>
+  </si>
+  <si>
+    <t>6.3.9.1</t>
+  </si>
+  <si>
+    <t>6.3.10.1</t>
+  </si>
+  <si>
+    <t>6.3.11.1</t>
+  </si>
+  <si>
+    <t>6.3.12.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="113" x14ac:knownFonts="1">
+  <fonts count="114" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3156,77 +3183,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="110" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="111" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="110" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="111" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="110" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="111" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="87" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="87" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="111" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="112" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="111" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="111" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="112" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="112" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3235,17 +3263,17 @@
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3260,19 +3288,19 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="110" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="111" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="111" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="112" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3287,44 +3315,44 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -20359,7 +20387,7 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21290,7 +21318,7 @@
         <v>797</v>
       </c>
       <c r="F45" s="134">
-        <f t="shared" ref="F45:F46" si="3">+G44</f>
+        <f t="shared" ref="F45" si="3">+G44</f>
         <v>33.549999999999997</v>
       </c>
       <c r="G45" s="134">
@@ -21319,31 +21347,37 @@
       <c r="B47" s="135">
         <v>44137</v>
       </c>
-      <c r="C47" s="134"/>
-      <c r="D47" s="140">
-        <v>1</v>
+      <c r="C47" s="152" t="s">
+        <v>695</v>
       </c>
       <c r="E47" s="151" t="s">
         <v>800</v>
       </c>
-      <c r="F47" s="134"/>
-      <c r="G47" s="134"/>
+      <c r="F47" s="134">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="G47" s="134">
+        <v>7.55</v>
+      </c>
       <c r="H47" s="134"/>
-      <c r="I47" s="134"/>
+      <c r="I47" s="134" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="134"/>
       <c r="B48" s="134"/>
       <c r="C48" s="134"/>
-      <c r="D48" s="140">
-        <f>+D47+1</f>
-        <v>2</v>
-      </c>
       <c r="E48" s="151" t="s">
         <v>801</v>
       </c>
-      <c r="F48" s="134"/>
-      <c r="G48" s="134"/>
+      <c r="F48" s="134">
+        <f>+G47</f>
+        <v>7.55</v>
+      </c>
+      <c r="G48" s="134">
+        <v>20.22</v>
+      </c>
       <c r="H48" s="134"/>
       <c r="I48" s="134"/>
     </row>
@@ -21351,15 +21385,16 @@
       <c r="A49" s="134"/>
       <c r="B49" s="134"/>
       <c r="C49" s="134"/>
-      <c r="D49" s="140">
-        <f>+D48+1</f>
-        <v>3</v>
-      </c>
       <c r="E49" s="151" t="s">
         <v>802</v>
       </c>
-      <c r="F49" s="134"/>
-      <c r="G49" s="134"/>
+      <c r="F49" s="134">
+        <f t="shared" ref="F49:F51" si="4">+G48</f>
+        <v>20.22</v>
+      </c>
+      <c r="G49" s="134">
+        <v>32.18</v>
+      </c>
       <c r="H49" s="134"/>
       <c r="I49" s="134"/>
     </row>
@@ -21367,15 +21402,16 @@
       <c r="A50" s="134"/>
       <c r="B50" s="134"/>
       <c r="C50" s="134"/>
-      <c r="D50" s="140">
-        <f>+D49+1</f>
-        <v>4</v>
-      </c>
       <c r="E50" s="151" t="s">
         <v>803</v>
       </c>
-      <c r="F50" s="134"/>
-      <c r="G50" s="134"/>
+      <c r="F50" s="134">
+        <f t="shared" si="4"/>
+        <v>32.18</v>
+      </c>
+      <c r="G50" s="134">
+        <v>49.37</v>
+      </c>
       <c r="H50" s="134"/>
       <c r="I50" s="134"/>
     </row>
@@ -21383,11 +21419,23 @@
       <c r="A51" s="134"/>
       <c r="B51" s="134"/>
       <c r="C51" s="134"/>
-      <c r="D51" s="134"/>
-      <c r="E51" s="134"/>
-      <c r="F51" s="134"/>
-      <c r="G51" s="134"/>
-      <c r="H51" s="134"/>
+      <c r="D51" s="140">
+        <f>+D56+1</f>
+        <v>5</v>
+      </c>
+      <c r="E51" s="152" t="s">
+        <v>805</v>
+      </c>
+      <c r="F51" s="134">
+        <f t="shared" si="4"/>
+        <v>49.37</v>
+      </c>
+      <c r="G51" s="134">
+        <v>59.49</v>
+      </c>
+      <c r="H51" s="152" t="s">
+        <v>806</v>
+      </c>
       <c r="I51" s="134"/>
     </row>
     <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -21402,11 +21450,19 @@
       <c r="I52" s="134"/>
     </row>
     <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="134"/>
-      <c r="B53" s="134"/>
+      <c r="A53" s="134">
+        <v>12</v>
+      </c>
+      <c r="B53" s="135">
+        <v>44138</v>
+      </c>
       <c r="C53" s="134"/>
-      <c r="D53" s="134"/>
-      <c r="E53" s="134"/>
+      <c r="D53" s="140">
+        <v>1</v>
+      </c>
+      <c r="E53" s="152" t="s">
+        <v>807</v>
+      </c>
       <c r="F53" s="134"/>
       <c r="G53" s="134"/>
       <c r="H53" s="134"/>
@@ -21416,8 +21472,13 @@
       <c r="A54" s="134"/>
       <c r="B54" s="134"/>
       <c r="C54" s="134"/>
-      <c r="D54" s="134"/>
-      <c r="E54" s="134"/>
+      <c r="D54" s="140">
+        <f>+D53+1</f>
+        <v>2</v>
+      </c>
+      <c r="E54" s="152" t="s">
+        <v>808</v>
+      </c>
       <c r="F54" s="134"/>
       <c r="G54" s="134"/>
       <c r="H54" s="134"/>
@@ -21427,8 +21488,13 @@
       <c r="A55" s="134"/>
       <c r="B55" s="134"/>
       <c r="C55" s="134"/>
-      <c r="D55" s="134"/>
-      <c r="E55" s="134"/>
+      <c r="D55" s="140">
+        <f>+D54+1</f>
+        <v>3</v>
+      </c>
+      <c r="E55" s="152" t="s">
+        <v>809</v>
+      </c>
       <c r="F55" s="134"/>
       <c r="G55" s="134"/>
       <c r="H55" s="134"/>
@@ -21438,8 +21504,13 @@
       <c r="A56" s="134"/>
       <c r="B56" s="134"/>
       <c r="C56" s="134"/>
-      <c r="D56" s="134"/>
-      <c r="E56" s="134"/>
+      <c r="D56" s="140">
+        <f>+D55+1</f>
+        <v>4</v>
+      </c>
+      <c r="E56" s="152" t="s">
+        <v>810</v>
+      </c>
       <c r="F56" s="134"/>
       <c r="G56" s="134"/>
       <c r="H56" s="134"/>

</xml_diff>

<commit_message>
Jata files changes 03/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="817">
   <si>
     <t>Date</t>
   </si>
@@ -2452,19 +2452,43 @@
   </si>
   <si>
     <t>6.3.12.1</t>
+  </si>
+  <si>
+    <t>1.07.30</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rnypIDwKaHU</t>
+  </si>
+  <si>
+    <t>1.06.26</t>
+  </si>
+  <si>
+    <t>6.4.1.1</t>
+  </si>
+  <si>
+    <t>6.4.2.1</t>
+  </si>
+  <si>
+    <t>6.4.3.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="114" x14ac:knownFonts="1">
+  <fonts count="115" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3183,77 +3207,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="111" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="112" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="111" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="112" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="111" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="112" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="87" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="87" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="112" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="113" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="112" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="112" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="113" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="113" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3262,17 +3287,17 @@
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3287,19 +3312,19 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="111" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="112" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="112" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="113" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3314,44 +3339,44 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -20386,8 +20411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21456,17 +21481,25 @@
       <c r="B53" s="135">
         <v>44138</v>
       </c>
-      <c r="C53" s="134"/>
+      <c r="C53" s="153" t="s">
+        <v>811</v>
+      </c>
       <c r="D53" s="140">
         <v>1</v>
       </c>
       <c r="E53" s="152" t="s">
         <v>807</v>
       </c>
-      <c r="F53" s="134"/>
-      <c r="G53" s="134"/>
+      <c r="F53" s="136">
+        <v>6.3</v>
+      </c>
+      <c r="G53" s="134">
+        <v>8.52</v>
+      </c>
       <c r="H53" s="134"/>
-      <c r="I53" s="134"/>
+      <c r="I53" s="134" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="134"/>
@@ -21479,8 +21512,13 @@
       <c r="E54" s="152" t="s">
         <v>808</v>
       </c>
-      <c r="F54" s="134"/>
-      <c r="G54" s="134"/>
+      <c r="F54" s="136">
+        <f>+G53</f>
+        <v>8.52</v>
+      </c>
+      <c r="G54" s="134">
+        <v>27.2</v>
+      </c>
       <c r="H54" s="134"/>
       <c r="I54" s="134"/>
     </row>
@@ -21495,8 +21533,13 @@
       <c r="E55" s="152" t="s">
         <v>809</v>
       </c>
-      <c r="F55" s="134"/>
-      <c r="G55" s="134"/>
+      <c r="F55" s="136">
+        <f t="shared" ref="F55:F56" si="5">+G54</f>
+        <v>27.2</v>
+      </c>
+      <c r="G55" s="134">
+        <v>46.42</v>
+      </c>
       <c r="H55" s="134"/>
       <c r="I55" s="134"/>
     </row>
@@ -21511,8 +21554,13 @@
       <c r="E56" s="152" t="s">
         <v>810</v>
       </c>
-      <c r="F56" s="134"/>
-      <c r="G56" s="134"/>
+      <c r="F56" s="136">
+        <f t="shared" si="5"/>
+        <v>46.42</v>
+      </c>
+      <c r="G56" s="153" t="s">
+        <v>813</v>
+      </c>
       <c r="H56" s="134"/>
       <c r="I56" s="134"/>
     </row>
@@ -21528,11 +21576,19 @@
       <c r="I57" s="134"/>
     </row>
     <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A58" s="134"/>
-      <c r="B58" s="134"/>
+      <c r="A58" s="134">
+        <v>13</v>
+      </c>
+      <c r="B58" s="135">
+        <v>44139</v>
+      </c>
       <c r="C58" s="134"/>
-      <c r="D58" s="134"/>
-      <c r="E58" s="134"/>
+      <c r="D58" s="140">
+        <v>1</v>
+      </c>
+      <c r="E58" s="153" t="s">
+        <v>814</v>
+      </c>
       <c r="F58" s="134"/>
       <c r="G58" s="134"/>
       <c r="H58" s="134"/>
@@ -21542,8 +21598,13 @@
       <c r="A59" s="134"/>
       <c r="B59" s="134"/>
       <c r="C59" s="134"/>
-      <c r="D59" s="134"/>
-      <c r="E59" s="134"/>
+      <c r="D59" s="140">
+        <f>+D58+1</f>
+        <v>2</v>
+      </c>
+      <c r="E59" s="153" t="s">
+        <v>815</v>
+      </c>
       <c r="F59" s="134"/>
       <c r="G59" s="134"/>
       <c r="H59" s="134"/>
@@ -21553,8 +21614,13 @@
       <c r="A60" s="134"/>
       <c r="B60" s="134"/>
       <c r="C60" s="134"/>
-      <c r="D60" s="134"/>
-      <c r="E60" s="134"/>
+      <c r="D60" s="140">
+        <f>+D59+1</f>
+        <v>3</v>
+      </c>
+      <c r="E60" s="153" t="s">
+        <v>816</v>
+      </c>
       <c r="F60" s="134"/>
       <c r="G60" s="134"/>
       <c r="H60" s="134"/>
@@ -21564,7 +21630,10 @@
       <c r="A61" s="134"/>
       <c r="B61" s="134"/>
       <c r="C61" s="134"/>
-      <c r="D61" s="134"/>
+      <c r="D61" s="140">
+        <f>+D60+1</f>
+        <v>4</v>
+      </c>
       <c r="E61" s="134"/>
       <c r="F61" s="134"/>
       <c r="G61" s="134"/>

</xml_diff>

<commit_message>
TB 1.1-1.4 Tamil 04/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="819">
   <si>
     <t>Date</t>
   </si>
@@ -2470,19 +2470,31 @@
   </si>
   <si>
     <t>6.4.3.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rmg81CDC2z0</t>
+  </si>
+  <si>
+    <t>6.4.4.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="115" x14ac:knownFonts="1">
+  <fonts count="116" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3207,77 +3219,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="112" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="112" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="113" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="112" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="113" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="112" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="112" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="113" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="105" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="105" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="113" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="114" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="113" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="113" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="114" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="114" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3286,17 +3299,17 @@
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3311,19 +3324,19 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="112" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="113" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="113" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="114" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3338,44 +3351,44 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -20412,7 +20425,7 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21582,17 +21595,25 @@
       <c r="B58" s="135">
         <v>44139</v>
       </c>
-      <c r="C58" s="134"/>
+      <c r="C58" s="134">
+        <v>59.22</v>
+      </c>
       <c r="D58" s="140">
         <v>1</v>
       </c>
       <c r="E58" s="153" t="s">
         <v>814</v>
       </c>
-      <c r="F58" s="134"/>
-      <c r="G58" s="134"/>
+      <c r="F58" s="134">
+        <v>2.02</v>
+      </c>
+      <c r="G58" s="134">
+        <v>18.13</v>
+      </c>
       <c r="H58" s="134"/>
-      <c r="I58" s="134"/>
+      <c r="I58" s="134" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="134"/>
@@ -21605,8 +21626,13 @@
       <c r="E59" s="153" t="s">
         <v>815</v>
       </c>
-      <c r="F59" s="134"/>
-      <c r="G59" s="134"/>
+      <c r="F59" s="134">
+        <f>+G58</f>
+        <v>18.13</v>
+      </c>
+      <c r="G59" s="134">
+        <v>39.56</v>
+      </c>
       <c r="H59" s="134"/>
       <c r="I59" s="134"/>
     </row>
@@ -21621,8 +21647,13 @@
       <c r="E60" s="153" t="s">
         <v>816</v>
       </c>
-      <c r="F60" s="134"/>
-      <c r="G60" s="134"/>
+      <c r="F60" s="136">
+        <f t="shared" ref="F60:F61" si="6">+G59</f>
+        <v>39.56</v>
+      </c>
+      <c r="G60" s="136">
+        <v>55.2</v>
+      </c>
       <c r="H60" s="134"/>
       <c r="I60" s="134"/>
     </row>
@@ -21634,9 +21665,16 @@
         <f>+D60+1</f>
         <v>4</v>
       </c>
-      <c r="E61" s="134"/>
-      <c r="F61" s="134"/>
-      <c r="G61" s="134"/>
+      <c r="E61" s="154" t="s">
+        <v>818</v>
+      </c>
+      <c r="F61" s="136">
+        <f t="shared" si="6"/>
+        <v>55.2</v>
+      </c>
+      <c r="G61" s="136">
+        <v>58.4</v>
+      </c>
       <c r="H61" s="134"/>
       <c r="I61" s="134"/>
     </row>

</xml_diff>

<commit_message>
TS Jatai  working 06/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -15,11 +15,12 @@
     <sheet name="Kandam6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="828">
   <si>
     <t>Date</t>
   </si>
@@ -2500,6 +2501,9 @@
   </si>
   <si>
     <t>6.4.10.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vVRTcBM6bW0</t>
   </si>
 </sst>
 </file>
@@ -20456,7 +20460,7 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21785,7 +21789,7 @@
         <f>+G64</f>
         <v>37.28</v>
       </c>
-      <c r="G65" s="134">
+      <c r="G65" s="136">
         <v>51.1</v>
       </c>
       <c r="H65" s="134"/>
@@ -21809,17 +21813,25 @@
       <c r="B67" s="135">
         <v>44141</v>
       </c>
-      <c r="C67" s="134"/>
+      <c r="C67" s="134">
+        <v>52.11</v>
+      </c>
       <c r="D67" s="140">
         <v>1</v>
       </c>
       <c r="E67" s="155" t="s">
         <v>823</v>
       </c>
-      <c r="F67" s="136"/>
-      <c r="G67" s="134"/>
+      <c r="F67" s="136">
+        <v>1.02</v>
+      </c>
+      <c r="G67" s="134">
+        <v>11.47</v>
+      </c>
       <c r="H67" s="134"/>
-      <c r="I67" s="134"/>
+      <c r="I67" s="134" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="134"/>
@@ -21832,8 +21844,13 @@
       <c r="E68" s="155" t="s">
         <v>824</v>
       </c>
-      <c r="F68" s="134"/>
-      <c r="G68" s="134"/>
+      <c r="F68" s="134">
+        <f>+G67</f>
+        <v>11.47</v>
+      </c>
+      <c r="G68" s="134">
+        <v>21.45</v>
+      </c>
       <c r="H68" s="134"/>
       <c r="I68" s="134"/>
     </row>
@@ -21848,8 +21865,13 @@
       <c r="E69" s="155" t="s">
         <v>825</v>
       </c>
-      <c r="F69" s="134"/>
-      <c r="G69" s="134"/>
+      <c r="F69" s="134">
+        <f t="shared" ref="F69:F70" si="7">+G68</f>
+        <v>21.45</v>
+      </c>
+      <c r="G69" s="134">
+        <v>37.07</v>
+      </c>
       <c r="H69" s="134"/>
       <c r="I69" s="134"/>
     </row>
@@ -21864,8 +21886,13 @@
       <c r="E70" s="155" t="s">
         <v>826</v>
       </c>
-      <c r="F70" s="134"/>
-      <c r="G70" s="134"/>
+      <c r="F70" s="134">
+        <f t="shared" si="7"/>
+        <v>37.07</v>
+      </c>
+      <c r="G70" s="134">
+        <v>51.33</v>
+      </c>
       <c r="H70" s="134"/>
       <c r="I70" s="134"/>
     </row>

</xml_diff>

<commit_message>
Jatai working files with U rule 08/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -15,12 +15,11 @@
     <sheet name="Kandam6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="839">
   <si>
     <t>Date</t>
   </si>
@@ -2504,19 +2503,58 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=vVRTcBM6bW0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=xrIQX69Ua9U</t>
+  </si>
+  <si>
+    <t>6.4.10.5</t>
+  </si>
+  <si>
+    <t>6.4.10.6</t>
+  </si>
+  <si>
+    <t>6.4.11.1</t>
+  </si>
+  <si>
+    <t>6.5.1.1</t>
+  </si>
+  <si>
+    <t>6.5.2.1</t>
+  </si>
+  <si>
+    <t>6.5.3.1</t>
+  </si>
+  <si>
+    <t>6.5.4.1</t>
+  </si>
+  <si>
+    <t>6.5.5.1</t>
+  </si>
+  <si>
+    <t>6.5.6.1</t>
+  </si>
+  <si>
+    <t>6.5.7.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="117" x14ac:knownFonts="1">
+  <fonts count="118" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3253,77 +3291,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="114" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="115" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="114" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="115" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="114" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="115" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="115" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="116" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="115" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="115" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="116" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="116" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3332,17 +3371,17 @@
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="70" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3357,19 +3396,19 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="114" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="115" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="115" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="116" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3384,44 +3423,44 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3737,7 +3776,7 @@
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="H107" sqref="H107"/>
     </sheetView>
@@ -13331,8 +13370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20459,8 +20498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21893,7 +21932,9 @@
       <c r="G70" s="134">
         <v>51.33</v>
       </c>
-      <c r="H70" s="134"/>
+      <c r="H70" s="156" t="s">
+        <v>829</v>
+      </c>
       <c r="I70" s="134"/>
     </row>
     <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -21908,24 +21949,50 @@
       <c r="I71" s="134"/>
     </row>
     <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="134"/>
-      <c r="B72" s="134"/>
-      <c r="C72" s="134"/>
-      <c r="D72" s="134"/>
-      <c r="E72" s="134"/>
-      <c r="F72" s="134"/>
-      <c r="G72" s="134"/>
+      <c r="A72" s="134">
+        <v>16</v>
+      </c>
+      <c r="B72" s="135">
+        <v>44142</v>
+      </c>
+      <c r="C72" s="134">
+        <v>59.11</v>
+      </c>
+      <c r="D72" s="140">
+        <v>1</v>
+      </c>
+      <c r="E72" s="156" t="s">
+        <v>830</v>
+      </c>
+      <c r="F72" s="156">
+        <v>5.51</v>
+      </c>
+      <c r="G72" s="134">
+        <v>8.32</v>
+      </c>
       <c r="H72" s="134"/>
-      <c r="I72" s="134"/>
+      <c r="I72" s="134" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="134"/>
       <c r="B73" s="134"/>
       <c r="C73" s="134"/>
-      <c r="D73" s="134"/>
-      <c r="E73" s="134"/>
-      <c r="F73" s="134"/>
-      <c r="G73" s="134"/>
+      <c r="D73" s="140">
+        <f>+D72+1</f>
+        <v>2</v>
+      </c>
+      <c r="E73" s="156" t="s">
+        <v>831</v>
+      </c>
+      <c r="F73" s="134">
+        <f>+G72</f>
+        <v>8.32</v>
+      </c>
+      <c r="G73" s="134">
+        <v>22.18</v>
+      </c>
       <c r="H73" s="134"/>
       <c r="I73" s="134"/>
     </row>
@@ -21933,10 +22000,20 @@
       <c r="A74" s="134"/>
       <c r="B74" s="134"/>
       <c r="C74" s="134"/>
-      <c r="D74" s="134"/>
-      <c r="E74" s="134"/>
-      <c r="F74" s="134"/>
-      <c r="G74" s="134"/>
+      <c r="D74" s="140">
+        <f>+D73+1</f>
+        <v>3</v>
+      </c>
+      <c r="E74" s="156" t="s">
+        <v>832</v>
+      </c>
+      <c r="F74" s="134">
+        <f t="shared" ref="F74:F76" si="8">+G73</f>
+        <v>22.18</v>
+      </c>
+      <c r="G74" s="134">
+        <v>35.409999999999997</v>
+      </c>
       <c r="H74" s="134"/>
       <c r="I74" s="134"/>
     </row>
@@ -21944,10 +22021,20 @@
       <c r="A75" s="134"/>
       <c r="B75" s="134"/>
       <c r="C75" s="134"/>
-      <c r="D75" s="134"/>
-      <c r="E75" s="134"/>
-      <c r="F75" s="134"/>
-      <c r="G75" s="134"/>
+      <c r="D75" s="140">
+        <f>+D74+1</f>
+        <v>4</v>
+      </c>
+      <c r="E75" s="156" t="s">
+        <v>833</v>
+      </c>
+      <c r="F75" s="134">
+        <f t="shared" si="8"/>
+        <v>35.409999999999997</v>
+      </c>
+      <c r="G75" s="134">
+        <v>45.57</v>
+      </c>
       <c r="H75" s="134"/>
       <c r="I75" s="134"/>
     </row>
@@ -21955,10 +22042,20 @@
       <c r="A76" s="134"/>
       <c r="B76" s="134"/>
       <c r="C76" s="134"/>
-      <c r="D76" s="134"/>
-      <c r="E76" s="134"/>
-      <c r="F76" s="134"/>
-      <c r="G76" s="134"/>
+      <c r="D76" s="140">
+        <f>+D75+1</f>
+        <v>5</v>
+      </c>
+      <c r="E76" s="156" t="s">
+        <v>834</v>
+      </c>
+      <c r="F76" s="134">
+        <f t="shared" si="8"/>
+        <v>45.57</v>
+      </c>
+      <c r="G76" s="134">
+        <v>57.55</v>
+      </c>
       <c r="H76" s="134"/>
       <c r="I76" s="134"/>
     </row>
@@ -21974,13 +22071,25 @@
       <c r="I77" s="134"/>
     </row>
     <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A78" s="134"/>
-      <c r="B78" s="134"/>
+      <c r="A78" s="134">
+        <v>16</v>
+      </c>
+      <c r="B78" s="135">
+        <v>44143</v>
+      </c>
       <c r="C78" s="134"/>
-      <c r="D78" s="134"/>
-      <c r="E78" s="134"/>
-      <c r="F78" s="134"/>
-      <c r="G78" s="134"/>
+      <c r="D78" s="140">
+        <v>1</v>
+      </c>
+      <c r="E78" s="156" t="s">
+        <v>835</v>
+      </c>
+      <c r="F78" s="134">
+        <v>7.18</v>
+      </c>
+      <c r="G78" s="134">
+        <v>13.43</v>
+      </c>
       <c r="H78" s="134"/>
       <c r="I78" s="134"/>
     </row>
@@ -21988,10 +22097,20 @@
       <c r="A79" s="134"/>
       <c r="B79" s="134"/>
       <c r="C79" s="134"/>
-      <c r="D79" s="134"/>
-      <c r="E79" s="134"/>
-      <c r="F79" s="134"/>
-      <c r="G79" s="134"/>
+      <c r="D79" s="140">
+        <f>+D78+1</f>
+        <v>2</v>
+      </c>
+      <c r="E79" s="156" t="s">
+        <v>836</v>
+      </c>
+      <c r="F79" s="134">
+        <f>+G78</f>
+        <v>13.43</v>
+      </c>
+      <c r="G79" s="134">
+        <v>25.29</v>
+      </c>
       <c r="H79" s="134"/>
       <c r="I79" s="134"/>
     </row>
@@ -21999,10 +22118,20 @@
       <c r="A80" s="134"/>
       <c r="B80" s="134"/>
       <c r="C80" s="134"/>
-      <c r="D80" s="134"/>
-      <c r="E80" s="134"/>
-      <c r="F80" s="134"/>
-      <c r="G80" s="134"/>
+      <c r="D80" s="140">
+        <f>+D79+1</f>
+        <v>3</v>
+      </c>
+      <c r="E80" s="156" t="s">
+        <v>837</v>
+      </c>
+      <c r="F80" s="134">
+        <f t="shared" ref="F80:F82" si="9">+G79</f>
+        <v>25.29</v>
+      </c>
+      <c r="G80" s="134">
+        <v>42.24</v>
+      </c>
       <c r="H80" s="134"/>
       <c r="I80" s="134"/>
     </row>
@@ -22010,10 +22139,20 @@
       <c r="A81" s="134"/>
       <c r="B81" s="134"/>
       <c r="C81" s="134"/>
-      <c r="D81" s="134"/>
-      <c r="E81" s="134"/>
-      <c r="F81" s="134"/>
-      <c r="G81" s="134"/>
+      <c r="D81" s="140">
+        <f>+D80+1</f>
+        <v>4</v>
+      </c>
+      <c r="E81" s="156" t="s">
+        <v>838</v>
+      </c>
+      <c r="F81" s="134">
+        <f t="shared" si="9"/>
+        <v>42.24</v>
+      </c>
+      <c r="G81" s="134">
+        <v>54.09</v>
+      </c>
       <c r="H81" s="134"/>
       <c r="I81" s="134"/>
     </row>
@@ -22021,7 +22160,7 @@
       <c r="A82" s="134"/>
       <c r="B82" s="134"/>
       <c r="C82" s="134"/>
-      <c r="D82" s="134"/>
+      <c r="D82" s="140"/>
       <c r="E82" s="134"/>
       <c r="F82" s="134"/>
       <c r="G82" s="134"/>

</xml_diff>

<commit_message>
TS PP 3.2 Sanskrit corrections sethu 13/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="870">
   <si>
     <t>Date</t>
   </si>
@@ -2569,29 +2569,104 @@
     <t>6.6.4.1</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=6Dtk41heBVU</t>
+  </si>
+  <si>
+    <t>H1/H2</t>
+  </si>
+  <si>
+    <t>1.5.8.3</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PF9qu0Z-Rog</t>
+  </si>
+  <si>
+    <t>1.04.38</t>
+  </si>
+  <si>
     <t>6.6.5.1</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=6Dtk41heBVU</t>
-  </si>
-  <si>
-    <t>H1/H2</t>
-  </si>
-  <si>
-    <t>1.5.8.3</t>
+    <t>6.6.6.1</t>
+  </si>
+  <si>
+    <t>6.6.7.1</t>
+  </si>
+  <si>
+    <t>6.6.8.1</t>
+  </si>
+  <si>
+    <t>6.6.9.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=x6cvrslUzr0</t>
+  </si>
+  <si>
+    <t>6.6.10.1</t>
+  </si>
+  <si>
+    <t>6.6.11.1</t>
+  </si>
+  <si>
+    <t>1.03.32</t>
+  </si>
+  <si>
+    <t>7.1.1.1</t>
+  </si>
+  <si>
+    <t>7.1.2.1</t>
+  </si>
+  <si>
+    <t>7.1.3.1</t>
+  </si>
+  <si>
+    <t>7.1.4.1</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>1.6.9.1/H1</t>
+  </si>
+  <si>
+    <t>7.1.5.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="121" x14ac:knownFonts="1">
+  <fonts count="125" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3352,54 +3427,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="117" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="118" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="121" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="122" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="118" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="122" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="117" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="121" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="118" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="122" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3407,41 +3487,40 @@
     <xf numFmtId="2" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="123" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="123" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="119" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="119" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3453,22 +3532,22 @@
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="122" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="123" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="118" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="119" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3482,57 +3561,66 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3839,10 +3927,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="H123" sqref="H123"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6333,7 +6421,7 @@
         <v>55.39</v>
       </c>
       <c r="H116" s="159" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="I116" s="1"/>
     </row>
@@ -6470,7 +6558,7 @@
         <v>5.59</v>
       </c>
       <c r="H123" s="156" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>164</v>
@@ -6493,7 +6581,9 @@
       <c r="G124" s="6">
         <v>15.35</v>
       </c>
-      <c r="H124" s="1"/>
+      <c r="H124" s="164" t="s">
+        <v>152</v>
+      </c>
       <c r="I124" s="1"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -6507,8 +6597,7 @@
         <v>144</v>
       </c>
       <c r="F125" s="6">
-        <f>+G124</f>
-        <v>15.35</v>
+        <v>20.21</v>
       </c>
       <c r="G125" s="6">
         <v>34.299999999999997</v>
@@ -6553,7 +6642,9 @@
       <c r="G127" s="6">
         <v>56.45</v>
       </c>
-      <c r="H127" s="1"/>
+      <c r="H127" s="165" t="s">
+        <v>867</v>
+      </c>
       <c r="I127" s="1"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -6671,8 +6762,8 @@
       <c r="G133" s="6">
         <v>59.01</v>
       </c>
-      <c r="H133" s="13" t="s">
-        <v>155</v>
+      <c r="H133" s="166" t="s">
+        <v>868</v>
       </c>
       <c r="I133" s="1"/>
     </row>
@@ -20562,8 +20653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22156,7 +22247,7 @@
       </c>
       <c r="H78" s="132"/>
       <c r="I78" s="132" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22424,17 +22515,25 @@
       <c r="B92" s="158">
         <v>44146</v>
       </c>
-      <c r="C92" s="157"/>
+      <c r="C92" s="157">
+        <v>41.48</v>
+      </c>
       <c r="D92" s="138">
         <v>1</v>
       </c>
       <c r="E92" s="157" t="s">
         <v>847</v>
       </c>
-      <c r="F92" s="157"/>
-      <c r="G92" s="157"/>
+      <c r="F92" s="157">
+        <v>2.11</v>
+      </c>
+      <c r="G92" s="157">
+        <v>20.059999999999999</v>
+      </c>
       <c r="H92" s="157"/>
-      <c r="I92" s="157"/>
+      <c r="I92" s="157" t="s">
+        <v>852</v>
+      </c>
       <c r="J92" s="157"/>
     </row>
     <row r="93" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -22448,8 +22547,13 @@
       <c r="E93" s="157" t="s">
         <v>848</v>
       </c>
-      <c r="F93" s="157"/>
-      <c r="G93" s="157"/>
+      <c r="F93" s="157">
+        <f>+G92</f>
+        <v>20.059999999999999</v>
+      </c>
+      <c r="G93" s="157">
+        <v>40.520000000000003</v>
+      </c>
       <c r="H93" s="157"/>
       <c r="I93" s="157"/>
       <c r="J93" s="157"/>
@@ -22458,13 +22562,8 @@
       <c r="A94" s="157"/>
       <c r="B94" s="157"/>
       <c r="C94" s="157"/>
-      <c r="D94" s="138">
-        <f>+D93+1</f>
-        <v>3</v>
-      </c>
-      <c r="E94" s="157" t="s">
-        <v>849</v>
-      </c>
+      <c r="D94" s="138"/>
+      <c r="E94" s="157"/>
       <c r="F94" s="157"/>
       <c r="G94" s="157"/>
       <c r="H94" s="157"/>
@@ -22472,28 +22571,51 @@
       <c r="J94" s="157"/>
     </row>
     <row r="95" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A95" s="157"/>
-      <c r="B95" s="157"/>
-      <c r="C95" s="157"/>
+      <c r="A95" s="157">
+        <v>21</v>
+      </c>
+      <c r="B95" s="158">
+        <v>44147</v>
+      </c>
+      <c r="C95" s="161" t="s">
+        <v>853</v>
+      </c>
       <c r="D95" s="138">
-        <f>+D94+1</f>
-        <v>4</v>
-      </c>
-      <c r="E95" s="157"/>
-      <c r="F95" s="157"/>
-      <c r="G95" s="157"/>
+        <v>1</v>
+      </c>
+      <c r="E95" s="160" t="s">
+        <v>854</v>
+      </c>
+      <c r="F95" s="157">
+        <v>3.33</v>
+      </c>
+      <c r="G95" s="157">
+        <v>12.52</v>
+      </c>
       <c r="H95" s="157"/>
-      <c r="I95" s="157"/>
+      <c r="I95" s="157" t="s">
+        <v>859</v>
+      </c>
       <c r="J95" s="157"/>
     </row>
     <row r="96" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="157"/>
       <c r="B96" s="157"/>
       <c r="C96" s="157"/>
-      <c r="D96" s="157"/>
-      <c r="E96" s="157"/>
-      <c r="F96" s="157"/>
-      <c r="G96" s="157"/>
+      <c r="D96" s="138">
+        <f>+D95+1</f>
+        <v>2</v>
+      </c>
+      <c r="E96" s="160" t="s">
+        <v>855</v>
+      </c>
+      <c r="F96" s="157">
+        <f>+G95</f>
+        <v>12.52</v>
+      </c>
+      <c r="G96" s="162">
+        <v>17</v>
+      </c>
       <c r="H96" s="157"/>
       <c r="I96" s="157"/>
       <c r="J96" s="157"/>
@@ -22502,10 +22624,20 @@
       <c r="A97" s="157"/>
       <c r="B97" s="157"/>
       <c r="C97" s="157"/>
-      <c r="D97" s="157"/>
-      <c r="E97" s="157"/>
-      <c r="F97" s="157"/>
-      <c r="G97" s="157"/>
+      <c r="D97" s="138">
+        <f>+D96+1</f>
+        <v>3</v>
+      </c>
+      <c r="E97" s="160" t="s">
+        <v>856</v>
+      </c>
+      <c r="F97" s="162">
+        <f t="shared" ref="F97:F101" si="11">+G96</f>
+        <v>17</v>
+      </c>
+      <c r="G97" s="162">
+        <v>27.36</v>
+      </c>
       <c r="H97" s="157"/>
       <c r="I97" s="157"/>
       <c r="J97" s="157"/>
@@ -22514,10 +22646,20 @@
       <c r="A98" s="157"/>
       <c r="B98" s="157"/>
       <c r="C98" s="157"/>
-      <c r="D98" s="157"/>
-      <c r="E98" s="157"/>
-      <c r="F98" s="157"/>
-      <c r="G98" s="157"/>
+      <c r="D98" s="138">
+        <f>+D97+1</f>
+        <v>4</v>
+      </c>
+      <c r="E98" s="160" t="s">
+        <v>857</v>
+      </c>
+      <c r="F98" s="162">
+        <f t="shared" si="11"/>
+        <v>27.36</v>
+      </c>
+      <c r="G98" s="157">
+        <v>37.479999999999997</v>
+      </c>
       <c r="H98" s="157"/>
       <c r="I98" s="157"/>
       <c r="J98" s="157"/>
@@ -22526,10 +22668,20 @@
       <c r="A99" s="157"/>
       <c r="B99" s="157"/>
       <c r="C99" s="157"/>
-      <c r="D99" s="157"/>
-      <c r="E99" s="157"/>
-      <c r="F99" s="157"/>
-      <c r="G99" s="157"/>
+      <c r="D99" s="138">
+        <f t="shared" ref="D99:D101" si="12">+D98+1</f>
+        <v>5</v>
+      </c>
+      <c r="E99" s="160" t="s">
+        <v>858</v>
+      </c>
+      <c r="F99" s="162">
+        <f t="shared" si="11"/>
+        <v>37.479999999999997</v>
+      </c>
+      <c r="G99" s="157">
+        <v>43.29</v>
+      </c>
       <c r="H99" s="157"/>
       <c r="I99" s="157"/>
       <c r="J99" s="157"/>
@@ -22538,10 +22690,20 @@
       <c r="A100" s="157"/>
       <c r="B100" s="157"/>
       <c r="C100" s="157"/>
-      <c r="D100" s="157"/>
-      <c r="E100" s="157"/>
-      <c r="F100" s="157"/>
-      <c r="G100" s="157"/>
+      <c r="D100" s="138">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="E100" s="160" t="s">
+        <v>860</v>
+      </c>
+      <c r="F100" s="162">
+        <f t="shared" si="11"/>
+        <v>43.29</v>
+      </c>
+      <c r="G100" s="157">
+        <v>48.56</v>
+      </c>
       <c r="H100" s="157"/>
       <c r="I100" s="157"/>
       <c r="J100" s="157"/>
@@ -22550,10 +22712,20 @@
       <c r="A101" s="157"/>
       <c r="B101" s="157"/>
       <c r="C101" s="157"/>
-      <c r="D101" s="157"/>
-      <c r="E101" s="157"/>
-      <c r="F101" s="157"/>
-      <c r="G101" s="157"/>
+      <c r="D101" s="138">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="E101" s="160" t="s">
+        <v>861</v>
+      </c>
+      <c r="F101" s="162">
+        <f t="shared" si="11"/>
+        <v>48.56</v>
+      </c>
+      <c r="G101" s="160" t="s">
+        <v>862</v>
+      </c>
       <c r="H101" s="157"/>
       <c r="I101" s="157"/>
       <c r="J101" s="157"/>
@@ -22614,21 +22786,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="58.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22681,7 +22853,1413 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="160">
+        <v>1</v>
+      </c>
+      <c r="B3" s="163">
+        <v>44148</v>
+      </c>
+      <c r="C3" s="160"/>
+      <c r="D3" s="167">
+        <v>1</v>
+      </c>
+      <c r="E3" s="160" t="s">
+        <v>863</v>
+      </c>
+      <c r="F3" s="160">
+        <v>2.38</v>
+      </c>
+      <c r="G3" s="160">
+        <v>23.38</v>
+      </c>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="160"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="167">
+        <f>+D3+1</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="160" t="s">
+        <v>864</v>
+      </c>
+      <c r="F4" s="160">
+        <f>+G3</f>
+        <v>23.38</v>
+      </c>
+      <c r="G4" s="160">
+        <v>28.12</v>
+      </c>
+      <c r="H4" s="160"/>
+      <c r="I4" s="160"/>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="160"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="160"/>
+      <c r="D5" s="167">
+        <f t="shared" ref="D5:D7" si="0">+D4+1</f>
+        <v>3</v>
+      </c>
+      <c r="E5" s="160" t="s">
+        <v>865</v>
+      </c>
+      <c r="F5" s="160">
+        <f t="shared" ref="F5:F7" si="1">+G4</f>
+        <v>28.12</v>
+      </c>
+      <c r="G5" s="160">
+        <v>36.24</v>
+      </c>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="160"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="167">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E6" s="160" t="s">
+        <v>866</v>
+      </c>
+      <c r="F6" s="160">
+        <f t="shared" si="1"/>
+        <v>36.24</v>
+      </c>
+      <c r="G6" s="160">
+        <v>47.02</v>
+      </c>
+      <c r="H6" s="160"/>
+      <c r="I6" s="160"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="160"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="160"/>
+      <c r="D7" s="167">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E7" s="168" t="s">
+        <v>869</v>
+      </c>
+      <c r="F7" s="160">
+        <f t="shared" si="1"/>
+        <v>47.02</v>
+      </c>
+      <c r="G7" s="160">
+        <v>49.51</v>
+      </c>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="160"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="160"/>
+      <c r="D8" s="160"/>
+      <c r="E8" s="160"/>
+      <c r="F8" s="160"/>
+      <c r="G8" s="160"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
+    </row>
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="160"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="160"/>
+      <c r="D9" s="160"/>
+      <c r="E9" s="160"/>
+      <c r="F9" s="160"/>
+      <c r="G9" s="160"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="160"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="160"/>
+      <c r="B10" s="160"/>
+      <c r="C10" s="160"/>
+      <c r="D10" s="160"/>
+      <c r="E10" s="160"/>
+      <c r="F10" s="160"/>
+      <c r="G10" s="160"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="160"/>
+    </row>
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="160"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="160"/>
+      <c r="D11" s="160"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="160"/>
+      <c r="G11" s="160"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="160"/>
+      <c r="B12" s="160"/>
+      <c r="C12" s="160"/>
+      <c r="D12" s="160"/>
+      <c r="E12" s="160"/>
+      <c r="F12" s="160"/>
+      <c r="G12" s="160"/>
+      <c r="H12" s="160"/>
+      <c r="I12" s="160"/>
+    </row>
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="160"/>
+      <c r="B13" s="160"/>
+      <c r="C13" s="160"/>
+      <c r="D13" s="160"/>
+      <c r="E13" s="160"/>
+      <c r="F13" s="160"/>
+      <c r="G13" s="160"/>
+      <c r="H13" s="160"/>
+      <c r="I13" s="160"/>
+    </row>
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="160"/>
+      <c r="B14" s="160"/>
+      <c r="C14" s="160"/>
+      <c r="D14" s="160"/>
+      <c r="E14" s="160"/>
+      <c r="F14" s="160"/>
+      <c r="G14" s="160"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+    </row>
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="160"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="160"/>
+      <c r="D15" s="160"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="160"/>
+    </row>
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="160"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="160"/>
+      <c r="D16" s="160"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="160"/>
+      <c r="G16" s="160"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="160"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="160"/>
+      <c r="D17" s="160"/>
+      <c r="E17" s="160"/>
+      <c r="F17" s="160"/>
+      <c r="G17" s="160"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="160"/>
+      <c r="B18" s="160"/>
+      <c r="C18" s="160"/>
+      <c r="D18" s="160"/>
+      <c r="E18" s="160"/>
+      <c r="F18" s="160"/>
+      <c r="G18" s="160"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="160"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="160"/>
+      <c r="B19" s="160"/>
+      <c r="C19" s="160"/>
+      <c r="D19" s="160"/>
+      <c r="E19" s="160"/>
+      <c r="F19" s="160"/>
+      <c r="G19" s="160"/>
+      <c r="H19" s="160"/>
+      <c r="I19" s="160"/>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="160"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="160"/>
+      <c r="D20" s="160"/>
+      <c r="E20" s="160"/>
+      <c r="F20" s="160"/>
+      <c r="G20" s="160"/>
+      <c r="H20" s="160"/>
+      <c r="I20" s="160"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="160"/>
+      <c r="B21" s="160"/>
+      <c r="C21" s="160"/>
+      <c r="D21" s="160"/>
+      <c r="E21" s="160"/>
+      <c r="F21" s="160"/>
+      <c r="G21" s="160"/>
+      <c r="H21" s="160"/>
+      <c r="I21" s="160"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="160"/>
+      <c r="B22" s="160"/>
+      <c r="C22" s="160"/>
+      <c r="D22" s="160"/>
+      <c r="E22" s="160"/>
+      <c r="F22" s="160"/>
+      <c r="G22" s="160"/>
+      <c r="H22" s="160"/>
+      <c r="I22" s="160"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="160"/>
+      <c r="B23" s="160"/>
+      <c r="C23" s="160"/>
+      <c r="D23" s="160"/>
+      <c r="E23" s="160"/>
+      <c r="F23" s="160"/>
+      <c r="G23" s="160"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="160"/>
+    </row>
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="160"/>
+      <c r="B24" s="160"/>
+      <c r="C24" s="160"/>
+      <c r="D24" s="160"/>
+      <c r="E24" s="160"/>
+      <c r="F24" s="160"/>
+      <c r="G24" s="160"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="160"/>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="160"/>
+      <c r="B25" s="160"/>
+      <c r="C25" s="160"/>
+      <c r="D25" s="160"/>
+      <c r="E25" s="160"/>
+      <c r="F25" s="160"/>
+      <c r="G25" s="160"/>
+      <c r="H25" s="160"/>
+      <c r="I25" s="160"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="160"/>
+      <c r="B26" s="160"/>
+      <c r="C26" s="160"/>
+      <c r="D26" s="160"/>
+      <c r="E26" s="160"/>
+      <c r="F26" s="160"/>
+      <c r="G26" s="160"/>
+      <c r="H26" s="160"/>
+      <c r="I26" s="160"/>
+    </row>
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="160"/>
+      <c r="B27" s="160"/>
+      <c r="C27" s="160"/>
+      <c r="D27" s="160"/>
+      <c r="E27" s="160"/>
+      <c r="F27" s="160"/>
+      <c r="G27" s="160"/>
+      <c r="H27" s="160"/>
+      <c r="I27" s="160"/>
+    </row>
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="160"/>
+      <c r="B28" s="160"/>
+      <c r="C28" s="160"/>
+      <c r="D28" s="160"/>
+      <c r="E28" s="160"/>
+      <c r="F28" s="160"/>
+      <c r="G28" s="160"/>
+      <c r="H28" s="160"/>
+      <c r="I28" s="160"/>
+    </row>
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="160"/>
+      <c r="B29" s="160"/>
+      <c r="C29" s="160"/>
+      <c r="D29" s="160"/>
+      <c r="E29" s="160"/>
+      <c r="F29" s="160"/>
+      <c r="G29" s="160"/>
+      <c r="H29" s="160"/>
+      <c r="I29" s="160"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="160"/>
+      <c r="B30" s="160"/>
+      <c r="C30" s="160"/>
+      <c r="D30" s="160"/>
+      <c r="E30" s="160"/>
+      <c r="F30" s="160"/>
+      <c r="G30" s="160"/>
+      <c r="H30" s="160"/>
+      <c r="I30" s="160"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="160"/>
+      <c r="B31" s="160"/>
+      <c r="C31" s="160"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="160"/>
+      <c r="F31" s="160"/>
+      <c r="G31" s="160"/>
+      <c r="H31" s="160"/>
+      <c r="I31" s="160"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="160"/>
+      <c r="B32" s="160"/>
+      <c r="C32" s="160"/>
+      <c r="D32" s="160"/>
+      <c r="E32" s="160"/>
+      <c r="F32" s="160"/>
+      <c r="G32" s="160"/>
+      <c r="H32" s="160"/>
+      <c r="I32" s="160"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="160"/>
+      <c r="B33" s="160"/>
+      <c r="C33" s="160"/>
+      <c r="D33" s="160"/>
+      <c r="E33" s="160"/>
+      <c r="F33" s="160"/>
+      <c r="G33" s="160"/>
+      <c r="H33" s="160"/>
+      <c r="I33" s="160"/>
+    </row>
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="160"/>
+      <c r="B34" s="160"/>
+      <c r="C34" s="160"/>
+      <c r="D34" s="160"/>
+      <c r="E34" s="160"/>
+      <c r="F34" s="160"/>
+      <c r="G34" s="160"/>
+      <c r="H34" s="160"/>
+      <c r="I34" s="160"/>
+    </row>
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="160"/>
+      <c r="B35" s="160"/>
+      <c r="C35" s="160"/>
+      <c r="D35" s="160"/>
+      <c r="E35" s="160"/>
+      <c r="F35" s="160"/>
+      <c r="G35" s="160"/>
+      <c r="H35" s="160"/>
+      <c r="I35" s="160"/>
+    </row>
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="160"/>
+      <c r="B36" s="160"/>
+      <c r="C36" s="160"/>
+      <c r="D36" s="160"/>
+      <c r="E36" s="160"/>
+      <c r="F36" s="160"/>
+      <c r="G36" s="160"/>
+      <c r="H36" s="160"/>
+      <c r="I36" s="160"/>
+    </row>
+    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A37" s="160"/>
+      <c r="B37" s="160"/>
+      <c r="C37" s="160"/>
+      <c r="D37" s="160"/>
+      <c r="E37" s="160"/>
+      <c r="F37" s="160"/>
+      <c r="G37" s="160"/>
+      <c r="H37" s="160"/>
+      <c r="I37" s="160"/>
+    </row>
+    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="160"/>
+      <c r="B38" s="160"/>
+      <c r="C38" s="160"/>
+      <c r="D38" s="160"/>
+      <c r="E38" s="160"/>
+      <c r="F38" s="160"/>
+      <c r="G38" s="160"/>
+      <c r="H38" s="160"/>
+      <c r="I38" s="160"/>
+    </row>
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="160"/>
+      <c r="B39" s="160"/>
+      <c r="C39" s="160"/>
+      <c r="D39" s="160"/>
+      <c r="E39" s="160"/>
+      <c r="F39" s="160"/>
+      <c r="G39" s="160"/>
+      <c r="H39" s="160"/>
+      <c r="I39" s="160"/>
+    </row>
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A40" s="160"/>
+      <c r="B40" s="160"/>
+      <c r="C40" s="160"/>
+      <c r="D40" s="160"/>
+      <c r="E40" s="160"/>
+      <c r="F40" s="160"/>
+      <c r="G40" s="160"/>
+      <c r="H40" s="160"/>
+      <c r="I40" s="160"/>
+    </row>
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A41" s="160"/>
+      <c r="B41" s="160"/>
+      <c r="C41" s="160"/>
+      <c r="D41" s="160"/>
+      <c r="E41" s="160"/>
+      <c r="F41" s="160"/>
+      <c r="G41" s="160"/>
+      <c r="H41" s="160"/>
+      <c r="I41" s="160"/>
+    </row>
+    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" s="160"/>
+      <c r="B42" s="160"/>
+      <c r="C42" s="160"/>
+      <c r="D42" s="160"/>
+      <c r="E42" s="160"/>
+      <c r="F42" s="160"/>
+      <c r="G42" s="160"/>
+      <c r="H42" s="160"/>
+      <c r="I42" s="160"/>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" s="160"/>
+      <c r="B43" s="160"/>
+      <c r="C43" s="160"/>
+      <c r="D43" s="160"/>
+      <c r="E43" s="160"/>
+      <c r="F43" s="160"/>
+      <c r="G43" s="160"/>
+      <c r="H43" s="160"/>
+      <c r="I43" s="160"/>
+    </row>
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A44" s="160"/>
+      <c r="B44" s="160"/>
+      <c r="C44" s="160"/>
+      <c r="D44" s="160"/>
+      <c r="E44" s="160"/>
+      <c r="F44" s="160"/>
+      <c r="G44" s="160"/>
+      <c r="H44" s="160"/>
+      <c r="I44" s="160"/>
+    </row>
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A45" s="160"/>
+      <c r="B45" s="160"/>
+      <c r="C45" s="160"/>
+      <c r="D45" s="160"/>
+      <c r="E45" s="160"/>
+      <c r="F45" s="160"/>
+      <c r="G45" s="160"/>
+      <c r="H45" s="160"/>
+      <c r="I45" s="160"/>
+    </row>
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A46" s="160"/>
+      <c r="B46" s="160"/>
+      <c r="C46" s="160"/>
+      <c r="D46" s="160"/>
+      <c r="E46" s="160"/>
+      <c r="F46" s="160"/>
+      <c r="G46" s="160"/>
+      <c r="H46" s="160"/>
+      <c r="I46" s="160"/>
+    </row>
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A47" s="160"/>
+      <c r="B47" s="160"/>
+      <c r="C47" s="160"/>
+      <c r="D47" s="160"/>
+      <c r="E47" s="160"/>
+      <c r="F47" s="160"/>
+      <c r="G47" s="160"/>
+      <c r="H47" s="160"/>
+      <c r="I47" s="160"/>
+    </row>
+    <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A48" s="160"/>
+      <c r="B48" s="160"/>
+      <c r="C48" s="160"/>
+      <c r="D48" s="160"/>
+      <c r="E48" s="160"/>
+      <c r="F48" s="160"/>
+      <c r="G48" s="160"/>
+      <c r="H48" s="160"/>
+      <c r="I48" s="160"/>
+    </row>
+    <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A49" s="160"/>
+      <c r="B49" s="160"/>
+      <c r="C49" s="160"/>
+      <c r="D49" s="160"/>
+      <c r="E49" s="160"/>
+      <c r="F49" s="160"/>
+      <c r="G49" s="160"/>
+      <c r="H49" s="160"/>
+      <c r="I49" s="160"/>
+    </row>
+    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A50" s="160"/>
+      <c r="B50" s="160"/>
+      <c r="C50" s="160"/>
+      <c r="D50" s="160"/>
+      <c r="E50" s="160"/>
+      <c r="F50" s="160"/>
+      <c r="G50" s="160"/>
+      <c r="H50" s="160"/>
+      <c r="I50" s="160"/>
+    </row>
+    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A51" s="160"/>
+      <c r="B51" s="160"/>
+      <c r="C51" s="160"/>
+      <c r="D51" s="160"/>
+      <c r="E51" s="160"/>
+      <c r="F51" s="160"/>
+      <c r="G51" s="160"/>
+      <c r="H51" s="160"/>
+      <c r="I51" s="160"/>
+    </row>
+    <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A52" s="160"/>
+      <c r="B52" s="160"/>
+      <c r="C52" s="160"/>
+      <c r="D52" s="160"/>
+      <c r="E52" s="160"/>
+      <c r="F52" s="160"/>
+      <c r="G52" s="160"/>
+      <c r="H52" s="160"/>
+      <c r="I52" s="160"/>
+    </row>
+    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A53" s="160"/>
+      <c r="B53" s="160"/>
+      <c r="C53" s="160"/>
+      <c r="D53" s="160"/>
+      <c r="E53" s="160"/>
+      <c r="F53" s="160"/>
+      <c r="G53" s="160"/>
+      <c r="H53" s="160"/>
+      <c r="I53" s="160"/>
+    </row>
+    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A54" s="160"/>
+      <c r="B54" s="160"/>
+      <c r="C54" s="160"/>
+      <c r="D54" s="160"/>
+      <c r="E54" s="160"/>
+      <c r="F54" s="160"/>
+      <c r="G54" s="160"/>
+      <c r="H54" s="160"/>
+      <c r="I54" s="160"/>
+    </row>
+    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A55" s="160"/>
+      <c r="B55" s="160"/>
+      <c r="C55" s="160"/>
+      <c r="D55" s="160"/>
+      <c r="E55" s="160"/>
+      <c r="F55" s="160"/>
+      <c r="G55" s="160"/>
+      <c r="H55" s="160"/>
+      <c r="I55" s="160"/>
+    </row>
+    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A56" s="160"/>
+      <c r="B56" s="160"/>
+      <c r="C56" s="160"/>
+      <c r="D56" s="160"/>
+      <c r="E56" s="160"/>
+      <c r="F56" s="160"/>
+      <c r="G56" s="160"/>
+      <c r="H56" s="160"/>
+      <c r="I56" s="160"/>
+    </row>
+    <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A57" s="160"/>
+      <c r="B57" s="160"/>
+      <c r="C57" s="160"/>
+      <c r="D57" s="160"/>
+      <c r="E57" s="160"/>
+      <c r="F57" s="160"/>
+      <c r="G57" s="160"/>
+      <c r="H57" s="160"/>
+      <c r="I57" s="160"/>
+    </row>
+    <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A58" s="160"/>
+      <c r="B58" s="160"/>
+      <c r="C58" s="160"/>
+      <c r="D58" s="160"/>
+      <c r="E58" s="160"/>
+      <c r="F58" s="160"/>
+      <c r="G58" s="160"/>
+      <c r="H58" s="160"/>
+      <c r="I58" s="160"/>
+    </row>
+    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A59" s="160"/>
+      <c r="B59" s="160"/>
+      <c r="C59" s="160"/>
+      <c r="D59" s="160"/>
+      <c r="E59" s="160"/>
+      <c r="F59" s="160"/>
+      <c r="G59" s="160"/>
+      <c r="H59" s="160"/>
+      <c r="I59" s="160"/>
+    </row>
+    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A60" s="160"/>
+      <c r="B60" s="160"/>
+      <c r="C60" s="160"/>
+      <c r="D60" s="160"/>
+      <c r="E60" s="160"/>
+      <c r="F60" s="160"/>
+      <c r="G60" s="160"/>
+      <c r="H60" s="160"/>
+      <c r="I60" s="160"/>
+    </row>
+    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A61" s="160"/>
+      <c r="B61" s="160"/>
+      <c r="C61" s="160"/>
+      <c r="D61" s="160"/>
+      <c r="E61" s="160"/>
+      <c r="F61" s="160"/>
+      <c r="G61" s="160"/>
+      <c r="H61" s="160"/>
+      <c r="I61" s="160"/>
+    </row>
+    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A62" s="160"/>
+      <c r="B62" s="160"/>
+      <c r="C62" s="160"/>
+      <c r="D62" s="160"/>
+      <c r="E62" s="160"/>
+      <c r="F62" s="160"/>
+      <c r="G62" s="160"/>
+      <c r="H62" s="160"/>
+      <c r="I62" s="160"/>
+    </row>
+    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A63" s="160"/>
+      <c r="B63" s="160"/>
+      <c r="C63" s="160"/>
+      <c r="D63" s="160"/>
+      <c r="E63" s="160"/>
+      <c r="F63" s="160"/>
+      <c r="G63" s="160"/>
+      <c r="H63" s="160"/>
+      <c r="I63" s="160"/>
+    </row>
+    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A64" s="160"/>
+      <c r="B64" s="160"/>
+      <c r="C64" s="160"/>
+      <c r="D64" s="160"/>
+      <c r="E64" s="160"/>
+      <c r="F64" s="160"/>
+      <c r="G64" s="160"/>
+      <c r="H64" s="160"/>
+      <c r="I64" s="160"/>
+    </row>
+    <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A65" s="160"/>
+      <c r="B65" s="160"/>
+      <c r="C65" s="160"/>
+      <c r="D65" s="160"/>
+      <c r="E65" s="160"/>
+      <c r="F65" s="160"/>
+      <c r="G65" s="160"/>
+      <c r="H65" s="160"/>
+      <c r="I65" s="160"/>
+    </row>
+    <row r="66" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A66" s="160"/>
+      <c r="B66" s="160"/>
+      <c r="C66" s="160"/>
+      <c r="D66" s="160"/>
+      <c r="E66" s="160"/>
+      <c r="F66" s="160"/>
+      <c r="G66" s="160"/>
+      <c r="H66" s="160"/>
+      <c r="I66" s="160"/>
+    </row>
+    <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A67" s="160"/>
+      <c r="B67" s="160"/>
+      <c r="C67" s="160"/>
+      <c r="D67" s="160"/>
+      <c r="E67" s="160"/>
+      <c r="F67" s="160"/>
+      <c r="G67" s="160"/>
+      <c r="H67" s="160"/>
+      <c r="I67" s="160"/>
+    </row>
+    <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A68" s="160"/>
+      <c r="B68" s="160"/>
+      <c r="C68" s="160"/>
+      <c r="D68" s="160"/>
+      <c r="E68" s="160"/>
+      <c r="F68" s="160"/>
+      <c r="G68" s="160"/>
+      <c r="H68" s="160"/>
+      <c r="I68" s="160"/>
+    </row>
+    <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A69" s="160"/>
+      <c r="B69" s="160"/>
+      <c r="C69" s="160"/>
+      <c r="D69" s="160"/>
+      <c r="E69" s="160"/>
+      <c r="F69" s="160"/>
+      <c r="G69" s="160"/>
+      <c r="H69" s="160"/>
+      <c r="I69" s="160"/>
+    </row>
+    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A70" s="160"/>
+      <c r="B70" s="160"/>
+      <c r="C70" s="160"/>
+      <c r="D70" s="160"/>
+      <c r="E70" s="160"/>
+      <c r="F70" s="160"/>
+      <c r="G70" s="160"/>
+      <c r="H70" s="160"/>
+      <c r="I70" s="160"/>
+    </row>
+    <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A71" s="160"/>
+      <c r="B71" s="160"/>
+      <c r="C71" s="160"/>
+      <c r="D71" s="160"/>
+      <c r="E71" s="160"/>
+      <c r="F71" s="160"/>
+      <c r="G71" s="160"/>
+      <c r="H71" s="160"/>
+      <c r="I71" s="160"/>
+    </row>
+    <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A72" s="160"/>
+      <c r="B72" s="160"/>
+      <c r="C72" s="160"/>
+      <c r="D72" s="160"/>
+      <c r="E72" s="160"/>
+      <c r="F72" s="160"/>
+      <c r="G72" s="160"/>
+      <c r="H72" s="160"/>
+      <c r="I72" s="160"/>
+    </row>
+    <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A73" s="160"/>
+      <c r="B73" s="160"/>
+      <c r="C73" s="160"/>
+      <c r="D73" s="160"/>
+      <c r="E73" s="160"/>
+      <c r="F73" s="160"/>
+      <c r="G73" s="160"/>
+      <c r="H73" s="160"/>
+      <c r="I73" s="160"/>
+    </row>
+    <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A74" s="160"/>
+      <c r="B74" s="160"/>
+      <c r="C74" s="160"/>
+      <c r="D74" s="160"/>
+      <c r="E74" s="160"/>
+      <c r="F74" s="160"/>
+      <c r="G74" s="160"/>
+      <c r="H74" s="160"/>
+      <c r="I74" s="160"/>
+    </row>
+    <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A75" s="160"/>
+      <c r="B75" s="160"/>
+      <c r="C75" s="160"/>
+      <c r="D75" s="160"/>
+      <c r="E75" s="160"/>
+      <c r="F75" s="160"/>
+      <c r="G75" s="160"/>
+      <c r="H75" s="160"/>
+      <c r="I75" s="160"/>
+    </row>
+    <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A76" s="160"/>
+      <c r="B76" s="160"/>
+      <c r="C76" s="160"/>
+      <c r="D76" s="160"/>
+      <c r="E76" s="160"/>
+      <c r="F76" s="160"/>
+      <c r="G76" s="160"/>
+      <c r="H76" s="160"/>
+      <c r="I76" s="160"/>
+    </row>
+    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A77" s="160"/>
+      <c r="B77" s="160"/>
+      <c r="C77" s="160"/>
+      <c r="D77" s="160"/>
+      <c r="E77" s="160"/>
+      <c r="F77" s="160"/>
+      <c r="G77" s="160"/>
+      <c r="H77" s="160"/>
+      <c r="I77" s="160"/>
+    </row>
+    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A78" s="160"/>
+      <c r="B78" s="160"/>
+      <c r="C78" s="160"/>
+      <c r="D78" s="160"/>
+      <c r="E78" s="160"/>
+      <c r="F78" s="160"/>
+      <c r="G78" s="160"/>
+      <c r="H78" s="160"/>
+      <c r="I78" s="160"/>
+    </row>
+    <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A79" s="160"/>
+      <c r="B79" s="160"/>
+      <c r="C79" s="160"/>
+      <c r="D79" s="160"/>
+      <c r="E79" s="160"/>
+      <c r="F79" s="160"/>
+      <c r="G79" s="160"/>
+      <c r="H79" s="160"/>
+      <c r="I79" s="160"/>
+    </row>
+    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A80" s="160"/>
+      <c r="B80" s="160"/>
+      <c r="C80" s="160"/>
+      <c r="D80" s="160"/>
+      <c r="E80" s="160"/>
+      <c r="F80" s="160"/>
+      <c r="G80" s="160"/>
+      <c r="H80" s="160"/>
+      <c r="I80" s="160"/>
+    </row>
+    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A81" s="160"/>
+      <c r="B81" s="160"/>
+      <c r="C81" s="160"/>
+      <c r="D81" s="160"/>
+      <c r="E81" s="160"/>
+      <c r="F81" s="160"/>
+      <c r="G81" s="160"/>
+      <c r="H81" s="160"/>
+      <c r="I81" s="160"/>
+    </row>
+    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A82" s="160"/>
+      <c r="B82" s="160"/>
+      <c r="C82" s="160"/>
+      <c r="D82" s="160"/>
+      <c r="E82" s="160"/>
+      <c r="F82" s="160"/>
+      <c r="G82" s="160"/>
+      <c r="H82" s="160"/>
+      <c r="I82" s="160"/>
+    </row>
+    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A83" s="160"/>
+      <c r="B83" s="160"/>
+      <c r="C83" s="160"/>
+      <c r="D83" s="160"/>
+      <c r="E83" s="160"/>
+      <c r="F83" s="160"/>
+      <c r="G83" s="160"/>
+      <c r="H83" s="160"/>
+      <c r="I83" s="160"/>
+    </row>
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A84" s="160"/>
+      <c r="B84" s="160"/>
+      <c r="C84" s="160"/>
+      <c r="D84" s="160"/>
+      <c r="E84" s="160"/>
+      <c r="F84" s="160"/>
+      <c r="G84" s="160"/>
+      <c r="H84" s="160"/>
+      <c r="I84" s="160"/>
+    </row>
+    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A85" s="160"/>
+      <c r="B85" s="160"/>
+      <c r="C85" s="160"/>
+      <c r="D85" s="160"/>
+      <c r="E85" s="160"/>
+      <c r="F85" s="160"/>
+      <c r="G85" s="160"/>
+      <c r="H85" s="160"/>
+      <c r="I85" s="160"/>
+    </row>
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A86" s="160"/>
+      <c r="B86" s="160"/>
+      <c r="C86" s="160"/>
+      <c r="D86" s="160"/>
+      <c r="E86" s="160"/>
+      <c r="F86" s="160"/>
+      <c r="G86" s="160"/>
+      <c r="H86" s="160"/>
+      <c r="I86" s="160"/>
+    </row>
+    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A87" s="160"/>
+      <c r="B87" s="160"/>
+      <c r="C87" s="160"/>
+      <c r="D87" s="160"/>
+      <c r="E87" s="160"/>
+      <c r="F87" s="160"/>
+      <c r="G87" s="160"/>
+      <c r="H87" s="160"/>
+      <c r="I87" s="160"/>
+    </row>
+    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A88" s="160"/>
+      <c r="B88" s="160"/>
+      <c r="C88" s="160"/>
+      <c r="D88" s="160"/>
+      <c r="E88" s="160"/>
+      <c r="F88" s="160"/>
+      <c r="G88" s="160"/>
+      <c r="H88" s="160"/>
+      <c r="I88" s="160"/>
+    </row>
+    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A89" s="160"/>
+      <c r="B89" s="160"/>
+      <c r="C89" s="160"/>
+      <c r="D89" s="160"/>
+      <c r="E89" s="160"/>
+      <c r="F89" s="160"/>
+      <c r="G89" s="160"/>
+      <c r="H89" s="160"/>
+      <c r="I89" s="160"/>
+    </row>
+    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A90" s="160"/>
+      <c r="B90" s="160"/>
+      <c r="C90" s="160"/>
+      <c r="D90" s="160"/>
+      <c r="E90" s="160"/>
+      <c r="F90" s="160"/>
+      <c r="G90" s="160"/>
+      <c r="H90" s="160"/>
+      <c r="I90" s="160"/>
+    </row>
+    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A91" s="160"/>
+      <c r="B91" s="160"/>
+      <c r="C91" s="160"/>
+      <c r="D91" s="160"/>
+      <c r="E91" s="160"/>
+      <c r="F91" s="160"/>
+      <c r="G91" s="160"/>
+      <c r="H91" s="160"/>
+      <c r="I91" s="160"/>
+    </row>
+    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A92" s="160"/>
+      <c r="B92" s="160"/>
+      <c r="C92" s="160"/>
+      <c r="D92" s="160"/>
+      <c r="E92" s="160"/>
+      <c r="F92" s="160"/>
+      <c r="G92" s="160"/>
+      <c r="H92" s="160"/>
+      <c r="I92" s="160"/>
+    </row>
+    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A93" s="160"/>
+      <c r="B93" s="160"/>
+      <c r="C93" s="160"/>
+      <c r="D93" s="160"/>
+      <c r="E93" s="160"/>
+      <c r="F93" s="160"/>
+      <c r="G93" s="160"/>
+      <c r="H93" s="160"/>
+      <c r="I93" s="160"/>
+    </row>
+    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A94" s="160"/>
+      <c r="B94" s="160"/>
+      <c r="C94" s="160"/>
+      <c r="D94" s="160"/>
+      <c r="E94" s="160"/>
+      <c r="F94" s="160"/>
+      <c r="G94" s="160"/>
+      <c r="H94" s="160"/>
+      <c r="I94" s="160"/>
+    </row>
+    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A95" s="160"/>
+      <c r="B95" s="160"/>
+      <c r="C95" s="160"/>
+      <c r="D95" s="160"/>
+      <c r="E95" s="160"/>
+      <c r="F95" s="160"/>
+      <c r="G95" s="160"/>
+      <c r="H95" s="160"/>
+      <c r="I95" s="160"/>
+    </row>
+    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A96" s="160"/>
+      <c r="B96" s="160"/>
+      <c r="C96" s="160"/>
+      <c r="D96" s="160"/>
+      <c r="E96" s="160"/>
+      <c r="F96" s="160"/>
+      <c r="G96" s="160"/>
+      <c r="H96" s="160"/>
+      <c r="I96" s="160"/>
+    </row>
+    <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A97" s="160"/>
+      <c r="B97" s="160"/>
+      <c r="C97" s="160"/>
+      <c r="D97" s="160"/>
+      <c r="E97" s="160"/>
+      <c r="F97" s="160"/>
+      <c r="G97" s="160"/>
+      <c r="H97" s="160"/>
+      <c r="I97" s="160"/>
+    </row>
+    <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A98" s="160"/>
+      <c r="B98" s="160"/>
+      <c r="C98" s="160"/>
+      <c r="D98" s="160"/>
+      <c r="E98" s="160"/>
+      <c r="F98" s="160"/>
+      <c r="G98" s="160"/>
+      <c r="H98" s="160"/>
+      <c r="I98" s="160"/>
+    </row>
+    <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A99" s="160"/>
+      <c r="B99" s="160"/>
+      <c r="C99" s="160"/>
+      <c r="D99" s="160"/>
+      <c r="E99" s="160"/>
+      <c r="F99" s="160"/>
+      <c r="G99" s="160"/>
+      <c r="H99" s="160"/>
+      <c r="I99" s="160"/>
+    </row>
+    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A100" s="160"/>
+      <c r="B100" s="160"/>
+      <c r="C100" s="160"/>
+      <c r="D100" s="160"/>
+      <c r="E100" s="160"/>
+      <c r="F100" s="160"/>
+      <c r="G100" s="160"/>
+      <c r="H100" s="160"/>
+      <c r="I100" s="160"/>
+    </row>
+    <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A101" s="160"/>
+      <c r="B101" s="160"/>
+      <c r="C101" s="160"/>
+      <c r="D101" s="160"/>
+      <c r="E101" s="160"/>
+      <c r="F101" s="160"/>
+      <c r="G101" s="160"/>
+      <c r="H101" s="160"/>
+      <c r="I101" s="160"/>
+    </row>
+    <row r="102" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A102" s="160"/>
+      <c r="B102" s="160"/>
+      <c r="C102" s="160"/>
+      <c r="D102" s="160"/>
+      <c r="E102" s="160"/>
+      <c r="F102" s="160"/>
+      <c r="G102" s="160"/>
+      <c r="H102" s="160"/>
+      <c r="I102" s="160"/>
+    </row>
+    <row r="103" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A103" s="160"/>
+      <c r="B103" s="160"/>
+      <c r="C103" s="160"/>
+      <c r="D103" s="160"/>
+      <c r="E103" s="160"/>
+      <c r="F103" s="160"/>
+      <c r="G103" s="160"/>
+      <c r="H103" s="160"/>
+      <c r="I103" s="160"/>
+    </row>
+    <row r="104" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A104" s="160"/>
+      <c r="B104" s="160"/>
+      <c r="C104" s="160"/>
+      <c r="D104" s="160"/>
+      <c r="E104" s="160"/>
+      <c r="F104" s="160"/>
+      <c r="G104" s="160"/>
+      <c r="H104" s="160"/>
+      <c r="I104" s="160"/>
+    </row>
+    <row r="105" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A105" s="160"/>
+      <c r="B105" s="160"/>
+      <c r="C105" s="160"/>
+      <c r="D105" s="160"/>
+      <c r="E105" s="160"/>
+      <c r="F105" s="160"/>
+      <c r="G105" s="160"/>
+      <c r="H105" s="160"/>
+      <c r="I105" s="160"/>
+    </row>
+    <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A106" s="160"/>
+      <c r="B106" s="160"/>
+      <c r="C106" s="160"/>
+      <c r="D106" s="160"/>
+      <c r="E106" s="160"/>
+      <c r="F106" s="160"/>
+      <c r="G106" s="160"/>
+      <c r="H106" s="160"/>
+      <c r="I106" s="160"/>
+    </row>
+    <row r="107" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A107" s="160"/>
+      <c r="B107" s="160"/>
+      <c r="C107" s="160"/>
+      <c r="D107" s="160"/>
+      <c r="E107" s="160"/>
+      <c r="F107" s="160"/>
+      <c r="G107" s="160"/>
+      <c r="H107" s="160"/>
+      <c r="I107" s="160"/>
+    </row>
+    <row r="108" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A108" s="160"/>
+      <c r="B108" s="160"/>
+      <c r="C108" s="160"/>
+      <c r="D108" s="160"/>
+      <c r="E108" s="160"/>
+      <c r="F108" s="160"/>
+      <c r="G108" s="160"/>
+      <c r="H108" s="160"/>
+      <c r="I108" s="160"/>
+    </row>
+    <row r="109" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A109" s="160"/>
+      <c r="B109" s="160"/>
+      <c r="C109" s="160"/>
+      <c r="D109" s="160"/>
+      <c r="E109" s="160"/>
+      <c r="F109" s="160"/>
+      <c r="G109" s="160"/>
+      <c r="H109" s="160"/>
+      <c r="I109" s="160"/>
+    </row>
+    <row r="110" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A110" s="160"/>
+      <c r="B110" s="160"/>
+      <c r="C110" s="160"/>
+      <c r="D110" s="160"/>
+      <c r="E110" s="160"/>
+      <c r="F110" s="160"/>
+      <c r="G110" s="160"/>
+      <c r="H110" s="160"/>
+      <c r="I110" s="160"/>
+    </row>
+    <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A111" s="160"/>
+      <c r="B111" s="160"/>
+      <c r="C111" s="160"/>
+      <c r="D111" s="160"/>
+      <c r="E111" s="160"/>
+      <c r="F111" s="160"/>
+      <c r="G111" s="160"/>
+      <c r="H111" s="160"/>
+      <c r="I111" s="160"/>
+    </row>
+    <row r="112" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A112" s="160"/>
+      <c r="B112" s="160"/>
+      <c r="C112" s="160"/>
+      <c r="D112" s="160"/>
+      <c r="E112" s="160"/>
+      <c r="F112" s="160"/>
+      <c r="G112" s="160"/>
+      <c r="H112" s="160"/>
+      <c r="I112" s="160"/>
+    </row>
+    <row r="113" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A113" s="160"/>
+      <c r="B113" s="160"/>
+      <c r="C113" s="160"/>
+      <c r="D113" s="160"/>
+      <c r="E113" s="160"/>
+      <c r="F113" s="160"/>
+      <c r="G113" s="160"/>
+      <c r="H113" s="160"/>
+      <c r="I113" s="160"/>
+    </row>
+    <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A114" s="160"/>
+      <c r="B114" s="160"/>
+      <c r="C114" s="160"/>
+      <c r="D114" s="160"/>
+      <c r="E114" s="160"/>
+      <c r="F114" s="160"/>
+      <c r="G114" s="160"/>
+      <c r="H114" s="160"/>
+      <c r="I114" s="160"/>
+    </row>
+    <row r="115" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A115" s="160"/>
+      <c r="B115" s="160"/>
+      <c r="C115" s="160"/>
+      <c r="D115" s="160"/>
+      <c r="E115" s="160"/>
+      <c r="F115" s="160"/>
+      <c r="G115" s="160"/>
+      <c r="H115" s="160"/>
+      <c r="I115" s="160"/>
+    </row>
+    <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A116" s="160"/>
+      <c r="B116" s="160"/>
+      <c r="C116" s="160"/>
+      <c r="D116" s="160"/>
+      <c r="E116" s="160"/>
+      <c r="F116" s="160"/>
+      <c r="G116" s="160"/>
+      <c r="H116" s="160"/>
+      <c r="I116" s="160"/>
+    </row>
+    <row r="117" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A117" s="160"/>
+      <c r="B117" s="160"/>
+      <c r="C117" s="160"/>
+      <c r="D117" s="160"/>
+      <c r="E117" s="160"/>
+      <c r="F117" s="160"/>
+      <c r="G117" s="160"/>
+      <c r="H117" s="160"/>
+      <c r="I117" s="160"/>
+    </row>
+    <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A118" s="160"/>
+      <c r="B118" s="160"/>
+      <c r="C118" s="160"/>
+      <c r="D118" s="160"/>
+      <c r="E118" s="160"/>
+      <c r="F118" s="160"/>
+      <c r="G118" s="160"/>
+      <c r="H118" s="160"/>
+      <c r="I118" s="160"/>
+    </row>
+    <row r="119" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A119" s="160"/>
+      <c r="B119" s="160"/>
+      <c r="C119" s="160"/>
+      <c r="D119" s="160"/>
+      <c r="E119" s="160"/>
+      <c r="F119" s="160"/>
+      <c r="G119" s="160"/>
+      <c r="H119" s="160"/>
+      <c r="I119" s="160"/>
+    </row>
+    <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A120" s="160"/>
+      <c r="B120" s="160"/>
+      <c r="C120" s="160"/>
+      <c r="D120" s="160"/>
+      <c r="E120" s="160"/>
+      <c r="F120" s="160"/>
+      <c r="G120" s="160"/>
+      <c r="H120" s="160"/>
+      <c r="I120" s="160"/>
+    </row>
+    <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A121" s="160"/>
+      <c r="B121" s="160"/>
+      <c r="C121" s="160"/>
+      <c r="D121" s="160"/>
+      <c r="E121" s="160"/>
+      <c r="F121" s="160"/>
+      <c r="G121" s="160"/>
+      <c r="H121" s="160"/>
+      <c r="I121" s="160"/>
+    </row>
+    <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A122" s="160"/>
+      <c r="B122" s="160"/>
+      <c r="C122" s="160"/>
+      <c r="D122" s="160"/>
+      <c r="E122" s="160"/>
+      <c r="F122" s="160"/>
+      <c r="G122" s="160"/>
+      <c r="H122" s="160"/>
+      <c r="I122" s="160"/>
+    </row>
+    <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A123" s="160"/>
+      <c r="B123" s="160"/>
+      <c r="C123" s="160"/>
+      <c r="D123" s="160"/>
+      <c r="E123" s="160"/>
+      <c r="F123" s="160"/>
+      <c r="G123" s="160"/>
+      <c r="H123" s="160"/>
+      <c r="I123" s="160"/>
+    </row>
+    <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A124" s="160"/>
+      <c r="B124" s="160"/>
+      <c r="C124" s="160"/>
+      <c r="D124" s="160"/>
+      <c r="E124" s="160"/>
+      <c r="F124" s="160"/>
+      <c r="G124" s="160"/>
+      <c r="H124" s="160"/>
+      <c r="I124" s="160"/>
+    </row>
+    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A125" s="160"/>
+      <c r="B125" s="160"/>
+      <c r="C125" s="160"/>
+      <c r="D125" s="160"/>
+      <c r="E125" s="160"/>
+      <c r="F125" s="160"/>
+      <c r="G125" s="160"/>
+      <c r="H125" s="160"/>
+      <c r="I125" s="160"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TS 3.2 Pada Paatam and Jatai files 14/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="880">
   <si>
     <t>Date</t>
   </si>
@@ -2630,19 +2630,61 @@
   </si>
   <si>
     <t>7.1.5.1</t>
+  </si>
+  <si>
+    <t>Speech/H1</t>
+  </si>
+  <si>
+    <t>7.1.5.2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=uGsJiqU8MYg</t>
+  </si>
+  <si>
+    <t>7.1.6.1</t>
+  </si>
+  <si>
+    <t>7.1.7.1</t>
+  </si>
+  <si>
+    <t>7.1.8.1</t>
+  </si>
+  <si>
+    <t>7.1.9.1</t>
+  </si>
+  <si>
+    <t>7.1.10.1</t>
+  </si>
+  <si>
+    <t>7.1.11.1</t>
+  </si>
+  <si>
+    <t>7.1.12.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="125" x14ac:knownFonts="1">
+  <fonts count="127" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3427,77 +3469,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="121" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="122" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="124" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="122" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="124" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="121" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="122" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="124" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="116" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="116" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="105" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="123" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="125" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="123" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="123" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="125" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="125" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3505,18 +3549,18 @@
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3530,20 +3574,20 @@
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="122" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="124" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="123" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="125" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3559,41 +3603,41 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3602,25 +3646,26 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3928,9 +3973,9 @@
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6899,8 +6944,8 @@
       <c r="G140" s="6">
         <v>26.55</v>
       </c>
-      <c r="H140" s="11" t="s">
-        <v>152</v>
+      <c r="H140" s="169" t="s">
+        <v>870</v>
       </c>
       <c r="I140" s="1"/>
     </row>
@@ -22789,7 +22834,7 @@
   <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22860,7 +22905,9 @@
       <c r="B3" s="163">
         <v>44148</v>
       </c>
-      <c r="C3" s="160"/>
+      <c r="C3" s="160">
+        <v>50.51</v>
+      </c>
       <c r="D3" s="167">
         <v>1</v>
       </c>
@@ -22874,7 +22921,9 @@
         <v>23.38</v>
       </c>
       <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
+      <c r="I3" s="160" t="s">
+        <v>872</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="160"/>
@@ -22972,13 +23021,27 @@
       <c r="I8" s="160"/>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
-      <c r="B9" s="160"/>
-      <c r="C9" s="160"/>
-      <c r="D9" s="160"/>
-      <c r="E9" s="160"/>
-      <c r="F9" s="160"/>
-      <c r="G9" s="160"/>
+      <c r="A9" s="160">
+        <v>2</v>
+      </c>
+      <c r="B9" s="163">
+        <v>44149</v>
+      </c>
+      <c r="C9" s="160">
+        <v>48.47</v>
+      </c>
+      <c r="D9" s="167">
+        <v>1</v>
+      </c>
+      <c r="E9" s="170" t="s">
+        <v>871</v>
+      </c>
+      <c r="F9" s="160">
+        <v>6.48</v>
+      </c>
+      <c r="G9" s="160">
+        <v>25.17</v>
+      </c>
       <c r="H9" s="160"/>
       <c r="I9" s="160"/>
     </row>
@@ -22986,10 +23049,20 @@
       <c r="A10" s="160"/>
       <c r="B10" s="160"/>
       <c r="C10" s="160"/>
-      <c r="D10" s="160"/>
-      <c r="E10" s="160"/>
-      <c r="F10" s="160"/>
-      <c r="G10" s="160"/>
+      <c r="D10" s="167">
+        <f>+D9+1</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="170" t="s">
+        <v>873</v>
+      </c>
+      <c r="F10" s="160">
+        <f>+G9</f>
+        <v>25.17</v>
+      </c>
+      <c r="G10" s="171">
+        <v>47.5</v>
+      </c>
       <c r="H10" s="160"/>
       <c r="I10" s="160"/>
     </row>
@@ -22997,19 +23070,27 @@
       <c r="A11" s="160"/>
       <c r="B11" s="160"/>
       <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="170"/>
       <c r="F11" s="160"/>
       <c r="G11" s="160"/>
       <c r="H11" s="160"/>
       <c r="I11" s="160"/>
     </row>
     <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="160"/>
-      <c r="B12" s="160"/>
+      <c r="A12" s="160">
+        <v>3</v>
+      </c>
+      <c r="B12" s="163">
+        <v>44150</v>
+      </c>
       <c r="C12" s="160"/>
-      <c r="D12" s="160"/>
-      <c r="E12" s="160"/>
+      <c r="D12" s="167">
+        <v>1</v>
+      </c>
+      <c r="E12" s="170" t="s">
+        <v>874</v>
+      </c>
       <c r="F12" s="160"/>
       <c r="G12" s="160"/>
       <c r="H12" s="160"/>
@@ -23019,8 +23100,13 @@
       <c r="A13" s="160"/>
       <c r="B13" s="160"/>
       <c r="C13" s="160"/>
-      <c r="D13" s="160"/>
-      <c r="E13" s="160"/>
+      <c r="D13" s="167">
+        <f>+D12+1</f>
+        <v>2</v>
+      </c>
+      <c r="E13" s="170" t="s">
+        <v>875</v>
+      </c>
       <c r="F13" s="160"/>
       <c r="G13" s="160"/>
       <c r="H13" s="160"/>
@@ -23030,8 +23116,13 @@
       <c r="A14" s="160"/>
       <c r="B14" s="160"/>
       <c r="C14" s="160"/>
-      <c r="D14" s="160"/>
-      <c r="E14" s="160"/>
+      <c r="D14" s="167">
+        <f t="shared" ref="D14:D17" si="2">+D13+1</f>
+        <v>3</v>
+      </c>
+      <c r="E14" s="170" t="s">
+        <v>876</v>
+      </c>
       <c r="F14" s="160"/>
       <c r="G14" s="160"/>
       <c r="H14" s="160"/>
@@ -23041,8 +23132,13 @@
       <c r="A15" s="160"/>
       <c r="B15" s="160"/>
       <c r="C15" s="160"/>
-      <c r="D15" s="160"/>
-      <c r="E15" s="160"/>
+      <c r="D15" s="167">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E15" s="170" t="s">
+        <v>877</v>
+      </c>
       <c r="F15" s="160"/>
       <c r="G15" s="160"/>
       <c r="H15" s="160"/>
@@ -23052,8 +23148,13 @@
       <c r="A16" s="160"/>
       <c r="B16" s="160"/>
       <c r="C16" s="160"/>
-      <c r="D16" s="160"/>
-      <c r="E16" s="160"/>
+      <c r="D16" s="167">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E16" s="170" t="s">
+        <v>878</v>
+      </c>
       <c r="F16" s="160"/>
       <c r="G16" s="160"/>
       <c r="H16" s="160"/>
@@ -23063,8 +23164,13 @@
       <c r="A17" s="160"/>
       <c r="B17" s="160"/>
       <c r="C17" s="160"/>
-      <c r="D17" s="160"/>
-      <c r="E17" s="160"/>
+      <c r="D17" s="167">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E17" s="170" t="s">
+        <v>879</v>
+      </c>
       <c r="F17" s="160"/>
       <c r="G17" s="160"/>
       <c r="H17" s="160"/>

</xml_diff>

<commit_message>
TS Jatai Excel+TS 2.2 Krama Paatam edit 18/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="902">
   <si>
     <t>Date</t>
   </si>
@@ -2660,19 +2660,103 @@
   </si>
   <si>
     <t>7.1.12.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZtXpcOlSRoc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nQR3G6lPxKo</t>
+  </si>
+  <si>
+    <t>7.1.13.1</t>
+  </si>
+  <si>
+    <t>7.1.14.1</t>
+  </si>
+  <si>
+    <t>7.1.15.1</t>
+  </si>
+  <si>
+    <t>7.1.16.1</t>
+  </si>
+  <si>
+    <t>7.1.17.1</t>
+  </si>
+  <si>
+    <t>7.1.18.1</t>
+  </si>
+  <si>
+    <t>7.1.19.1</t>
+  </si>
+  <si>
+    <t>7.1.20.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wjQRLFXA0Kk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7btHg8WV4FU</t>
+  </si>
+  <si>
+    <t>7.2.1.1</t>
+  </si>
+  <si>
+    <t>7.2.2.1</t>
+  </si>
+  <si>
+    <t>7.2.3.1</t>
+  </si>
+  <si>
+    <t>7.2.4.1</t>
+  </si>
+  <si>
+    <t>7.2.5.1</t>
+  </si>
+  <si>
+    <t>7.2.6.1</t>
+  </si>
+  <si>
+    <t>7.2.7.1</t>
+  </si>
+  <si>
+    <t>7.2.9.1</t>
+  </si>
+  <si>
+    <t>7.2.8.3</t>
+  </si>
+  <si>
+    <t>7.2.10.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="127" x14ac:knownFonts="1">
+  <fonts count="130" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3469,96 +3553,99 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="124" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="127" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="124" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="127" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="124" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="127" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="116" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="116" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="108" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="105" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="128" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="128" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="125" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="125" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="125" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3571,21 +3658,21 @@
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="124" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="127" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="125" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="128" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3600,42 +3687,42 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3643,29 +3730,30 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -22831,10 +22919,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I125"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23043,7 +23131,9 @@
         <v>25.17</v>
       </c>
       <c r="H9" s="160"/>
-      <c r="I9" s="160"/>
+      <c r="I9" s="160" t="s">
+        <v>881</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="160"/>
@@ -23084,17 +23174,25 @@
       <c r="B12" s="163">
         <v>44150</v>
       </c>
-      <c r="C12" s="160"/>
+      <c r="C12" s="160">
+        <v>46.05</v>
+      </c>
       <c r="D12" s="167">
         <v>1</v>
       </c>
       <c r="E12" s="170" t="s">
         <v>874</v>
       </c>
-      <c r="F12" s="160"/>
-      <c r="G12" s="160"/>
+      <c r="F12" s="160">
+        <v>5.44</v>
+      </c>
+      <c r="G12" s="160">
+        <v>18.14</v>
+      </c>
       <c r="H12" s="160"/>
-      <c r="I12" s="160"/>
+      <c r="I12" s="160" t="s">
+        <v>880</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="160"/>
@@ -23107,8 +23205,13 @@
       <c r="E13" s="170" t="s">
         <v>875</v>
       </c>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
+      <c r="F13" s="160">
+        <f>+G12</f>
+        <v>18.14</v>
+      </c>
+      <c r="G13" s="160">
+        <v>26.31</v>
+      </c>
       <c r="H13" s="160"/>
       <c r="I13" s="160"/>
     </row>
@@ -23117,14 +23220,19 @@
       <c r="B14" s="160"/>
       <c r="C14" s="160"/>
       <c r="D14" s="167">
-        <f t="shared" ref="D14:D17" si="2">+D13+1</f>
+        <f t="shared" ref="D14:D16" si="2">+D13+1</f>
         <v>3</v>
       </c>
       <c r="E14" s="170" t="s">
         <v>876</v>
       </c>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
+      <c r="F14" s="160">
+        <f t="shared" ref="F14:F16" si="3">+G13</f>
+        <v>26.31</v>
+      </c>
+      <c r="G14" s="160">
+        <v>29.32</v>
+      </c>
       <c r="H14" s="160"/>
       <c r="I14" s="160"/>
     </row>
@@ -23139,8 +23247,13 @@
       <c r="E15" s="170" t="s">
         <v>877</v>
       </c>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
+      <c r="F15" s="160">
+        <f t="shared" si="3"/>
+        <v>29.32</v>
+      </c>
+      <c r="G15" s="160">
+        <v>41.24</v>
+      </c>
       <c r="H15" s="160"/>
       <c r="I15" s="160"/>
     </row>
@@ -23155,8 +23268,13 @@
       <c r="E16" s="170" t="s">
         <v>878</v>
       </c>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
+      <c r="F16" s="160">
+        <f t="shared" si="3"/>
+        <v>41.24</v>
+      </c>
+      <c r="G16" s="160">
+        <v>45.29</v>
+      </c>
       <c r="H16" s="160"/>
       <c r="I16" s="160"/>
     </row>
@@ -23164,37 +23282,58 @@
       <c r="A17" s="160"/>
       <c r="B17" s="160"/>
       <c r="C17" s="160"/>
-      <c r="D17" s="167">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="E17" s="170" t="s">
-        <v>879</v>
-      </c>
+      <c r="D17" s="167"/>
+      <c r="E17" s="170"/>
       <c r="F17" s="160"/>
       <c r="G17" s="160"/>
       <c r="H17" s="160"/>
       <c r="I17" s="160"/>
     </row>
     <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="160"/>
-      <c r="B18" s="160"/>
-      <c r="C18" s="160"/>
-      <c r="D18" s="160"/>
-      <c r="E18" s="160"/>
-      <c r="F18" s="160"/>
-      <c r="G18" s="160"/>
+      <c r="A18" s="160">
+        <v>4</v>
+      </c>
+      <c r="B18" s="163">
+        <v>44151</v>
+      </c>
+      <c r="C18" s="171">
+        <v>45.5</v>
+      </c>
+      <c r="D18" s="167">
+        <v>1</v>
+      </c>
+      <c r="E18" s="172" t="s">
+        <v>879</v>
+      </c>
+      <c r="F18" s="171">
+        <v>5.2</v>
+      </c>
+      <c r="G18" s="160">
+        <v>9.57</v>
+      </c>
       <c r="H18" s="160"/>
-      <c r="I18" s="160"/>
+      <c r="I18" s="160" t="s">
+        <v>890</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="160"/>
       <c r="B19" s="160"/>
       <c r="C19" s="160"/>
-      <c r="D19" s="160"/>
-      <c r="E19" s="160"/>
-      <c r="F19" s="160"/>
-      <c r="G19" s="160"/>
+      <c r="D19" s="167">
+        <f>+D18+1</f>
+        <v>2</v>
+      </c>
+      <c r="E19" s="172" t="s">
+        <v>882</v>
+      </c>
+      <c r="F19" s="171">
+        <f>+G18</f>
+        <v>9.57</v>
+      </c>
+      <c r="G19" s="160">
+        <v>12.24</v>
+      </c>
       <c r="H19" s="160"/>
       <c r="I19" s="160"/>
     </row>
@@ -23202,10 +23341,20 @@
       <c r="A20" s="160"/>
       <c r="B20" s="160"/>
       <c r="C20" s="160"/>
-      <c r="D20" s="160"/>
-      <c r="E20" s="160"/>
-      <c r="F20" s="160"/>
-      <c r="G20" s="160"/>
+      <c r="D20" s="167">
+        <f t="shared" ref="D20:D26" si="4">+D19+1</f>
+        <v>3</v>
+      </c>
+      <c r="E20" s="172" t="s">
+        <v>883</v>
+      </c>
+      <c r="F20" s="171">
+        <f t="shared" ref="F20:F26" si="5">+G19</f>
+        <v>12.24</v>
+      </c>
+      <c r="G20" s="160">
+        <v>13.55</v>
+      </c>
       <c r="H20" s="160"/>
       <c r="I20" s="160"/>
     </row>
@@ -23213,10 +23362,20 @@
       <c r="A21" s="160"/>
       <c r="B21" s="160"/>
       <c r="C21" s="160"/>
-      <c r="D21" s="160"/>
-      <c r="E21" s="160"/>
-      <c r="F21" s="160"/>
-      <c r="G21" s="160"/>
+      <c r="D21" s="167">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E21" s="172" t="s">
+        <v>884</v>
+      </c>
+      <c r="F21" s="171">
+        <f t="shared" si="5"/>
+        <v>13.55</v>
+      </c>
+      <c r="G21" s="160">
+        <v>17.45</v>
+      </c>
       <c r="H21" s="160"/>
       <c r="I21" s="160"/>
     </row>
@@ -23224,10 +23383,20 @@
       <c r="A22" s="160"/>
       <c r="B22" s="160"/>
       <c r="C22" s="160"/>
-      <c r="D22" s="160"/>
-      <c r="E22" s="160"/>
-      <c r="F22" s="160"/>
-      <c r="G22" s="160"/>
+      <c r="D22" s="167">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="E22" s="172" t="s">
+        <v>885</v>
+      </c>
+      <c r="F22" s="171">
+        <f t="shared" si="5"/>
+        <v>17.45</v>
+      </c>
+      <c r="G22" s="160">
+        <v>19.14</v>
+      </c>
       <c r="H22" s="160"/>
       <c r="I22" s="160"/>
     </row>
@@ -23235,10 +23404,20 @@
       <c r="A23" s="160"/>
       <c r="B23" s="160"/>
       <c r="C23" s="160"/>
-      <c r="D23" s="160"/>
-      <c r="E23" s="160"/>
-      <c r="F23" s="160"/>
-      <c r="G23" s="160"/>
+      <c r="D23" s="167">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="E23" s="172" t="s">
+        <v>886</v>
+      </c>
+      <c r="F23" s="171">
+        <f t="shared" si="5"/>
+        <v>19.14</v>
+      </c>
+      <c r="G23" s="160">
+        <v>22.12</v>
+      </c>
       <c r="H23" s="160"/>
       <c r="I23" s="160"/>
     </row>
@@ -23246,10 +23425,20 @@
       <c r="A24" s="160"/>
       <c r="B24" s="160"/>
       <c r="C24" s="160"/>
-      <c r="D24" s="160"/>
-      <c r="E24" s="160"/>
-      <c r="F24" s="160"/>
-      <c r="G24" s="160"/>
+      <c r="D24" s="167">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="E24" s="172" t="s">
+        <v>887</v>
+      </c>
+      <c r="F24" s="171">
+        <f t="shared" si="5"/>
+        <v>22.12</v>
+      </c>
+      <c r="G24" s="160">
+        <v>28.08</v>
+      </c>
       <c r="H24" s="160"/>
       <c r="I24" s="160"/>
     </row>
@@ -23257,10 +23446,20 @@
       <c r="A25" s="160"/>
       <c r="B25" s="160"/>
       <c r="C25" s="160"/>
-      <c r="D25" s="160"/>
-      <c r="E25" s="160"/>
-      <c r="F25" s="160"/>
-      <c r="G25" s="160"/>
+      <c r="D25" s="167">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="E25" s="172" t="s">
+        <v>888</v>
+      </c>
+      <c r="F25" s="171">
+        <f t="shared" si="5"/>
+        <v>28.08</v>
+      </c>
+      <c r="G25" s="160">
+        <v>42.37</v>
+      </c>
       <c r="H25" s="160"/>
       <c r="I25" s="160"/>
     </row>
@@ -23268,10 +23467,20 @@
       <c r="A26" s="160"/>
       <c r="B26" s="160"/>
       <c r="C26" s="160"/>
-      <c r="D26" s="160"/>
-      <c r="E26" s="160"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="160"/>
+      <c r="D26" s="167">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="E26" s="172" t="s">
+        <v>889</v>
+      </c>
+      <c r="F26" s="171">
+        <f t="shared" si="5"/>
+        <v>42.37</v>
+      </c>
+      <c r="G26" s="160">
+        <v>45.13</v>
+      </c>
       <c r="H26" s="160"/>
       <c r="I26" s="160"/>
     </row>
@@ -23287,24 +23496,50 @@
       <c r="I27" s="160"/>
     </row>
     <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="160"/>
-      <c r="B28" s="160"/>
-      <c r="C28" s="160"/>
-      <c r="D28" s="160"/>
-      <c r="E28" s="160"/>
-      <c r="F28" s="160"/>
-      <c r="G28" s="160"/>
+      <c r="A28" s="160">
+        <v>5</v>
+      </c>
+      <c r="B28" s="174">
+        <v>44152</v>
+      </c>
+      <c r="C28" s="160">
+        <v>49.08</v>
+      </c>
+      <c r="D28" s="167">
+        <v>1</v>
+      </c>
+      <c r="E28" s="173" t="s">
+        <v>892</v>
+      </c>
+      <c r="F28" s="160">
+        <v>7.27</v>
+      </c>
+      <c r="G28" s="160">
+        <v>22.25</v>
+      </c>
       <c r="H28" s="160"/>
-      <c r="I28" s="160"/>
+      <c r="I28" s="160" t="s">
+        <v>891</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="160"/>
       <c r="B29" s="160"/>
       <c r="C29" s="160"/>
-      <c r="D29" s="160"/>
-      <c r="E29" s="160"/>
-      <c r="F29" s="160"/>
-      <c r="G29" s="160"/>
+      <c r="D29" s="167">
+        <f>+D28+1</f>
+        <v>2</v>
+      </c>
+      <c r="E29" s="173" t="s">
+        <v>893</v>
+      </c>
+      <c r="F29" s="160">
+        <f>+G28</f>
+        <v>22.25</v>
+      </c>
+      <c r="G29" s="160">
+        <v>32.270000000000003</v>
+      </c>
       <c r="H29" s="160"/>
       <c r="I29" s="160"/>
     </row>
@@ -23312,10 +23547,20 @@
       <c r="A30" s="160"/>
       <c r="B30" s="160"/>
       <c r="C30" s="160"/>
-      <c r="D30" s="160"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
-      <c r="G30" s="160"/>
+      <c r="D30" s="167">
+        <f t="shared" ref="D30:D31" si="6">+D29+1</f>
+        <v>3</v>
+      </c>
+      <c r="E30" s="173" t="s">
+        <v>894</v>
+      </c>
+      <c r="F30" s="160">
+        <f t="shared" ref="F30:F31" si="7">+G29</f>
+        <v>32.270000000000003</v>
+      </c>
+      <c r="G30" s="171">
+        <v>40</v>
+      </c>
       <c r="H30" s="160"/>
       <c r="I30" s="160"/>
     </row>
@@ -23323,10 +23568,20 @@
       <c r="A31" s="160"/>
       <c r="B31" s="160"/>
       <c r="C31" s="160"/>
-      <c r="D31" s="160"/>
-      <c r="E31" s="160"/>
-      <c r="F31" s="160"/>
-      <c r="G31" s="160"/>
+      <c r="D31" s="167">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E31" s="173" t="s">
+        <v>895</v>
+      </c>
+      <c r="F31" s="171">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="G31" s="160">
+        <v>48.05</v>
+      </c>
       <c r="H31" s="160"/>
       <c r="I31" s="160"/>
     </row>
@@ -23334,8 +23589,7 @@
       <c r="A32" s="160"/>
       <c r="B32" s="160"/>
       <c r="C32" s="160"/>
-      <c r="D32" s="160"/>
-      <c r="E32" s="160"/>
+      <c r="D32" s="167"/>
       <c r="F32" s="160"/>
       <c r="G32" s="160"/>
       <c r="H32" s="160"/>
@@ -23353,13 +23607,27 @@
       <c r="I33" s="160"/>
     </row>
     <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="160"/>
-      <c r="B34" s="160"/>
-      <c r="C34" s="160"/>
-      <c r="D34" s="160"/>
-      <c r="E34" s="160"/>
-      <c r="F34" s="160"/>
-      <c r="G34" s="160"/>
+      <c r="A34" s="160">
+        <v>6</v>
+      </c>
+      <c r="B34" s="163">
+        <v>44153</v>
+      </c>
+      <c r="C34" s="160">
+        <v>42.25</v>
+      </c>
+      <c r="D34" s="167">
+        <v>1</v>
+      </c>
+      <c r="E34" s="173" t="s">
+        <v>896</v>
+      </c>
+      <c r="F34" s="160">
+        <v>5.19</v>
+      </c>
+      <c r="G34" s="160">
+        <v>24.27</v>
+      </c>
       <c r="H34" s="160"/>
       <c r="I34" s="160"/>
     </row>
@@ -23367,10 +23635,20 @@
       <c r="A35" s="160"/>
       <c r="B35" s="160"/>
       <c r="C35" s="160"/>
-      <c r="D35" s="160"/>
-      <c r="E35" s="160"/>
-      <c r="F35" s="160"/>
-      <c r="G35" s="160"/>
+      <c r="D35" s="167">
+        <f>+D34+1</f>
+        <v>2</v>
+      </c>
+      <c r="E35" s="173" t="s">
+        <v>897</v>
+      </c>
+      <c r="F35" s="171">
+        <f>+G34</f>
+        <v>24.27</v>
+      </c>
+      <c r="G35" s="160">
+        <v>34.51</v>
+      </c>
       <c r="H35" s="160"/>
       <c r="I35" s="160"/>
     </row>
@@ -23378,10 +23656,20 @@
       <c r="A36" s="160"/>
       <c r="B36" s="160"/>
       <c r="C36" s="160"/>
-      <c r="D36" s="160"/>
-      <c r="E36" s="160"/>
-      <c r="F36" s="160"/>
-      <c r="G36" s="160"/>
+      <c r="D36" s="167">
+        <f t="shared" ref="D36" si="8">+D35+1</f>
+        <v>3</v>
+      </c>
+      <c r="E36" s="173" t="s">
+        <v>898</v>
+      </c>
+      <c r="F36" s="171">
+        <f>+G35</f>
+        <v>34.51</v>
+      </c>
+      <c r="G36" s="160">
+        <v>41.52</v>
+      </c>
       <c r="H36" s="160"/>
       <c r="I36" s="160"/>
     </row>
@@ -23397,11 +23685,20 @@
       <c r="I37" s="160"/>
     </row>
     <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="160"/>
-      <c r="B38" s="160"/>
+      <c r="A38" s="160">
+        <v>7</v>
+      </c>
+      <c r="B38" s="163">
+        <v>44154</v>
+      </c>
       <c r="C38" s="160"/>
-      <c r="D38" s="160"/>
-      <c r="E38" s="160"/>
+      <c r="D38" s="167">
+        <f>+D37+1</f>
+        <v>1</v>
+      </c>
+      <c r="E38" s="175" t="s">
+        <v>900</v>
+      </c>
       <c r="F38" s="160"/>
       <c r="G38" s="160"/>
       <c r="H38" s="160"/>
@@ -23411,8 +23708,13 @@
       <c r="A39" s="160"/>
       <c r="B39" s="160"/>
       <c r="C39" s="160"/>
-      <c r="D39" s="160"/>
-      <c r="E39" s="160"/>
+      <c r="D39" s="167">
+        <f t="shared" ref="D39:D40" si="9">+D38+1</f>
+        <v>2</v>
+      </c>
+      <c r="E39" s="175" t="s">
+        <v>899</v>
+      </c>
       <c r="F39" s="160"/>
       <c r="G39" s="160"/>
       <c r="H39" s="160"/>
@@ -23422,8 +23724,13 @@
       <c r="A40" s="160"/>
       <c r="B40" s="160"/>
       <c r="C40" s="160"/>
-      <c r="D40" s="160"/>
-      <c r="E40" s="160"/>
+      <c r="D40" s="167">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="E40" s="175" t="s">
+        <v>901</v>
+      </c>
       <c r="F40" s="160"/>
       <c r="G40" s="160"/>
       <c r="H40" s="160"/>
@@ -24353,17 +24660,6 @@
       <c r="H124" s="160"/>
       <c r="I124" s="160"/>
     </row>
-    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A125" s="160"/>
-      <c r="B125" s="160"/>
-      <c r="C125" s="160"/>
-      <c r="D125" s="160"/>
-      <c r="E125" s="160"/>
-      <c r="F125" s="160"/>
-      <c r="G125" s="160"/>
-      <c r="H125" s="160"/>
-      <c r="I125" s="160"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
TS 3.33 Pada Paatam pushed 20/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="913">
   <si>
     <t>Date</t>
   </si>
@@ -2722,10 +2722,43 @@
     <t>7.2.9.1</t>
   </si>
   <si>
-    <t>7.2.8.3</t>
-  </si>
-  <si>
     <t>7.2.10.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=X7zf06xcLWw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RB9Dlb_ryp8</t>
+  </si>
+  <si>
+    <t>7.2.7.3</t>
+  </si>
+  <si>
+    <t>7.2.8.1</t>
+  </si>
+  <si>
+    <t>7.2.7.2</t>
+  </si>
+  <si>
+    <t>7.2.9.2</t>
+  </si>
+  <si>
+    <t>7.2.9.3</t>
+  </si>
+  <si>
+    <t>7.2.11.1</t>
+  </si>
+  <si>
+    <t>7.2.12.1</t>
+  </si>
+  <si>
+    <t>7.2.13.1</t>
+  </si>
+  <si>
+    <t>7.2.14.1</t>
+  </si>
+  <si>
+    <t>7.2.15.1</t>
   </si>
 </sst>
 </file>
@@ -22921,8 +22954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23629,7 +23662,9 @@
         <v>24.27</v>
       </c>
       <c r="H34" s="160"/>
-      <c r="I34" s="160"/>
+      <c r="I34" s="160" t="s">
+        <v>902</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="160"/>
@@ -23670,7 +23705,9 @@
       <c r="G36" s="160">
         <v>41.52</v>
       </c>
-      <c r="H36" s="160"/>
+      <c r="H36" s="175" t="s">
+        <v>905</v>
+      </c>
       <c r="I36" s="160"/>
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23691,18 +23728,26 @@
       <c r="B38" s="163">
         <v>44154</v>
       </c>
-      <c r="C38" s="160"/>
+      <c r="C38" s="160">
+        <v>39.49</v>
+      </c>
       <c r="D38" s="167">
         <f>+D37+1</f>
         <v>1</v>
       </c>
       <c r="E38" s="175" t="s">
-        <v>900</v>
-      </c>
-      <c r="F38" s="160"/>
-      <c r="G38" s="160"/>
+        <v>903</v>
+      </c>
+      <c r="F38" s="160">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G38" s="160">
+        <v>11.54</v>
+      </c>
       <c r="H38" s="160"/>
-      <c r="I38" s="160"/>
+      <c r="I38" s="160" t="s">
+        <v>901</v>
+      </c>
     </row>
     <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="160"/>
@@ -23713,10 +23758,15 @@
         <v>2</v>
       </c>
       <c r="E39" s="175" t="s">
-        <v>899</v>
-      </c>
-      <c r="F39" s="160"/>
-      <c r="G39" s="160"/>
+        <v>904</v>
+      </c>
+      <c r="F39" s="160">
+        <f>+G38</f>
+        <v>11.54</v>
+      </c>
+      <c r="G39" s="160">
+        <v>33.31</v>
+      </c>
       <c r="H39" s="160"/>
       <c r="I39" s="160"/>
     </row>
@@ -23729,11 +23779,18 @@
         <v>3</v>
       </c>
       <c r="E40" s="175" t="s">
-        <v>901</v>
-      </c>
-      <c r="F40" s="160"/>
-      <c r="G40" s="160"/>
-      <c r="H40" s="160"/>
+        <v>899</v>
+      </c>
+      <c r="F40" s="160">
+        <f>+G39</f>
+        <v>33.31</v>
+      </c>
+      <c r="G40" s="160">
+        <v>39.090000000000003</v>
+      </c>
+      <c r="H40" s="175" t="s">
+        <v>906</v>
+      </c>
       <c r="I40" s="160"/>
     </row>
     <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23748,11 +23805,20 @@
       <c r="I41" s="160"/>
     </row>
     <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="160"/>
-      <c r="B42" s="160"/>
+      <c r="A42" s="160">
+        <v>8</v>
+      </c>
+      <c r="B42" s="163">
+        <v>44155</v>
+      </c>
       <c r="C42" s="160"/>
-      <c r="D42" s="160"/>
-      <c r="E42" s="160"/>
+      <c r="D42" s="167">
+        <f>+D41+1</f>
+        <v>1</v>
+      </c>
+      <c r="E42" s="175" t="s">
+        <v>907</v>
+      </c>
       <c r="F42" s="160"/>
       <c r="G42" s="160"/>
       <c r="H42" s="160"/>
@@ -23762,9 +23828,17 @@
       <c r="A43" s="160"/>
       <c r="B43" s="160"/>
       <c r="C43" s="160"/>
-      <c r="D43" s="160"/>
-      <c r="E43" s="160"/>
-      <c r="F43" s="160"/>
+      <c r="D43" s="167">
+        <f t="shared" ref="D43:D48" si="10">+D42+1</f>
+        <v>2</v>
+      </c>
+      <c r="E43" s="175" t="s">
+        <v>900</v>
+      </c>
+      <c r="F43" s="171">
+        <f>+G42</f>
+        <v>0</v>
+      </c>
       <c r="G43" s="160"/>
       <c r="H43" s="160"/>
       <c r="I43" s="160"/>
@@ -23773,9 +23847,17 @@
       <c r="A44" s="160"/>
       <c r="B44" s="160"/>
       <c r="C44" s="160"/>
-      <c r="D44" s="160"/>
-      <c r="E44" s="160"/>
-      <c r="F44" s="160"/>
+      <c r="D44" s="167">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="E44" s="175" t="s">
+        <v>908</v>
+      </c>
+      <c r="F44" s="171">
+        <f t="shared" ref="F44:F48" si="11">+G43</f>
+        <v>0</v>
+      </c>
       <c r="G44" s="160"/>
       <c r="H44" s="160"/>
       <c r="I44" s="160"/>
@@ -23784,9 +23866,17 @@
       <c r="A45" s="160"/>
       <c r="B45" s="160"/>
       <c r="C45" s="160"/>
-      <c r="D45" s="160"/>
-      <c r="E45" s="160"/>
-      <c r="F45" s="160"/>
+      <c r="D45" s="167">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="E45" s="175" t="s">
+        <v>909</v>
+      </c>
+      <c r="F45" s="171">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="G45" s="160"/>
       <c r="H45" s="160"/>
       <c r="I45" s="160"/>
@@ -23795,9 +23885,17 @@
       <c r="A46" s="160"/>
       <c r="B46" s="160"/>
       <c r="C46" s="160"/>
-      <c r="D46" s="160"/>
-      <c r="E46" s="160"/>
-      <c r="F46" s="160"/>
+      <c r="D46" s="167">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="E46" s="175" t="s">
+        <v>910</v>
+      </c>
+      <c r="F46" s="171">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="G46" s="160"/>
       <c r="H46" s="160"/>
       <c r="I46" s="160"/>
@@ -23806,9 +23904,17 @@
       <c r="A47" s="160"/>
       <c r="B47" s="160"/>
       <c r="C47" s="160"/>
-      <c r="D47" s="160"/>
-      <c r="E47" s="160"/>
-      <c r="F47" s="160"/>
+      <c r="D47" s="167">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="E47" s="175" t="s">
+        <v>911</v>
+      </c>
+      <c r="F47" s="171">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="G47" s="160"/>
       <c r="H47" s="160"/>
       <c r="I47" s="160"/>
@@ -23817,9 +23923,17 @@
       <c r="A48" s="160"/>
       <c r="B48" s="160"/>
       <c r="C48" s="160"/>
-      <c r="D48" s="160"/>
-      <c r="E48" s="160"/>
-      <c r="F48" s="160"/>
+      <c r="D48" s="167">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="E48" s="175" t="s">
+        <v>912</v>
+      </c>
+      <c r="F48" s="171">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="G48" s="160"/>
       <c r="H48" s="160"/>
       <c r="I48" s="160"/>

</xml_diff>

<commit_message>
TS Jatai working changes 22/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="937">
   <si>
     <t>Date</t>
   </si>
@@ -2759,19 +2759,109 @@
   </si>
   <si>
     <t>7.2.15.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-jIZuc4ooDc</t>
+  </si>
+  <si>
+    <t>7.2.16.1</t>
+  </si>
+  <si>
+    <t>7.2.17.1</t>
+  </si>
+  <si>
+    <t>7.2.18.1</t>
+  </si>
+  <si>
+    <t>7.2.19.1</t>
+  </si>
+  <si>
+    <t>7.2.20.1</t>
+  </si>
+  <si>
+    <t>7.3.1.1</t>
+  </si>
+  <si>
+    <t>7.3.1.2</t>
+  </si>
+  <si>
+    <t>7.3.2.1</t>
+  </si>
+  <si>
+    <t>7.3.3.1</t>
+  </si>
+  <si>
+    <t>7.3.4.1</t>
+  </si>
+  <si>
+    <t>7.3.5.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fWVHDASHQEc</t>
+  </si>
+  <si>
+    <t>7.3.6.1</t>
+  </si>
+  <si>
+    <t>7.3.7.1</t>
+  </si>
+  <si>
+    <t>7.3.8.1</t>
+  </si>
+  <si>
+    <t>7.3.9.1</t>
+  </si>
+  <si>
+    <t>7.3.10.1</t>
+  </si>
+  <si>
+    <t>7.3.11.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=SuG4jjAl1KQ</t>
+  </si>
+  <si>
+    <t>7.3.10.3</t>
+  </si>
+  <si>
+    <t>7.3.10.2</t>
+  </si>
+  <si>
+    <t>7.3.12.1</t>
+  </si>
+  <si>
+    <t>7.3.13.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="130" x14ac:knownFonts="1">
+  <fonts count="133" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3586,96 +3676,99 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="127" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="130" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="127" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="130" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="127" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="130" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="116" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="108" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="131" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="131" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="128" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="128" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="128" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3688,21 +3781,21 @@
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="127" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="130" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="128" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="131" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3717,42 +3810,42 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3760,32 +3853,32 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -22954,8 +23047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23811,7 +23904,9 @@
       <c r="B42" s="163">
         <v>44155</v>
       </c>
-      <c r="C42" s="160"/>
+      <c r="C42" s="171">
+        <v>49.1</v>
+      </c>
       <c r="D42" s="167">
         <f>+D41+1</f>
         <v>1</v>
@@ -23819,17 +23914,23 @@
       <c r="E42" s="175" t="s">
         <v>907</v>
       </c>
-      <c r="F42" s="160"/>
-      <c r="G42" s="160"/>
+      <c r="F42" s="160">
+        <v>2.37</v>
+      </c>
+      <c r="G42" s="160">
+        <v>6.15</v>
+      </c>
       <c r="H42" s="160"/>
-      <c r="I42" s="160"/>
+      <c r="I42" s="160" t="s">
+        <v>913</v>
+      </c>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="160"/>
       <c r="B43" s="160"/>
       <c r="C43" s="160"/>
       <c r="D43" s="167">
-        <f t="shared" ref="D43:D48" si="10">+D42+1</f>
+        <f t="shared" ref="D43:D54" si="10">+D42+1</f>
         <v>2</v>
       </c>
       <c r="E43" s="175" t="s">
@@ -23837,9 +23938,11 @@
       </c>
       <c r="F43" s="171">
         <f>+G42</f>
-        <v>0</v>
-      </c>
-      <c r="G43" s="160"/>
+        <v>6.15</v>
+      </c>
+      <c r="G43" s="160">
+        <v>18.28</v>
+      </c>
       <c r="H43" s="160"/>
       <c r="I43" s="160"/>
     </row>
@@ -23855,10 +23958,12 @@
         <v>908</v>
       </c>
       <c r="F44" s="171">
-        <f t="shared" ref="F44:F48" si="11">+G43</f>
-        <v>0</v>
-      </c>
-      <c r="G44" s="160"/>
+        <f t="shared" ref="F44:F54" si="11">+G43</f>
+        <v>18.28</v>
+      </c>
+      <c r="G44" s="160">
+        <v>24.23</v>
+      </c>
       <c r="H44" s="160"/>
       <c r="I44" s="160"/>
     </row>
@@ -23875,9 +23980,11 @@
       </c>
       <c r="F45" s="171">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="160"/>
+        <v>24.23</v>
+      </c>
+      <c r="G45" s="160">
+        <v>28.19</v>
+      </c>
       <c r="H45" s="160"/>
       <c r="I45" s="160"/>
     </row>
@@ -23894,9 +24001,11 @@
       </c>
       <c r="F46" s="171">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="160"/>
+        <v>28.19</v>
+      </c>
+      <c r="G46" s="160">
+        <v>30.34</v>
+      </c>
       <c r="H46" s="160"/>
       <c r="I46" s="160"/>
     </row>
@@ -23913,9 +24022,11 @@
       </c>
       <c r="F47" s="171">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="G47" s="160"/>
+        <v>30.34</v>
+      </c>
+      <c r="G47" s="160">
+        <v>34.200000000000003</v>
+      </c>
       <c r="H47" s="160"/>
       <c r="I47" s="160"/>
     </row>
@@ -23932,9 +24043,11 @@
       </c>
       <c r="F48" s="171">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="G48" s="160"/>
+        <v>34.200000000000003</v>
+      </c>
+      <c r="G48" s="160">
+        <v>35.43</v>
+      </c>
       <c r="H48" s="160"/>
       <c r="I48" s="160"/>
     </row>
@@ -23942,10 +24055,20 @@
       <c r="A49" s="160"/>
       <c r="B49" s="160"/>
       <c r="C49" s="160"/>
-      <c r="D49" s="160"/>
-      <c r="E49" s="160"/>
-      <c r="F49" s="160"/>
-      <c r="G49" s="160"/>
+      <c r="D49" s="167">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="E49" s="176" t="s">
+        <v>914</v>
+      </c>
+      <c r="F49" s="171">
+        <f t="shared" si="11"/>
+        <v>35.43</v>
+      </c>
+      <c r="G49" s="160">
+        <v>36.51</v>
+      </c>
       <c r="H49" s="160"/>
       <c r="I49" s="160"/>
     </row>
@@ -23953,10 +24076,20 @@
       <c r="A50" s="160"/>
       <c r="B50" s="160"/>
       <c r="C50" s="160"/>
-      <c r="D50" s="160"/>
-      <c r="E50" s="160"/>
-      <c r="F50" s="160"/>
-      <c r="G50" s="160"/>
+      <c r="D50" s="167">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="E50" s="176" t="s">
+        <v>915</v>
+      </c>
+      <c r="F50" s="171">
+        <f t="shared" si="11"/>
+        <v>36.51</v>
+      </c>
+      <c r="G50" s="160">
+        <v>38.31</v>
+      </c>
       <c r="H50" s="160"/>
       <c r="I50" s="160"/>
     </row>
@@ -23964,10 +24097,20 @@
       <c r="A51" s="160"/>
       <c r="B51" s="160"/>
       <c r="C51" s="160"/>
-      <c r="D51" s="160"/>
-      <c r="E51" s="160"/>
-      <c r="F51" s="160"/>
-      <c r="G51" s="160"/>
+      <c r="D51" s="167">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="E51" s="176" t="s">
+        <v>916</v>
+      </c>
+      <c r="F51" s="171">
+        <f t="shared" si="11"/>
+        <v>38.31</v>
+      </c>
+      <c r="G51" s="160">
+        <v>39.24</v>
+      </c>
       <c r="H51" s="160"/>
       <c r="I51" s="160"/>
     </row>
@@ -23975,10 +24118,20 @@
       <c r="A52" s="160"/>
       <c r="B52" s="160"/>
       <c r="C52" s="160"/>
-      <c r="D52" s="160"/>
-      <c r="E52" s="160"/>
-      <c r="F52" s="160"/>
-      <c r="G52" s="160"/>
+      <c r="D52" s="167">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="E52" s="176" t="s">
+        <v>917</v>
+      </c>
+      <c r="F52" s="171">
+        <f t="shared" si="11"/>
+        <v>39.24</v>
+      </c>
+      <c r="G52" s="160">
+        <v>42.04</v>
+      </c>
       <c r="H52" s="160"/>
       <c r="I52" s="160"/>
     </row>
@@ -23986,10 +24139,20 @@
       <c r="A53" s="160"/>
       <c r="B53" s="160"/>
       <c r="C53" s="160"/>
-      <c r="D53" s="160"/>
-      <c r="E53" s="160"/>
-      <c r="F53" s="160"/>
-      <c r="G53" s="160"/>
+      <c r="D53" s="167">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="E53" s="176" t="s">
+        <v>918</v>
+      </c>
+      <c r="F53" s="171">
+        <f t="shared" si="11"/>
+        <v>42.04</v>
+      </c>
+      <c r="G53" s="171">
+        <v>45.4</v>
+      </c>
       <c r="H53" s="160"/>
       <c r="I53" s="160"/>
     </row>
@@ -23997,11 +24160,23 @@
       <c r="A54" s="160"/>
       <c r="B54" s="160"/>
       <c r="C54" s="160"/>
-      <c r="D54" s="160"/>
-      <c r="E54" s="160"/>
-      <c r="F54" s="160"/>
-      <c r="G54" s="160"/>
-      <c r="H54" s="160"/>
+      <c r="D54" s="167">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="E54" s="176" t="s">
+        <v>919</v>
+      </c>
+      <c r="F54" s="171">
+        <f t="shared" si="11"/>
+        <v>45.4</v>
+      </c>
+      <c r="G54" s="160">
+        <v>48.36</v>
+      </c>
+      <c r="H54" s="176" t="s">
+        <v>919</v>
+      </c>
       <c r="I54" s="160"/>
     </row>
     <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24016,24 +24191,51 @@
       <c r="I55" s="160"/>
     </row>
     <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="160"/>
-      <c r="B56" s="160"/>
-      <c r="C56" s="160"/>
-      <c r="D56" s="160"/>
-      <c r="E56" s="160"/>
-      <c r="F56" s="160"/>
-      <c r="G56" s="160"/>
+      <c r="A56" s="160">
+        <v>9</v>
+      </c>
+      <c r="B56" s="163">
+        <v>44156</v>
+      </c>
+      <c r="C56" s="171">
+        <v>53</v>
+      </c>
+      <c r="D56" s="167">
+        <f>+D55+1</f>
+        <v>1</v>
+      </c>
+      <c r="E56" s="176" t="s">
+        <v>920</v>
+      </c>
+      <c r="F56" s="160">
+        <v>2.04</v>
+      </c>
+      <c r="G56" s="160">
+        <v>12.15</v>
+      </c>
       <c r="H56" s="160"/>
-      <c r="I56" s="160"/>
+      <c r="I56" s="160" t="s">
+        <v>925</v>
+      </c>
     </row>
     <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="160"/>
       <c r="B57" s="160"/>
       <c r="C57" s="160"/>
-      <c r="D57" s="160"/>
-      <c r="E57" s="160"/>
-      <c r="F57" s="160"/>
-      <c r="G57" s="160"/>
+      <c r="D57" s="167">
+        <f t="shared" ref="D57:D61" si="12">+D56+1</f>
+        <v>2</v>
+      </c>
+      <c r="E57" s="176" t="s">
+        <v>921</v>
+      </c>
+      <c r="F57" s="160">
+        <f>+G56</f>
+        <v>12.15</v>
+      </c>
+      <c r="G57" s="160">
+        <v>18.14</v>
+      </c>
       <c r="H57" s="160"/>
       <c r="I57" s="160"/>
     </row>
@@ -24041,10 +24243,20 @@
       <c r="A58" s="160"/>
       <c r="B58" s="160"/>
       <c r="C58" s="160"/>
-      <c r="D58" s="160"/>
-      <c r="E58" s="160"/>
-      <c r="F58" s="160"/>
-      <c r="G58" s="160"/>
+      <c r="D58" s="167">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="E58" s="176" t="s">
+        <v>922</v>
+      </c>
+      <c r="F58" s="160">
+        <f t="shared" ref="F58:F61" si="13">+G57</f>
+        <v>18.14</v>
+      </c>
+      <c r="G58" s="160">
+        <v>25.51</v>
+      </c>
       <c r="H58" s="160"/>
       <c r="I58" s="160"/>
     </row>
@@ -24052,10 +24264,20 @@
       <c r="A59" s="160"/>
       <c r="B59" s="160"/>
       <c r="C59" s="160"/>
-      <c r="D59" s="160"/>
-      <c r="E59" s="160"/>
-      <c r="F59" s="160"/>
-      <c r="G59" s="160"/>
+      <c r="D59" s="167">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="E59" s="176" t="s">
+        <v>923</v>
+      </c>
+      <c r="F59" s="160">
+        <f t="shared" si="13"/>
+        <v>25.51</v>
+      </c>
+      <c r="G59" s="160">
+        <v>31.52</v>
+      </c>
       <c r="H59" s="160"/>
       <c r="I59" s="160"/>
     </row>
@@ -24063,10 +24285,20 @@
       <c r="A60" s="160"/>
       <c r="B60" s="160"/>
       <c r="C60" s="160"/>
-      <c r="D60" s="160"/>
-      <c r="E60" s="160"/>
-      <c r="F60" s="160"/>
-      <c r="G60" s="160"/>
+      <c r="D60" s="167">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="E60" s="176" t="s">
+        <v>924</v>
+      </c>
+      <c r="F60" s="160">
+        <f t="shared" si="13"/>
+        <v>31.52</v>
+      </c>
+      <c r="G60" s="160">
+        <v>45.04</v>
+      </c>
       <c r="H60" s="160"/>
       <c r="I60" s="160"/>
     </row>
@@ -24074,10 +24306,20 @@
       <c r="A61" s="160"/>
       <c r="B61" s="160"/>
       <c r="C61" s="160"/>
-      <c r="D61" s="160"/>
-      <c r="E61" s="160"/>
-      <c r="F61" s="160"/>
-      <c r="G61" s="160"/>
+      <c r="D61" s="167">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="E61" s="177" t="s">
+        <v>926</v>
+      </c>
+      <c r="F61" s="160">
+        <f t="shared" si="13"/>
+        <v>45.04</v>
+      </c>
+      <c r="G61" s="171">
+        <v>52</v>
+      </c>
       <c r="H61" s="160"/>
       <c r="I61" s="160"/>
     </row>
@@ -24085,8 +24327,7 @@
       <c r="A62" s="160"/>
       <c r="B62" s="160"/>
       <c r="C62" s="160"/>
-      <c r="D62" s="160"/>
-      <c r="E62" s="160"/>
+      <c r="D62" s="167"/>
       <c r="F62" s="160"/>
       <c r="G62" s="160"/>
       <c r="H62" s="160"/>
@@ -24104,24 +24345,51 @@
       <c r="I63" s="160"/>
     </row>
     <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A64" s="160"/>
-      <c r="B64" s="160"/>
-      <c r="C64" s="160"/>
-      <c r="D64" s="160"/>
-      <c r="E64" s="160"/>
-      <c r="F64" s="160"/>
-      <c r="G64" s="160"/>
+      <c r="A64" s="160">
+        <v>10</v>
+      </c>
+      <c r="B64" s="163">
+        <v>44157</v>
+      </c>
+      <c r="C64" s="171">
+        <v>37.5</v>
+      </c>
+      <c r="D64" s="167">
+        <f>+D63+1</f>
+        <v>1</v>
+      </c>
+      <c r="E64" s="177" t="s">
+        <v>927</v>
+      </c>
+      <c r="F64" s="160">
+        <v>0.59</v>
+      </c>
+      <c r="G64" s="160">
+        <v>15.52</v>
+      </c>
       <c r="H64" s="160"/>
-      <c r="I64" s="160"/>
+      <c r="I64" s="160" t="s">
+        <v>932</v>
+      </c>
     </row>
     <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="160"/>
       <c r="B65" s="160"/>
       <c r="C65" s="160"/>
-      <c r="D65" s="160"/>
-      <c r="E65" s="160"/>
-      <c r="F65" s="160"/>
-      <c r="G65" s="160"/>
+      <c r="D65" s="167">
+        <f t="shared" ref="D65:D72" si="14">+D64+1</f>
+        <v>2</v>
+      </c>
+      <c r="E65" s="177" t="s">
+        <v>928</v>
+      </c>
+      <c r="F65" s="171">
+        <f>+G64</f>
+        <v>15.52</v>
+      </c>
+      <c r="G65" s="160">
+        <v>21.33</v>
+      </c>
       <c r="H65" s="160"/>
       <c r="I65" s="160"/>
     </row>
@@ -24129,10 +24397,20 @@
       <c r="A66" s="160"/>
       <c r="B66" s="160"/>
       <c r="C66" s="160"/>
-      <c r="D66" s="160"/>
-      <c r="E66" s="160"/>
-      <c r="F66" s="160"/>
-      <c r="G66" s="160"/>
+      <c r="D66" s="167">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="E66" s="177" t="s">
+        <v>929</v>
+      </c>
+      <c r="F66" s="171">
+        <f t="shared" ref="F66:F68" si="15">+G65</f>
+        <v>21.33</v>
+      </c>
+      <c r="G66" s="160">
+        <v>31.19</v>
+      </c>
       <c r="H66" s="160"/>
       <c r="I66" s="160"/>
     </row>
@@ -24140,30 +24418,51 @@
       <c r="A67" s="160"/>
       <c r="B67" s="160"/>
       <c r="C67" s="160"/>
-      <c r="D67" s="160"/>
-      <c r="E67" s="160"/>
-      <c r="F67" s="160"/>
-      <c r="G67" s="160"/>
-      <c r="H67" s="160"/>
+      <c r="D67" s="167">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="E67" s="177" t="s">
+        <v>930</v>
+      </c>
+      <c r="F67" s="171">
+        <f t="shared" si="15"/>
+        <v>31.19</v>
+      </c>
+      <c r="G67" s="160">
+        <v>37.15</v>
+      </c>
+      <c r="H67" s="178" t="s">
+        <v>934</v>
+      </c>
       <c r="I67" s="160"/>
     </row>
     <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="160"/>
       <c r="B68" s="160"/>
       <c r="C68" s="160"/>
-      <c r="D68" s="160"/>
-      <c r="E68" s="160"/>
-      <c r="F68" s="160"/>
+      <c r="D68" s="167"/>
+      <c r="E68" s="177"/>
+      <c r="F68" s="171"/>
       <c r="G68" s="160"/>
       <c r="H68" s="160"/>
       <c r="I68" s="160"/>
     </row>
     <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="160"/>
-      <c r="B69" s="160"/>
+      <c r="A69" s="160">
+        <v>11</v>
+      </c>
+      <c r="B69" s="163">
+        <v>44158</v>
+      </c>
       <c r="C69" s="160"/>
-      <c r="D69" s="160"/>
-      <c r="E69" s="160"/>
+      <c r="D69" s="167">
+        <f>+D68+1</f>
+        <v>1</v>
+      </c>
+      <c r="E69" s="178" t="s">
+        <v>933</v>
+      </c>
       <c r="F69" s="160"/>
       <c r="G69" s="160"/>
       <c r="H69" s="160"/>
@@ -24173,9 +24472,17 @@
       <c r="A70" s="160"/>
       <c r="B70" s="160"/>
       <c r="C70" s="160"/>
-      <c r="D70" s="160"/>
-      <c r="E70" s="160"/>
-      <c r="F70" s="160"/>
+      <c r="D70" s="167">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="E70" s="178" t="s">
+        <v>931</v>
+      </c>
+      <c r="F70" s="160">
+        <f>+G69</f>
+        <v>0</v>
+      </c>
       <c r="G70" s="160"/>
       <c r="H70" s="160"/>
       <c r="I70" s="160"/>
@@ -24184,9 +24491,17 @@
       <c r="A71" s="160"/>
       <c r="B71" s="160"/>
       <c r="C71" s="160"/>
-      <c r="D71" s="160"/>
-      <c r="E71" s="160"/>
-      <c r="F71" s="160"/>
+      <c r="D71" s="167">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="E71" s="178" t="s">
+        <v>935</v>
+      </c>
+      <c r="F71" s="160">
+        <f t="shared" ref="F71:F72" si="16">+G70</f>
+        <v>0</v>
+      </c>
       <c r="G71" s="160"/>
       <c r="H71" s="160"/>
       <c r="I71" s="160"/>
@@ -24195,9 +24510,17 @@
       <c r="A72" s="160"/>
       <c r="B72" s="160"/>
       <c r="C72" s="160"/>
-      <c r="D72" s="160"/>
-      <c r="E72" s="160"/>
-      <c r="F72" s="160"/>
+      <c r="D72" s="167">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="E72" s="178" t="s">
+        <v>936</v>
+      </c>
+      <c r="F72" s="160">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
       <c r="G72" s="160"/>
       <c r="H72" s="160"/>
       <c r="I72" s="160"/>

</xml_diff>

<commit_message>
TS PP 3.4 and Jatai Excel, TTD 23/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="946">
   <si>
     <t>Date</t>
   </si>
@@ -2831,19 +2831,52 @@
   </si>
   <si>
     <t>7.3.13.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=z--7cLE1FPs</t>
+  </si>
+  <si>
+    <t>7.3.14.1</t>
+  </si>
+  <si>
+    <t>7.3.15.1</t>
+  </si>
+  <si>
+    <t>7.3.16.1</t>
+  </si>
+  <si>
+    <t>7.3.17.1</t>
+  </si>
+  <si>
+    <t>7.3.18.1</t>
+  </si>
+  <si>
+    <t>7.3.19.1</t>
+  </si>
+  <si>
+    <t>7.3.20.1</t>
+  </si>
+  <si>
+    <t>7.4.1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="133" x14ac:knownFonts="1">
+  <fonts count="134" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3676,77 +3709,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="130" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="130" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="131" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="130" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="131" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="130" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="130" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="131" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="120" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="112" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="131" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="132" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="131" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="131" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="132" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="132" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3755,17 +3789,17 @@
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3780,19 +3814,19 @@
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="130" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="131" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="131" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="132" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3809,40 +3843,40 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3852,30 +3886,30 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -23048,7 +23082,7 @@
   <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24377,7 +24411,7 @@
       <c r="B65" s="160"/>
       <c r="C65" s="160"/>
       <c r="D65" s="167">
-        <f t="shared" ref="D65:D72" si="14">+D64+1</f>
+        <f t="shared" ref="D65:D74" si="14">+D64+1</f>
         <v>2</v>
       </c>
       <c r="E65" s="177" t="s">
@@ -24405,7 +24439,7 @@
         <v>929</v>
       </c>
       <c r="F66" s="171">
-        <f t="shared" ref="F66:F68" si="15">+G65</f>
+        <f t="shared" ref="F66:F67" si="15">+G65</f>
         <v>21.33</v>
       </c>
       <c r="G66" s="160">
@@ -24455,7 +24489,9 @@
       <c r="B69" s="163">
         <v>44158</v>
       </c>
-      <c r="C69" s="160"/>
+      <c r="C69" s="160">
+        <v>43.32</v>
+      </c>
       <c r="D69" s="167">
         <f>+D68+1</f>
         <v>1</v>
@@ -24463,10 +24499,16 @@
       <c r="E69" s="178" t="s">
         <v>933</v>
       </c>
-      <c r="F69" s="160"/>
-      <c r="G69" s="160"/>
+      <c r="F69" s="160">
+        <v>4.01</v>
+      </c>
+      <c r="G69" s="160">
+        <v>17.329999999999998</v>
+      </c>
       <c r="H69" s="160"/>
-      <c r="I69" s="160"/>
+      <c r="I69" s="160" t="s">
+        <v>937</v>
+      </c>
     </row>
     <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="160"/>
@@ -24481,9 +24523,11 @@
       </c>
       <c r="F70" s="160">
         <f>+G69</f>
-        <v>0</v>
-      </c>
-      <c r="G70" s="160"/>
+        <v>17.329999999999998</v>
+      </c>
+      <c r="G70" s="160">
+        <v>26.15</v>
+      </c>
       <c r="H70" s="160"/>
       <c r="I70" s="160"/>
     </row>
@@ -24499,10 +24543,12 @@
         <v>935</v>
       </c>
       <c r="F71" s="160">
-        <f t="shared" ref="F71:F72" si="16">+G70</f>
-        <v>0</v>
-      </c>
-      <c r="G71" s="160"/>
+        <f t="shared" ref="F71:F74" si="16">+G70</f>
+        <v>26.15</v>
+      </c>
+      <c r="G71" s="171">
+        <v>29.3</v>
+      </c>
       <c r="H71" s="160"/>
       <c r="I71" s="160"/>
     </row>
@@ -24517,11 +24563,13 @@
       <c r="E72" s="178" t="s">
         <v>936</v>
       </c>
-      <c r="F72" s="160">
+      <c r="F72" s="171">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="G72" s="160"/>
+        <v>29.3</v>
+      </c>
+      <c r="G72" s="160">
+        <v>33.24</v>
+      </c>
       <c r="H72" s="160"/>
       <c r="I72" s="160"/>
     </row>
@@ -24529,10 +24577,20 @@
       <c r="A73" s="160"/>
       <c r="B73" s="160"/>
       <c r="C73" s="160"/>
-      <c r="D73" s="160"/>
-      <c r="E73" s="160"/>
-      <c r="F73" s="160"/>
-      <c r="G73" s="160"/>
+      <c r="D73" s="167">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="E73" s="179" t="s">
+        <v>938</v>
+      </c>
+      <c r="F73" s="171">
+        <f t="shared" si="16"/>
+        <v>33.24</v>
+      </c>
+      <c r="G73" s="160">
+        <v>37.26</v>
+      </c>
       <c r="H73" s="160"/>
       <c r="I73" s="160"/>
     </row>
@@ -24540,10 +24598,20 @@
       <c r="A74" s="160"/>
       <c r="B74" s="160"/>
       <c r="C74" s="160"/>
-      <c r="D74" s="160"/>
-      <c r="E74" s="160"/>
-      <c r="F74" s="160"/>
-      <c r="G74" s="160"/>
+      <c r="D74" s="167">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="E74" s="179" t="s">
+        <v>939</v>
+      </c>
+      <c r="F74" s="171">
+        <f t="shared" si="16"/>
+        <v>37.26</v>
+      </c>
+      <c r="G74" s="160">
+        <v>42.33</v>
+      </c>
       <c r="H74" s="160"/>
       <c r="I74" s="160"/>
     </row>
@@ -24559,11 +24627,20 @@
       <c r="I75" s="160"/>
     </row>
     <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="160"/>
-      <c r="B76" s="160"/>
+      <c r="A76" s="160">
+        <v>12</v>
+      </c>
+      <c r="B76" s="163">
+        <v>44159</v>
+      </c>
       <c r="C76" s="160"/>
-      <c r="D76" s="160"/>
-      <c r="E76" s="160"/>
+      <c r="D76" s="167">
+        <f>+D75+1</f>
+        <v>1</v>
+      </c>
+      <c r="E76" s="179" t="s">
+        <v>940</v>
+      </c>
       <c r="F76" s="160"/>
       <c r="G76" s="160"/>
       <c r="H76" s="160"/>
@@ -24573,9 +24650,17 @@
       <c r="A77" s="160"/>
       <c r="B77" s="160"/>
       <c r="C77" s="160"/>
-      <c r="D77" s="160"/>
-      <c r="E77" s="160"/>
-      <c r="F77" s="160"/>
+      <c r="D77" s="167">
+        <f t="shared" ref="D77:D81" si="17">+D76+1</f>
+        <v>2</v>
+      </c>
+      <c r="E77" s="179" t="s">
+        <v>941</v>
+      </c>
+      <c r="F77" s="171">
+        <f>+G76</f>
+        <v>0</v>
+      </c>
       <c r="G77" s="160"/>
       <c r="H77" s="160"/>
       <c r="I77" s="160"/>
@@ -24584,9 +24669,17 @@
       <c r="A78" s="160"/>
       <c r="B78" s="160"/>
       <c r="C78" s="160"/>
-      <c r="D78" s="160"/>
-      <c r="E78" s="160"/>
-      <c r="F78" s="160"/>
+      <c r="D78" s="167">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="E78" s="179" t="s">
+        <v>942</v>
+      </c>
+      <c r="F78" s="171">
+        <f t="shared" ref="F78:F81" si="18">+G77</f>
+        <v>0</v>
+      </c>
       <c r="G78" s="160"/>
       <c r="H78" s="160"/>
       <c r="I78" s="160"/>
@@ -24595,9 +24688,17 @@
       <c r="A79" s="160"/>
       <c r="B79" s="160"/>
       <c r="C79" s="160"/>
-      <c r="D79" s="160"/>
-      <c r="E79" s="160"/>
-      <c r="F79" s="160"/>
+      <c r="D79" s="167">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="E79" s="179" t="s">
+        <v>943</v>
+      </c>
+      <c r="F79" s="171">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
       <c r="G79" s="160"/>
       <c r="H79" s="160"/>
       <c r="I79" s="160"/>
@@ -24606,9 +24707,17 @@
       <c r="A80" s="160"/>
       <c r="B80" s="160"/>
       <c r="C80" s="160"/>
-      <c r="D80" s="160"/>
-      <c r="E80" s="160"/>
-      <c r="F80" s="160"/>
+      <c r="D80" s="167">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="E80" s="179" t="s">
+        <v>944</v>
+      </c>
+      <c r="F80" s="171">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
       <c r="G80" s="160"/>
       <c r="H80" s="160"/>
       <c r="I80" s="160"/>
@@ -24617,9 +24726,17 @@
       <c r="A81" s="160"/>
       <c r="B81" s="160"/>
       <c r="C81" s="160"/>
-      <c r="D81" s="160"/>
-      <c r="E81" s="160"/>
-      <c r="F81" s="160"/>
+      <c r="D81" s="167">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="E81" s="179" t="s">
+        <v>945</v>
+      </c>
+      <c r="F81" s="171">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
       <c r="G81" s="160"/>
       <c r="H81" s="160"/>
       <c r="I81" s="160"/>

</xml_diff>

<commit_message>
Padam Input edits 25/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="955">
   <si>
     <t>Date</t>
   </si>
@@ -2632,9 +2632,6 @@
     <t>7.1.5.1</t>
   </si>
   <si>
-    <t>Speech/H1</t>
-  </si>
-  <si>
     <t>7.1.5.2</t>
   </si>
   <si>
@@ -2858,19 +2855,61 @@
   </si>
   <si>
     <t>7.4.1.1</t>
+  </si>
+  <si>
+    <t>H1/Archive</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iO0ystneX1c</t>
+  </si>
+  <si>
+    <t>7.4.1.2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cXbLzMhnjVs</t>
+  </si>
+  <si>
+    <t>7.4.3.3</t>
+  </si>
+  <si>
+    <t>7.4.2.1</t>
+  </si>
+  <si>
+    <t>7.4.3.1</t>
+  </si>
+  <si>
+    <t>7.4.4.1</t>
+  </si>
+  <si>
+    <t>7.4.5.1</t>
+  </si>
+  <si>
+    <t>7.4.6.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="134" x14ac:knownFonts="1">
+  <fonts count="136" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3709,77 +3748,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="130" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="131" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="133" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="131" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="133" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="130" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="131" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="133" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="125" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="125" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="120" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="112" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="132" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="134" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="132" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="132" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="134" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="134" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3787,18 +3828,18 @@
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="87" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="86" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3812,20 +3853,20 @@
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="131" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="133" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="132" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="134" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3841,41 +3882,41 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3884,36 +3925,36 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4220,10 +4261,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
+      <selection pane="bottomLeft" activeCell="I146" sqref="I146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -7156,7 +7197,7 @@
         <v>161</v>
       </c>
       <c r="C139" s="1">
-        <v>52.45</v>
+        <v>52.46</v>
       </c>
       <c r="D139" s="4">
         <v>1</v>
@@ -7192,8 +7233,8 @@
       <c r="G140" s="6">
         <v>26.55</v>
       </c>
-      <c r="H140" s="169" t="s">
-        <v>870</v>
+      <c r="H140" s="179" t="s">
+        <v>945</v>
       </c>
       <c r="I140" s="1"/>
     </row>
@@ -7550,7 +7591,9 @@
       <c r="I158" s="1"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B159" s="1"/>
+      <c r="B159" s="181" t="s">
+        <v>867</v>
+      </c>
       <c r="C159" s="1"/>
       <c r="D159" s="4">
         <f>+D158+1</f>
@@ -23081,8 +23124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23170,7 +23213,7 @@
       </c>
       <c r="H3" s="160"/>
       <c r="I3" s="160" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23281,8 +23324,8 @@
       <c r="D9" s="167">
         <v>1</v>
       </c>
-      <c r="E9" s="170" t="s">
-        <v>871</v>
+      <c r="E9" s="169" t="s">
+        <v>870</v>
       </c>
       <c r="F9" s="160">
         <v>6.48</v>
@@ -23292,7 +23335,7 @@
       </c>
       <c r="H9" s="160"/>
       <c r="I9" s="160" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23303,14 +23346,14 @@
         <f>+D9+1</f>
         <v>2</v>
       </c>
-      <c r="E10" s="170" t="s">
-        <v>873</v>
+      <c r="E10" s="169" t="s">
+        <v>872</v>
       </c>
       <c r="F10" s="160">
         <f>+G9</f>
         <v>25.17</v>
       </c>
-      <c r="G10" s="171">
+      <c r="G10" s="170">
         <v>47.5</v>
       </c>
       <c r="H10" s="160"/>
@@ -23321,7 +23364,7 @@
       <c r="B11" s="160"/>
       <c r="C11" s="160"/>
       <c r="D11" s="167"/>
-      <c r="E11" s="170"/>
+      <c r="E11" s="169"/>
       <c r="F11" s="160"/>
       <c r="G11" s="160"/>
       <c r="H11" s="160"/>
@@ -23340,8 +23383,8 @@
       <c r="D12" s="167">
         <v>1</v>
       </c>
-      <c r="E12" s="170" t="s">
-        <v>874</v>
+      <c r="E12" s="169" t="s">
+        <v>873</v>
       </c>
       <c r="F12" s="160">
         <v>5.44</v>
@@ -23351,7 +23394,7 @@
       </c>
       <c r="H12" s="160"/>
       <c r="I12" s="160" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23362,8 +23405,8 @@
         <f>+D12+1</f>
         <v>2</v>
       </c>
-      <c r="E13" s="170" t="s">
-        <v>875</v>
+      <c r="E13" s="169" t="s">
+        <v>874</v>
       </c>
       <c r="F13" s="160">
         <f>+G12</f>
@@ -23383,8 +23426,8 @@
         <f t="shared" ref="D14:D16" si="2">+D13+1</f>
         <v>3</v>
       </c>
-      <c r="E14" s="170" t="s">
-        <v>876</v>
+      <c r="E14" s="169" t="s">
+        <v>875</v>
       </c>
       <c r="F14" s="160">
         <f t="shared" ref="F14:F16" si="3">+G13</f>
@@ -23404,8 +23447,8 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E15" s="170" t="s">
-        <v>877</v>
+      <c r="E15" s="169" t="s">
+        <v>876</v>
       </c>
       <c r="F15" s="160">
         <f t="shared" si="3"/>
@@ -23425,8 +23468,8 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="E16" s="170" t="s">
-        <v>878</v>
+      <c r="E16" s="169" t="s">
+        <v>877</v>
       </c>
       <c r="F16" s="160">
         <f t="shared" si="3"/>
@@ -23443,7 +23486,7 @@
       <c r="B17" s="160"/>
       <c r="C17" s="160"/>
       <c r="D17" s="167"/>
-      <c r="E17" s="170"/>
+      <c r="E17" s="169"/>
       <c r="F17" s="160"/>
       <c r="G17" s="160"/>
       <c r="H17" s="160"/>
@@ -23456,16 +23499,16 @@
       <c r="B18" s="163">
         <v>44151</v>
       </c>
-      <c r="C18" s="171">
+      <c r="C18" s="170">
         <v>45.5</v>
       </c>
       <c r="D18" s="167">
         <v>1</v>
       </c>
-      <c r="E18" s="172" t="s">
-        <v>879</v>
-      </c>
-      <c r="F18" s="171">
+      <c r="E18" s="171" t="s">
+        <v>878</v>
+      </c>
+      <c r="F18" s="170">
         <v>5.2</v>
       </c>
       <c r="G18" s="160">
@@ -23473,7 +23516,7 @@
       </c>
       <c r="H18" s="160"/>
       <c r="I18" s="160" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23484,10 +23527,10 @@
         <f>+D18+1</f>
         <v>2</v>
       </c>
-      <c r="E19" s="172" t="s">
-        <v>882</v>
-      </c>
-      <c r="F19" s="171">
+      <c r="E19" s="171" t="s">
+        <v>881</v>
+      </c>
+      <c r="F19" s="170">
         <f>+G18</f>
         <v>9.57</v>
       </c>
@@ -23505,10 +23548,10 @@
         <f t="shared" ref="D20:D26" si="4">+D19+1</f>
         <v>3</v>
       </c>
-      <c r="E20" s="172" t="s">
-        <v>883</v>
-      </c>
-      <c r="F20" s="171">
+      <c r="E20" s="171" t="s">
+        <v>882</v>
+      </c>
+      <c r="F20" s="170">
         <f t="shared" ref="F20:F26" si="5">+G19</f>
         <v>12.24</v>
       </c>
@@ -23526,10 +23569,10 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="E21" s="172" t="s">
-        <v>884</v>
-      </c>
-      <c r="F21" s="171">
+      <c r="E21" s="171" t="s">
+        <v>883</v>
+      </c>
+      <c r="F21" s="170">
         <f t="shared" si="5"/>
         <v>13.55</v>
       </c>
@@ -23547,10 +23590,10 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="E22" s="172" t="s">
-        <v>885</v>
-      </c>
-      <c r="F22" s="171">
+      <c r="E22" s="171" t="s">
+        <v>884</v>
+      </c>
+      <c r="F22" s="170">
         <f t="shared" si="5"/>
         <v>17.45</v>
       </c>
@@ -23568,10 +23611,10 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="E23" s="172" t="s">
-        <v>886</v>
-      </c>
-      <c r="F23" s="171">
+      <c r="E23" s="171" t="s">
+        <v>885</v>
+      </c>
+      <c r="F23" s="170">
         <f t="shared" si="5"/>
         <v>19.14</v>
       </c>
@@ -23589,10 +23632,10 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="E24" s="172" t="s">
-        <v>887</v>
-      </c>
-      <c r="F24" s="171">
+      <c r="E24" s="171" t="s">
+        <v>886</v>
+      </c>
+      <c r="F24" s="170">
         <f t="shared" si="5"/>
         <v>22.12</v>
       </c>
@@ -23610,10 +23653,10 @@
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="E25" s="172" t="s">
-        <v>888</v>
-      </c>
-      <c r="F25" s="171">
+      <c r="E25" s="171" t="s">
+        <v>887</v>
+      </c>
+      <c r="F25" s="170">
         <f t="shared" si="5"/>
         <v>28.08</v>
       </c>
@@ -23631,10 +23674,10 @@
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="E26" s="172" t="s">
-        <v>889</v>
-      </c>
-      <c r="F26" s="171">
+      <c r="E26" s="171" t="s">
+        <v>888</v>
+      </c>
+      <c r="F26" s="170">
         <f t="shared" si="5"/>
         <v>42.37</v>
       </c>
@@ -23659,7 +23702,7 @@
       <c r="A28" s="160">
         <v>5</v>
       </c>
-      <c r="B28" s="174">
+      <c r="B28" s="173">
         <v>44152</v>
       </c>
       <c r="C28" s="160">
@@ -23668,8 +23711,8 @@
       <c r="D28" s="167">
         <v>1</v>
       </c>
-      <c r="E28" s="173" t="s">
-        <v>892</v>
+      <c r="E28" s="172" t="s">
+        <v>891</v>
       </c>
       <c r="F28" s="160">
         <v>7.27</v>
@@ -23679,7 +23722,7 @@
       </c>
       <c r="H28" s="160"/>
       <c r="I28" s="160" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23690,8 +23733,8 @@
         <f>+D28+1</f>
         <v>2</v>
       </c>
-      <c r="E29" s="173" t="s">
-        <v>893</v>
+      <c r="E29" s="172" t="s">
+        <v>892</v>
       </c>
       <c r="F29" s="160">
         <f>+G28</f>
@@ -23711,14 +23754,14 @@
         <f t="shared" ref="D30:D31" si="6">+D29+1</f>
         <v>3</v>
       </c>
-      <c r="E30" s="173" t="s">
-        <v>894</v>
+      <c r="E30" s="172" t="s">
+        <v>893</v>
       </c>
       <c r="F30" s="160">
         <f t="shared" ref="F30:F31" si="7">+G29</f>
         <v>32.270000000000003</v>
       </c>
-      <c r="G30" s="171">
+      <c r="G30" s="170">
         <v>40</v>
       </c>
       <c r="H30" s="160"/>
@@ -23732,10 +23775,10 @@
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="E31" s="173" t="s">
-        <v>895</v>
-      </c>
-      <c r="F31" s="171">
+      <c r="E31" s="172" t="s">
+        <v>894</v>
+      </c>
+      <c r="F31" s="170">
         <f t="shared" si="7"/>
         <v>40</v>
       </c>
@@ -23779,8 +23822,8 @@
       <c r="D34" s="167">
         <v>1</v>
       </c>
-      <c r="E34" s="173" t="s">
-        <v>896</v>
+      <c r="E34" s="172" t="s">
+        <v>895</v>
       </c>
       <c r="F34" s="160">
         <v>5.19</v>
@@ -23790,7 +23833,7 @@
       </c>
       <c r="H34" s="160"/>
       <c r="I34" s="160" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23801,10 +23844,10 @@
         <f>+D34+1</f>
         <v>2</v>
       </c>
-      <c r="E35" s="173" t="s">
-        <v>897</v>
-      </c>
-      <c r="F35" s="171">
+      <c r="E35" s="172" t="s">
+        <v>896</v>
+      </c>
+      <c r="F35" s="170">
         <f>+G34</f>
         <v>24.27</v>
       </c>
@@ -23822,18 +23865,18 @@
         <f t="shared" ref="D36" si="8">+D35+1</f>
         <v>3</v>
       </c>
-      <c r="E36" s="173" t="s">
-        <v>898</v>
-      </c>
-      <c r="F36" s="171">
+      <c r="E36" s="172" t="s">
+        <v>897</v>
+      </c>
+      <c r="F36" s="170">
         <f>+G35</f>
         <v>34.51</v>
       </c>
       <c r="G36" s="160">
         <v>41.52</v>
       </c>
-      <c r="H36" s="175" t="s">
-        <v>905</v>
+      <c r="H36" s="174" t="s">
+        <v>904</v>
       </c>
       <c r="I36" s="160"/>
     </row>
@@ -23862,8 +23905,8 @@
         <f>+D37+1</f>
         <v>1</v>
       </c>
-      <c r="E38" s="175" t="s">
-        <v>903</v>
+      <c r="E38" s="174" t="s">
+        <v>902</v>
       </c>
       <c r="F38" s="160">
         <v>2.4500000000000002</v>
@@ -23873,7 +23916,7 @@
       </c>
       <c r="H38" s="160"/>
       <c r="I38" s="160" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23884,8 +23927,8 @@
         <f t="shared" ref="D39:D40" si="9">+D38+1</f>
         <v>2</v>
       </c>
-      <c r="E39" s="175" t="s">
-        <v>904</v>
+      <c r="E39" s="174" t="s">
+        <v>903</v>
       </c>
       <c r="F39" s="160">
         <f>+G38</f>
@@ -23905,8 +23948,8 @@
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="E40" s="175" t="s">
-        <v>899</v>
+      <c r="E40" s="174" t="s">
+        <v>898</v>
       </c>
       <c r="F40" s="160">
         <f>+G39</f>
@@ -23915,8 +23958,8 @@
       <c r="G40" s="160">
         <v>39.090000000000003</v>
       </c>
-      <c r="H40" s="175" t="s">
-        <v>906</v>
+      <c r="H40" s="174" t="s">
+        <v>905</v>
       </c>
       <c r="I40" s="160"/>
     </row>
@@ -23938,15 +23981,15 @@
       <c r="B42" s="163">
         <v>44155</v>
       </c>
-      <c r="C42" s="171">
+      <c r="C42" s="170">
         <v>49.1</v>
       </c>
       <c r="D42" s="167">
         <f>+D41+1</f>
         <v>1</v>
       </c>
-      <c r="E42" s="175" t="s">
-        <v>907</v>
+      <c r="E42" s="174" t="s">
+        <v>906</v>
       </c>
       <c r="F42" s="160">
         <v>2.37</v>
@@ -23956,7 +23999,7 @@
       </c>
       <c r="H42" s="160"/>
       <c r="I42" s="160" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23967,10 +24010,10 @@
         <f t="shared" ref="D43:D54" si="10">+D42+1</f>
         <v>2</v>
       </c>
-      <c r="E43" s="175" t="s">
-        <v>900</v>
-      </c>
-      <c r="F43" s="171">
+      <c r="E43" s="174" t="s">
+        <v>899</v>
+      </c>
+      <c r="F43" s="170">
         <f>+G42</f>
         <v>6.15</v>
       </c>
@@ -23988,10 +24031,10 @@
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="E44" s="175" t="s">
-        <v>908</v>
-      </c>
-      <c r="F44" s="171">
+      <c r="E44" s="174" t="s">
+        <v>907</v>
+      </c>
+      <c r="F44" s="170">
         <f t="shared" ref="F44:F54" si="11">+G43</f>
         <v>18.28</v>
       </c>
@@ -24009,10 +24052,10 @@
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="E45" s="175" t="s">
-        <v>909</v>
-      </c>
-      <c r="F45" s="171">
+      <c r="E45" s="174" t="s">
+        <v>908</v>
+      </c>
+      <c r="F45" s="170">
         <f t="shared" si="11"/>
         <v>24.23</v>
       </c>
@@ -24030,10 +24073,10 @@
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="E46" s="175" t="s">
-        <v>910</v>
-      </c>
-      <c r="F46" s="171">
+      <c r="E46" s="174" t="s">
+        <v>909</v>
+      </c>
+      <c r="F46" s="170">
         <f t="shared" si="11"/>
         <v>28.19</v>
       </c>
@@ -24051,10 +24094,10 @@
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
-      <c r="E47" s="175" t="s">
-        <v>911</v>
-      </c>
-      <c r="F47" s="171">
+      <c r="E47" s="174" t="s">
+        <v>910</v>
+      </c>
+      <c r="F47" s="170">
         <f t="shared" si="11"/>
         <v>30.34</v>
       </c>
@@ -24072,10 +24115,10 @@
         <f t="shared" si="10"/>
         <v>7</v>
       </c>
-      <c r="E48" s="175" t="s">
-        <v>912</v>
-      </c>
-      <c r="F48" s="171">
+      <c r="E48" s="174" t="s">
+        <v>911</v>
+      </c>
+      <c r="F48" s="170">
         <f t="shared" si="11"/>
         <v>34.200000000000003</v>
       </c>
@@ -24093,10 +24136,10 @@
         <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="E49" s="176" t="s">
-        <v>914</v>
-      </c>
-      <c r="F49" s="171">
+      <c r="E49" s="175" t="s">
+        <v>913</v>
+      </c>
+      <c r="F49" s="170">
         <f t="shared" si="11"/>
         <v>35.43</v>
       </c>
@@ -24114,10 +24157,10 @@
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
-      <c r="E50" s="176" t="s">
-        <v>915</v>
-      </c>
-      <c r="F50" s="171">
+      <c r="E50" s="175" t="s">
+        <v>914</v>
+      </c>
+      <c r="F50" s="170">
         <f t="shared" si="11"/>
         <v>36.51</v>
       </c>
@@ -24135,10 +24178,10 @@
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="E51" s="176" t="s">
-        <v>916</v>
-      </c>
-      <c r="F51" s="171">
+      <c r="E51" s="175" t="s">
+        <v>915</v>
+      </c>
+      <c r="F51" s="170">
         <f t="shared" si="11"/>
         <v>38.31</v>
       </c>
@@ -24156,10 +24199,10 @@
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="E52" s="176" t="s">
-        <v>917</v>
-      </c>
-      <c r="F52" s="171">
+      <c r="E52" s="175" t="s">
+        <v>916</v>
+      </c>
+      <c r="F52" s="170">
         <f t="shared" si="11"/>
         <v>39.24</v>
       </c>
@@ -24177,14 +24220,14 @@
         <f t="shared" si="10"/>
         <v>12</v>
       </c>
-      <c r="E53" s="176" t="s">
-        <v>918</v>
-      </c>
-      <c r="F53" s="171">
+      <c r="E53" s="175" t="s">
+        <v>917</v>
+      </c>
+      <c r="F53" s="170">
         <f t="shared" si="11"/>
         <v>42.04</v>
       </c>
-      <c r="G53" s="171">
+      <c r="G53" s="170">
         <v>45.4</v>
       </c>
       <c r="H53" s="160"/>
@@ -24198,18 +24241,18 @@
         <f t="shared" si="10"/>
         <v>13</v>
       </c>
-      <c r="E54" s="176" t="s">
-        <v>919</v>
-      </c>
-      <c r="F54" s="171">
+      <c r="E54" s="175" t="s">
+        <v>918</v>
+      </c>
+      <c r="F54" s="170">
         <f t="shared" si="11"/>
         <v>45.4</v>
       </c>
       <c r="G54" s="160">
         <v>48.36</v>
       </c>
-      <c r="H54" s="176" t="s">
-        <v>919</v>
+      <c r="H54" s="175" t="s">
+        <v>918</v>
       </c>
       <c r="I54" s="160"/>
     </row>
@@ -24231,15 +24274,15 @@
       <c r="B56" s="163">
         <v>44156</v>
       </c>
-      <c r="C56" s="171">
+      <c r="C56" s="170">
         <v>53</v>
       </c>
       <c r="D56" s="167">
         <f>+D55+1</f>
         <v>1</v>
       </c>
-      <c r="E56" s="176" t="s">
-        <v>920</v>
+      <c r="E56" s="175" t="s">
+        <v>919</v>
       </c>
       <c r="F56" s="160">
         <v>2.04</v>
@@ -24249,7 +24292,7 @@
       </c>
       <c r="H56" s="160"/>
       <c r="I56" s="160" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24260,8 +24303,8 @@
         <f t="shared" ref="D57:D61" si="12">+D56+1</f>
         <v>2</v>
       </c>
-      <c r="E57" s="176" t="s">
-        <v>921</v>
+      <c r="E57" s="175" t="s">
+        <v>920</v>
       </c>
       <c r="F57" s="160">
         <f>+G56</f>
@@ -24281,8 +24324,8 @@
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="E58" s="176" t="s">
-        <v>922</v>
+      <c r="E58" s="175" t="s">
+        <v>921</v>
       </c>
       <c r="F58" s="160">
         <f t="shared" ref="F58:F61" si="13">+G57</f>
@@ -24302,8 +24345,8 @@
         <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="E59" s="176" t="s">
-        <v>923</v>
+      <c r="E59" s="175" t="s">
+        <v>922</v>
       </c>
       <c r="F59" s="160">
         <f t="shared" si="13"/>
@@ -24323,8 +24366,8 @@
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="E60" s="176" t="s">
-        <v>924</v>
+      <c r="E60" s="175" t="s">
+        <v>923</v>
       </c>
       <c r="F60" s="160">
         <f t="shared" si="13"/>
@@ -24344,14 +24387,14 @@
         <f t="shared" si="12"/>
         <v>6</v>
       </c>
-      <c r="E61" s="177" t="s">
-        <v>926</v>
+      <c r="E61" s="176" t="s">
+        <v>925</v>
       </c>
       <c r="F61" s="160">
         <f t="shared" si="13"/>
         <v>45.04</v>
       </c>
-      <c r="G61" s="171">
+      <c r="G61" s="170">
         <v>52</v>
       </c>
       <c r="H61" s="160"/>
@@ -24385,15 +24428,15 @@
       <c r="B64" s="163">
         <v>44157</v>
       </c>
-      <c r="C64" s="171">
+      <c r="C64" s="170">
         <v>37.5</v>
       </c>
       <c r="D64" s="167">
         <f>+D63+1</f>
         <v>1</v>
       </c>
-      <c r="E64" s="177" t="s">
-        <v>927</v>
+      <c r="E64" s="176" t="s">
+        <v>926</v>
       </c>
       <c r="F64" s="160">
         <v>0.59</v>
@@ -24403,7 +24446,7 @@
       </c>
       <c r="H64" s="160"/>
       <c r="I64" s="160" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24414,10 +24457,10 @@
         <f t="shared" ref="D65:D74" si="14">+D64+1</f>
         <v>2</v>
       </c>
-      <c r="E65" s="177" t="s">
-        <v>928</v>
-      </c>
-      <c r="F65" s="171">
+      <c r="E65" s="176" t="s">
+        <v>927</v>
+      </c>
+      <c r="F65" s="170">
         <f>+G64</f>
         <v>15.52</v>
       </c>
@@ -24435,10 +24478,10 @@
         <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="E66" s="177" t="s">
-        <v>929</v>
-      </c>
-      <c r="F66" s="171">
+      <c r="E66" s="176" t="s">
+        <v>928</v>
+      </c>
+      <c r="F66" s="170">
         <f t="shared" ref="F66:F67" si="15">+G65</f>
         <v>21.33</v>
       </c>
@@ -24456,18 +24499,18 @@
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="E67" s="177" t="s">
-        <v>930</v>
-      </c>
-      <c r="F67" s="171">
+      <c r="E67" s="176" t="s">
+        <v>929</v>
+      </c>
+      <c r="F67" s="170">
         <f t="shared" si="15"/>
         <v>31.19</v>
       </c>
       <c r="G67" s="160">
         <v>37.15</v>
       </c>
-      <c r="H67" s="178" t="s">
-        <v>934</v>
+      <c r="H67" s="177" t="s">
+        <v>933</v>
       </c>
       <c r="I67" s="160"/>
     </row>
@@ -24476,8 +24519,8 @@
       <c r="B68" s="160"/>
       <c r="C68" s="160"/>
       <c r="D68" s="167"/>
-      <c r="E68" s="177"/>
-      <c r="F68" s="171"/>
+      <c r="E68" s="176"/>
+      <c r="F68" s="170"/>
       <c r="G68" s="160"/>
       <c r="H68" s="160"/>
       <c r="I68" s="160"/>
@@ -24496,8 +24539,8 @@
         <f>+D68+1</f>
         <v>1</v>
       </c>
-      <c r="E69" s="178" t="s">
-        <v>933</v>
+      <c r="E69" s="177" t="s">
+        <v>932</v>
       </c>
       <c r="F69" s="160">
         <v>4.01</v>
@@ -24507,7 +24550,7 @@
       </c>
       <c r="H69" s="160"/>
       <c r="I69" s="160" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24518,8 +24561,8 @@
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="E70" s="178" t="s">
-        <v>931</v>
+      <c r="E70" s="177" t="s">
+        <v>930</v>
       </c>
       <c r="F70" s="160">
         <f>+G69</f>
@@ -24539,14 +24582,14 @@
         <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="E71" s="178" t="s">
-        <v>935</v>
+      <c r="E71" s="177" t="s">
+        <v>934</v>
       </c>
       <c r="F71" s="160">
         <f t="shared" ref="F71:F74" si="16">+G70</f>
         <v>26.15</v>
       </c>
-      <c r="G71" s="171">
+      <c r="G71" s="170">
         <v>29.3</v>
       </c>
       <c r="H71" s="160"/>
@@ -24560,10 +24603,10 @@
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="E72" s="178" t="s">
-        <v>936</v>
-      </c>
-      <c r="F72" s="171">
+      <c r="E72" s="177" t="s">
+        <v>935</v>
+      </c>
+      <c r="F72" s="170">
         <f t="shared" si="16"/>
         <v>29.3</v>
       </c>
@@ -24581,10 +24624,10 @@
         <f t="shared" si="14"/>
         <v>5</v>
       </c>
-      <c r="E73" s="179" t="s">
-        <v>938</v>
-      </c>
-      <c r="F73" s="171">
+      <c r="E73" s="178" t="s">
+        <v>937</v>
+      </c>
+      <c r="F73" s="170">
         <f t="shared" si="16"/>
         <v>33.24</v>
       </c>
@@ -24602,10 +24645,10 @@
         <f t="shared" si="14"/>
         <v>6</v>
       </c>
-      <c r="E74" s="179" t="s">
-        <v>939</v>
-      </c>
-      <c r="F74" s="171">
+      <c r="E74" s="178" t="s">
+        <v>938</v>
+      </c>
+      <c r="F74" s="170">
         <f t="shared" si="16"/>
         <v>37.26</v>
       </c>
@@ -24633,18 +24676,26 @@
       <c r="B76" s="163">
         <v>44159</v>
       </c>
-      <c r="C76" s="160"/>
+      <c r="C76" s="160">
+        <v>34.32</v>
+      </c>
       <c r="D76" s="167">
         <f>+D75+1</f>
         <v>1</v>
       </c>
-      <c r="E76" s="179" t="s">
-        <v>940</v>
-      </c>
-      <c r="F76" s="160"/>
-      <c r="G76" s="160"/>
+      <c r="E76" s="178" t="s">
+        <v>939</v>
+      </c>
+      <c r="F76" s="160">
+        <v>1.44</v>
+      </c>
+      <c r="G76" s="160">
+        <v>12.56</v>
+      </c>
       <c r="H76" s="160"/>
-      <c r="I76" s="160"/>
+      <c r="I76" s="160" t="s">
+        <v>946</v>
+      </c>
     </row>
     <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="160"/>
@@ -24654,14 +24705,16 @@
         <f t="shared" ref="D77:D81" si="17">+D76+1</f>
         <v>2</v>
       </c>
-      <c r="E77" s="179" t="s">
-        <v>941</v>
-      </c>
-      <c r="F77" s="171">
+      <c r="E77" s="178" t="s">
+        <v>940</v>
+      </c>
+      <c r="F77" s="170">
         <f>+G76</f>
-        <v>0</v>
-      </c>
-      <c r="G77" s="160"/>
+        <v>12.56</v>
+      </c>
+      <c r="G77" s="160">
+        <v>18.399999999999999</v>
+      </c>
       <c r="H77" s="160"/>
       <c r="I77" s="160"/>
     </row>
@@ -24673,14 +24726,16 @@
         <f t="shared" si="17"/>
         <v>3</v>
       </c>
-      <c r="E78" s="179" t="s">
-        <v>942</v>
-      </c>
-      <c r="F78" s="171">
+      <c r="E78" s="178" t="s">
+        <v>941</v>
+      </c>
+      <c r="F78" s="170">
         <f t="shared" ref="F78:F81" si="18">+G77</f>
-        <v>0</v>
-      </c>
-      <c r="G78" s="160"/>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G78" s="160">
+        <v>22.55</v>
+      </c>
       <c r="H78" s="160"/>
       <c r="I78" s="160"/>
     </row>
@@ -24692,14 +24747,16 @@
         <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="E79" s="179" t="s">
-        <v>943</v>
-      </c>
-      <c r="F79" s="171">
+      <c r="E79" s="178" t="s">
+        <v>942</v>
+      </c>
+      <c r="F79" s="170">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="G79" s="160"/>
+        <v>22.55</v>
+      </c>
+      <c r="G79" s="160">
+        <v>25.21</v>
+      </c>
       <c r="H79" s="160"/>
       <c r="I79" s="160"/>
     </row>
@@ -24711,14 +24768,16 @@
         <f t="shared" si="17"/>
         <v>5</v>
       </c>
-      <c r="E80" s="179" t="s">
-        <v>944</v>
-      </c>
-      <c r="F80" s="171">
+      <c r="E80" s="178" t="s">
+        <v>943</v>
+      </c>
+      <c r="F80" s="170">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="G80" s="160"/>
+        <v>25.21</v>
+      </c>
+      <c r="G80" s="160">
+        <v>30.07</v>
+      </c>
       <c r="H80" s="160"/>
       <c r="I80" s="160"/>
     </row>
@@ -24730,14 +24789,16 @@
         <f t="shared" si="17"/>
         <v>6</v>
       </c>
-      <c r="E81" s="179" t="s">
-        <v>945</v>
-      </c>
-      <c r="F81" s="171">
+      <c r="E81" s="178" t="s">
+        <v>944</v>
+      </c>
+      <c r="F81" s="170">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="G81" s="160"/>
+        <v>30.07</v>
+      </c>
+      <c r="G81" s="160">
+        <v>33.19</v>
+      </c>
       <c r="H81" s="160"/>
       <c r="I81" s="160"/>
     </row>
@@ -24753,24 +24814,51 @@
       <c r="I82" s="160"/>
     </row>
     <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A83" s="160"/>
-      <c r="B83" s="160"/>
-      <c r="C83" s="160"/>
-      <c r="D83" s="160"/>
-      <c r="E83" s="160"/>
-      <c r="F83" s="160"/>
-      <c r="G83" s="160"/>
+      <c r="A83" s="160">
+        <v>13</v>
+      </c>
+      <c r="B83" s="163">
+        <v>44160</v>
+      </c>
+      <c r="C83" s="160">
+        <v>41.35</v>
+      </c>
+      <c r="D83" s="167">
+        <f>+D82+1</f>
+        <v>1</v>
+      </c>
+      <c r="E83" s="180" t="s">
+        <v>947</v>
+      </c>
+      <c r="F83" s="160">
+        <v>3.57</v>
+      </c>
+      <c r="G83" s="160">
+        <v>12.05</v>
+      </c>
       <c r="H83" s="160"/>
-      <c r="I83" s="160"/>
+      <c r="I83" s="160" t="s">
+        <v>948</v>
+      </c>
     </row>
     <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="160"/>
       <c r="B84" s="160"/>
       <c r="C84" s="160"/>
-      <c r="D84" s="160"/>
-      <c r="E84" s="160"/>
-      <c r="F84" s="160"/>
-      <c r="G84" s="160"/>
+      <c r="D84" s="167">
+        <f t="shared" ref="D84:D85" si="19">+D83+1</f>
+        <v>2</v>
+      </c>
+      <c r="E84" s="180" t="s">
+        <v>950</v>
+      </c>
+      <c r="F84" s="160">
+        <f>+G83</f>
+        <v>12.05</v>
+      </c>
+      <c r="G84" s="160">
+        <v>33.39</v>
+      </c>
       <c r="H84" s="160"/>
       <c r="I84" s="160"/>
     </row>
@@ -24778,10 +24866,20 @@
       <c r="A85" s="160"/>
       <c r="B85" s="160"/>
       <c r="C85" s="160"/>
-      <c r="D85" s="160"/>
-      <c r="E85" s="160"/>
-      <c r="F85" s="160"/>
-      <c r="G85" s="160"/>
+      <c r="D85" s="167">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="E85" s="180" t="s">
+        <v>951</v>
+      </c>
+      <c r="F85" s="160">
+        <f t="shared" ref="F85" si="20">+G84</f>
+        <v>33.39</v>
+      </c>
+      <c r="G85" s="160">
+        <v>40.35</v>
+      </c>
       <c r="H85" s="160"/>
       <c r="I85" s="160"/>
     </row>
@@ -24789,7 +24887,7 @@
       <c r="A86" s="160"/>
       <c r="B86" s="160"/>
       <c r="C86" s="160"/>
-      <c r="D86" s="160"/>
+      <c r="D86" s="167"/>
       <c r="E86" s="160"/>
       <c r="F86" s="160"/>
       <c r="G86" s="160"/>
@@ -24797,11 +24895,20 @@
       <c r="I86" s="160"/>
     </row>
     <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A87" s="160"/>
-      <c r="B87" s="160"/>
+      <c r="A87" s="160">
+        <v>14</v>
+      </c>
+      <c r="B87" s="163">
+        <v>44161</v>
+      </c>
       <c r="C87" s="160"/>
-      <c r="D87" s="160"/>
-      <c r="E87" s="160"/>
+      <c r="D87" s="167">
+        <f>+D86+1</f>
+        <v>1</v>
+      </c>
+      <c r="E87" s="180" t="s">
+        <v>949</v>
+      </c>
       <c r="F87" s="160"/>
       <c r="G87" s="160"/>
       <c r="H87" s="160"/>
@@ -24811,8 +24918,13 @@
       <c r="A88" s="160"/>
       <c r="B88" s="160"/>
       <c r="C88" s="160"/>
-      <c r="D88" s="160"/>
-      <c r="E88" s="160"/>
+      <c r="D88" s="167">
+        <f t="shared" ref="D88:D90" si="21">+D87+1</f>
+        <v>2</v>
+      </c>
+      <c r="E88" s="180" t="s">
+        <v>952</v>
+      </c>
       <c r="F88" s="160"/>
       <c r="G88" s="160"/>
       <c r="H88" s="160"/>
@@ -24822,8 +24934,13 @@
       <c r="A89" s="160"/>
       <c r="B89" s="160"/>
       <c r="C89" s="160"/>
-      <c r="D89" s="160"/>
-      <c r="E89" s="160"/>
+      <c r="D89" s="167">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="E89" s="180" t="s">
+        <v>953</v>
+      </c>
       <c r="F89" s="160"/>
       <c r="G89" s="160"/>
       <c r="H89" s="160"/>
@@ -24833,8 +24950,13 @@
       <c r="A90" s="160"/>
       <c r="B90" s="160"/>
       <c r="C90" s="160"/>
-      <c r="D90" s="160"/>
-      <c r="E90" s="160"/>
+      <c r="D90" s="167">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="E90" s="180" t="s">
+        <v>954</v>
+      </c>
       <c r="F90" s="160"/>
       <c r="G90" s="160"/>
       <c r="H90" s="160"/>

</xml_diff>

<commit_message>
TS Padam Template 1.7 +2.6
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="954">
   <si>
     <t>Date</t>
   </si>
@@ -2881,23 +2881,32 @@
     <t>7.4.4.1</t>
   </si>
   <si>
-    <t>7.4.5.1</t>
-  </si>
-  <si>
-    <t>7.4.6.1</t>
+    <t>7.4.4.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="136" x14ac:knownFonts="1">
+  <fonts count="138" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3748,77 +3757,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="133" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="135" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="133" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="135" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="133" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="135" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="125" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="124" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="125" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="116" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="115" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="134" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="136" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="134" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="134" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="136" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="136" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3826,18 +3837,18 @@
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="88" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="87" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3851,20 +3862,20 @@
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="133" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="135" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="134" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="136" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3880,41 +3891,41 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3923,38 +3934,38 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4261,10 +4272,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B146" sqref="B146"/>
+      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -7374,7 +7385,7 @@
         <v>173</v>
       </c>
       <c r="C148" s="1">
-        <v>57.51</v>
+        <v>57.52</v>
       </c>
       <c r="D148" s="4">
         <v>1</v>
@@ -7454,7 +7465,9 @@
       <c r="I151" s="1"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B152" s="1"/>
+      <c r="B152" s="182" t="s">
+        <v>867</v>
+      </c>
       <c r="C152" s="1"/>
       <c r="D152" s="4">
         <f>+D151+1</f>
@@ -23123,8 +23136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24908,8 +24921,12 @@
       <c r="E87" s="180" t="s">
         <v>949</v>
       </c>
-      <c r="F87" s="160"/>
-      <c r="G87" s="160"/>
+      <c r="F87" s="160">
+        <v>4.03</v>
+      </c>
+      <c r="G87" s="160">
+        <v>23.32</v>
+      </c>
       <c r="H87" s="160"/>
       <c r="I87" s="160"/>
     </row>
@@ -24924,22 +24941,24 @@
       <c r="E88" s="180" t="s">
         <v>952</v>
       </c>
-      <c r="F88" s="160"/>
-      <c r="G88" s="160"/>
-      <c r="H88" s="160"/>
+      <c r="F88" s="160">
+        <f>+G87</f>
+        <v>23.32</v>
+      </c>
+      <c r="G88" s="160">
+        <v>33.19</v>
+      </c>
+      <c r="H88" s="183" t="s">
+        <v>953</v>
+      </c>
       <c r="I88" s="160"/>
     </row>
     <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="160"/>
       <c r="B89" s="160"/>
       <c r="C89" s="160"/>
-      <c r="D89" s="167">
-        <f t="shared" si="21"/>
-        <v>3</v>
-      </c>
-      <c r="E89" s="180" t="s">
-        <v>953</v>
-      </c>
+      <c r="D89" s="167"/>
+      <c r="E89" s="180"/>
       <c r="F89" s="160"/>
       <c r="G89" s="160"/>
       <c r="H89" s="160"/>
@@ -24949,13 +24968,8 @@
       <c r="A90" s="160"/>
       <c r="B90" s="160"/>
       <c r="C90" s="160"/>
-      <c r="D90" s="167">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="E90" s="180" t="s">
-        <v>954</v>
-      </c>
+      <c r="D90" s="167"/>
+      <c r="E90" s="180"/>
       <c r="F90" s="160"/>
       <c r="G90" s="160"/>
       <c r="H90" s="160"/>

</xml_diff>

<commit_message>
Jatai TTD Padam Input 03/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="1011">
   <si>
     <t>Date</t>
   </si>
@@ -2987,19 +2987,97 @@
   </si>
   <si>
     <t>7.5.7.1</t>
+  </si>
+  <si>
+    <t>7.5.7.3</t>
+  </si>
+  <si>
+    <t>7.5.8.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lWISxXV9GEQ</t>
+  </si>
+  <si>
+    <t>7.5.9.1</t>
+  </si>
+  <si>
+    <t>7.5.10.1</t>
+  </si>
+  <si>
+    <t>7.5.11.1</t>
+  </si>
+  <si>
+    <t>7.5.12.1</t>
+  </si>
+  <si>
+    <t>7.5.13.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GDVmaTIF1M8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=BtxhyKKSSe8</t>
+  </si>
+  <si>
+    <t>7.5.14.1</t>
+  </si>
+  <si>
+    <t>7.5.15.1</t>
+  </si>
+  <si>
+    <t>7.5.16.1</t>
+  </si>
+  <si>
+    <t>7.5.17.1</t>
+  </si>
+  <si>
+    <t>7.5.18.1</t>
+  </si>
+  <si>
+    <t>7.5.19.1</t>
+  </si>
+  <si>
+    <t>7.5.20.1</t>
+  </si>
+  <si>
+    <t>7.5.21.1</t>
+  </si>
+  <si>
+    <t>7.5.22.1</t>
+  </si>
+  <si>
+    <t>7.5.23.1</t>
+  </si>
+  <si>
+    <t>7.5.24.1</t>
+  </si>
+  <si>
+    <t>7.5.25.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="143" x14ac:knownFonts="1">
+  <fonts count="145" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3892,77 +3970,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="140" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="141" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="142" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="140" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="142" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="141" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="140" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="142" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="131" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="121" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="120" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="116" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="116" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="141" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="143" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="141" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="141" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="143" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="143" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3970,18 +4050,18 @@
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="94" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3995,20 +4075,20 @@
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="140" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="142" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="141" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="143" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4024,41 +4104,41 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4067,45 +4147,47 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23276,10 +23358,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="H142" sqref="H142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25647,7 +25729,7 @@
         <v>983</v>
       </c>
       <c r="F115" s="160">
-        <f t="shared" ref="F115:F116" si="29">+G114</f>
+        <f t="shared" ref="F115" si="29">+G114</f>
         <v>33.26</v>
       </c>
       <c r="G115" s="160">
@@ -25674,7 +25756,9 @@
       <c r="B117" s="163">
         <v>44166</v>
       </c>
-      <c r="C117" s="160"/>
+      <c r="C117" s="160">
+        <v>40.28</v>
+      </c>
       <c r="D117" s="167">
         <f>+D116+1</f>
         <v>1</v>
@@ -25682,10 +25766,16 @@
       <c r="E117" s="188" t="s">
         <v>984</v>
       </c>
-      <c r="F117" s="160"/>
-      <c r="G117" s="160"/>
+      <c r="F117" s="160">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G117" s="160">
+        <v>8.4700000000000006</v>
+      </c>
       <c r="H117" s="160"/>
-      <c r="I117" s="160"/>
+      <c r="I117" s="160" t="s">
+        <v>997</v>
+      </c>
     </row>
     <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="160"/>
@@ -25700,9 +25790,11 @@
       </c>
       <c r="F118" s="160">
         <f>+G117</f>
-        <v>0</v>
-      </c>
-      <c r="G118" s="160"/>
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="G118" s="160">
+        <v>17.190000000000001</v>
+      </c>
       <c r="H118" s="160"/>
       <c r="I118" s="160"/>
     </row>
@@ -25719,9 +25811,11 @@
       </c>
       <c r="F119" s="160">
         <f t="shared" ref="F119:F120" si="30">+G118</f>
-        <v>0</v>
-      </c>
-      <c r="G119" s="160"/>
+        <v>17.190000000000001</v>
+      </c>
+      <c r="G119" s="160">
+        <v>31.17</v>
+      </c>
       <c r="H119" s="160"/>
       <c r="I119" s="160"/>
     </row>
@@ -25738,9 +25832,11 @@
       </c>
       <c r="F120" s="160">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="G120" s="160"/>
+        <v>31.17</v>
+      </c>
+      <c r="G120" s="160">
+        <v>39.520000000000003</v>
+      </c>
       <c r="H120" s="160"/>
       <c r="I120" s="160"/>
     </row>
@@ -25756,24 +25852,51 @@
       <c r="I121" s="160"/>
     </row>
     <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A122" s="160"/>
-      <c r="B122" s="160"/>
-      <c r="C122" s="160"/>
-      <c r="D122" s="160"/>
-      <c r="E122" s="160"/>
-      <c r="F122" s="160"/>
-      <c r="G122" s="160"/>
+      <c r="A122" s="160">
+        <v>20</v>
+      </c>
+      <c r="B122" s="163">
+        <v>44167</v>
+      </c>
+      <c r="C122" s="160">
+        <v>51.34</v>
+      </c>
+      <c r="D122" s="167">
+        <f>+D121+1</f>
+        <v>1</v>
+      </c>
+      <c r="E122" s="189" t="s">
+        <v>989</v>
+      </c>
+      <c r="F122" s="160">
+        <v>8.51</v>
+      </c>
+      <c r="G122" s="170">
+        <v>17.399999999999999</v>
+      </c>
       <c r="H122" s="160"/>
-      <c r="I122" s="160"/>
+      <c r="I122" s="160" t="s">
+        <v>998</v>
+      </c>
     </row>
     <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="160"/>
       <c r="B123" s="160"/>
       <c r="C123" s="160"/>
-      <c r="D123" s="160"/>
-      <c r="E123" s="160"/>
-      <c r="F123" s="160"/>
-      <c r="G123" s="160"/>
+      <c r="D123" s="167">
+        <f t="shared" ref="D123" si="31">+D122+1</f>
+        <v>2</v>
+      </c>
+      <c r="E123" s="189" t="s">
+        <v>990</v>
+      </c>
+      <c r="F123" s="170">
+        <f>+G122</f>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G123" s="170">
+        <v>39.44</v>
+      </c>
       <c r="H123" s="160"/>
       <c r="I123" s="160"/>
     </row>
@@ -25781,12 +25904,475 @@
       <c r="A124" s="160"/>
       <c r="B124" s="160"/>
       <c r="C124" s="160"/>
-      <c r="D124" s="160"/>
-      <c r="E124" s="160"/>
-      <c r="F124" s="160"/>
-      <c r="G124" s="160"/>
+      <c r="D124" s="167"/>
+      <c r="E124" s="189"/>
+      <c r="F124" s="170"/>
+      <c r="G124" s="170"/>
       <c r="H124" s="160"/>
       <c r="I124" s="160"/>
+    </row>
+    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A125" s="190">
+        <v>21</v>
+      </c>
+      <c r="B125" s="192">
+        <v>44168</v>
+      </c>
+      <c r="C125" s="190">
+        <v>45.02</v>
+      </c>
+      <c r="D125" s="167">
+        <f>+D124+1</f>
+        <v>1</v>
+      </c>
+      <c r="E125" s="190" t="s">
+        <v>992</v>
+      </c>
+      <c r="F125" s="191">
+        <v>10.48</v>
+      </c>
+      <c r="G125" s="191">
+        <v>23.36</v>
+      </c>
+      <c r="H125" s="190"/>
+      <c r="I125" s="190" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A126" s="190"/>
+      <c r="B126" s="190"/>
+      <c r="C126" s="190"/>
+      <c r="D126" s="167">
+        <f t="shared" ref="D126:D135" si="32">+D125+1</f>
+        <v>2</v>
+      </c>
+      <c r="E126" s="190" t="s">
+        <v>993</v>
+      </c>
+      <c r="F126" s="191">
+        <f>+G125</f>
+        <v>23.36</v>
+      </c>
+      <c r="G126" s="190">
+        <v>26.38</v>
+      </c>
+      <c r="H126" s="190"/>
+      <c r="I126" s="190"/>
+    </row>
+    <row r="127" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A127" s="190"/>
+      <c r="B127" s="190"/>
+      <c r="C127" s="190"/>
+      <c r="D127" s="167">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="E127" s="190" t="s">
+        <v>994</v>
+      </c>
+      <c r="F127" s="191">
+        <f t="shared" ref="F127:F129" si="33">+G126</f>
+        <v>26.38</v>
+      </c>
+      <c r="G127" s="190">
+        <v>35.590000000000003</v>
+      </c>
+      <c r="H127" s="190"/>
+      <c r="I127" s="190"/>
+    </row>
+    <row r="128" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A128" s="190"/>
+      <c r="B128" s="190"/>
+      <c r="C128" s="190"/>
+      <c r="D128" s="167">
+        <f t="shared" si="32"/>
+        <v>4</v>
+      </c>
+      <c r="E128" s="190" t="s">
+        <v>995</v>
+      </c>
+      <c r="F128" s="191">
+        <f t="shared" si="33"/>
+        <v>35.590000000000003</v>
+      </c>
+      <c r="G128" s="191">
+        <v>44.1</v>
+      </c>
+      <c r="H128" s="190"/>
+      <c r="I128" s="190"/>
+    </row>
+    <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A129" s="190"/>
+      <c r="B129" s="190"/>
+      <c r="C129" s="190"/>
+      <c r="D129" s="167"/>
+      <c r="E129" s="190"/>
+      <c r="F129" s="191"/>
+      <c r="G129" s="190"/>
+      <c r="H129" s="190"/>
+      <c r="I129" s="190"/>
+    </row>
+    <row r="130" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A130" s="190">
+        <v>22</v>
+      </c>
+      <c r="B130" s="192">
+        <v>44169</v>
+      </c>
+      <c r="C130" s="190"/>
+      <c r="D130" s="167">
+        <f>+D129+1</f>
+        <v>1</v>
+      </c>
+      <c r="E130" s="190" t="s">
+        <v>996</v>
+      </c>
+      <c r="F130" s="190"/>
+      <c r="G130" s="191">
+        <v>0</v>
+      </c>
+      <c r="H130" s="190"/>
+      <c r="I130" s="190"/>
+    </row>
+    <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A131" s="190"/>
+      <c r="B131" s="190"/>
+      <c r="C131" s="190"/>
+      <c r="D131" s="167">
+        <f t="shared" si="32"/>
+        <v>2</v>
+      </c>
+      <c r="E131" s="190" t="s">
+        <v>999</v>
+      </c>
+      <c r="F131" s="191">
+        <f>+G130</f>
+        <v>0</v>
+      </c>
+      <c r="G131" s="190"/>
+      <c r="H131" s="190"/>
+      <c r="I131" s="190"/>
+    </row>
+    <row r="132" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A132" s="190"/>
+      <c r="B132" s="190"/>
+      <c r="C132" s="190"/>
+      <c r="D132" s="167">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="E132" s="190" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F132" s="191">
+        <f t="shared" ref="F132:F135" si="34">+G131</f>
+        <v>0</v>
+      </c>
+      <c r="G132" s="190"/>
+      <c r="H132" s="190"/>
+      <c r="I132" s="190"/>
+    </row>
+    <row r="133" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A133" s="190"/>
+      <c r="B133" s="190"/>
+      <c r="C133" s="190"/>
+      <c r="D133" s="167">
+        <f t="shared" si="32"/>
+        <v>4</v>
+      </c>
+      <c r="E133" s="190" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F133" s="191">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="G133" s="190"/>
+      <c r="H133" s="190"/>
+      <c r="I133" s="190"/>
+    </row>
+    <row r="134" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A134" s="190"/>
+      <c r="B134" s="190"/>
+      <c r="C134" s="190"/>
+      <c r="D134" s="167">
+        <f t="shared" si="32"/>
+        <v>5</v>
+      </c>
+      <c r="E134" s="190" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F134" s="191">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="G134" s="190"/>
+      <c r="H134" s="190"/>
+      <c r="I134" s="190"/>
+    </row>
+    <row r="135" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A135" s="190"/>
+      <c r="B135" s="190"/>
+      <c r="C135" s="190"/>
+      <c r="D135" s="167">
+        <f t="shared" si="32"/>
+        <v>6</v>
+      </c>
+      <c r="E135" s="190" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F135" s="191">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="G135" s="190"/>
+      <c r="H135" s="190"/>
+      <c r="I135" s="190"/>
+    </row>
+    <row r="136" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A136" s="190"/>
+      <c r="B136" s="190"/>
+      <c r="C136" s="190"/>
+      <c r="D136" s="190"/>
+      <c r="E136" s="190"/>
+      <c r="F136" s="190"/>
+      <c r="G136" s="190"/>
+      <c r="H136" s="190"/>
+      <c r="I136" s="190"/>
+    </row>
+    <row r="137" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A137" s="190"/>
+      <c r="B137" s="190"/>
+      <c r="C137" s="190"/>
+      <c r="D137" s="190"/>
+      <c r="E137" s="190"/>
+      <c r="F137" s="190"/>
+      <c r="G137" s="190"/>
+      <c r="H137" s="190"/>
+      <c r="I137" s="190"/>
+    </row>
+    <row r="138" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A138" s="190">
+        <v>23</v>
+      </c>
+      <c r="B138" s="192">
+        <v>44170</v>
+      </c>
+      <c r="C138" s="190"/>
+      <c r="D138" s="167">
+        <f>+D137+1</f>
+        <v>1</v>
+      </c>
+      <c r="E138" s="190" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F138" s="190"/>
+      <c r="G138" s="190"/>
+      <c r="H138" s="190"/>
+      <c r="I138" s="190"/>
+    </row>
+    <row r="139" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A139" s="190"/>
+      <c r="B139" s="190"/>
+      <c r="C139" s="190"/>
+      <c r="D139" s="167">
+        <f t="shared" ref="D139:D144" si="35">+D138+1</f>
+        <v>2</v>
+      </c>
+      <c r="E139" s="190" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F139" s="191">
+        <f t="shared" ref="F139:F144" si="36">+G138</f>
+        <v>0</v>
+      </c>
+      <c r="G139" s="190"/>
+      <c r="H139" s="190"/>
+      <c r="I139" s="190"/>
+    </row>
+    <row r="140" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A140" s="190"/>
+      <c r="B140" s="190"/>
+      <c r="C140" s="190"/>
+      <c r="D140" s="167">
+        <f t="shared" si="35"/>
+        <v>3</v>
+      </c>
+      <c r="E140" s="190" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F140" s="191">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="G140" s="190"/>
+      <c r="H140" s="190"/>
+      <c r="I140" s="190"/>
+    </row>
+    <row r="141" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A141" s="190"/>
+      <c r="B141" s="190"/>
+      <c r="C141" s="190"/>
+      <c r="D141" s="167">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
+      <c r="E141" s="190" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F141" s="191">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="G141" s="190"/>
+      <c r="H141" s="190"/>
+      <c r="I141" s="190"/>
+    </row>
+    <row r="142" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A142" s="190"/>
+      <c r="B142" s="190"/>
+      <c r="C142" s="190"/>
+      <c r="D142" s="167">
+        <f t="shared" si="35"/>
+        <v>5</v>
+      </c>
+      <c r="E142" s="190" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F142" s="191">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="G142" s="190"/>
+      <c r="H142" s="190"/>
+      <c r="I142" s="190"/>
+    </row>
+    <row r="143" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A143" s="190"/>
+      <c r="B143" s="190"/>
+      <c r="C143" s="190"/>
+      <c r="D143" s="167">
+        <f t="shared" si="35"/>
+        <v>6</v>
+      </c>
+      <c r="E143" s="190" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F143" s="191">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="G143" s="190"/>
+      <c r="H143" s="190"/>
+      <c r="I143" s="190"/>
+    </row>
+    <row r="144" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A144" s="190"/>
+      <c r="B144" s="190"/>
+      <c r="C144" s="190"/>
+      <c r="D144" s="167">
+        <f t="shared" si="35"/>
+        <v>7</v>
+      </c>
+      <c r="E144" s="190" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F144" s="191">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="G144" s="190"/>
+      <c r="H144" s="190"/>
+      <c r="I144" s="190"/>
+    </row>
+    <row r="145" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A145" s="190"/>
+      <c r="B145" s="190"/>
+      <c r="C145" s="190"/>
+      <c r="D145" s="190"/>
+      <c r="E145" s="190"/>
+      <c r="F145" s="190"/>
+      <c r="G145" s="190"/>
+      <c r="H145" s="190"/>
+      <c r="I145" s="190"/>
+    </row>
+    <row r="146" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A146" s="190"/>
+      <c r="B146" s="190"/>
+      <c r="C146" s="190"/>
+      <c r="D146" s="190"/>
+      <c r="E146" s="190"/>
+      <c r="F146" s="190"/>
+      <c r="G146" s="190"/>
+      <c r="H146" s="190"/>
+      <c r="I146" s="190"/>
+    </row>
+    <row r="147" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A147" s="190"/>
+      <c r="B147" s="190"/>
+      <c r="C147" s="190"/>
+      <c r="D147" s="190"/>
+      <c r="E147" s="190"/>
+      <c r="F147" s="190"/>
+      <c r="G147" s="190"/>
+      <c r="H147" s="190"/>
+      <c r="I147" s="190"/>
+    </row>
+    <row r="148" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A148" s="190"/>
+      <c r="B148" s="190"/>
+      <c r="C148" s="190"/>
+      <c r="D148" s="190"/>
+      <c r="E148" s="190"/>
+      <c r="F148" s="190"/>
+      <c r="G148" s="190"/>
+      <c r="H148" s="190"/>
+      <c r="I148" s="190"/>
+    </row>
+    <row r="149" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A149" s="190"/>
+      <c r="B149" s="190"/>
+      <c r="C149" s="190"/>
+      <c r="D149" s="190"/>
+      <c r="E149" s="190"/>
+      <c r="F149" s="190"/>
+      <c r="G149" s="190"/>
+      <c r="H149" s="190"/>
+      <c r="I149" s="190"/>
+    </row>
+    <row r="150" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A150" s="190"/>
+      <c r="B150" s="190"/>
+      <c r="C150" s="190"/>
+      <c r="D150" s="190"/>
+      <c r="E150" s="190"/>
+      <c r="F150" s="190"/>
+      <c r="G150" s="190"/>
+      <c r="H150" s="190"/>
+      <c r="I150" s="190"/>
+    </row>
+    <row r="151" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A151" s="190"/>
+      <c r="B151" s="190"/>
+      <c r="C151" s="190"/>
+      <c r="D151" s="190"/>
+      <c r="E151" s="190"/>
+      <c r="F151" s="190"/>
+      <c r="G151" s="190"/>
+      <c r="H151" s="190"/>
+      <c r="I151" s="190"/>
+    </row>
+    <row r="152" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A152" s="190"/>
+      <c r="B152" s="190"/>
+      <c r="C152" s="190"/>
+      <c r="D152" s="190"/>
+      <c r="E152" s="190"/>
+      <c r="F152" s="190"/>
+      <c r="G152" s="190"/>
+      <c r="H152" s="190"/>
+      <c r="I152" s="190"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TS 2.1-2.3 Template changes 04/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="1011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="1012">
   <si>
     <t>Date</t>
   </si>
@@ -3053,19 +3053,28 @@
   </si>
   <si>
     <t>7.5.25.1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=doE4wuv5XYM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="145" x14ac:knownFonts="1">
+  <fonts count="146" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3970,77 +3979,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="141" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="142" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="142" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="143" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="142" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="143" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="141" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="142" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="142" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="143" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="135" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="131" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="135" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="124" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="109" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="143" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="144" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="143" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="143" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="144" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="144" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4049,17 +4059,17 @@
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="92" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4074,19 +4084,19 @@
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="142" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="143" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="143" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="144" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4103,40 +4113,40 @@
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4146,48 +4156,48 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9287,7 +9297,7 @@
   <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I132" sqref="I132"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9298,7 +9308,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="86.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
@@ -9367,7 +9377,7 @@
         <v>44044</v>
       </c>
       <c r="C4" s="1">
-        <v>57.23</v>
+        <v>57.24</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -23360,8 +23370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="H142" sqref="H142"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="G137" sqref="G137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25944,7 +25954,7 @@
       <c r="B126" s="190"/>
       <c r="C126" s="190"/>
       <c r="D126" s="167">
-        <f t="shared" ref="D126:D135" si="32">+D125+1</f>
+        <f t="shared" ref="D126:D136" si="32">+D125+1</f>
         <v>2</v>
       </c>
       <c r="E126" s="190" t="s">
@@ -25972,7 +25982,7 @@
         <v>994</v>
       </c>
       <c r="F127" s="191">
-        <f t="shared" ref="F127:F129" si="33">+G126</f>
+        <f t="shared" ref="F127:F128" si="33">+G126</f>
         <v>26.38</v>
       </c>
       <c r="G127" s="190">
@@ -26020,7 +26030,9 @@
       <c r="B130" s="192">
         <v>44169</v>
       </c>
-      <c r="C130" s="190"/>
+      <c r="C130" s="190">
+        <v>46.44</v>
+      </c>
       <c r="D130" s="167">
         <f>+D129+1</f>
         <v>1</v>
@@ -26028,12 +26040,16 @@
       <c r="E130" s="190" t="s">
         <v>996</v>
       </c>
-      <c r="F130" s="190"/>
+      <c r="F130" s="190">
+        <v>11.36</v>
+      </c>
       <c r="G130" s="191">
-        <v>0</v>
+        <v>14.39</v>
       </c>
       <c r="H130" s="190"/>
-      <c r="I130" s="190"/>
+      <c r="I130" s="190" t="s">
+        <v>1011</v>
+      </c>
     </row>
     <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="190"/>
@@ -26048,9 +26064,11 @@
       </c>
       <c r="F131" s="191">
         <f>+G130</f>
-        <v>0</v>
-      </c>
-      <c r="G131" s="190"/>
+        <v>14.39</v>
+      </c>
+      <c r="G131" s="190">
+        <v>21.04</v>
+      </c>
       <c r="H131" s="190"/>
       <c r="I131" s="190"/>
     </row>
@@ -26066,10 +26084,12 @@
         <v>1000</v>
       </c>
       <c r="F132" s="191">
-        <f t="shared" ref="F132:F135" si="34">+G131</f>
-        <v>0</v>
-      </c>
-      <c r="G132" s="190"/>
+        <f t="shared" ref="F132:F136" si="34">+G131</f>
+        <v>21.04</v>
+      </c>
+      <c r="G132" s="190">
+        <v>32.270000000000003</v>
+      </c>
       <c r="H132" s="190"/>
       <c r="I132" s="190"/>
     </row>
@@ -26086,9 +26106,11 @@
       </c>
       <c r="F133" s="191">
         <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="G133" s="190"/>
+        <v>32.270000000000003</v>
+      </c>
+      <c r="G133" s="190">
+        <v>35.17</v>
+      </c>
       <c r="H133" s="190"/>
       <c r="I133" s="190"/>
     </row>
@@ -26105,9 +26127,11 @@
       </c>
       <c r="F134" s="191">
         <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="G134" s="190"/>
+        <v>35.17</v>
+      </c>
+      <c r="G134" s="190">
+        <v>38.15</v>
+      </c>
       <c r="H134" s="190"/>
       <c r="I134" s="190"/>
     </row>
@@ -26124,9 +26148,11 @@
       </c>
       <c r="F135" s="191">
         <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="G135" s="190"/>
+        <v>38.15</v>
+      </c>
+      <c r="G135" s="190">
+        <v>41.46</v>
+      </c>
       <c r="H135" s="190"/>
       <c r="I135" s="190"/>
     </row>
@@ -26134,10 +26160,20 @@
       <c r="A136" s="190"/>
       <c r="B136" s="190"/>
       <c r="C136" s="190"/>
-      <c r="D136" s="190"/>
-      <c r="E136" s="190"/>
-      <c r="F136" s="190"/>
-      <c r="G136" s="190"/>
+      <c r="D136" s="167">
+        <f t="shared" si="32"/>
+        <v>7</v>
+      </c>
+      <c r="E136" s="193" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F136" s="191">
+        <f t="shared" si="34"/>
+        <v>41.46</v>
+      </c>
+      <c r="G136" s="190">
+        <v>46.06</v>
+      </c>
       <c r="H136" s="190"/>
       <c r="I136" s="190"/>
     </row>
@@ -26161,13 +26197,16 @@
       </c>
       <c r="C138" s="190"/>
       <c r="D138" s="167">
-        <f>+D137+1</f>
+        <f>1</f>
         <v>1</v>
       </c>
       <c r="E138" s="190" t="s">
-        <v>1004</v>
-      </c>
-      <c r="F138" s="190"/>
+        <v>1005</v>
+      </c>
+      <c r="F138" s="191">
+        <f>+G138</f>
+        <v>0</v>
+      </c>
       <c r="G138" s="190"/>
       <c r="H138" s="190"/>
       <c r="I138" s="190"/>
@@ -26177,14 +26216,14 @@
       <c r="B139" s="190"/>
       <c r="C139" s="190"/>
       <c r="D139" s="167">
-        <f t="shared" ref="D139:D144" si="35">+D138+1</f>
+        <f>+D138+1</f>
         <v>2</v>
       </c>
       <c r="E139" s="190" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="F139" s="191">
-        <f t="shared" ref="F139:F144" si="36">+G138</f>
+        <f>+G139</f>
         <v>0</v>
       </c>
       <c r="G139" s="190"/>
@@ -26196,14 +26235,14 @@
       <c r="B140" s="190"/>
       <c r="C140" s="190"/>
       <c r="D140" s="167">
-        <f t="shared" si="35"/>
+        <f>+D139+1</f>
         <v>3</v>
       </c>
       <c r="E140" s="190" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="F140" s="191">
-        <f t="shared" si="36"/>
+        <f>+G140</f>
         <v>0</v>
       </c>
       <c r="G140" s="190"/>
@@ -26215,14 +26254,14 @@
       <c r="B141" s="190"/>
       <c r="C141" s="190"/>
       <c r="D141" s="167">
-        <f t="shared" si="35"/>
+        <f>+D140+1</f>
         <v>4</v>
       </c>
       <c r="E141" s="190" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="F141" s="191">
-        <f t="shared" si="36"/>
+        <f>+G141</f>
         <v>0</v>
       </c>
       <c r="G141" s="190"/>
@@ -26234,14 +26273,14 @@
       <c r="B142" s="190"/>
       <c r="C142" s="190"/>
       <c r="D142" s="167">
-        <f t="shared" si="35"/>
+        <f>+D141+1</f>
         <v>5</v>
       </c>
       <c r="E142" s="190" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="F142" s="191">
-        <f t="shared" si="36"/>
+        <f>+G142</f>
         <v>0</v>
       </c>
       <c r="G142" s="190"/>
@@ -26253,14 +26292,14 @@
       <c r="B143" s="190"/>
       <c r="C143" s="190"/>
       <c r="D143" s="167">
-        <f t="shared" si="35"/>
+        <f>+D142+1</f>
         <v>6</v>
       </c>
       <c r="E143" s="190" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="F143" s="191">
-        <f t="shared" si="36"/>
+        <f>+G143</f>
         <v>0</v>
       </c>
       <c r="G143" s="190"/>
@@ -26271,17 +26310,6 @@
       <c r="A144" s="190"/>
       <c r="B144" s="190"/>
       <c r="C144" s="190"/>
-      <c r="D144" s="167">
-        <f t="shared" si="35"/>
-        <v>7</v>
-      </c>
-      <c r="E144" s="190" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F144" s="191">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
       <c r="G144" s="190"/>
       <c r="H144" s="190"/>
       <c r="I144" s="190"/>

</xml_diff>

<commit_message>
Shanti Japam, Padam Input 07/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -3065,13 +3065,31 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="146" x14ac:knownFonts="1">
+  <fonts count="149" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3944,7 +3962,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3969,6 +3987,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3982,96 +4006,99 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="142" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="143" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="146" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="143" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="146" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="142" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="143" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="146" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="138" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="135" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="138" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="135" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="124" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="117" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="147" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="147" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="144" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="144" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="144" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4084,21 +4111,21 @@
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="143" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="146" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="144" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="147" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4113,42 +4140,42 @@
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="57" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="54" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4156,51 +4183,52 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9297,10 +9325,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K133"/>
+  <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9311,10 +9339,11 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="86.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="86.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -9335,13 +9364,14 @@
       <c r="H1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -9365,14 +9395,15 @@
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="1"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -9395,13 +9426,14 @@
         <v>22.28</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
@@ -9421,8 +9453,9 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
@@ -9443,9 +9476,12 @@
       <c r="H6" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="I6" s="195" t="s">
+        <v>867</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
@@ -9455,8 +9491,9 @@
       <c r="G7" s="16"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -9479,11 +9516,12 @@
         <v>16.13</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
@@ -9504,9 +9542,10 @@
       <c r="H9" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="I9" s="17"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
@@ -9526,9 +9565,12 @@
       <c r="H10" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="I10" s="194" t="s">
+        <v>867</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
@@ -9538,8 +9580,9 @@
       <c r="G11" s="16"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -9562,11 +9605,12 @@
         <v>13.19</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
@@ -9586,8 +9630,9 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
@@ -9608,9 +9653,12 @@
       <c r="H14" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="I14" s="194" t="s">
+        <v>867</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
@@ -9620,8 +9668,9 @@
       <c r="G15" s="16"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -9644,11 +9693,12 @@
         <v>12.42</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
@@ -9668,8 +9718,9 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
@@ -9689,8 +9740,9 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
@@ -9710,8 +9762,9 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
@@ -9732,11 +9785,14 @@
       <c r="H20" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="196" t="s">
+        <v>867</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
@@ -9746,8 +9802,9 @@
       <c r="G21" s="16"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>5</v>
       </c>
@@ -9772,11 +9829,14 @@
       <c r="H22" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="197" t="s">
+        <v>867</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
@@ -9795,8 +9855,9 @@
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
@@ -9817,9 +9878,10 @@
       <c r="H24" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I24" s="21"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -9829,8 +9891,9 @@
       <c r="G25" s="16"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
-    </row>
-    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J25" s="15"/>
+    </row>
+    <row r="26" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>6</v>
       </c>
@@ -9853,11 +9916,12 @@
         <v>6.08</v>
       </c>
       <c r="H26" s="15"/>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="15"/>
+      <c r="J26" s="15" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -9877,8 +9941,9 @@
       </c>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
-    </row>
-    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -9899,9 +9964,10 @@
       <c r="H28" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="I28" s="15"/>
-    </row>
-    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I28" s="23"/>
+      <c r="J28" s="15"/>
+    </row>
+    <row r="29" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -9921,9 +9987,10 @@
       <c r="H29" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="I29" s="15"/>
-    </row>
-    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I29" s="24"/>
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -9933,8 +10000,9 @@
       <c r="G30" s="16"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
-    </row>
-    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>7</v>
       </c>
@@ -9959,11 +10027,12 @@
       <c r="H31" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="I31" s="24"/>
+      <c r="J31" s="15" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -9982,8 +10051,9 @@
       </c>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
-    </row>
-    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J32" s="15"/>
+    </row>
+    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -10004,9 +10074,10 @@
       <c r="H33" s="24" t="s">
         <v>260</v>
       </c>
-      <c r="I33" s="15"/>
-    </row>
-    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I33" s="24"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -10019,8 +10090,9 @@
       <c r="G34" s="16"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
-    </row>
-    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -10030,8 +10102,9 @@
       <c r="G35" s="16"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
-    </row>
-    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J35" s="15"/>
+    </row>
+    <row r="36" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>8</v>
       </c>
@@ -10054,11 +10127,12 @@
         <v>15.48</v>
       </c>
       <c r="H36" s="15"/>
-      <c r="I36" s="15" t="s">
+      <c r="I36" s="15"/>
+      <c r="J36" s="15" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -10078,8 +10152,9 @@
       </c>
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
-    </row>
-    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -10100,9 +10175,10 @@
       <c r="H38" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="I38" s="15"/>
-    </row>
-    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I38" s="26"/>
+      <c r="J38" s="15"/>
+    </row>
+    <row r="39" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="22"/>
       <c r="C39" s="15"/>
@@ -10112,8 +10188,9 @@
       <c r="G39" s="16"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15"/>
-    </row>
-    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J39" s="15"/>
+    </row>
+    <row r="40" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>9</v>
       </c>
@@ -10136,11 +10213,12 @@
         <v>10.54</v>
       </c>
       <c r="H40" s="15"/>
-      <c r="I40" s="15" t="s">
+      <c r="I40" s="15"/>
+      <c r="J40" s="15" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -10160,8 +10238,9 @@
       </c>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
-    </row>
-    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J41" s="15"/>
+    </row>
+    <row r="42" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="22"/>
       <c r="C42" s="15"/>
@@ -10182,9 +10261,10 @@
       <c r="H42" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="I42" s="15"/>
-    </row>
-    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I42" s="26"/>
+      <c r="J42" s="15"/>
+    </row>
+    <row r="43" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -10194,8 +10274,9 @@
       <c r="G43" s="16"/>
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
-    </row>
-    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J43" s="15"/>
+    </row>
+    <row r="44" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>10</v>
       </c>
@@ -10218,11 +10299,12 @@
         <v>9.07</v>
       </c>
       <c r="H44" s="15"/>
-      <c r="I44" s="15" t="s">
+      <c r="I44" s="15"/>
+      <c r="J44" s="15" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="22"/>
       <c r="C45" s="15"/>
@@ -10243,9 +10325,10 @@
       <c r="H45" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="I45" s="15"/>
-    </row>
-    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I45" s="29"/>
+      <c r="J45" s="15"/>
+    </row>
+    <row r="46" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -10264,8 +10347,9 @@
       </c>
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
-    </row>
-    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J46" s="15"/>
+    </row>
+    <row r="47" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -10286,9 +10370,10 @@
       <c r="H47" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="I47" s="15"/>
-    </row>
-    <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I47" s="30"/>
+      <c r="J47" s="15"/>
+    </row>
+    <row r="48" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="B48" s="22"/>
       <c r="C48" s="15"/>
@@ -10298,8 +10383,9 @@
       <c r="G48" s="16"/>
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
-    </row>
-    <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J48" s="15"/>
+    </row>
+    <row r="49" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>11</v>
       </c>
@@ -10322,11 +10408,12 @@
         <v>23.44</v>
       </c>
       <c r="H49" s="15"/>
-      <c r="I49" s="15" t="s">
+      <c r="I49" s="15"/>
+      <c r="J49" s="15" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -10346,8 +10433,9 @@
       </c>
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
-    </row>
-    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J50" s="15"/>
+    </row>
+    <row r="51" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
       <c r="B51" s="22"/>
       <c r="C51" s="15"/>
@@ -10367,8 +10455,9 @@
       </c>
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
-    </row>
-    <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J51" s="15"/>
+    </row>
+    <row r="52" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
@@ -10389,9 +10478,10 @@
       <c r="H52" s="30" t="s">
         <v>282</v>
       </c>
-      <c r="I52" s="15"/>
-    </row>
-    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I52" s="30"/>
+      <c r="J52" s="15"/>
+    </row>
+    <row r="53" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -10401,8 +10491,9 @@
       <c r="G53" s="16"/>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
-    </row>
-    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J53" s="15"/>
+    </row>
+    <row r="54" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <v>12</v>
       </c>
@@ -10425,11 +10516,12 @@
         <v>9.48</v>
       </c>
       <c r="H54" s="15"/>
-      <c r="I54" s="15" t="s">
+      <c r="I54" s="15"/>
+      <c r="J54" s="15" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
@@ -10449,8 +10541,9 @@
       </c>
       <c r="H55" s="15"/>
       <c r="I55" s="15"/>
-    </row>
-    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J55" s="15"/>
+    </row>
+    <row r="56" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
@@ -10470,8 +10563,9 @@
       </c>
       <c r="H56" s="15"/>
       <c r="I56" s="15"/>
-    </row>
-    <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J56" s="15"/>
+    </row>
+    <row r="57" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
       <c r="B57" s="22"/>
       <c r="C57" s="15"/>
@@ -10491,8 +10585,9 @@
       </c>
       <c r="H57" s="15"/>
       <c r="I57" s="15"/>
-    </row>
-    <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J57" s="15"/>
+    </row>
+    <row r="58" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
@@ -10512,8 +10607,9 @@
       </c>
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
-    </row>
-    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J58" s="15"/>
+    </row>
+    <row r="59" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
@@ -10534,9 +10630,10 @@
       <c r="H59" s="32" t="s">
         <v>292</v>
       </c>
-      <c r="I59" s="15"/>
-    </row>
-    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I59" s="32"/>
+      <c r="J59" s="15"/>
+    </row>
+    <row r="60" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="22"/>
       <c r="C60" s="15"/>
@@ -10546,8 +10643,9 @@
       <c r="G60" s="16"/>
       <c r="H60" s="15"/>
       <c r="I60" s="15"/>
-    </row>
-    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J60" s="15"/>
+    </row>
+    <row r="61" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
@@ -10557,8 +10655,9 @@
       <c r="G61" s="16"/>
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
-    </row>
-    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J61" s="15"/>
+    </row>
+    <row r="62" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>13</v>
       </c>
@@ -10581,11 +10680,12 @@
         <v>7.19</v>
       </c>
       <c r="H62" s="15"/>
-      <c r="I62" s="15" t="s">
+      <c r="I62" s="15"/>
+      <c r="J62" s="15" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="B63" s="22"/>
       <c r="C63" s="15"/>
@@ -10605,8 +10705,9 @@
       </c>
       <c r="H63" s="15"/>
       <c r="I63" s="15"/>
-    </row>
-    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J63" s="15"/>
+    </row>
+    <row r="64" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -10627,9 +10728,10 @@
       <c r="H64" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="I64" s="15"/>
-    </row>
-    <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I64" s="32"/>
+      <c r="J64" s="15"/>
+    </row>
+    <row r="65" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
@@ -10648,8 +10750,9 @@
       </c>
       <c r="H65" s="15"/>
       <c r="I65" s="15"/>
-    </row>
-    <row r="66" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J65" s="15"/>
+    </row>
+    <row r="66" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="15"/>
       <c r="B66" s="22"/>
       <c r="C66" s="15"/>
@@ -10670,9 +10773,10 @@
       <c r="H66" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="I66" s="15"/>
-    </row>
-    <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I66" s="32"/>
+      <c r="J66" s="15"/>
+    </row>
+    <row r="67" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
@@ -10682,8 +10786,9 @@
       <c r="G67" s="16"/>
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
-    </row>
-    <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J67" s="15"/>
+    </row>
+    <row r="68" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <v>14</v>
       </c>
@@ -10708,11 +10813,12 @@
       <c r="H68" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="I68" s="15" t="s">
+      <c r="I68" s="34"/>
+      <c r="J68" s="15" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="15"/>
       <c r="B69" s="22"/>
       <c r="C69" s="15"/>
@@ -10731,8 +10837,9 @@
       </c>
       <c r="H69" s="15"/>
       <c r="I69" s="15"/>
-    </row>
-    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J69" s="15"/>
+    </row>
+    <row r="70" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
@@ -10752,8 +10859,9 @@
       </c>
       <c r="H70" s="15"/>
       <c r="I70" s="15"/>
-    </row>
-    <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J70" s="15"/>
+    </row>
+    <row r="71" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="15"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
@@ -10773,8 +10881,9 @@
       </c>
       <c r="H71" s="15"/>
       <c r="I71" s="15"/>
-    </row>
-    <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J71" s="15"/>
+    </row>
+    <row r="72" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
       <c r="B72" s="22"/>
       <c r="C72" s="15"/>
@@ -10784,8 +10893,9 @@
       <c r="G72" s="16"/>
       <c r="H72" s="15"/>
       <c r="I72" s="15"/>
-    </row>
-    <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J72" s="15"/>
+    </row>
+    <row r="73" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>15</v>
       </c>
@@ -10808,11 +10918,12 @@
         <v>14.04</v>
       </c>
       <c r="H73" s="15"/>
-      <c r="I73" s="15" t="s">
+      <c r="I73" s="15"/>
+      <c r="J73" s="15" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="15"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
@@ -10832,8 +10943,9 @@
       </c>
       <c r="H74" s="15"/>
       <c r="I74" s="15"/>
-    </row>
-    <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J74" s="15"/>
+    </row>
+    <row r="75" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="15"/>
       <c r="B75" s="22"/>
       <c r="C75" s="15"/>
@@ -10853,8 +10965,9 @@
       </c>
       <c r="H75" s="15"/>
       <c r="I75" s="15"/>
-    </row>
-    <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J75" s="15"/>
+    </row>
+    <row r="76" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="15"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
@@ -10874,8 +10987,9 @@
       </c>
       <c r="H76" s="15"/>
       <c r="I76" s="15"/>
-    </row>
-    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J76" s="15"/>
+    </row>
+    <row r="77" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="15"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
@@ -10895,8 +11009,9 @@
       </c>
       <c r="H77" s="15"/>
       <c r="I77" s="15"/>
-    </row>
-    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J77" s="15"/>
+    </row>
+    <row r="78" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="15"/>
       <c r="B78" s="22"/>
       <c r="C78" s="15"/>
@@ -10916,8 +11031,9 @@
       </c>
       <c r="H78" s="15"/>
       <c r="I78" s="15"/>
-    </row>
-    <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J78" s="15"/>
+    </row>
+    <row r="79" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="15"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
@@ -10927,8 +11043,9 @@
       <c r="G79" s="16"/>
       <c r="H79" s="15"/>
       <c r="I79" s="15"/>
-    </row>
-    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J79" s="15"/>
+    </row>
+    <row r="80" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <v>16</v>
       </c>
@@ -10951,11 +11068,12 @@
         <v>14.46</v>
       </c>
       <c r="H80" s="15"/>
-      <c r="I80" s="15" t="s">
+      <c r="I80" s="15"/>
+      <c r="J80" s="15" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="15"/>
       <c r="B81" s="22"/>
       <c r="C81" s="15"/>
@@ -10976,9 +11094,10 @@
       <c r="H81" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="I81" s="15"/>
-    </row>
-    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I81" s="36"/>
+      <c r="J81" s="15"/>
+    </row>
+    <row r="82" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="15"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
@@ -10998,12 +11117,13 @@
       <c r="H82" s="37" t="s">
         <v>317</v>
       </c>
-      <c r="I82" s="15"/>
-    </row>
-    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I82" s="37"/>
+      <c r="J82" s="15"/>
+    </row>
+    <row r="83" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="37">
         <v>17</v>
       </c>
@@ -11026,11 +11146,12 @@
         <v>10.06</v>
       </c>
       <c r="H84" s="37"/>
-      <c r="I84" s="37" t="s">
+      <c r="I84" s="37"/>
+      <c r="J84" s="37" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="37"/>
       <c r="B85" s="37"/>
       <c r="C85" s="37"/>
@@ -11050,8 +11171,9 @@
       </c>
       <c r="H85" s="37"/>
       <c r="I85" s="37"/>
-    </row>
-    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J85" s="37"/>
+    </row>
+    <row r="86" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="37"/>
       <c r="B86" s="37"/>
       <c r="C86" s="37"/>
@@ -11071,8 +11193,9 @@
       </c>
       <c r="H86" s="37"/>
       <c r="I86" s="37"/>
-    </row>
-    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J86" s="37"/>
+    </row>
+    <row r="87" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="37"/>
       <c r="B87" s="37"/>
       <c r="C87" s="37"/>
@@ -11092,9 +11215,10 @@
       <c r="H87" s="40" t="s">
         <v>323</v>
       </c>
-      <c r="I87" s="37"/>
-    </row>
-    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I87" s="40"/>
+      <c r="J87" s="37"/>
+    </row>
+    <row r="88" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="37"/>
       <c r="B88" s="37"/>
       <c r="C88" s="37"/>
@@ -11104,8 +11228,9 @@
       <c r="G88" s="39"/>
       <c r="H88" s="37"/>
       <c r="I88" s="37"/>
-    </row>
-    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J88" s="37"/>
+    </row>
+    <row r="89" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="37">
         <v>18</v>
       </c>
@@ -11128,11 +11253,12 @@
         <v>12.32</v>
       </c>
       <c r="H89" s="37"/>
-      <c r="I89" s="37" t="s">
+      <c r="I89" s="37"/>
+      <c r="J89" s="37" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="37"/>
       <c r="B90" s="37"/>
       <c r="C90" s="37"/>
@@ -11151,11 +11277,12 @@
       <c r="H90" s="40" t="s">
         <v>326</v>
       </c>
-      <c r="I90" s="40" t="s">
+      <c r="I90" s="40"/>
+      <c r="J90" s="40" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="37"/>
       <c r="B91" s="37"/>
       <c r="C91" s="37"/>
@@ -11173,9 +11300,10 @@
       <c r="H91" s="41" t="s">
         <v>330</v>
       </c>
-      <c r="I91" s="37"/>
-    </row>
-    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I91" s="41"/>
+      <c r="J91" s="37"/>
+    </row>
+    <row r="92" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="37"/>
       <c r="B92" s="37"/>
       <c r="C92" s="37"/>
@@ -11185,8 +11313,9 @@
       <c r="G92" s="39"/>
       <c r="H92" s="37"/>
       <c r="I92" s="37"/>
-    </row>
-    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J92" s="37"/>
+    </row>
+    <row r="93" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="37">
         <v>19</v>
       </c>
@@ -11209,11 +11338,12 @@
         <v>9.5299999999999994</v>
       </c>
       <c r="H93" s="37"/>
-      <c r="I93" s="37" t="s">
+      <c r="I93" s="37"/>
+      <c r="J93" s="37" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="37"/>
       <c r="B94" s="37"/>
       <c r="C94" s="37"/>
@@ -11234,9 +11364,10 @@
       <c r="H94" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="I94" s="37"/>
-    </row>
-    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I94" s="41"/>
+      <c r="J94" s="37"/>
+    </row>
+    <row r="95" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="37"/>
       <c r="B95" s="37"/>
       <c r="C95" s="37"/>
@@ -11255,8 +11386,9 @@
       </c>
       <c r="H95" s="37"/>
       <c r="I95" s="37"/>
-    </row>
-    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J95" s="37"/>
+    </row>
+    <row r="96" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="37"/>
       <c r="B96" s="37"/>
       <c r="C96" s="37"/>
@@ -11266,8 +11398,9 @@
       <c r="G96" s="39"/>
       <c r="H96" s="37"/>
       <c r="I96" s="37"/>
-    </row>
-    <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J96" s="37"/>
+    </row>
+    <row r="97" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="37">
         <v>20</v>
       </c>
@@ -11290,11 +11423,12 @@
         <v>29.18</v>
       </c>
       <c r="H97" s="37"/>
-      <c r="I97" s="37" t="s">
+      <c r="I97" s="37"/>
+      <c r="J97" s="37" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="37"/>
       <c r="B98" s="37"/>
       <c r="C98" s="37"/>
@@ -11312,8 +11446,9 @@
       <c r="G98" s="39"/>
       <c r="H98" s="37"/>
       <c r="I98" s="37"/>
-    </row>
-    <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J98" s="37"/>
+    </row>
+    <row r="99" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
       <c r="C99" s="37"/>
@@ -11331,9 +11466,10 @@
       <c r="H99" s="42" t="s">
         <v>338</v>
       </c>
-      <c r="I99" s="37"/>
-    </row>
-    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I99" s="42"/>
+      <c r="J99" s="37"/>
+    </row>
+    <row r="100" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="37"/>
       <c r="B100" s="37"/>
       <c r="C100" s="37"/>
@@ -11343,8 +11479,9 @@
       <c r="G100" s="39"/>
       <c r="H100" s="37"/>
       <c r="I100" s="37"/>
-    </row>
-    <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J100" s="37"/>
+    </row>
+    <row r="101" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="37">
         <v>21</v>
       </c>
@@ -11369,11 +11506,12 @@
       <c r="H101" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="I101" s="37" t="s">
+      <c r="I101" s="43"/>
+      <c r="J101" s="37" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="37"/>
@@ -11392,8 +11530,9 @@
       </c>
       <c r="H102" s="37"/>
       <c r="I102" s="37"/>
-    </row>
-    <row r="103" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J102" s="37"/>
+    </row>
+    <row r="103" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="37"/>
       <c r="B103" s="37"/>
       <c r="C103" s="37"/>
@@ -11414,9 +11553,10 @@
       <c r="H103" s="43" t="s">
         <v>343</v>
       </c>
-      <c r="I103" s="37"/>
-    </row>
-    <row r="104" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I103" s="43"/>
+      <c r="J103" s="37"/>
+    </row>
+    <row r="104" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="37"/>
       <c r="B104" s="37"/>
       <c r="C104" s="37"/>
@@ -11426,8 +11566,9 @@
       <c r="G104" s="39"/>
       <c r="H104" s="37"/>
       <c r="I104" s="37"/>
-    </row>
-    <row r="105" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J104" s="37"/>
+    </row>
+    <row r="105" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="37">
         <v>22</v>
       </c>
@@ -11451,8 +11592,9 @@
       </c>
       <c r="H105" s="37"/>
       <c r="I105" s="37"/>
-    </row>
-    <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J105" s="37"/>
+    </row>
+    <row r="106" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
       <c r="C106" s="37"/>
@@ -11472,8 +11614,9 @@
       </c>
       <c r="H106" s="37"/>
       <c r="I106" s="37"/>
-    </row>
-    <row r="107" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J106" s="37"/>
+    </row>
+    <row r="107" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="37"/>
       <c r="B107" s="37"/>
       <c r="C107" s="37"/>
@@ -11494,9 +11637,10 @@
       <c r="H107" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="I107" s="37"/>
-    </row>
-    <row r="108" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I107" s="44"/>
+      <c r="J107" s="37"/>
+    </row>
+    <row r="108" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="37"/>
       <c r="B108" s="37"/>
       <c r="C108" s="37"/>
@@ -11516,9 +11660,10 @@
       <c r="H108" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="I108" s="37"/>
-    </row>
-    <row r="109" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I108" s="46"/>
+      <c r="J108" s="37"/>
+    </row>
+    <row r="109" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="37"/>
       <c r="B109" s="37"/>
       <c r="C109" s="37"/>
@@ -11528,8 +11673,9 @@
       <c r="G109" s="39"/>
       <c r="H109" s="37"/>
       <c r="I109" s="37"/>
-    </row>
-    <row r="110" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J109" s="37"/>
+    </row>
+    <row r="110" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="37">
         <v>23</v>
       </c>
@@ -11552,11 +11698,12 @@
         <v>25.05</v>
       </c>
       <c r="H110" s="37"/>
-      <c r="I110" s="37" t="s">
+      <c r="I110" s="37"/>
+      <c r="J110" s="37" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="37"/>
       <c r="B111" s="37"/>
       <c r="C111" s="37"/>
@@ -11576,8 +11723,9 @@
       </c>
       <c r="H111" s="37"/>
       <c r="I111" s="37"/>
-    </row>
-    <row r="112" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J111" s="37"/>
+    </row>
+    <row r="112" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="37"/>
       <c r="B112" s="37"/>
       <c r="C112" s="37"/>
@@ -11598,9 +11746,10 @@
       <c r="H112" s="47" t="s">
         <v>353</v>
       </c>
-      <c r="I112" s="37"/>
-    </row>
-    <row r="113" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I112" s="47"/>
+      <c r="J112" s="37"/>
+    </row>
+    <row r="113" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="37"/>
       <c r="B113" s="37"/>
       <c r="C113" s="37"/>
@@ -11610,8 +11759,9 @@
       <c r="G113" s="39"/>
       <c r="H113" s="37"/>
       <c r="I113" s="37"/>
-    </row>
-    <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J113" s="37"/>
+    </row>
+    <row r="114" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="37">
         <v>24</v>
       </c>
@@ -11634,11 +11784,12 @@
         <v>18.22</v>
       </c>
       <c r="H114" s="37"/>
-      <c r="I114" s="37" t="s">
+      <c r="I114" s="37"/>
+      <c r="J114" s="37" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="37"/>
       <c r="B115" s="37"/>
       <c r="C115" s="37"/>
@@ -11658,8 +11809,9 @@
       </c>
       <c r="H115" s="37"/>
       <c r="I115" s="37"/>
-    </row>
-    <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J115" s="37"/>
+    </row>
+    <row r="116" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="37"/>
       <c r="B116" s="37"/>
       <c r="C116" s="37"/>
@@ -11679,8 +11831,9 @@
       </c>
       <c r="H116" s="37"/>
       <c r="I116" s="37"/>
-    </row>
-    <row r="117" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J116" s="37"/>
+    </row>
+    <row r="117" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="37"/>
       <c r="B117" s="37"/>
       <c r="C117" s="37"/>
@@ -11701,9 +11854,10 @@
       <c r="H117" s="49" t="s">
         <v>358</v>
       </c>
-      <c r="I117" s="37"/>
-    </row>
-    <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I117" s="49"/>
+      <c r="J117" s="37"/>
+    </row>
+    <row r="118" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="37"/>
       <c r="B118" s="37"/>
       <c r="C118" s="37"/>
@@ -11713,8 +11867,9 @@
       <c r="G118" s="39"/>
       <c r="H118" s="37"/>
       <c r="I118" s="37"/>
-    </row>
-    <row r="119" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J118" s="37"/>
+    </row>
+    <row r="119" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="37">
         <v>25</v>
       </c>
@@ -11737,11 +11892,12 @@
         <v>20.29</v>
       </c>
       <c r="H119" s="37"/>
-      <c r="I119" s="37" t="s">
+      <c r="I119" s="37"/>
+      <c r="J119" s="37" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="37"/>
       <c r="B120" s="37"/>
       <c r="C120" s="37"/>
@@ -11762,9 +11918,10 @@
       <c r="H120" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="I120" s="37"/>
-    </row>
-    <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I120" s="49"/>
+      <c r="J120" s="37"/>
+    </row>
+    <row r="121" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="37"/>
       <c r="B121" s="37"/>
       <c r="C121" s="37"/>
@@ -11784,9 +11941,10 @@
       <c r="H121" s="51" t="s">
         <v>364</v>
       </c>
-      <c r="I121" s="37"/>
-    </row>
-    <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I121" s="51"/>
+      <c r="J121" s="37"/>
+    </row>
+    <row r="122" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="37"/>
       <c r="B122" s="37"/>
       <c r="C122" s="37"/>
@@ -11796,8 +11954,9 @@
       <c r="G122" s="39"/>
       <c r="H122" s="37"/>
       <c r="I122" s="37"/>
-    </row>
-    <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J122" s="37"/>
+    </row>
+    <row r="123" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="37">
         <v>26</v>
       </c>
@@ -11820,11 +11979,12 @@
       <c r="H123" s="51" t="s">
         <v>367</v>
       </c>
-      <c r="I123" s="37" t="s">
+      <c r="I123" s="51"/>
+      <c r="J123" s="37" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="37"/>
       <c r="B124" s="37"/>
       <c r="C124" s="37"/>
@@ -11841,8 +12001,9 @@
       </c>
       <c r="H124" s="37"/>
       <c r="I124" s="37"/>
-    </row>
-    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J124" s="37"/>
+    </row>
+    <row r="125" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="37"/>
       <c r="B125" s="37"/>
       <c r="C125" s="37"/>
@@ -11862,8 +12023,9 @@
       </c>
       <c r="H125" s="37"/>
       <c r="I125" s="37"/>
-    </row>
-    <row r="126" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J125" s="37"/>
+    </row>
+    <row r="126" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="37"/>
       <c r="B126" s="37"/>
       <c r="C126" s="37"/>
@@ -11873,8 +12035,9 @@
       <c r="G126" s="39"/>
       <c r="H126" s="37"/>
       <c r="I126" s="37"/>
-    </row>
-    <row r="127" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J126" s="37"/>
+    </row>
+    <row r="127" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="37">
         <v>27</v>
       </c>
@@ -11897,11 +12060,12 @@
         <v>14.09</v>
       </c>
       <c r="H127" s="37"/>
-      <c r="I127" s="37" t="s">
+      <c r="I127" s="37"/>
+      <c r="J127" s="37" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="37"/>
       <c r="B128" s="37"/>
       <c r="C128" s="37"/>
@@ -11922,9 +12086,10 @@
       <c r="H128" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="I128" s="37"/>
-    </row>
-    <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I128" s="52"/>
+      <c r="J128" s="37"/>
+    </row>
+    <row r="129" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="37"/>
       <c r="B129" s="37"/>
       <c r="C129" s="37"/>
@@ -11943,8 +12108,9 @@
       </c>
       <c r="H129" s="37"/>
       <c r="I129" s="37"/>
-    </row>
-    <row r="130" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J129" s="37"/>
+    </row>
+    <row r="130" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="37"/>
       <c r="B130" s="37"/>
       <c r="C130" s="37"/>
@@ -11965,9 +12131,10 @@
       <c r="H130" s="52" t="s">
         <v>374</v>
       </c>
-      <c r="I130" s="37"/>
-    </row>
-    <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="I130" s="52"/>
+      <c r="J130" s="37"/>
+    </row>
+    <row r="131" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="37"/>
       <c r="B131" s="37"/>
       <c r="C131" s="37"/>
@@ -11977,8 +12144,9 @@
       <c r="G131" s="39"/>
       <c r="H131" s="37"/>
       <c r="I131" s="37"/>
-    </row>
-    <row r="132" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J131" s="37"/>
+    </row>
+    <row r="132" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="37"/>
       <c r="B132" s="37"/>
       <c r="C132" s="37"/>
@@ -11988,8 +12156,9 @@
       <c r="G132" s="39"/>
       <c r="H132" s="37"/>
       <c r="I132" s="37"/>
-    </row>
-    <row r="133" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J132" s="37"/>
+    </row>
+    <row r="133" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="37"/>
       <c r="B133" s="37"/>
       <c r="C133" s="37"/>
@@ -11999,6 +12168,7 @@
       <c r="G133" s="39"/>
       <c r="H133" s="37"/>
       <c r="I133" s="37"/>
+      <c r="J133" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23373,8 +23543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="G144" sqref="G144"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS Padam Templates and GS 2.1.-2.6
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -3065,13 +3065,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="151" x14ac:knownFonts="1">
+  <fonts count="153" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4018,77 +4030,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="147" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="148" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="150" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="148" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="150" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="147" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="148" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="150" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="142" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="140" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="142" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="137" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="140" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="131" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="130" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="128" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="124" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="124" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="121" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="117" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="115" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="149" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="151" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="149" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="149" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="112" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="151" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="151" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="112" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4096,18 +4110,18 @@
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="105" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4121,20 +4135,20 @@
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="148" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="150" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="149" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="151" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4150,41 +4164,41 @@
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="61" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="59" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4193,55 +4207,55 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -9341,8 +9355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10192,7 +10206,9 @@
       <c r="H38" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="I38" s="26"/>
+      <c r="I38" s="200" t="s">
+        <v>867</v>
+      </c>
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -10278,7 +10294,9 @@
       <c r="H42" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="I42" s="26"/>
+      <c r="I42" s="201" t="s">
+        <v>867</v>
+      </c>
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Udaka Shanti Corrections 18/12/2020 2.40 am
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -9390,8 +9390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I87" sqref="I87"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11388,7 +11388,9 @@
       <c r="H91" s="41" t="s">
         <v>330</v>
       </c>
-      <c r="I91" s="41"/>
+      <c r="I91" s="206" t="s">
+        <v>867</v>
+      </c>
       <c r="J91" s="37"/>
     </row>
     <row r="92" spans="1:10" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TS 3.1 Kramam, TS 2.6 template 25/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -9397,8 +9397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="H124" sqref="H124"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="H132" sqref="H132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12199,7 +12199,9 @@
       <c r="H128" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="I128" s="52"/>
+      <c r="I128" s="206" t="s">
+        <v>865</v>
+      </c>
       <c r="J128" s="37"/>
     </row>
     <row r="129" spans="1:10" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Jatai and padam files 26/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -3065,13 +3065,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="159" x14ac:knownFonts="1">
+  <fonts count="160" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4066,77 +4072,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="155" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="156" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="156" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="157" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="156" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="157" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="155" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="156" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="156" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="157" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="148" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="146" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="148" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="138" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="137" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="137" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="136" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="133" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="133" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="128" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="124" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="157" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="158" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="157" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="157" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="120" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="158" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="158" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="121" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="120" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="121" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4145,17 +4152,17 @@
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="112" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="111" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="110" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="107" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="106" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4170,19 +4177,19 @@
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="156" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="157" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="157" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="158" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="90" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4199,40 +4206,40 @@
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="67" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="68" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="62" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="57" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4242,54 +4249,54 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4297,8 +4304,8 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9397,8 +9404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="H132" sqref="H132"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="I130" sqref="I130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12158,7 +12165,7 @@
         <v>44070</v>
       </c>
       <c r="C127" s="37">
-        <v>56.05</v>
+        <v>56.06</v>
       </c>
       <c r="D127" s="4">
         <v>1</v>
@@ -12246,7 +12253,9 @@
       <c r="H130" s="52" t="s">
         <v>372</v>
       </c>
-      <c r="I130" s="52"/>
+      <c r="I130" s="206" t="s">
+        <v>865</v>
+      </c>
       <c r="J130" s="37"/>
     </row>
     <row r="131" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -12295,8 +12304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12449,8 +12458,8 @@
       <c r="G7" s="39">
         <v>55.04</v>
       </c>
-      <c r="H7" s="52" t="s">
-        <v>372</v>
+      <c r="H7" s="208" t="s">
+        <v>865</v>
       </c>
       <c r="I7" s="37"/>
     </row>
@@ -12578,7 +12587,9 @@
       <c r="G13" s="56">
         <v>54.55</v>
       </c>
-      <c r="H13" s="56"/>
+      <c r="H13" s="208" t="s">
+        <v>865</v>
+      </c>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
       <c r="K13" s="56"/>
@@ -14395,7 +14406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TS PP Template TU English/Baraha etc. 29/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -12304,8 +12304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12619,7 +12619,7 @@
         <v>44072</v>
       </c>
       <c r="C15" s="56">
-        <v>57.42</v>
+        <v>57.43</v>
       </c>
       <c r="D15" s="58">
         <v>1</v>
@@ -12710,7 +12710,9 @@
       <c r="G18" s="56">
         <v>56.32</v>
       </c>
-      <c r="H18" s="56"/>
+      <c r="H18" s="208" t="s">
+        <v>865</v>
+      </c>
       <c r="I18" s="56"/>
       <c r="J18" s="56"/>
       <c r="K18" s="56"/>

</xml_diff>

<commit_message>
Gana Sandhi and Templates 31/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -12304,8 +12304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12834,7 +12834,9 @@
       <c r="G23" s="56">
         <v>58.58</v>
       </c>
-      <c r="H23" s="56"/>
+      <c r="H23" s="208" t="s">
+        <v>865</v>
+      </c>
       <c r="I23" s="56"/>
       <c r="J23" s="56"/>
       <c r="K23" s="56"/>
@@ -12864,7 +12866,7 @@
         <v>389</v>
       </c>
       <c r="C25" s="56">
-        <v>59.38</v>
+        <v>59.39</v>
       </c>
       <c r="D25" s="58">
         <v>1</v>
@@ -12930,7 +12932,9 @@
       <c r="G27" s="56">
         <v>58.45</v>
       </c>
-      <c r="H27" s="56"/>
+      <c r="H27" s="208" t="s">
+        <v>865</v>
+      </c>
       <c r="I27" s="56"/>
       <c r="J27" s="56"/>
       <c r="K27" s="56"/>
@@ -12960,7 +12964,7 @@
         <v>44075</v>
       </c>
       <c r="C29" s="56">
-        <v>58.2</v>
+        <v>58.21</v>
       </c>
       <c r="D29" s="58">
         <v>1</v>
@@ -13051,10 +13055,12 @@
       <c r="G32" s="56">
         <v>57.46</v>
       </c>
-      <c r="H32" s="63" t="s">
+      <c r="H32" s="208" t="s">
+        <v>865</v>
+      </c>
+      <c r="I32" s="63" t="s">
         <v>399</v>
       </c>
-      <c r="I32" s="56"/>
       <c r="J32" s="56"/>
       <c r="K32" s="56"/>
       <c r="L32" s="56"/>

</xml_diff>

<commit_message>
Pada Paatam edits 04/01/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -12304,8 +12304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13825,7 +13825,10 @@
       <c r="G63" s="69">
         <v>54.5</v>
       </c>
-      <c r="H63" s="68" t="s">
+      <c r="H63" s="208" t="s">
+        <v>865</v>
+      </c>
+      <c r="I63" s="68" t="s">
         <v>431</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to Padam Template 06/01/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -12304,8 +12304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13737,7 +13737,7 @@
         <v>44080</v>
       </c>
       <c r="C60" s="56">
-        <v>56.02</v>
+        <v>56.03</v>
       </c>
       <c r="D60" s="58">
         <v>1</v>
@@ -13851,7 +13851,7 @@
         <v>44081</v>
       </c>
       <c r="C65" s="70">
-        <v>57.23</v>
+        <v>57.24</v>
       </c>
       <c r="D65" s="58">
         <v>1</v>
@@ -13909,7 +13909,6 @@
       <c r="G67" s="70">
         <v>53.42</v>
       </c>
-      <c r="H67" s="70"/>
       <c r="I67" s="70"/>
     </row>
     <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -13930,10 +13929,12 @@
       <c r="G68" s="70">
         <v>56.51</v>
       </c>
-      <c r="H68" s="72" t="s">
+      <c r="H68" s="208" t="s">
+        <v>865</v>
+      </c>
+      <c r="I68" s="72" t="s">
         <v>436</v>
       </c>
-      <c r="I68" s="70"/>
     </row>
     <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="70"/>
@@ -13954,7 +13955,7 @@
         <v>44082</v>
       </c>
       <c r="C70" s="70">
-        <v>57.25</v>
+        <v>57.26</v>
       </c>
       <c r="D70" s="58">
         <v>1</v>
@@ -14033,7 +14034,9 @@
       <c r="G73" s="70">
         <v>56.26</v>
       </c>
-      <c r="H73" s="70"/>
+      <c r="H73" s="208" t="s">
+        <v>865</v>
+      </c>
       <c r="I73" s="70"/>
     </row>
     <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TS Template 3.2& 3.5 and TTD 07/01/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -12304,8 +12304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14058,7 +14058,7 @@
         <v>44083</v>
       </c>
       <c r="C75" s="70">
-        <v>55.46</v>
+        <v>55.47</v>
       </c>
       <c r="D75" s="58">
         <v>1</v>
@@ -14179,7 +14179,9 @@
       <c r="G80" s="70">
         <v>55.12</v>
       </c>
-      <c r="H80" s="70"/>
+      <c r="H80" s="208" t="s">
+        <v>865</v>
+      </c>
       <c r="I80" s="70"/>
     </row>
     <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -14201,7 +14203,7 @@
         <v>44084</v>
       </c>
       <c r="C82" s="70">
-        <v>55.27</v>
+        <v>55.28</v>
       </c>
       <c r="D82" s="58">
         <v>1</v>
@@ -14215,7 +14217,9 @@
       <c r="G82" s="70">
         <v>21.12</v>
       </c>
-      <c r="H82" s="70"/>
+      <c r="H82" s="208" t="s">
+        <v>865</v>
+      </c>
       <c r="I82" s="70" t="s">
         <v>450</v>
       </c>
@@ -14224,10 +14228,7 @@
       <c r="A83" s="70"/>
       <c r="B83" s="70"/>
       <c r="C83" s="70"/>
-      <c r="D83" s="58">
-        <f>+D82+1</f>
-        <v>2</v>
-      </c>
+      <c r="D83" s="58"/>
       <c r="E83" s="70"/>
       <c r="F83" s="70"/>
       <c r="G83" s="70"/>
@@ -14238,10 +14239,7 @@
       <c r="A84" s="70"/>
       <c r="B84" s="70"/>
       <c r="C84" s="70"/>
-      <c r="D84" s="58">
-        <f>+D83+1</f>
-        <v>3</v>
-      </c>
+      <c r="D84" s="58"/>
       <c r="E84" s="70"/>
       <c r="F84" s="70"/>
       <c r="G84" s="70"/>
@@ -14252,10 +14250,7 @@
       <c r="A85" s="70"/>
       <c r="B85" s="70"/>
       <c r="C85" s="70"/>
-      <c r="D85" s="58">
-        <f>+D84+1</f>
-        <v>4</v>
-      </c>
+      <c r="D85" s="58"/>
       <c r="E85" s="70"/>
       <c r="F85" s="70"/>
       <c r="G85" s="70"/>
@@ -14266,10 +14261,7 @@
       <c r="A86" s="70"/>
       <c r="B86" s="70"/>
       <c r="C86" s="70"/>
-      <c r="D86" s="58">
-        <f>+D85+1</f>
-        <v>5</v>
-      </c>
+      <c r="D86" s="58"/>
       <c r="E86" s="70"/>
       <c r="F86" s="70"/>
       <c r="G86" s="70"/>

</xml_diff>

<commit_message>
TS 1.1 Ghanam files 04/03/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5150C9-4EA6-4E34-8D12-2538D71D28EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C208403B-D18C-4E11-9E5A-E05F4C574B39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="3075" windowWidth="15360" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
TS 4.3 PP and TTD
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54EB22C-E41D-4A87-9E96-098EEBFDD449}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9595CD59-E2CE-48A0-A17E-1FDF88DFB284}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -3066,13 +3066,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="166" x14ac:knownFonts="1">
+  <fonts count="167" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4110,79 +4116,80 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="165" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="166" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="161" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="162" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="162" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="163" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="162" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="163" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="161" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="162" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="162" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="163" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="155" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="154" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="152" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="151" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="155" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="154" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="144" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="143" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="143" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="142" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="138" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="138" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="133" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="130" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="163" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="164" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="163" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="163" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="164" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="164" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4191,17 +4198,17 @@
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="117" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="117" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="116" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="112" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="112" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4216,19 +4223,19 @@
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="162" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="163" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="163" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="164" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4245,40 +4252,40 @@
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="73" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="74" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="63" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="62" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="58" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4288,54 +4295,54 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4343,15 +4350,16 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14505,8 +14513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15361,7 +15369,7 @@
       <c r="G41" s="75">
         <v>43.52</v>
       </c>
-      <c r="H41" s="75"/>
+      <c r="H41" s="216"/>
       <c r="I41" s="75"/>
     </row>
     <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15403,7 +15411,9 @@
       <c r="G43" s="75">
         <v>55.58</v>
       </c>
-      <c r="H43" s="75"/>
+      <c r="H43" s="215" t="s">
+        <v>865</v>
+      </c>
       <c r="I43" s="75"/>
     </row>
     <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New Padam Templates 5.3,5.4
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9595CD59-E2CE-48A0-A17E-1FDF88DFB284}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9679C486-6CB6-4289-BB7E-C5472E4A6C72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="1013">
   <si>
     <t>Date</t>
   </si>
@@ -3066,13 +3066,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="167" x14ac:knownFonts="1">
+  <fonts count="169" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4116,79 +4128,81 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="166" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="168" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="162" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="163" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="164" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="165" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="163" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="165" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="162" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="164" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="163" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="165" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="157" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="155" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="154" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="157" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="152" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="155" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="146" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="144" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="143" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="141" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="141" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="136" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="130" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="164" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="166" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="164" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="164" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="166" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="166" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4196,18 +4210,18 @@
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="120" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="117" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="115" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="115" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4221,20 +4235,20 @@
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="97" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="163" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="165" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="164" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="166" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4250,41 +4264,41 @@
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="76" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="74" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="71" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="65" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="63" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="58" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4293,73 +4307,73 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14513,8 +14527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15538,7 +15552,9 @@
       <c r="H49" s="84" t="s">
         <v>499</v>
       </c>
-      <c r="I49" s="75"/>
+      <c r="I49" s="217" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="75"/>
@@ -15559,7 +15575,7 @@
         <v>44093</v>
       </c>
       <c r="C51" s="75">
-        <v>38.21</v>
+        <v>38.22</v>
       </c>
       <c r="D51" s="58">
         <v>1</v>
@@ -15617,7 +15633,9 @@
       <c r="G53" s="75">
         <v>37.42</v>
       </c>
-      <c r="H53" s="75"/>
+      <c r="H53" s="218" t="s">
+        <v>865</v>
+      </c>
       <c r="I53" s="75"/>
     </row>
     <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15697,7 +15715,9 @@
       <c r="G57" s="75">
         <v>59.12</v>
       </c>
-      <c r="H57" s="75"/>
+      <c r="H57" s="218" t="s">
+        <v>865</v>
+      </c>
       <c r="I57" s="75"/>
     </row>
     <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15885,7 +15905,9 @@
       <c r="H66" s="87" t="s">
         <v>516</v>
       </c>
-      <c r="I66" s="75"/>
+      <c r="I66" s="218" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="75"/>
@@ -17484,7 +17506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>